<commit_message>
Added more engines questions
</commit_message>
<xml_diff>
--- a/public/questions.xlsx
+++ b/public/questions.xlsx
@@ -6,14 +6,14 @@
     <sheet state="visible" name="Sheet1" sheetId="1" r:id="rId4"/>
   </sheets>
   <definedNames>
-    <definedName hidden="1" localSheetId="0" name="_xlnm._FilterDatabase">Sheet1!$A$1:$H$282</definedName>
+    <definedName hidden="1" localSheetId="0" name="_xlnm._FilterDatabase">Sheet1!$A$1:$H$303</definedName>
   </definedNames>
   <calcPr/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1662" uniqueCount="1259">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1793" uniqueCount="1361">
   <si>
     <t>Topic</t>
   </si>
@@ -3120,9 +3120,6 @@
     <t>First scheduled ground event, 10 hours</t>
   </si>
   <si>
-    <t xml:space="preserve">ground </t>
-  </si>
-  <si>
     <t>Stall recoveries SHALL be completed above</t>
   </si>
   <si>
@@ -3222,9 +3219,6 @@
     <t>As inlet air velocity increases, gross thrust ______</t>
   </si>
   <si>
-    <t xml:space="preserve">engines </t>
-  </si>
-  <si>
     <t>Which of these measurements will give the value closest to the aircrafts gross thrust?</t>
   </si>
   <si>
@@ -3790,6 +3784,318 @@
   </si>
   <si>
     <t>Starter</t>
+  </si>
+  <si>
+    <t>What is the purpose of the fuel-oil heat exchanger for the fuel system?</t>
+  </si>
+  <si>
+    <t>Preheating fuel to remove any ice crystals and increases volatility</t>
+  </si>
+  <si>
+    <t>Cooling fuel to prevent pre-ignition or detonation</t>
+  </si>
+  <si>
+    <t>Preheating fuel as required for the afterburner fuel to ignited</t>
+  </si>
+  <si>
+    <t>Preheating fuel to simply enable cooling engine lubricant without adding additional weight and components</t>
+  </si>
+  <si>
+    <t>What is the boost pump?</t>
+  </si>
+  <si>
+    <t>An electrically powered pump which ensure adequate supply of fuel from the tanks</t>
+  </si>
+  <si>
+    <t>An engine driven pump which delievers fuel from the tanks in all flight attitudes</t>
+  </si>
+  <si>
+    <t>A pneumatically powered pump which prevents aeration in the fuel by maintaining stable pressures</t>
+  </si>
+  <si>
+    <t>A hydraulically powered pump which delivers fuel to the control units and prevents aeration in the fuel which may result from rapid pressure change</t>
+  </si>
+  <si>
+    <t>What jet fuel is used aboard ships?</t>
+  </si>
+  <si>
+    <t>JP-5</t>
+  </si>
+  <si>
+    <t>JP-4</t>
+  </si>
+  <si>
+    <t>JP-8</t>
+  </si>
+  <si>
+    <t>Avgas 100LL</t>
+  </si>
+  <si>
+    <t>What color is avgas 100?</t>
+  </si>
+  <si>
+    <t>Green</t>
+  </si>
+  <si>
+    <t>Blue</t>
+  </si>
+  <si>
+    <t>Red</t>
+  </si>
+  <si>
+    <t>Green and Blue</t>
+  </si>
+  <si>
+    <t>What color is avgas 100LL?</t>
+  </si>
+  <si>
+    <t>Clear</t>
+  </si>
+  <si>
+    <t>The measurement of the ability of a fluid to evaporate is called ______. It is _____ related to flash point and _____ related to temperature</t>
+  </si>
+  <si>
+    <t>Volatility, inversely, directly</t>
+  </si>
+  <si>
+    <t>Viscosity, inversely, directly</t>
+  </si>
+  <si>
+    <t>Volatility, directly, directly</t>
+  </si>
+  <si>
+    <t>Viscosity, directly, inversely</t>
+  </si>
+  <si>
+    <t>What is the flash point of a liquid?</t>
+  </si>
+  <si>
+    <t>The lowest temperature at which the liquid would ignite with a momentary application of a flame</t>
+  </si>
+  <si>
+    <t>The lowest temperature at which the liquid would spontaneously and independently ignite</t>
+  </si>
+  <si>
+    <t>The lowest temperature at which the liquid can be sufficiently atomized for efficient combustion</t>
+  </si>
+  <si>
+    <t>The lowest temperature at which the entire liquid transitions into combustable gas.</t>
+  </si>
+  <si>
+    <t>What component controls if fuel flows into the afterburner system?</t>
+  </si>
+  <si>
+    <t>Fuel Control Unit</t>
+  </si>
+  <si>
+    <t>Engine-Driven Pump</t>
+  </si>
+  <si>
+    <t>Selector Valve</t>
+  </si>
+  <si>
+    <t>The fuel pressure gauge reports pressure measured where?</t>
+  </si>
+  <si>
+    <t>At the boost pump outlet</t>
+  </si>
+  <si>
+    <t>At the engine driven pump outlet</t>
+  </si>
+  <si>
+    <t>At the primary manifold</t>
+  </si>
+  <si>
+    <t>At the fuel control unit outlet</t>
+  </si>
+  <si>
+    <t>On engine start, the pressurizing valve is ______ and the dump valve is ______</t>
+  </si>
+  <si>
+    <t>Closed, closed</t>
+  </si>
+  <si>
+    <t>Closed, open</t>
+  </si>
+  <si>
+    <t>Open, closed</t>
+  </si>
+  <si>
+    <t>Open, open</t>
+  </si>
+  <si>
+    <t>All of these are major considerations in designing a fuel system EXCEPT</t>
+  </si>
+  <si>
+    <t>Operation at all aircraft attitudes</t>
+  </si>
+  <si>
+    <t>Complexity of the piping system</t>
+  </si>
+  <si>
+    <t>Cold weather starting</t>
+  </si>
+  <si>
+    <t>High fuel flow pressure</t>
+  </si>
+  <si>
+    <t>What component relieves pressure by bypassing oil back to the pressure pump inlet?</t>
+  </si>
+  <si>
+    <t>Pressure unloader valve</t>
+  </si>
+  <si>
+    <t>Pressure bypass valve</t>
+  </si>
+  <si>
+    <t>Temperature regulator valve</t>
+  </si>
+  <si>
+    <t>What component directs the flow of oil into the fuel-oil heat exchanger?</t>
+  </si>
+  <si>
+    <t>Temperature regulating valve</t>
+  </si>
+  <si>
+    <t>Selector valve</t>
+  </si>
+  <si>
+    <t>Fuel temperature switch</t>
+  </si>
+  <si>
+    <t>On a standard day at sea level, the breather pressurizing valve is ______</t>
+  </si>
+  <si>
+    <t>Open to the atmosphere</t>
+  </si>
+  <si>
+    <t>Entirely closed to the atmosphere</t>
+  </si>
+  <si>
+    <t>Partially closed to the atmosphere as necessary to maintain 29.92 inHg</t>
+  </si>
+  <si>
+    <t>In a state dictated by lubrication system design</t>
+  </si>
+  <si>
+    <t>_____ is the property of fluid that resists the force tending to cause the fluid to flow. It is _____ related to temperature</t>
+  </si>
+  <si>
+    <t>Viscosity, Inversely</t>
+  </si>
+  <si>
+    <t>Volatility, Inversely</t>
+  </si>
+  <si>
+    <t>Viscosity, Directly</t>
+  </si>
+  <si>
+    <t>Volatility, Directly</t>
+  </si>
+  <si>
+    <t>The fuel temperature switch activates the ______ if it detects that the ______ is too hot</t>
+  </si>
+  <si>
+    <t>Air-Oil Cooler, Fuel</t>
+  </si>
+  <si>
+    <t>Fuel-Oil Cooler, Fuel</t>
+  </si>
+  <si>
+    <t>Air-Oil Cooler, Oil</t>
+  </si>
+  <si>
+    <t>Fuel-Oil Cooler, Oil</t>
+  </si>
+  <si>
+    <t xml:space="preserve">The Magnetic-Chip detector is located after the ________ and illuminates a warning light in the cockpit when excess metal chips are detected, indicating ______. </t>
+  </si>
+  <si>
+    <t xml:space="preserve">Engine and accessory gear box, potential engine failure </t>
+  </si>
+  <si>
+    <t>Engine, extreme back pressure within the engine</t>
+  </si>
+  <si>
+    <t>Accessory gear box, malfunctioning generator</t>
+  </si>
+  <si>
+    <t>Engine and accessory gear box, potential hydraulic failure</t>
+  </si>
+  <si>
+    <t>The breather pressurizing subsystem use pressurized air from where?</t>
+  </si>
+  <si>
+    <t>Compressor bleed air</t>
+  </si>
+  <si>
+    <t>Interstage bleed air</t>
+  </si>
+  <si>
+    <t>The atmosphere</t>
+  </si>
+  <si>
+    <t>The power control system</t>
+  </si>
+  <si>
+    <t>What is interstage bleed air used for?</t>
+  </si>
+  <si>
+    <t>Only compressor stability</t>
+  </si>
+  <si>
+    <t>To drive accessory components</t>
+  </si>
+  <si>
+    <t>Life support and environmental systems</t>
+  </si>
+  <si>
+    <t>Anti-ice the engine air inlet guide vanes and parts of the aircraft air inlet duct</t>
+  </si>
+  <si>
+    <t>Where is low pressure bleed air sourced?</t>
+  </si>
+  <si>
+    <t>From between the compressor stages</t>
+  </si>
+  <si>
+    <t>From between the low pressure and high pressure spools</t>
+  </si>
+  <si>
+    <t>After the high pressure spool</t>
+  </si>
+  <si>
+    <t>Before the low pressure spool</t>
+  </si>
+  <si>
+    <t>What type of spark igniter extends the spark beyond the face of the chamber liner?</t>
+  </si>
+  <si>
+    <t>Constrained-gap</t>
+  </si>
+  <si>
+    <t>Annular-gap</t>
+  </si>
+  <si>
+    <t>High Heat-Intensity Capacitor</t>
+  </si>
+  <si>
+    <t>Air Turbine Starter</t>
+  </si>
+  <si>
+    <t>The most dangerous type of abnormal start is?</t>
+  </si>
+  <si>
+    <t>Wet Start</t>
+  </si>
+  <si>
+    <t>False Start</t>
+  </si>
+  <si>
+    <t>Hot Start</t>
+  </si>
+  <si>
+    <t>Hung Start</t>
   </si>
 </sst>
 </file>
@@ -3953,10 +4259,10 @@
         <color rgb="FF284E3F"/>
       </left>
       <right style="thin">
-        <color rgb="FFFFFFFF"/>
+        <color rgb="FFF6F8F9"/>
       </right>
       <top style="thin">
-        <color rgb="FFFFFFFF"/>
+        <color rgb="FFF6F8F9"/>
       </top>
       <bottom style="thin">
         <color rgb="FF284E3F"/>
@@ -3964,13 +4270,13 @@
     </border>
     <border>
       <left style="thin">
-        <color rgb="FFFFFFFF"/>
+        <color rgb="FFF6F8F9"/>
       </left>
       <right style="thin">
-        <color rgb="FFFFFFFF"/>
+        <color rgb="FFF6F8F9"/>
       </right>
       <top style="thin">
-        <color rgb="FFFFFFFF"/>
+        <color rgb="FFF6F8F9"/>
       </top>
       <bottom style="thin">
         <color rgb="FF284E3F"/>
@@ -3978,13 +4284,13 @@
     </border>
     <border>
       <left style="thin">
-        <color rgb="FFFFFFFF"/>
+        <color rgb="FFF6F8F9"/>
       </left>
       <right style="thin">
         <color rgb="FF284E3F"/>
       </right>
       <top style="thin">
-        <color rgb="FFFFFFFF"/>
+        <color rgb="FFF6F8F9"/>
       </top>
       <bottom style="thin">
         <color rgb="FF284E3F"/>
@@ -4049,10 +4355,10 @@
     <xf borderId="5" fillId="0" fontId="1" numFmtId="164" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1" applyNumberFormat="1">
       <alignment readingOrder="0" shrinkToFit="0" vertical="center" wrapText="0"/>
     </xf>
-    <xf borderId="5" fillId="0" fontId="1" numFmtId="9" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1" applyNumberFormat="1">
+    <xf borderId="8" fillId="0" fontId="1" numFmtId="9" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1" applyNumberFormat="1">
       <alignment readingOrder="0" shrinkToFit="0" vertical="center" wrapText="0"/>
     </xf>
-    <xf borderId="8" fillId="0" fontId="1" numFmtId="9" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1" applyNumberFormat="1">
+    <xf borderId="5" fillId="0" fontId="1" numFmtId="9" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1" applyNumberFormat="1">
       <alignment readingOrder="0" shrinkToFit="0" vertical="center" wrapText="0"/>
     </xf>
     <xf borderId="10" fillId="0" fontId="1" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
@@ -4122,8 +4428,14 @@
 </file>
 
 <file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" ref="A1:H282" displayName="Table1" name="Table1" id="1">
-  <autoFilter ref="$A$1:$H$282"/>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" ref="A1:H303" displayName="Table1" name="Table1" id="1">
+  <autoFilter ref="$A$1:$H$303">
+    <filterColumn colId="0">
+      <filters>
+        <filter val="engines"/>
+      </filters>
+    </filterColumn>
+  </autoFilter>
   <tableColumns count="8">
     <tableColumn name="Topic" id="1"/>
     <tableColumn name="Lecture" id="2"/>
@@ -4376,7 +4688,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="2">
+    <row r="2" hidden="1">
       <c r="A2" s="4" t="s">
         <v>8</v>
       </c>
@@ -4399,11 +4711,11 @@
         <v>13</v>
       </c>
       <c r="H2" s="6">
-        <f t="shared" ref="H2:H282" si="1">ROW()</f>
+        <f t="shared" ref="H2:H303" si="1">ROW()</f>
         <v>2</v>
       </c>
     </row>
-    <row r="3">
+    <row r="3" hidden="1">
       <c r="A3" s="7" t="s">
         <v>8</v>
       </c>
@@ -4430,7 +4742,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="4">
+    <row r="4" hidden="1">
       <c r="A4" s="4" t="s">
         <v>8</v>
       </c>
@@ -4457,7 +4769,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="5">
+    <row r="5" hidden="1">
       <c r="A5" s="7" t="s">
         <v>8</v>
       </c>
@@ -4484,7 +4796,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="6">
+    <row r="6" hidden="1">
       <c r="A6" s="4" t="s">
         <v>8</v>
       </c>
@@ -4511,7 +4823,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="7">
+    <row r="7" hidden="1">
       <c r="A7" s="7" t="s">
         <v>34</v>
       </c>
@@ -4538,7 +4850,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="8">
+    <row r="8" hidden="1">
       <c r="A8" s="4" t="s">
         <v>34</v>
       </c>
@@ -4565,7 +4877,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="9">
+    <row r="9" hidden="1">
       <c r="A9" s="7" t="s">
         <v>34</v>
       </c>
@@ -4592,7 +4904,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="10">
+    <row r="10" hidden="1">
       <c r="A10" s="4" t="s">
         <v>34</v>
       </c>
@@ -4619,7 +4931,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="11">
+    <row r="11" hidden="1">
       <c r="A11" s="10" t="s">
         <v>34</v>
       </c>
@@ -4646,7 +4958,7 @@
         <v>11</v>
       </c>
     </row>
-    <row r="12">
+    <row r="12" hidden="1">
       <c r="A12" s="13" t="s">
         <v>34</v>
       </c>
@@ -4673,7 +4985,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="13">
+    <row r="13" hidden="1">
       <c r="A13" s="10" t="s">
         <v>34</v>
       </c>
@@ -4700,7 +5012,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="14">
+    <row r="14" hidden="1">
       <c r="A14" s="13" t="s">
         <v>34</v>
       </c>
@@ -4727,7 +5039,7 @@
         <v>14</v>
       </c>
     </row>
-    <row r="15">
+    <row r="15" hidden="1">
       <c r="A15" s="10" t="s">
         <v>34</v>
       </c>
@@ -4754,7 +5066,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="16">
+    <row r="16" hidden="1">
       <c r="A16" s="13" t="s">
         <v>34</v>
       </c>
@@ -4781,7 +5093,7 @@
         <v>16</v>
       </c>
     </row>
-    <row r="17">
+    <row r="17" hidden="1">
       <c r="A17" s="10" t="s">
         <v>34</v>
       </c>
@@ -4808,7 +5120,7 @@
         <v>17</v>
       </c>
     </row>
-    <row r="18">
+    <row r="18" hidden="1">
       <c r="A18" s="13" t="s">
         <v>34</v>
       </c>
@@ -4835,7 +5147,7 @@
         <v>18</v>
       </c>
     </row>
-    <row r="19">
+    <row r="19" hidden="1">
       <c r="A19" s="10" t="s">
         <v>34</v>
       </c>
@@ -4862,7 +5174,7 @@
         <v>19</v>
       </c>
     </row>
-    <row r="20">
+    <row r="20" hidden="1">
       <c r="A20" s="13" t="s">
         <v>34</v>
       </c>
@@ -4889,7 +5201,7 @@
         <v>20</v>
       </c>
     </row>
-    <row r="21">
+    <row r="21" hidden="1">
       <c r="A21" s="10" t="s">
         <v>34</v>
       </c>
@@ -4916,7 +5228,7 @@
         <v>21</v>
       </c>
     </row>
-    <row r="22">
+    <row r="22" hidden="1">
       <c r="A22" s="13" t="s">
         <v>34</v>
       </c>
@@ -4943,7 +5255,7 @@
         <v>22</v>
       </c>
     </row>
-    <row r="23">
+    <row r="23" hidden="1">
       <c r="A23" s="10" t="s">
         <v>34</v>
       </c>
@@ -4970,7 +5282,7 @@
         <v>23</v>
       </c>
     </row>
-    <row r="24">
+    <row r="24" hidden="1">
       <c r="A24" s="4" t="s">
         <v>107</v>
       </c>
@@ -4997,7 +5309,7 @@
         <v>24</v>
       </c>
     </row>
-    <row r="25">
+    <row r="25" hidden="1">
       <c r="A25" s="7" t="s">
         <v>107</v>
       </c>
@@ -5024,7 +5336,7 @@
         <v>25</v>
       </c>
     </row>
-    <row r="26">
+    <row r="26" hidden="1">
       <c r="A26" s="4" t="s">
         <v>107</v>
       </c>
@@ -5051,7 +5363,7 @@
         <v>26</v>
       </c>
     </row>
-    <row r="27">
+    <row r="27" hidden="1">
       <c r="A27" s="7" t="s">
         <v>107</v>
       </c>
@@ -5078,7 +5390,7 @@
         <v>27</v>
       </c>
     </row>
-    <row r="28">
+    <row r="28" hidden="1">
       <c r="A28" s="4" t="s">
         <v>107</v>
       </c>
@@ -5105,7 +5417,7 @@
         <v>28</v>
       </c>
     </row>
-    <row r="29">
+    <row r="29" hidden="1">
       <c r="A29" s="7" t="s">
         <v>107</v>
       </c>
@@ -5132,7 +5444,7 @@
         <v>29</v>
       </c>
     </row>
-    <row r="30">
+    <row r="30" hidden="1">
       <c r="A30" s="4" t="s">
         <v>107</v>
       </c>
@@ -5159,7 +5471,7 @@
         <v>30</v>
       </c>
     </row>
-    <row r="31">
+    <row r="31" hidden="1">
       <c r="A31" s="7" t="s">
         <v>107</v>
       </c>
@@ -5186,7 +5498,7 @@
         <v>31</v>
       </c>
     </row>
-    <row r="32">
+    <row r="32" hidden="1">
       <c r="A32" s="4" t="s">
         <v>107</v>
       </c>
@@ -5213,7 +5525,7 @@
         <v>32</v>
       </c>
     </row>
-    <row r="33">
+    <row r="33" hidden="1">
       <c r="A33" s="7" t="s">
         <v>107</v>
       </c>
@@ -5240,7 +5552,7 @@
         <v>33</v>
       </c>
     </row>
-    <row r="34">
+    <row r="34" hidden="1">
       <c r="A34" s="4" t="s">
         <v>107</v>
       </c>
@@ -5267,7 +5579,7 @@
         <v>34</v>
       </c>
     </row>
-    <row r="35">
+    <row r="35" hidden="1">
       <c r="A35" s="7" t="s">
         <v>107</v>
       </c>
@@ -5294,7 +5606,7 @@
         <v>35</v>
       </c>
     </row>
-    <row r="36">
+    <row r="36" hidden="1">
       <c r="A36" s="4" t="s">
         <v>107</v>
       </c>
@@ -5321,7 +5633,7 @@
         <v>36</v>
       </c>
     </row>
-    <row r="37">
+    <row r="37" hidden="1">
       <c r="A37" s="7" t="s">
         <v>107</v>
       </c>
@@ -5348,7 +5660,7 @@
         <v>37</v>
       </c>
     </row>
-    <row r="38">
+    <row r="38" hidden="1">
       <c r="A38" s="4" t="s">
         <v>107</v>
       </c>
@@ -5375,7 +5687,7 @@
         <v>38</v>
       </c>
     </row>
-    <row r="39">
+    <row r="39" hidden="1">
       <c r="A39" s="7" t="s">
         <v>107</v>
       </c>
@@ -5402,7 +5714,7 @@
         <v>39</v>
       </c>
     </row>
-    <row r="40">
+    <row r="40" hidden="1">
       <c r="A40" s="4" t="s">
         <v>107</v>
       </c>
@@ -5429,7 +5741,7 @@
         <v>40</v>
       </c>
     </row>
-    <row r="41">
+    <row r="41" hidden="1">
       <c r="A41" s="7" t="s">
         <v>107</v>
       </c>
@@ -5456,7 +5768,7 @@
         <v>41</v>
       </c>
     </row>
-    <row r="42">
+    <row r="42" hidden="1">
       <c r="A42" s="4" t="s">
         <v>107</v>
       </c>
@@ -5483,7 +5795,7 @@
         <v>42</v>
       </c>
     </row>
-    <row r="43">
+    <row r="43" hidden="1">
       <c r="A43" s="7" t="s">
         <v>107</v>
       </c>
@@ -5510,7 +5822,7 @@
         <v>43</v>
       </c>
     </row>
-    <row r="44">
+    <row r="44" hidden="1">
       <c r="A44" s="4" t="s">
         <v>107</v>
       </c>
@@ -5537,7 +5849,7 @@
         <v>44</v>
       </c>
     </row>
-    <row r="45">
+    <row r="45" hidden="1">
       <c r="A45" s="7" t="s">
         <v>107</v>
       </c>
@@ -5564,7 +5876,7 @@
         <v>45</v>
       </c>
     </row>
-    <row r="46">
+    <row r="46" hidden="1">
       <c r="A46" s="4" t="s">
         <v>107</v>
       </c>
@@ -5591,7 +5903,7 @@
         <v>46</v>
       </c>
     </row>
-    <row r="47">
+    <row r="47" hidden="1">
       <c r="A47" s="7" t="s">
         <v>107</v>
       </c>
@@ -5618,7 +5930,7 @@
         <v>47</v>
       </c>
     </row>
-    <row r="48">
+    <row r="48" hidden="1">
       <c r="A48" s="4" t="s">
         <v>220</v>
       </c>
@@ -5642,7 +5954,7 @@
         <v>48</v>
       </c>
     </row>
-    <row r="49">
+    <row r="49" hidden="1">
       <c r="A49" s="7" t="s">
         <v>220</v>
       </c>
@@ -5666,7 +5978,7 @@
         <v>49</v>
       </c>
     </row>
-    <row r="50">
+    <row r="50" hidden="1">
       <c r="A50" s="4" t="s">
         <v>220</v>
       </c>
@@ -5690,7 +6002,7 @@
         <v>50</v>
       </c>
     </row>
-    <row r="51">
+    <row r="51" hidden="1">
       <c r="A51" s="7" t="s">
         <v>107</v>
       </c>
@@ -5717,7 +6029,7 @@
         <v>51</v>
       </c>
     </row>
-    <row r="52">
+    <row r="52" hidden="1">
       <c r="A52" s="4" t="s">
         <v>220</v>
       </c>
@@ -5741,7 +6053,7 @@
         <v>52</v>
       </c>
     </row>
-    <row r="53">
+    <row r="53" hidden="1">
       <c r="A53" s="7" t="s">
         <v>220</v>
       </c>
@@ -5765,7 +6077,7 @@
         <v>53</v>
       </c>
     </row>
-    <row r="54">
+    <row r="54" hidden="1">
       <c r="A54" s="4" t="s">
         <v>251</v>
       </c>
@@ -5789,7 +6101,7 @@
         <v>54</v>
       </c>
     </row>
-    <row r="55">
+    <row r="55" hidden="1">
       <c r="A55" s="7" t="s">
         <v>220</v>
       </c>
@@ -5813,7 +6125,7 @@
         <v>55</v>
       </c>
     </row>
-    <row r="56">
+    <row r="56" hidden="1">
       <c r="A56" s="4" t="s">
         <v>251</v>
       </c>
@@ -5837,7 +6149,7 @@
         <v>56</v>
       </c>
     </row>
-    <row r="57">
+    <row r="57" hidden="1">
       <c r="A57" s="7" t="s">
         <v>107</v>
       </c>
@@ -5864,7 +6176,7 @@
         <v>57</v>
       </c>
     </row>
-    <row r="58">
+    <row r="58" hidden="1">
       <c r="A58" s="4" t="s">
         <v>107</v>
       </c>
@@ -5891,7 +6203,7 @@
         <v>58</v>
       </c>
     </row>
-    <row r="59">
+    <row r="59" hidden="1">
       <c r="A59" s="7" t="s">
         <v>107</v>
       </c>
@@ -5918,7 +6230,7 @@
         <v>59</v>
       </c>
     </row>
-    <row r="60">
+    <row r="60" hidden="1">
       <c r="A60" s="4" t="s">
         <v>107</v>
       </c>
@@ -5945,7 +6257,7 @@
         <v>60</v>
       </c>
     </row>
-    <row r="61">
+    <row r="61" hidden="1">
       <c r="A61" s="7" t="s">
         <v>107</v>
       </c>
@@ -5972,7 +6284,7 @@
         <v>61</v>
       </c>
     </row>
-    <row r="62">
+    <row r="62" hidden="1">
       <c r="A62" s="4" t="s">
         <v>107</v>
       </c>
@@ -5999,7 +6311,7 @@
         <v>62</v>
       </c>
     </row>
-    <row r="63">
+    <row r="63" hidden="1">
       <c r="A63" s="7" t="s">
         <v>107</v>
       </c>
@@ -6026,7 +6338,7 @@
         <v>63</v>
       </c>
     </row>
-    <row r="64">
+    <row r="64" hidden="1">
       <c r="A64" s="4" t="s">
         <v>107</v>
       </c>
@@ -6053,7 +6365,7 @@
         <v>64</v>
       </c>
     </row>
-    <row r="65">
+    <row r="65" hidden="1">
       <c r="A65" s="7" t="s">
         <v>107</v>
       </c>
@@ -6080,7 +6392,7 @@
         <v>65</v>
       </c>
     </row>
-    <row r="66">
+    <row r="66" hidden="1">
       <c r="A66" s="4" t="s">
         <v>107</v>
       </c>
@@ -6107,7 +6419,7 @@
         <v>66</v>
       </c>
     </row>
-    <row r="67">
+    <row r="67" hidden="1">
       <c r="A67" s="7" t="s">
         <v>107</v>
       </c>
@@ -6134,7 +6446,7 @@
         <v>67</v>
       </c>
     </row>
-    <row r="68">
+    <row r="68" hidden="1">
       <c r="A68" s="4" t="s">
         <v>220</v>
       </c>
@@ -6158,7 +6470,7 @@
         <v>68</v>
       </c>
     </row>
-    <row r="69">
+    <row r="69" hidden="1">
       <c r="A69" s="7" t="s">
         <v>220</v>
       </c>
@@ -6182,7 +6494,7 @@
         <v>69</v>
       </c>
     </row>
-    <row r="70">
+    <row r="70" hidden="1">
       <c r="A70" s="4" t="s">
         <v>220</v>
       </c>
@@ -6206,7 +6518,7 @@
         <v>70</v>
       </c>
     </row>
-    <row r="71">
+    <row r="71" hidden="1">
       <c r="A71" s="7" t="s">
         <v>220</v>
       </c>
@@ -6230,7 +6542,7 @@
         <v>71</v>
       </c>
     </row>
-    <row r="72">
+    <row r="72" hidden="1">
       <c r="A72" s="4" t="s">
         <v>220</v>
       </c>
@@ -6254,7 +6566,7 @@
         <v>72</v>
       </c>
     </row>
-    <row r="73">
+    <row r="73" hidden="1">
       <c r="A73" s="7" t="s">
         <v>107</v>
       </c>
@@ -6281,7 +6593,7 @@
         <v>73</v>
       </c>
     </row>
-    <row r="74">
+    <row r="74" hidden="1">
       <c r="A74" s="4" t="s">
         <v>107</v>
       </c>
@@ -6308,7 +6620,7 @@
         <v>74</v>
       </c>
     </row>
-    <row r="75">
+    <row r="75" hidden="1">
       <c r="A75" s="7" t="s">
         <v>107</v>
       </c>
@@ -6335,7 +6647,7 @@
         <v>75</v>
       </c>
     </row>
-    <row r="76">
+    <row r="76" hidden="1">
       <c r="A76" s="4" t="s">
         <v>107</v>
       </c>
@@ -6362,7 +6674,7 @@
         <v>76</v>
       </c>
     </row>
-    <row r="77">
+    <row r="77" hidden="1">
       <c r="A77" s="7" t="s">
         <v>107</v>
       </c>
@@ -6389,7 +6701,7 @@
         <v>77</v>
       </c>
     </row>
-    <row r="78">
+    <row r="78" hidden="1">
       <c r="A78" s="4" t="s">
         <v>107</v>
       </c>
@@ -6416,7 +6728,7 @@
         <v>78</v>
       </c>
     </row>
-    <row r="79">
+    <row r="79" hidden="1">
       <c r="A79" s="7" t="s">
         <v>8</v>
       </c>
@@ -6443,7 +6755,7 @@
         <v>79</v>
       </c>
     </row>
-    <row r="80">
+    <row r="80" hidden="1">
       <c r="A80" s="4" t="s">
         <v>107</v>
       </c>
@@ -6470,7 +6782,7 @@
         <v>80</v>
       </c>
     </row>
-    <row r="81">
+    <row r="81" hidden="1">
       <c r="A81" s="7" t="s">
         <v>107</v>
       </c>
@@ -6497,7 +6809,7 @@
         <v>81</v>
       </c>
     </row>
-    <row r="82">
+    <row r="82" hidden="1">
       <c r="A82" s="4" t="s">
         <v>107</v>
       </c>
@@ -6524,7 +6836,7 @@
         <v>82</v>
       </c>
     </row>
-    <row r="83">
+    <row r="83" hidden="1">
       <c r="A83" s="7" t="s">
         <v>220</v>
       </c>
@@ -6548,7 +6860,7 @@
         <v>83</v>
       </c>
     </row>
-    <row r="84">
+    <row r="84" hidden="1">
       <c r="A84" s="4" t="s">
         <v>220</v>
       </c>
@@ -6572,7 +6884,7 @@
         <v>84</v>
       </c>
     </row>
-    <row r="85">
+    <row r="85" hidden="1">
       <c r="A85" s="7" t="s">
         <v>220</v>
       </c>
@@ -6596,7 +6908,7 @@
         <v>85</v>
       </c>
     </row>
-    <row r="86">
+    <row r="86" hidden="1">
       <c r="A86" s="4" t="s">
         <v>220</v>
       </c>
@@ -6620,7 +6932,7 @@
         <v>86</v>
       </c>
     </row>
-    <row r="87">
+    <row r="87" hidden="1">
       <c r="A87" s="7" t="s">
         <v>220</v>
       </c>
@@ -6644,7 +6956,7 @@
         <v>87</v>
       </c>
     </row>
-    <row r="88">
+    <row r="88" hidden="1">
       <c r="A88" s="4" t="s">
         <v>220</v>
       </c>
@@ -6668,7 +6980,7 @@
         <v>88</v>
       </c>
     </row>
-    <row r="89">
+    <row r="89" hidden="1">
       <c r="A89" s="7" t="s">
         <v>220</v>
       </c>
@@ -6692,7 +7004,7 @@
         <v>89</v>
       </c>
     </row>
-    <row r="90">
+    <row r="90" hidden="1">
       <c r="A90" s="4" t="s">
         <v>220</v>
       </c>
@@ -6716,7 +7028,7 @@
         <v>90</v>
       </c>
     </row>
-    <row r="91">
+    <row r="91" hidden="1">
       <c r="A91" s="7" t="s">
         <v>220</v>
       </c>
@@ -6740,7 +7052,7 @@
         <v>91</v>
       </c>
     </row>
-    <row r="92">
+    <row r="92" hidden="1">
       <c r="A92" s="4" t="s">
         <v>220</v>
       </c>
@@ -6764,7 +7076,7 @@
         <v>92</v>
       </c>
     </row>
-    <row r="93">
+    <row r="93" hidden="1">
       <c r="A93" s="7" t="s">
         <v>220</v>
       </c>
@@ -6788,7 +7100,7 @@
         <v>93</v>
       </c>
     </row>
-    <row r="94">
+    <row r="94" hidden="1">
       <c r="A94" s="4" t="s">
         <v>220</v>
       </c>
@@ -6812,7 +7124,7 @@
         <v>94</v>
       </c>
     </row>
-    <row r="95">
+    <row r="95" hidden="1">
       <c r="A95" s="7" t="s">
         <v>220</v>
       </c>
@@ -6836,7 +7148,7 @@
         <v>95</v>
       </c>
     </row>
-    <row r="96">
+    <row r="96" hidden="1">
       <c r="A96" s="4" t="s">
         <v>220</v>
       </c>
@@ -6860,7 +7172,7 @@
         <v>96</v>
       </c>
     </row>
-    <row r="97">
+    <row r="97" hidden="1">
       <c r="A97" s="7" t="s">
         <v>220</v>
       </c>
@@ -6884,7 +7196,7 @@
         <v>97</v>
       </c>
     </row>
-    <row r="98">
+    <row r="98" hidden="1">
       <c r="A98" s="4" t="s">
         <v>220</v>
       </c>
@@ -6908,7 +7220,7 @@
         <v>98</v>
       </c>
     </row>
-    <row r="99">
+    <row r="99" hidden="1">
       <c r="A99" s="7" t="s">
         <v>220</v>
       </c>
@@ -6932,7 +7244,7 @@
         <v>99</v>
       </c>
     </row>
-    <row r="100">
+    <row r="100" hidden="1">
       <c r="A100" s="4" t="s">
         <v>220</v>
       </c>
@@ -6956,7 +7268,7 @@
         <v>100</v>
       </c>
     </row>
-    <row r="101">
+    <row r="101" hidden="1">
       <c r="A101" s="7" t="s">
         <v>220</v>
       </c>
@@ -6980,7 +7292,7 @@
         <v>101</v>
       </c>
     </row>
-    <row r="102">
+    <row r="102" hidden="1">
       <c r="A102" s="4" t="s">
         <v>220</v>
       </c>
@@ -7004,7 +7316,7 @@
         <v>102</v>
       </c>
     </row>
-    <row r="103">
+    <row r="103" hidden="1">
       <c r="A103" s="7" t="s">
         <v>220</v>
       </c>
@@ -7028,7 +7340,7 @@
         <v>103</v>
       </c>
     </row>
-    <row r="104">
+    <row r="104" hidden="1">
       <c r="A104" s="4" t="s">
         <v>220</v>
       </c>
@@ -7052,7 +7364,7 @@
         <v>104</v>
       </c>
     </row>
-    <row r="105">
+    <row r="105" hidden="1">
       <c r="A105" s="7" t="s">
         <v>220</v>
       </c>
@@ -7616,7 +7928,7 @@
         <v>125</v>
       </c>
     </row>
-    <row r="126">
+    <row r="126" hidden="1">
       <c r="A126" s="13" t="s">
         <v>107</v>
       </c>
@@ -7643,7 +7955,7 @@
         <v>126</v>
       </c>
     </row>
-    <row r="127">
+    <row r="127" hidden="1">
       <c r="A127" s="10" t="s">
         <v>107</v>
       </c>
@@ -7670,7 +7982,7 @@
         <v>127</v>
       </c>
     </row>
-    <row r="128">
+    <row r="128" hidden="1">
       <c r="A128" s="13" t="s">
         <v>107</v>
       </c>
@@ -7697,7 +8009,7 @@
         <v>128</v>
       </c>
     </row>
-    <row r="129">
+    <row r="129" hidden="1">
       <c r="A129" s="10" t="s">
         <v>107</v>
       </c>
@@ -7724,7 +8036,7 @@
         <v>129</v>
       </c>
     </row>
-    <row r="130">
+    <row r="130" hidden="1">
       <c r="A130" s="13" t="s">
         <v>107</v>
       </c>
@@ -7751,7 +8063,7 @@
         <v>130</v>
       </c>
     </row>
-    <row r="131">
+    <row r="131" hidden="1">
       <c r="A131" s="10" t="s">
         <v>107</v>
       </c>
@@ -7778,7 +8090,7 @@
         <v>131</v>
       </c>
     </row>
-    <row r="132">
+    <row r="132" hidden="1">
       <c r="A132" s="13" t="s">
         <v>107</v>
       </c>
@@ -7805,7 +8117,7 @@
         <v>132</v>
       </c>
     </row>
-    <row r="133">
+    <row r="133" hidden="1">
       <c r="A133" s="10" t="s">
         <v>107</v>
       </c>
@@ -7832,7 +8144,7 @@
         <v>133</v>
       </c>
     </row>
-    <row r="134">
+    <row r="134" hidden="1">
       <c r="A134" s="13" t="s">
         <v>107</v>
       </c>
@@ -7859,7 +8171,7 @@
         <v>134</v>
       </c>
     </row>
-    <row r="135">
+    <row r="135" hidden="1">
       <c r="A135" s="10" t="s">
         <v>107</v>
       </c>
@@ -7886,7 +8198,7 @@
         <v>135</v>
       </c>
     </row>
-    <row r="136">
+    <row r="136" hidden="1">
       <c r="A136" s="13" t="s">
         <v>107</v>
       </c>
@@ -7913,7 +8225,7 @@
         <v>136</v>
       </c>
     </row>
-    <row r="137">
+    <row r="137" hidden="1">
       <c r="A137" s="10" t="s">
         <v>107</v>
       </c>
@@ -7940,7 +8252,7 @@
         <v>137</v>
       </c>
     </row>
-    <row r="138">
+    <row r="138" hidden="1">
       <c r="A138" s="13" t="s">
         <v>107</v>
       </c>
@@ -7967,7 +8279,7 @@
         <v>138</v>
       </c>
     </row>
-    <row r="139">
+    <row r="139" hidden="1">
       <c r="A139" s="10" t="s">
         <v>107</v>
       </c>
@@ -7994,7 +8306,7 @@
         <v>139</v>
       </c>
     </row>
-    <row r="140">
+    <row r="140" hidden="1">
       <c r="A140" s="13" t="s">
         <v>107</v>
       </c>
@@ -8021,7 +8333,7 @@
         <v>140</v>
       </c>
     </row>
-    <row r="141">
+    <row r="141" hidden="1">
       <c r="A141" s="10" t="s">
         <v>107</v>
       </c>
@@ -8048,7 +8360,7 @@
         <v>141</v>
       </c>
     </row>
-    <row r="142">
+    <row r="142" hidden="1">
       <c r="A142" s="13" t="s">
         <v>107</v>
       </c>
@@ -8075,7 +8387,7 @@
         <v>142</v>
       </c>
     </row>
-    <row r="143">
+    <row r="143" hidden="1">
       <c r="A143" s="10" t="s">
         <v>107</v>
       </c>
@@ -8102,7 +8414,7 @@
         <v>143</v>
       </c>
     </row>
-    <row r="144">
+    <row r="144" hidden="1">
       <c r="A144" s="13" t="s">
         <v>107</v>
       </c>
@@ -8129,7 +8441,7 @@
         <v>144</v>
       </c>
     </row>
-    <row r="145">
+    <row r="145" hidden="1">
       <c r="A145" s="10" t="s">
         <v>107</v>
       </c>
@@ -8156,7 +8468,7 @@
         <v>145</v>
       </c>
     </row>
-    <row r="146">
+    <row r="146" hidden="1">
       <c r="A146" s="13" t="s">
         <v>107</v>
       </c>
@@ -8183,7 +8495,7 @@
         <v>146</v>
       </c>
     </row>
-    <row r="147">
+    <row r="147" hidden="1">
       <c r="A147" s="10" t="s">
         <v>107</v>
       </c>
@@ -8210,7 +8522,7 @@
         <v>147</v>
       </c>
     </row>
-    <row r="148">
+    <row r="148" hidden="1">
       <c r="A148" s="13" t="s">
         <v>107</v>
       </c>
@@ -8237,7 +8549,7 @@
         <v>148</v>
       </c>
     </row>
-    <row r="149">
+    <row r="149" hidden="1">
       <c r="A149" s="10" t="s">
         <v>107</v>
       </c>
@@ -8264,7 +8576,7 @@
         <v>149</v>
       </c>
     </row>
-    <row r="150">
+    <row r="150" hidden="1">
       <c r="A150" s="13" t="s">
         <v>107</v>
       </c>
@@ -8291,7 +8603,7 @@
         <v>150</v>
       </c>
     </row>
-    <row r="151">
+    <row r="151" hidden="1">
       <c r="A151" s="10" t="s">
         <v>107</v>
       </c>
@@ -8318,7 +8630,7 @@
         <v>151</v>
       </c>
     </row>
-    <row r="152">
+    <row r="152" hidden="1">
       <c r="A152" s="13" t="s">
         <v>107</v>
       </c>
@@ -8345,7 +8657,7 @@
         <v>152</v>
       </c>
     </row>
-    <row r="153">
+    <row r="153" hidden="1">
       <c r="A153" s="10" t="s">
         <v>107</v>
       </c>
@@ -8372,7 +8684,7 @@
         <v>153</v>
       </c>
     </row>
-    <row r="154">
+    <row r="154" hidden="1">
       <c r="A154" s="13" t="s">
         <v>107</v>
       </c>
@@ -8399,7 +8711,7 @@
         <v>154</v>
       </c>
     </row>
-    <row r="155">
+    <row r="155" hidden="1">
       <c r="A155" s="10" t="s">
         <v>107</v>
       </c>
@@ -8426,7 +8738,7 @@
         <v>155</v>
       </c>
     </row>
-    <row r="156">
+    <row r="156" hidden="1">
       <c r="A156" s="13" t="s">
         <v>107</v>
       </c>
@@ -8453,7 +8765,7 @@
         <v>156</v>
       </c>
     </row>
-    <row r="157">
+    <row r="157" hidden="1">
       <c r="A157" s="7" t="s">
         <v>107</v>
       </c>
@@ -8480,7 +8792,7 @@
         <v>157</v>
       </c>
     </row>
-    <row r="158">
+    <row r="158" hidden="1">
       <c r="A158" s="13" t="s">
         <v>107</v>
       </c>
@@ -8507,7 +8819,7 @@
         <v>158</v>
       </c>
     </row>
-    <row r="159">
+    <row r="159" hidden="1">
       <c r="A159" s="10" t="s">
         <v>107</v>
       </c>
@@ -8534,7 +8846,7 @@
         <v>159</v>
       </c>
     </row>
-    <row r="160">
+    <row r="160" hidden="1">
       <c r="A160" s="13" t="s">
         <v>107</v>
       </c>
@@ -8561,7 +8873,7 @@
         <v>160</v>
       </c>
     </row>
-    <row r="161">
+    <row r="161" hidden="1">
       <c r="A161" s="10" t="s">
         <v>107</v>
       </c>
@@ -8588,7 +8900,7 @@
         <v>161</v>
       </c>
     </row>
-    <row r="162">
+    <row r="162" hidden="1">
       <c r="A162" s="13" t="s">
         <v>34</v>
       </c>
@@ -8615,7 +8927,7 @@
         <v>162</v>
       </c>
     </row>
-    <row r="163">
+    <row r="163" hidden="1">
       <c r="A163" s="10" t="s">
         <v>34</v>
       </c>
@@ -8642,7 +8954,7 @@
         <v>163</v>
       </c>
     </row>
-    <row r="164">
+    <row r="164" hidden="1">
       <c r="A164" s="13" t="s">
         <v>34</v>
       </c>
@@ -8669,7 +8981,7 @@
         <v>164</v>
       </c>
     </row>
-    <row r="165">
+    <row r="165" hidden="1">
       <c r="A165" s="10" t="s">
         <v>34</v>
       </c>
@@ -8696,7 +9008,7 @@
         <v>165</v>
       </c>
     </row>
-    <row r="166">
+    <row r="166" hidden="1">
       <c r="A166" s="13" t="s">
         <v>34</v>
       </c>
@@ -8723,7 +9035,7 @@
         <v>166</v>
       </c>
     </row>
-    <row r="167">
+    <row r="167" hidden="1">
       <c r="A167" s="10" t="s">
         <v>34</v>
       </c>
@@ -8750,7 +9062,7 @@
         <v>167</v>
       </c>
     </row>
-    <row r="168">
+    <row r="168" hidden="1">
       <c r="A168" s="13" t="s">
         <v>34</v>
       </c>
@@ -8777,7 +9089,7 @@
         <v>168</v>
       </c>
     </row>
-    <row r="169">
+    <row r="169" hidden="1">
       <c r="A169" s="10" t="s">
         <v>34</v>
       </c>
@@ -8804,7 +9116,7 @@
         <v>169</v>
       </c>
     </row>
-    <row r="170">
+    <row r="170" hidden="1">
       <c r="A170" s="13" t="s">
         <v>34</v>
       </c>
@@ -8831,7 +9143,7 @@
         <v>170</v>
       </c>
     </row>
-    <row r="171">
+    <row r="171" hidden="1">
       <c r="A171" s="10" t="s">
         <v>34</v>
       </c>
@@ -8858,7 +9170,7 @@
         <v>171</v>
       </c>
     </row>
-    <row r="172">
+    <row r="172" hidden="1">
       <c r="A172" s="13" t="s">
         <v>34</v>
       </c>
@@ -8885,7 +9197,7 @@
         <v>172</v>
       </c>
     </row>
-    <row r="173">
+    <row r="173" hidden="1">
       <c r="A173" s="10" t="s">
         <v>34</v>
       </c>
@@ -8912,7 +9224,7 @@
         <v>173</v>
       </c>
     </row>
-    <row r="174">
+    <row r="174" hidden="1">
       <c r="A174" s="13" t="s">
         <v>34</v>
       </c>
@@ -8939,7 +9251,7 @@
         <v>174</v>
       </c>
     </row>
-    <row r="175">
+    <row r="175" hidden="1">
       <c r="A175" s="10" t="s">
         <v>34</v>
       </c>
@@ -8966,7 +9278,7 @@
         <v>175</v>
       </c>
     </row>
-    <row r="176">
+    <row r="176" hidden="1">
       <c r="A176" s="13" t="s">
         <v>34</v>
       </c>
@@ -8993,7 +9305,7 @@
         <v>176</v>
       </c>
     </row>
-    <row r="177">
+    <row r="177" hidden="1">
       <c r="A177" s="10" t="s">
         <v>34</v>
       </c>
@@ -9020,7 +9332,7 @@
         <v>177</v>
       </c>
     </row>
-    <row r="178">
+    <row r="178" hidden="1">
       <c r="A178" s="13" t="s">
         <v>812</v>
       </c>
@@ -9047,7 +9359,7 @@
         <v>178</v>
       </c>
     </row>
-    <row r="179">
+    <row r="179" hidden="1">
       <c r="A179" s="10" t="s">
         <v>34</v>
       </c>
@@ -9074,7 +9386,7 @@
         <v>179</v>
       </c>
     </row>
-    <row r="180">
+    <row r="180" hidden="1">
       <c r="A180" s="4" t="s">
         <v>34</v>
       </c>
@@ -9101,7 +9413,7 @@
         <v>180</v>
       </c>
     </row>
-    <row r="181">
+    <row r="181" hidden="1">
       <c r="A181" s="7" t="s">
         <v>34</v>
       </c>
@@ -9128,7 +9440,7 @@
         <v>181</v>
       </c>
     </row>
-    <row r="182">
+    <row r="182" hidden="1">
       <c r="A182" s="4" t="s">
         <v>34</v>
       </c>
@@ -9155,7 +9467,7 @@
         <v>182</v>
       </c>
     </row>
-    <row r="183">
+    <row r="183" hidden="1">
       <c r="A183" s="7" t="s">
         <v>34</v>
       </c>
@@ -9182,7 +9494,7 @@
         <v>183</v>
       </c>
     </row>
-    <row r="184">
+    <row r="184" hidden="1">
       <c r="A184" s="4" t="s">
         <v>34</v>
       </c>
@@ -9209,7 +9521,7 @@
         <v>184</v>
       </c>
     </row>
-    <row r="185">
+    <row r="185" hidden="1">
       <c r="A185" s="7" t="s">
         <v>34</v>
       </c>
@@ -9236,7 +9548,7 @@
         <v>185</v>
       </c>
     </row>
-    <row r="186">
+    <row r="186" hidden="1">
       <c r="A186" s="4" t="s">
         <v>34</v>
       </c>
@@ -9263,7 +9575,7 @@
         <v>186</v>
       </c>
     </row>
-    <row r="187">
+    <row r="187" hidden="1">
       <c r="A187" s="10" t="s">
         <v>34</v>
       </c>
@@ -9290,7 +9602,7 @@
         <v>187</v>
       </c>
     </row>
-    <row r="188">
+    <row r="188" hidden="1">
       <c r="A188" s="13" t="s">
         <v>34</v>
       </c>
@@ -9317,7 +9629,7 @@
         <v>188</v>
       </c>
     </row>
-    <row r="189">
+    <row r="189" hidden="1">
       <c r="A189" s="10" t="s">
         <v>34</v>
       </c>
@@ -9344,7 +9656,7 @@
         <v>189</v>
       </c>
     </row>
-    <row r="190">
+    <row r="190" hidden="1">
       <c r="A190" s="13" t="s">
         <v>34</v>
       </c>
@@ -9371,7 +9683,7 @@
         <v>190</v>
       </c>
     </row>
-    <row r="191">
+    <row r="191" hidden="1">
       <c r="A191" s="10" t="s">
         <v>34</v>
       </c>
@@ -9398,7 +9710,7 @@
         <v>191</v>
       </c>
     </row>
-    <row r="192">
+    <row r="192" hidden="1">
       <c r="A192" s="4" t="s">
         <v>34</v>
       </c>
@@ -9425,7 +9737,7 @@
         <v>192</v>
       </c>
     </row>
-    <row r="193">
+    <row r="193" hidden="1">
       <c r="A193" s="7" t="s">
         <v>34</v>
       </c>
@@ -9452,7 +9764,7 @@
         <v>193</v>
       </c>
     </row>
-    <row r="194">
+    <row r="194" hidden="1">
       <c r="A194" s="4" t="s">
         <v>34</v>
       </c>
@@ -9479,7 +9791,7 @@
         <v>194</v>
       </c>
     </row>
-    <row r="195">
+    <row r="195" hidden="1">
       <c r="A195" s="7" t="s">
         <v>34</v>
       </c>
@@ -9506,7 +9818,7 @@
         <v>195</v>
       </c>
     </row>
-    <row r="196">
+    <row r="196" hidden="1">
       <c r="A196" s="4" t="s">
         <v>34</v>
       </c>
@@ -9533,7 +9845,7 @@
         <v>196</v>
       </c>
     </row>
-    <row r="197">
+    <row r="197" hidden="1">
       <c r="A197" s="7" t="s">
         <v>34</v>
       </c>
@@ -9560,7 +9872,7 @@
         <v>197</v>
       </c>
     </row>
-    <row r="198">
+    <row r="198" hidden="1">
       <c r="A198" s="4" t="s">
         <v>34</v>
       </c>
@@ -9587,7 +9899,7 @@
         <v>198</v>
       </c>
     </row>
-    <row r="199">
+    <row r="199" hidden="1">
       <c r="A199" s="10" t="s">
         <v>34</v>
       </c>
@@ -9614,7 +9926,7 @@
         <v>199</v>
       </c>
     </row>
-    <row r="200">
+    <row r="200" hidden="1">
       <c r="A200" s="13" t="s">
         <v>34</v>
       </c>
@@ -9641,7 +9953,7 @@
         <v>200</v>
       </c>
     </row>
-    <row r="201">
+    <row r="201" hidden="1">
       <c r="A201" s="10" t="s">
         <v>34</v>
       </c>
@@ -9668,7 +9980,7 @@
         <v>201</v>
       </c>
     </row>
-    <row r="202">
+    <row r="202" hidden="1">
       <c r="A202" s="13" t="s">
         <v>34</v>
       </c>
@@ -9695,7 +10007,7 @@
         <v>202</v>
       </c>
     </row>
-    <row r="203">
+    <row r="203" hidden="1">
       <c r="A203" s="10" t="s">
         <v>34</v>
       </c>
@@ -9722,7 +10034,7 @@
         <v>203</v>
       </c>
     </row>
-    <row r="204">
+    <row r="204" hidden="1">
       <c r="A204" s="13" t="s">
         <v>34</v>
       </c>
@@ -9749,7 +10061,7 @@
         <v>204</v>
       </c>
     </row>
-    <row r="205">
+    <row r="205" hidden="1">
       <c r="A205" s="10" t="s">
         <v>34</v>
       </c>
@@ -9776,7 +10088,7 @@
         <v>205</v>
       </c>
     </row>
-    <row r="206">
+    <row r="206" hidden="1">
       <c r="A206" s="13" t="s">
         <v>34</v>
       </c>
@@ -9803,7 +10115,7 @@
         <v>206</v>
       </c>
     </row>
-    <row r="207">
+    <row r="207" hidden="1">
       <c r="A207" s="10" t="s">
         <v>34</v>
       </c>
@@ -9830,7 +10142,7 @@
         <v>207</v>
       </c>
     </row>
-    <row r="208">
+    <row r="208" hidden="1">
       <c r="A208" s="13" t="s">
         <v>34</v>
       </c>
@@ -9857,7 +10169,7 @@
         <v>208</v>
       </c>
     </row>
-    <row r="209">
+    <row r="209" hidden="1">
       <c r="A209" s="10" t="s">
         <v>34</v>
       </c>
@@ -9884,7 +10196,7 @@
         <v>209</v>
       </c>
     </row>
-    <row r="210">
+    <row r="210" hidden="1">
       <c r="A210" s="13" t="s">
         <v>34</v>
       </c>
@@ -9911,7 +10223,7 @@
         <v>210</v>
       </c>
     </row>
-    <row r="211">
+    <row r="211" hidden="1">
       <c r="A211" s="10" t="s">
         <v>34</v>
       </c>
@@ -9938,7 +10250,7 @@
         <v>211</v>
       </c>
     </row>
-    <row r="212">
+    <row r="212" hidden="1">
       <c r="A212" s="13" t="s">
         <v>34</v>
       </c>
@@ -9965,7 +10277,7 @@
         <v>212</v>
       </c>
     </row>
-    <row r="213">
+    <row r="213" hidden="1">
       <c r="A213" s="10" t="s">
         <v>34</v>
       </c>
@@ -9992,7 +10304,7 @@
         <v>213</v>
       </c>
     </row>
-    <row r="214">
+    <row r="214" hidden="1">
       <c r="A214" s="13" t="s">
         <v>34</v>
       </c>
@@ -10019,7 +10331,7 @@
         <v>214</v>
       </c>
     </row>
-    <row r="215">
+    <row r="215" hidden="1">
       <c r="A215" s="10" t="s">
         <v>34</v>
       </c>
@@ -10046,7 +10358,7 @@
         <v>215</v>
       </c>
     </row>
-    <row r="216">
+    <row r="216" hidden="1">
       <c r="A216" s="13" t="s">
         <v>34</v>
       </c>
@@ -10073,7 +10385,7 @@
         <v>216</v>
       </c>
     </row>
-    <row r="217">
+    <row r="217" hidden="1">
       <c r="A217" s="10" t="s">
         <v>34</v>
       </c>
@@ -10100,7 +10412,7 @@
         <v>217</v>
       </c>
     </row>
-    <row r="218">
+    <row r="218" hidden="1">
       <c r="A218" s="13" t="s">
         <v>34</v>
       </c>
@@ -10127,7 +10439,7 @@
         <v>218</v>
       </c>
     </row>
-    <row r="219">
+    <row r="219" hidden="1">
       <c r="A219" s="10" t="s">
         <v>34</v>
       </c>
@@ -10154,7 +10466,7 @@
         <v>219</v>
       </c>
     </row>
-    <row r="220">
+    <row r="220" hidden="1">
       <c r="A220" s="13" t="s">
         <v>34</v>
       </c>
@@ -10181,7 +10493,7 @@
         <v>220</v>
       </c>
     </row>
-    <row r="221">
+    <row r="221" hidden="1">
       <c r="A221" s="10" t="s">
         <v>34</v>
       </c>
@@ -10208,7 +10520,7 @@
         <v>221</v>
       </c>
     </row>
-    <row r="222">
+    <row r="222" hidden="1">
       <c r="A222" s="13" t="s">
         <v>34</v>
       </c>
@@ -10235,7 +10547,7 @@
         <v>222</v>
       </c>
     </row>
-    <row r="223">
+    <row r="223" hidden="1">
       <c r="A223" s="10" t="s">
         <v>34</v>
       </c>
@@ -10262,7 +10574,7 @@
         <v>223</v>
       </c>
     </row>
-    <row r="224">
+    <row r="224" hidden="1">
       <c r="A224" s="13" t="s">
         <v>34</v>
       </c>
@@ -10289,7 +10601,7 @@
         <v>224</v>
       </c>
     </row>
-    <row r="225">
+    <row r="225" hidden="1">
       <c r="A225" s="10" t="s">
         <v>34</v>
       </c>
@@ -10316,7 +10628,7 @@
         <v>225</v>
       </c>
     </row>
-    <row r="226">
+    <row r="226" hidden="1">
       <c r="A226" s="13" t="s">
         <v>34</v>
       </c>
@@ -10343,7 +10655,7 @@
         <v>226</v>
       </c>
     </row>
-    <row r="227">
+    <row r="227" hidden="1">
       <c r="A227" s="10" t="s">
         <v>34</v>
       </c>
@@ -10370,7 +10682,7 @@
         <v>227</v>
       </c>
     </row>
-    <row r="228">
+    <row r="228" hidden="1">
       <c r="A228" s="13" t="s">
         <v>34</v>
       </c>
@@ -10397,7 +10709,7 @@
         <v>228</v>
       </c>
     </row>
-    <row r="229">
+    <row r="229" hidden="1">
       <c r="A229" s="10" t="s">
         <v>251</v>
       </c>
@@ -10424,15 +10736,15 @@
         <v>229</v>
       </c>
     </row>
-    <row r="230">
+    <row r="230" hidden="1">
       <c r="A230" s="13" t="s">
-        <v>1035</v>
+        <v>251</v>
       </c>
       <c r="B230" s="14">
         <v>1.0</v>
       </c>
       <c r="C230" s="14" t="s">
-        <v>1036</v>
+        <v>1035</v>
       </c>
       <c r="D230" s="14" t="s">
         <v>208</v>
@@ -10444,14 +10756,14 @@
         <v>209</v>
       </c>
       <c r="G230" s="14" t="s">
-        <v>1037</v>
+        <v>1036</v>
       </c>
       <c r="H230" s="15">
         <f t="shared" si="1"/>
         <v>230</v>
       </c>
     </row>
-    <row r="231">
+    <row r="231" hidden="1">
       <c r="A231" s="10" t="s">
         <v>251</v>
       </c>
@@ -10459,26 +10771,26 @@
         <v>1.0</v>
       </c>
       <c r="C231" s="11" t="s">
+        <v>1037</v>
+      </c>
+      <c r="D231" s="11" t="s">
         <v>1038</v>
       </c>
-      <c r="D231" s="11" t="s">
+      <c r="E231" s="11" t="s">
         <v>1039</v>
       </c>
-      <c r="E231" s="11" t="s">
+      <c r="F231" s="11" t="s">
         <v>1040</v>
       </c>
-      <c r="F231" s="11" t="s">
+      <c r="G231" s="11" t="s">
         <v>1041</v>
       </c>
-      <c r="G231" s="11" t="s">
-        <v>1042</v>
-      </c>
       <c r="H231" s="12">
         <f t="shared" si="1"/>
         <v>231</v>
       </c>
     </row>
-    <row r="232">
+    <row r="232" hidden="1">
       <c r="A232" s="13" t="s">
         <v>251</v>
       </c>
@@ -10486,26 +10798,26 @@
         <v>1.0</v>
       </c>
       <c r="C232" s="14" t="s">
+        <v>1042</v>
+      </c>
+      <c r="D232" s="14" t="s">
         <v>1043</v>
       </c>
-      <c r="D232" s="14" t="s">
+      <c r="E232" s="14" t="s">
         <v>1044</v>
       </c>
-      <c r="E232" s="14" t="s">
+      <c r="F232" s="5" t="s">
         <v>1045</v>
       </c>
-      <c r="F232" s="5" t="s">
+      <c r="G232" s="14" t="s">
         <v>1046</v>
       </c>
-      <c r="G232" s="14" t="s">
-        <v>1047</v>
-      </c>
       <c r="H232" s="15">
         <f t="shared" si="1"/>
         <v>232</v>
       </c>
     </row>
-    <row r="233">
+    <row r="233" hidden="1">
       <c r="A233" s="10" t="s">
         <v>251</v>
       </c>
@@ -10513,26 +10825,26 @@
         <v>1.0</v>
       </c>
       <c r="C233" s="11" t="s">
+        <v>1047</v>
+      </c>
+      <c r="D233" s="11" t="s">
         <v>1048</v>
       </c>
-      <c r="D233" s="11" t="s">
+      <c r="E233" s="11" t="s">
         <v>1049</v>
       </c>
-      <c r="E233" s="11" t="s">
+      <c r="F233" s="11" t="s">
         <v>1050</v>
       </c>
-      <c r="F233" s="11" t="s">
+      <c r="G233" s="11" t="s">
         <v>1051</v>
       </c>
-      <c r="G233" s="11" t="s">
-        <v>1052</v>
-      </c>
       <c r="H233" s="12">
         <f t="shared" si="1"/>
         <v>233</v>
       </c>
     </row>
-    <row r="234">
+    <row r="234" hidden="1">
       <c r="A234" s="13" t="s">
         <v>251</v>
       </c>
@@ -10540,26 +10852,26 @@
         <v>1.0</v>
       </c>
       <c r="C234" s="14" t="s">
+        <v>1052</v>
+      </c>
+      <c r="D234" s="14" t="s">
         <v>1053</v>
       </c>
-      <c r="D234" s="14" t="s">
+      <c r="E234" s="14" t="s">
         <v>1054</v>
       </c>
-      <c r="E234" s="14" t="s">
+      <c r="F234" s="14" t="s">
         <v>1055</v>
       </c>
-      <c r="F234" s="14" t="s">
+      <c r="G234" s="14" t="s">
         <v>1056</v>
       </c>
-      <c r="G234" s="14" t="s">
-        <v>1057</v>
-      </c>
       <c r="H234" s="15">
         <f t="shared" si="1"/>
         <v>234</v>
       </c>
     </row>
-    <row r="235">
+    <row r="235" hidden="1">
       <c r="A235" s="10" t="s">
         <v>251</v>
       </c>
@@ -10567,26 +10879,26 @@
         <v>1.0</v>
       </c>
       <c r="C235" s="11" t="s">
+        <v>1057</v>
+      </c>
+      <c r="D235" s="11" t="s">
         <v>1058</v>
       </c>
-      <c r="D235" s="11" t="s">
+      <c r="E235" s="11" t="s">
         <v>1059</v>
       </c>
-      <c r="E235" s="11" t="s">
+      <c r="F235" s="11" t="s">
         <v>1060</v>
       </c>
-      <c r="F235" s="11" t="s">
+      <c r="G235" s="11" t="s">
         <v>1061</v>
       </c>
-      <c r="G235" s="11" t="s">
-        <v>1062</v>
-      </c>
       <c r="H235" s="12">
         <f t="shared" si="1"/>
         <v>235</v>
       </c>
     </row>
-    <row r="236">
+    <row r="236" hidden="1">
       <c r="A236" s="13" t="s">
         <v>251</v>
       </c>
@@ -10594,44 +10906,54 @@
         <v>2.0</v>
       </c>
       <c r="C236" s="14" t="s">
+        <v>1062</v>
+      </c>
+      <c r="D236" s="14" t="s">
         <v>1063</v>
       </c>
-      <c r="D236" s="14" t="s">
+      <c r="E236" s="14" t="s">
         <v>1064</v>
       </c>
-      <c r="E236" s="14" t="s">
+      <c r="F236" s="14" t="s">
         <v>1065</v>
       </c>
-      <c r="F236" s="14" t="s">
+      <c r="G236" s="14" t="s">
         <v>1066</v>
       </c>
-      <c r="G236" s="14" t="s">
+      <c r="H236" s="15">
+        <f t="shared" si="1"/>
+        <v>236</v>
+      </c>
+    </row>
+    <row r="237">
+      <c r="A237" s="7" t="s">
+        <v>485</v>
+      </c>
+      <c r="B237" s="11">
+        <v>1.0</v>
+      </c>
+      <c r="C237" s="11" t="s">
         <v>1067</v>
       </c>
-      <c r="H236" s="15">
-        <f t="shared" si="1"/>
-        <v>236</v>
-      </c>
-    </row>
-    <row r="237">
-      <c r="A237" s="10" t="s">
-        <v>251</v>
-      </c>
-      <c r="B237" s="11">
-        <v>2.0</v>
-      </c>
-      <c r="C237" s="11"/>
-      <c r="D237" s="11"/>
-      <c r="E237" s="11"/>
-      <c r="F237" s="11"/>
-      <c r="G237" s="11"/>
+      <c r="D237" s="11" t="s">
+        <v>98</v>
+      </c>
+      <c r="E237" s="11" t="s">
+        <v>99</v>
+      </c>
+      <c r="F237" s="11" t="s">
+        <v>100</v>
+      </c>
+      <c r="G237" s="11" t="s">
+        <v>96</v>
+      </c>
       <c r="H237" s="12">
         <f t="shared" si="1"/>
         <v>237</v>
       </c>
     </row>
     <row r="238">
-      <c r="A238" s="13" t="s">
+      <c r="A238" s="4" t="s">
         <v>485</v>
       </c>
       <c r="B238" s="14">
@@ -10641,16 +10963,16 @@
         <v>1068</v>
       </c>
       <c r="D238" s="14" t="s">
-        <v>98</v>
+        <v>1069</v>
       </c>
       <c r="E238" s="14" t="s">
-        <v>99</v>
+        <v>1070</v>
       </c>
       <c r="F238" s="14" t="s">
-        <v>100</v>
+        <v>1071</v>
       </c>
       <c r="G238" s="14" t="s">
-        <v>96</v>
+        <v>1072</v>
       </c>
       <c r="H238" s="15">
         <f t="shared" si="1"/>
@@ -10658,26 +10980,26 @@
       </c>
     </row>
     <row r="239">
-      <c r="A239" s="10" t="s">
-        <v>1069</v>
+      <c r="A239" s="7" t="s">
+        <v>485</v>
       </c>
       <c r="B239" s="11">
         <v>1.0</v>
       </c>
       <c r="C239" s="11" t="s">
-        <v>1070</v>
+        <v>1073</v>
       </c>
       <c r="D239" s="11" t="s">
-        <v>1071</v>
+        <v>1074</v>
       </c>
       <c r="E239" s="11" t="s">
-        <v>1072</v>
+        <v>1075</v>
       </c>
       <c r="F239" s="11" t="s">
-        <v>1073</v>
+        <v>1076</v>
       </c>
       <c r="G239" s="11" t="s">
-        <v>1074</v>
+        <v>1077</v>
       </c>
       <c r="H239" s="12">
         <f t="shared" si="1"/>
@@ -10685,26 +11007,26 @@
       </c>
     </row>
     <row r="240">
-      <c r="A240" s="13" t="s">
+      <c r="A240" s="4" t="s">
         <v>485</v>
       </c>
       <c r="B240" s="14">
         <v>1.0</v>
       </c>
       <c r="C240" s="14" t="s">
-        <v>1075</v>
+        <v>1078</v>
       </c>
       <c r="D240" s="14" t="s">
-        <v>1076</v>
+        <v>1079</v>
       </c>
       <c r="E240" s="14" t="s">
-        <v>1077</v>
+        <v>1080</v>
       </c>
       <c r="F240" s="14" t="s">
-        <v>1078</v>
+        <v>1081</v>
       </c>
       <c r="G240" s="14" t="s">
-        <v>1079</v>
+        <v>1082</v>
       </c>
       <c r="H240" s="15">
         <f t="shared" si="1"/>
@@ -10712,26 +11034,26 @@
       </c>
     </row>
     <row r="241">
-      <c r="A241" s="10" t="s">
+      <c r="A241" s="7" t="s">
         <v>485</v>
       </c>
       <c r="B241" s="11">
-        <v>1.0</v>
+        <v>2.0</v>
       </c>
       <c r="C241" s="11" t="s">
-        <v>1080</v>
+        <v>1083</v>
       </c>
       <c r="D241" s="11" t="s">
-        <v>1081</v>
+        <v>1084</v>
       </c>
       <c r="E241" s="11" t="s">
-        <v>1082</v>
+        <v>1085</v>
       </c>
       <c r="F241" s="11" t="s">
-        <v>1083</v>
+        <v>1086</v>
       </c>
       <c r="G241" s="11" t="s">
-        <v>1084</v>
+        <v>1087</v>
       </c>
       <c r="H241" s="12">
         <f t="shared" si="1"/>
@@ -10739,26 +11061,26 @@
       </c>
     </row>
     <row r="242">
-      <c r="A242" s="13" t="s">
+      <c r="A242" s="4" t="s">
         <v>485</v>
       </c>
       <c r="B242" s="14">
         <v>2.0</v>
       </c>
       <c r="C242" s="14" t="s">
-        <v>1085</v>
+        <v>1088</v>
       </c>
       <c r="D242" s="14" t="s">
-        <v>1086</v>
+        <v>1089</v>
       </c>
       <c r="E242" s="14" t="s">
-        <v>1087</v>
+        <v>1090</v>
       </c>
       <c r="F242" s="14" t="s">
-        <v>1088</v>
+        <v>1091</v>
       </c>
       <c r="G242" s="14" t="s">
-        <v>1089</v>
+        <v>1092</v>
       </c>
       <c r="H242" s="15">
         <f t="shared" si="1"/>
@@ -10766,26 +11088,26 @@
       </c>
     </row>
     <row r="243">
-      <c r="A243" s="10" t="s">
+      <c r="A243" s="7" t="s">
         <v>485</v>
       </c>
       <c r="B243" s="11">
         <v>2.0</v>
       </c>
       <c r="C243" s="11" t="s">
-        <v>1090</v>
+        <v>1093</v>
       </c>
       <c r="D243" s="11" t="s">
-        <v>1091</v>
+        <v>1094</v>
       </c>
       <c r="E243" s="11" t="s">
-        <v>1092</v>
+        <v>1095</v>
       </c>
       <c r="F243" s="11" t="s">
-        <v>1093</v>
+        <v>1096</v>
       </c>
       <c r="G243" s="11" t="s">
-        <v>1094</v>
+        <v>1097</v>
       </c>
       <c r="H243" s="12">
         <f t="shared" si="1"/>
@@ -10793,26 +11115,26 @@
       </c>
     </row>
     <row r="244">
-      <c r="A244" s="13" t="s">
+      <c r="A244" s="4" t="s">
         <v>485</v>
       </c>
       <c r="B244" s="14">
         <v>2.0</v>
       </c>
       <c r="C244" s="14" t="s">
-        <v>1095</v>
+        <v>1098</v>
       </c>
       <c r="D244" s="14" t="s">
-        <v>1096</v>
+        <v>1099</v>
       </c>
       <c r="E244" s="14" t="s">
-        <v>1097</v>
+        <v>1100</v>
       </c>
       <c r="F244" s="14" t="s">
-        <v>1098</v>
+        <v>1101</v>
       </c>
       <c r="G244" s="14" t="s">
-        <v>1099</v>
+        <v>1102</v>
       </c>
       <c r="H244" s="15">
         <f t="shared" si="1"/>
@@ -10820,26 +11142,26 @@
       </c>
     </row>
     <row r="245">
-      <c r="A245" s="10" t="s">
+      <c r="A245" s="7" t="s">
         <v>485</v>
       </c>
       <c r="B245" s="11">
         <v>2.0</v>
       </c>
       <c r="C245" s="11" t="s">
-        <v>1100</v>
+        <v>1103</v>
       </c>
       <c r="D245" s="11" t="s">
-        <v>1101</v>
+        <v>1104</v>
       </c>
       <c r="E245" s="11" t="s">
-        <v>1102</v>
+        <v>1105</v>
       </c>
       <c r="F245" s="11" t="s">
-        <v>1103</v>
+        <v>1106</v>
       </c>
       <c r="G245" s="11" t="s">
-        <v>1104</v>
+        <v>1107</v>
       </c>
       <c r="H245" s="12">
         <f t="shared" si="1"/>
@@ -10847,26 +11169,26 @@
       </c>
     </row>
     <row r="246">
-      <c r="A246" s="13" t="s">
+      <c r="A246" s="4" t="s">
         <v>485</v>
       </c>
       <c r="B246" s="14">
         <v>2.0</v>
       </c>
       <c r="C246" s="14" t="s">
-        <v>1105</v>
+        <v>1108</v>
       </c>
       <c r="D246" s="14" t="s">
-        <v>1106</v>
+        <v>1109</v>
       </c>
       <c r="E246" s="14" t="s">
-        <v>1107</v>
+        <v>1110</v>
       </c>
       <c r="F246" s="14" t="s">
-        <v>1108</v>
+        <v>1111</v>
       </c>
       <c r="G246" s="14" t="s">
-        <v>1109</v>
+        <v>1112</v>
       </c>
       <c r="H246" s="15">
         <f t="shared" si="1"/>
@@ -10874,26 +11196,26 @@
       </c>
     </row>
     <row r="247">
-      <c r="A247" s="10" t="s">
+      <c r="A247" s="7" t="s">
         <v>485</v>
       </c>
       <c r="B247" s="11">
         <v>2.0</v>
       </c>
       <c r="C247" s="11" t="s">
-        <v>1110</v>
-      </c>
-      <c r="D247" s="11" t="s">
-        <v>1111</v>
-      </c>
-      <c r="E247" s="11" t="s">
-        <v>1112</v>
-      </c>
-      <c r="F247" s="11" t="s">
         <v>1113</v>
       </c>
-      <c r="G247" s="11" t="s">
-        <v>1114</v>
+      <c r="D247" s="18">
+        <v>0.75</v>
+      </c>
+      <c r="E247" s="18">
+        <v>0.25</v>
+      </c>
+      <c r="F247" s="18">
+        <v>0.1</v>
+      </c>
+      <c r="G247" s="18">
+        <v>0.9</v>
       </c>
       <c r="H247" s="12">
         <f t="shared" si="1"/>
@@ -10901,25 +11223,25 @@
       </c>
     </row>
     <row r="248">
-      <c r="A248" s="13" t="s">
+      <c r="A248" s="4" t="s">
         <v>485</v>
       </c>
       <c r="B248" s="14">
         <v>2.0</v>
       </c>
       <c r="C248" s="14" t="s">
-        <v>1115</v>
-      </c>
-      <c r="D248" s="18">
+        <v>1114</v>
+      </c>
+      <c r="D248" s="19">
+        <v>0.25</v>
+      </c>
+      <c r="E248" s="19">
         <v>0.75</v>
       </c>
-      <c r="E248" s="18">
-        <v>0.25</v>
-      </c>
-      <c r="F248" s="18">
+      <c r="F248" s="19">
         <v>0.1</v>
       </c>
-      <c r="G248" s="18">
+      <c r="G248" s="19">
         <v>0.9</v>
       </c>
       <c r="H248" s="15">
@@ -10928,26 +11250,26 @@
       </c>
     </row>
     <row r="249">
-      <c r="A249" s="10" t="s">
+      <c r="A249" s="7" t="s">
         <v>485</v>
       </c>
       <c r="B249" s="11">
         <v>2.0</v>
       </c>
       <c r="C249" s="11" t="s">
+        <v>1115</v>
+      </c>
+      <c r="D249" s="11" t="s">
         <v>1116</v>
       </c>
-      <c r="D249" s="19">
-        <v>0.25</v>
-      </c>
-      <c r="E249" s="19">
-        <v>0.75</v>
-      </c>
-      <c r="F249" s="19">
-        <v>0.1</v>
-      </c>
-      <c r="G249" s="19">
-        <v>0.9</v>
+      <c r="E249" s="11" t="s">
+        <v>1117</v>
+      </c>
+      <c r="F249" s="11" t="s">
+        <v>1118</v>
+      </c>
+      <c r="G249" s="11" t="s">
+        <v>1119</v>
       </c>
       <c r="H249" s="12">
         <f t="shared" si="1"/>
@@ -10955,26 +11277,26 @@
       </c>
     </row>
     <row r="250">
-      <c r="A250" s="13" t="s">
+      <c r="A250" s="4" t="s">
         <v>485</v>
       </c>
       <c r="B250" s="14">
         <v>2.0</v>
       </c>
       <c r="C250" s="14" t="s">
-        <v>1117</v>
+        <v>1120</v>
       </c>
       <c r="D250" s="14" t="s">
-        <v>1118</v>
+        <v>1121</v>
       </c>
       <c r="E250" s="14" t="s">
-        <v>1119</v>
+        <v>1122</v>
       </c>
       <c r="F250" s="14" t="s">
-        <v>1120</v>
+        <v>1123</v>
       </c>
       <c r="G250" s="14" t="s">
-        <v>1121</v>
+        <v>1124</v>
       </c>
       <c r="H250" s="15">
         <f t="shared" si="1"/>
@@ -10982,26 +11304,26 @@
       </c>
     </row>
     <row r="251">
-      <c r="A251" s="10" t="s">
-        <v>1069</v>
+      <c r="A251" s="7" t="s">
+        <v>485</v>
       </c>
       <c r="B251" s="11">
         <v>2.0</v>
       </c>
       <c r="C251" s="11" t="s">
-        <v>1122</v>
+        <v>1125</v>
       </c>
       <c r="D251" s="11" t="s">
-        <v>1123</v>
+        <v>1126</v>
       </c>
       <c r="E251" s="11" t="s">
-        <v>1124</v>
+        <v>1127</v>
       </c>
       <c r="F251" s="11" t="s">
-        <v>1125</v>
+        <v>1128</v>
       </c>
       <c r="G251" s="11" t="s">
-        <v>1126</v>
+        <v>1129</v>
       </c>
       <c r="H251" s="12">
         <f t="shared" si="1"/>
@@ -11009,80 +11331,80 @@
       </c>
     </row>
     <row r="252">
-      <c r="A252" s="13" t="s">
+      <c r="A252" s="4" t="s">
         <v>485</v>
       </c>
       <c r="B252" s="14">
         <v>2.0</v>
       </c>
       <c r="C252" s="14" t="s">
-        <v>1127</v>
+        <v>1130</v>
       </c>
       <c r="D252" s="14" t="s">
-        <v>1128</v>
+        <v>1131</v>
       </c>
       <c r="E252" s="14" t="s">
-        <v>1129</v>
+        <v>1132</v>
       </c>
       <c r="F252" s="14" t="s">
-        <v>1130</v>
+        <v>1133</v>
       </c>
       <c r="G252" s="14" t="s">
+        <v>1134</v>
+      </c>
+      <c r="H252" s="15">
+        <f t="shared" si="1"/>
+        <v>252</v>
+      </c>
+    </row>
+    <row r="253">
+      <c r="A253" s="7" t="s">
+        <v>485</v>
+      </c>
+      <c r="B253" s="11">
+        <v>7.0</v>
+      </c>
+      <c r="C253" s="11" t="s">
+        <v>1135</v>
+      </c>
+      <c r="D253" s="11" t="s">
+        <v>1136</v>
+      </c>
+      <c r="E253" s="11" t="s">
+        <v>1132</v>
+      </c>
+      <c r="F253" s="11" t="s">
+        <v>1137</v>
+      </c>
+      <c r="G253" s="11" t="s">
+        <v>1138</v>
+      </c>
+      <c r="H253" s="12">
+        <f t="shared" si="1"/>
+        <v>253</v>
+      </c>
+    </row>
+    <row r="254">
+      <c r="A254" s="4" t="s">
+        <v>485</v>
+      </c>
+      <c r="B254" s="14">
+        <v>2.0</v>
+      </c>
+      <c r="C254" s="14" t="s">
+        <v>1139</v>
+      </c>
+      <c r="D254" s="14" t="s">
+        <v>1140</v>
+      </c>
+      <c r="E254" s="14" t="s">
+        <v>1132</v>
+      </c>
+      <c r="F254" s="14" t="s">
         <v>1131</v>
       </c>
-      <c r="H252" s="15">
-        <f t="shared" si="1"/>
-        <v>252</v>
-      </c>
-    </row>
-    <row r="253">
-      <c r="A253" s="10" t="s">
-        <v>1069</v>
-      </c>
-      <c r="B253" s="11">
-        <v>2.0</v>
-      </c>
-      <c r="C253" s="11" t="s">
-        <v>1132</v>
-      </c>
-      <c r="D253" s="11" t="s">
-        <v>1133</v>
-      </c>
-      <c r="E253" s="11" t="s">
-        <v>1134</v>
-      </c>
-      <c r="F253" s="11" t="s">
-        <v>1135</v>
-      </c>
-      <c r="G253" s="11" t="s">
-        <v>1136</v>
-      </c>
-      <c r="H253" s="12">
-        <f t="shared" si="1"/>
-        <v>253</v>
-      </c>
-    </row>
-    <row r="254">
-      <c r="A254" s="13" t="s">
-        <v>485</v>
-      </c>
-      <c r="B254" s="14">
-        <v>7.0</v>
-      </c>
-      <c r="C254" s="14" t="s">
-        <v>1137</v>
-      </c>
-      <c r="D254" s="14" t="s">
-        <v>1138</v>
-      </c>
-      <c r="E254" s="14" t="s">
-        <v>1134</v>
-      </c>
-      <c r="F254" s="14" t="s">
-        <v>1139</v>
-      </c>
       <c r="G254" s="14" t="s">
-        <v>1140</v>
+        <v>1141</v>
       </c>
       <c r="H254" s="15">
         <f t="shared" si="1"/>
@@ -11090,26 +11412,26 @@
       </c>
     </row>
     <row r="255">
-      <c r="A255" s="10" t="s">
+      <c r="A255" s="7" t="s">
         <v>485</v>
       </c>
       <c r="B255" s="11">
         <v>2.0</v>
       </c>
       <c r="C255" s="11" t="s">
-        <v>1141</v>
+        <v>1142</v>
       </c>
       <c r="D255" s="11" t="s">
-        <v>1142</v>
+        <v>1143</v>
       </c>
       <c r="E255" s="11" t="s">
-        <v>1134</v>
+        <v>1144</v>
       </c>
       <c r="F255" s="11" t="s">
-        <v>1133</v>
+        <v>1145</v>
       </c>
       <c r="G255" s="11" t="s">
-        <v>1143</v>
+        <v>1146</v>
       </c>
       <c r="H255" s="12">
         <f t="shared" si="1"/>
@@ -11117,26 +11439,26 @@
       </c>
     </row>
     <row r="256">
-      <c r="A256" s="13" t="s">
+      <c r="A256" s="4" t="s">
         <v>485</v>
       </c>
       <c r="B256" s="14">
-        <v>2.0</v>
+        <v>3.0</v>
       </c>
       <c r="C256" s="14" t="s">
-        <v>1144</v>
+        <v>1147</v>
       </c>
       <c r="D256" s="14" t="s">
-        <v>1145</v>
+        <v>1148</v>
       </c>
       <c r="E256" s="14" t="s">
-        <v>1146</v>
+        <v>1149</v>
       </c>
       <c r="F256" s="14" t="s">
-        <v>1147</v>
+        <v>1150</v>
       </c>
       <c r="G256" s="14" t="s">
-        <v>1148</v>
+        <v>1151</v>
       </c>
       <c r="H256" s="15">
         <f t="shared" si="1"/>
@@ -11144,53 +11466,53 @@
       </c>
     </row>
     <row r="257">
-      <c r="A257" s="10" t="s">
+      <c r="A257" s="7" t="s">
         <v>485</v>
       </c>
       <c r="B257" s="11">
         <v>3.0</v>
       </c>
       <c r="C257" s="11" t="s">
+        <v>1152</v>
+      </c>
+      <c r="D257" s="11" t="s">
         <v>1149</v>
       </c>
-      <c r="D257" s="11" t="s">
+      <c r="E257" s="11" t="s">
+        <v>1148</v>
+      </c>
+      <c r="F257" s="11" t="s">
         <v>1150</v>
       </c>
-      <c r="E257" s="11" t="s">
+      <c r="G257" s="11" t="s">
         <v>1151</v>
       </c>
-      <c r="F257" s="11" t="s">
-        <v>1152</v>
-      </c>
-      <c r="G257" s="11" t="s">
-        <v>1153</v>
-      </c>
       <c r="H257" s="12">
         <f t="shared" si="1"/>
         <v>257</v>
       </c>
     </row>
     <row r="258">
-      <c r="A258" s="13" t="s">
+      <c r="A258" s="4" t="s">
         <v>485</v>
       </c>
       <c r="B258" s="14">
         <v>3.0</v>
       </c>
       <c r="C258" s="14" t="s">
+        <v>1153</v>
+      </c>
+      <c r="D258" s="14" t="s">
         <v>1154</v>
       </c>
-      <c r="D258" s="14" t="s">
-        <v>1151</v>
-      </c>
       <c r="E258" s="14" t="s">
-        <v>1150</v>
+        <v>1155</v>
       </c>
       <c r="F258" s="14" t="s">
-        <v>1152</v>
+        <v>1156</v>
       </c>
       <c r="G258" s="14" t="s">
-        <v>1153</v>
+        <v>1157</v>
       </c>
       <c r="H258" s="15">
         <f t="shared" si="1"/>
@@ -11198,26 +11520,26 @@
       </c>
     </row>
     <row r="259">
-      <c r="A259" s="10" t="s">
+      <c r="A259" s="7" t="s">
         <v>485</v>
       </c>
       <c r="B259" s="11">
         <v>3.0</v>
       </c>
       <c r="C259" s="11" t="s">
-        <v>1155</v>
+        <v>1158</v>
       </c>
       <c r="D259" s="11" t="s">
-        <v>1156</v>
+        <v>1159</v>
       </c>
       <c r="E259" s="11" t="s">
-        <v>1157</v>
+        <v>1160</v>
       </c>
       <c r="F259" s="11" t="s">
-        <v>1158</v>
+        <v>1161</v>
       </c>
       <c r="G259" s="11" t="s">
-        <v>1159</v>
+        <v>1162</v>
       </c>
       <c r="H259" s="12">
         <f t="shared" si="1"/>
@@ -11225,26 +11547,26 @@
       </c>
     </row>
     <row r="260">
-      <c r="A260" s="13" t="s">
+      <c r="A260" s="4" t="s">
         <v>485</v>
       </c>
       <c r="B260" s="14">
         <v>3.0</v>
       </c>
       <c r="C260" s="14" t="s">
-        <v>1160</v>
+        <v>1163</v>
       </c>
       <c r="D260" s="14" t="s">
-        <v>1161</v>
+        <v>1164</v>
       </c>
       <c r="E260" s="14" t="s">
-        <v>1162</v>
+        <v>1165</v>
       </c>
       <c r="F260" s="14" t="s">
-        <v>1163</v>
+        <v>1166</v>
       </c>
       <c r="G260" s="14" t="s">
-        <v>1164</v>
+        <v>1167</v>
       </c>
       <c r="H260" s="15">
         <f t="shared" si="1"/>
@@ -11252,26 +11574,26 @@
       </c>
     </row>
     <row r="261">
-      <c r="A261" s="10" t="s">
+      <c r="A261" s="7" t="s">
         <v>485</v>
       </c>
       <c r="B261" s="11">
         <v>3.0</v>
       </c>
       <c r="C261" s="11" t="s">
-        <v>1165</v>
+        <v>1168</v>
       </c>
       <c r="D261" s="11" t="s">
-        <v>1166</v>
+        <v>1169</v>
       </c>
       <c r="E261" s="11" t="s">
-        <v>1167</v>
+        <v>1170</v>
       </c>
       <c r="F261" s="11" t="s">
-        <v>1168</v>
+        <v>1171</v>
       </c>
       <c r="G261" s="11" t="s">
-        <v>1169</v>
+        <v>1172</v>
       </c>
       <c r="H261" s="12">
         <f t="shared" si="1"/>
@@ -11279,26 +11601,26 @@
       </c>
     </row>
     <row r="262">
-      <c r="A262" s="13" t="s">
+      <c r="A262" s="4" t="s">
         <v>485</v>
       </c>
       <c r="B262" s="14">
-        <v>3.0</v>
+        <v>4.0</v>
       </c>
       <c r="C262" s="14" t="s">
-        <v>1170</v>
+        <v>1173</v>
       </c>
       <c r="D262" s="14" t="s">
-        <v>1171</v>
+        <v>1174</v>
       </c>
       <c r="E262" s="14" t="s">
-        <v>1172</v>
+        <v>1175</v>
       </c>
       <c r="F262" s="14" t="s">
-        <v>1173</v>
+        <v>1176</v>
       </c>
       <c r="G262" s="14" t="s">
-        <v>1174</v>
+        <v>1177</v>
       </c>
       <c r="H262" s="15">
         <f t="shared" si="1"/>
@@ -11306,34 +11628,34 @@
       </c>
     </row>
     <row r="263">
-      <c r="A263" s="10" t="s">
+      <c r="A263" s="7" t="s">
         <v>485</v>
       </c>
       <c r="B263" s="11">
         <v>4.0</v>
       </c>
       <c r="C263" s="11" t="s">
-        <v>1175</v>
+        <v>1178</v>
       </c>
       <c r="D263" s="11" t="s">
-        <v>1176</v>
-      </c>
-      <c r="E263" s="11" t="s">
-        <v>1177</v>
-      </c>
-      <c r="F263" s="11" t="s">
-        <v>1178</v>
-      </c>
-      <c r="G263" s="11" t="s">
         <v>1179</v>
       </c>
+      <c r="E263" s="18">
+        <v>0.1</v>
+      </c>
+      <c r="F263" s="18">
+        <v>0.25</v>
+      </c>
+      <c r="G263" s="18">
+        <v>0.4</v>
+      </c>
       <c r="H263" s="12">
         <f t="shared" si="1"/>
         <v>263</v>
       </c>
     </row>
     <row r="264">
-      <c r="A264" s="13" t="s">
+      <c r="A264" s="4" t="s">
         <v>485</v>
       </c>
       <c r="B264" s="14">
@@ -11342,44 +11664,44 @@
       <c r="C264" s="14" t="s">
         <v>1180</v>
       </c>
-      <c r="D264" s="14" t="s">
-        <v>1181</v>
-      </c>
-      <c r="E264" s="18">
-        <v>0.1</v>
-      </c>
-      <c r="F264" s="18">
-        <v>0.25</v>
-      </c>
-      <c r="G264" s="18">
+      <c r="D264" s="19">
+        <v>0.3</v>
+      </c>
+      <c r="E264" s="19">
+        <v>0.6</v>
+      </c>
+      <c r="F264" s="19">
         <v>0.4</v>
       </c>
+      <c r="G264" s="19">
+        <v>0.7</v>
+      </c>
       <c r="H264" s="15">
         <f t="shared" si="1"/>
         <v>264</v>
       </c>
     </row>
     <row r="265">
-      <c r="A265" s="10" t="s">
+      <c r="A265" s="7" t="s">
         <v>485</v>
       </c>
       <c r="B265" s="11">
         <v>4.0</v>
       </c>
       <c r="C265" s="11" t="s">
+        <v>1181</v>
+      </c>
+      <c r="D265" s="11" t="s">
         <v>1182</v>
       </c>
-      <c r="D265" s="19">
-        <v>0.3</v>
-      </c>
-      <c r="E265" s="19">
-        <v>0.6</v>
-      </c>
-      <c r="F265" s="19">
-        <v>0.4</v>
-      </c>
-      <c r="G265" s="19">
-        <v>0.7</v>
+      <c r="E265" s="11" t="s">
+        <v>1183</v>
+      </c>
+      <c r="F265" s="11" t="s">
+        <v>1184</v>
+      </c>
+      <c r="G265" s="11" t="s">
+        <v>1185</v>
       </c>
       <c r="H265" s="12">
         <f t="shared" si="1"/>
@@ -11387,26 +11709,26 @@
       </c>
     </row>
     <row r="266">
-      <c r="A266" s="13" t="s">
+      <c r="A266" s="4" t="s">
         <v>485</v>
       </c>
       <c r="B266" s="14">
-        <v>4.0</v>
+        <v>5.0</v>
       </c>
       <c r="C266" s="14" t="s">
-        <v>1183</v>
+        <v>1186</v>
       </c>
       <c r="D266" s="14" t="s">
-        <v>1184</v>
+        <v>1187</v>
       </c>
       <c r="E266" s="14" t="s">
-        <v>1185</v>
+        <v>1188</v>
       </c>
       <c r="F266" s="14" t="s">
-        <v>1186</v>
+        <v>1189</v>
       </c>
       <c r="G266" s="14" t="s">
-        <v>1187</v>
+        <v>1190</v>
       </c>
       <c r="H266" s="15">
         <f t="shared" si="1"/>
@@ -11414,26 +11736,26 @@
       </c>
     </row>
     <row r="267">
-      <c r="A267" s="10" t="s">
+      <c r="A267" s="7" t="s">
         <v>485</v>
       </c>
       <c r="B267" s="11">
         <v>5.0</v>
       </c>
       <c r="C267" s="11" t="s">
-        <v>1188</v>
+        <v>1191</v>
       </c>
       <c r="D267" s="11" t="s">
-        <v>1189</v>
+        <v>1192</v>
       </c>
       <c r="E267" s="11" t="s">
-        <v>1190</v>
+        <v>1193</v>
       </c>
       <c r="F267" s="11" t="s">
-        <v>1191</v>
+        <v>1194</v>
       </c>
       <c r="G267" s="11" t="s">
-        <v>1192</v>
+        <v>1195</v>
       </c>
       <c r="H267" s="12">
         <f t="shared" si="1"/>
@@ -11441,26 +11763,26 @@
       </c>
     </row>
     <row r="268">
-      <c r="A268" s="13" t="s">
+      <c r="A268" s="4" t="s">
         <v>485</v>
       </c>
       <c r="B268" s="14">
         <v>5.0</v>
       </c>
       <c r="C268" s="14" t="s">
-        <v>1193</v>
+        <v>1196</v>
       </c>
       <c r="D268" s="14" t="s">
-        <v>1194</v>
+        <v>1197</v>
       </c>
       <c r="E268" s="14" t="s">
-        <v>1195</v>
+        <v>1198</v>
       </c>
       <c r="F268" s="14" t="s">
-        <v>1196</v>
+        <v>1199</v>
       </c>
       <c r="G268" s="14" t="s">
-        <v>1197</v>
+        <v>1200</v>
       </c>
       <c r="H268" s="15">
         <f t="shared" si="1"/>
@@ -11468,26 +11790,26 @@
       </c>
     </row>
     <row r="269">
-      <c r="A269" s="10" t="s">
+      <c r="A269" s="7" t="s">
         <v>485</v>
       </c>
       <c r="B269" s="11">
         <v>5.0</v>
       </c>
       <c r="C269" s="11" t="s">
-        <v>1198</v>
+        <v>1201</v>
       </c>
       <c r="D269" s="11" t="s">
-        <v>1199</v>
+        <v>492</v>
       </c>
       <c r="E269" s="11" t="s">
-        <v>1200</v>
+        <v>1202</v>
       </c>
       <c r="F269" s="11" t="s">
-        <v>1201</v>
+        <v>1203</v>
       </c>
       <c r="G269" s="11" t="s">
-        <v>1202</v>
+        <v>1204</v>
       </c>
       <c r="H269" s="12">
         <f t="shared" si="1"/>
@@ -11495,26 +11817,26 @@
       </c>
     </row>
     <row r="270">
-      <c r="A270" s="13" t="s">
+      <c r="A270" s="4" t="s">
         <v>485</v>
       </c>
       <c r="B270" s="14">
         <v>5.0</v>
       </c>
       <c r="C270" s="14" t="s">
-        <v>1203</v>
+        <v>1205</v>
       </c>
       <c r="D270" s="14" t="s">
-        <v>492</v>
+        <v>1206</v>
       </c>
       <c r="E270" s="14" t="s">
-        <v>1204</v>
+        <v>1207</v>
       </c>
       <c r="F270" s="14" t="s">
-        <v>1205</v>
+        <v>1208</v>
       </c>
       <c r="G270" s="14" t="s">
-        <v>1206</v>
+        <v>1209</v>
       </c>
       <c r="H270" s="15">
         <f t="shared" si="1"/>
@@ -11522,26 +11844,26 @@
       </c>
     </row>
     <row r="271">
-      <c r="A271" s="10" t="s">
+      <c r="A271" s="7" t="s">
         <v>485</v>
       </c>
       <c r="B271" s="11">
         <v>5.0</v>
       </c>
       <c r="C271" s="11" t="s">
-        <v>1207</v>
+        <v>1210</v>
       </c>
       <c r="D271" s="11" t="s">
-        <v>1208</v>
+        <v>1211</v>
       </c>
       <c r="E271" s="11" t="s">
-        <v>1209</v>
+        <v>1212</v>
       </c>
       <c r="F271" s="11" t="s">
-        <v>1210</v>
+        <v>1213</v>
       </c>
       <c r="G271" s="11" t="s">
-        <v>1211</v>
+        <v>1214</v>
       </c>
       <c r="H271" s="12">
         <f t="shared" si="1"/>
@@ -11549,26 +11871,26 @@
       </c>
     </row>
     <row r="272">
-      <c r="A272" s="13" t="s">
+      <c r="A272" s="4" t="s">
         <v>485</v>
       </c>
       <c r="B272" s="14">
         <v>5.0</v>
       </c>
       <c r="C272" s="14" t="s">
-        <v>1212</v>
+        <v>1215</v>
       </c>
       <c r="D272" s="14" t="s">
-        <v>1213</v>
+        <v>1202</v>
       </c>
       <c r="E272" s="14" t="s">
-        <v>1214</v>
+        <v>1203</v>
       </c>
       <c r="F272" s="14" t="s">
-        <v>1215</v>
+        <v>1216</v>
       </c>
       <c r="G272" s="14" t="s">
-        <v>1216</v>
+        <v>495</v>
       </c>
       <c r="H272" s="15">
         <f t="shared" si="1"/>
@@ -11576,7 +11898,7 @@
       </c>
     </row>
     <row r="273">
-      <c r="A273" s="10" t="s">
+      <c r="A273" s="7" t="s">
         <v>485</v>
       </c>
       <c r="B273" s="11">
@@ -11586,16 +11908,16 @@
         <v>1217</v>
       </c>
       <c r="D273" s="11" t="s">
-        <v>1204</v>
+        <v>1218</v>
       </c>
       <c r="E273" s="11" t="s">
-        <v>1205</v>
+        <v>1219</v>
       </c>
       <c r="F273" s="11" t="s">
-        <v>1218</v>
+        <v>1220</v>
       </c>
       <c r="G273" s="11" t="s">
-        <v>495</v>
+        <v>1221</v>
       </c>
       <c r="H273" s="12">
         <f t="shared" si="1"/>
@@ -11603,26 +11925,26 @@
       </c>
     </row>
     <row r="274">
-      <c r="A274" s="13" t="s">
+      <c r="A274" s="4" t="s">
         <v>485</v>
       </c>
       <c r="B274" s="14">
         <v>5.0</v>
       </c>
       <c r="C274" s="14" t="s">
-        <v>1219</v>
+        <v>1222</v>
       </c>
       <c r="D274" s="14" t="s">
-        <v>1220</v>
+        <v>1223</v>
       </c>
       <c r="E274" s="14" t="s">
-        <v>1221</v>
+        <v>1137</v>
       </c>
       <c r="F274" s="14" t="s">
-        <v>1222</v>
+        <v>1203</v>
       </c>
       <c r="G274" s="14" t="s">
-        <v>1223</v>
+        <v>1224</v>
       </c>
       <c r="H274" s="15">
         <f t="shared" si="1"/>
@@ -11630,23 +11952,23 @@
       </c>
     </row>
     <row r="275">
-      <c r="A275" s="10" t="s">
+      <c r="A275" s="7" t="s">
         <v>485</v>
       </c>
       <c r="B275" s="11">
         <v>5.0</v>
       </c>
       <c r="C275" s="11" t="s">
-        <v>1224</v>
+        <v>1225</v>
       </c>
       <c r="D275" s="11" t="s">
-        <v>1225</v>
+        <v>1203</v>
       </c>
       <c r="E275" s="11" t="s">
-        <v>1139</v>
+        <v>1202</v>
       </c>
       <c r="F275" s="11" t="s">
-        <v>1205</v>
+        <v>492</v>
       </c>
       <c r="G275" s="11" t="s">
         <v>1226</v>
@@ -11657,26 +11979,26 @@
       </c>
     </row>
     <row r="276">
-      <c r="A276" s="13" t="s">
+      <c r="A276" s="4" t="s">
         <v>485</v>
       </c>
       <c r="B276" s="14">
-        <v>5.0</v>
+        <v>6.0</v>
       </c>
       <c r="C276" s="14" t="s">
         <v>1227</v>
       </c>
       <c r="D276" s="14" t="s">
-        <v>1205</v>
+        <v>1228</v>
       </c>
       <c r="E276" s="14" t="s">
-        <v>1204</v>
+        <v>1229</v>
       </c>
       <c r="F276" s="14" t="s">
-        <v>492</v>
+        <v>1230</v>
       </c>
       <c r="G276" s="14" t="s">
-        <v>1228</v>
+        <v>1231</v>
       </c>
       <c r="H276" s="15">
         <f t="shared" si="1"/>
@@ -11684,26 +12006,26 @@
       </c>
     </row>
     <row r="277">
-      <c r="A277" s="10" t="s">
+      <c r="A277" s="7" t="s">
         <v>485</v>
       </c>
       <c r="B277" s="11">
         <v>6.0</v>
       </c>
       <c r="C277" s="11" t="s">
-        <v>1229</v>
+        <v>1232</v>
       </c>
       <c r="D277" s="11" t="s">
-        <v>1230</v>
+        <v>1233</v>
       </c>
       <c r="E277" s="11" t="s">
-        <v>1231</v>
+        <v>1234</v>
       </c>
       <c r="F277" s="11" t="s">
-        <v>1232</v>
+        <v>1235</v>
       </c>
       <c r="G277" s="11" t="s">
-        <v>1233</v>
+        <v>1236</v>
       </c>
       <c r="H277" s="12">
         <f t="shared" si="1"/>
@@ -11711,26 +12033,26 @@
       </c>
     </row>
     <row r="278">
-      <c r="A278" s="13" t="s">
+      <c r="A278" s="4" t="s">
         <v>485</v>
       </c>
       <c r="B278" s="14">
         <v>6.0</v>
       </c>
       <c r="C278" s="14" t="s">
-        <v>1234</v>
+        <v>1237</v>
       </c>
       <c r="D278" s="14" t="s">
-        <v>1235</v>
+        <v>1238</v>
       </c>
       <c r="E278" s="14" t="s">
-        <v>1236</v>
+        <v>1239</v>
       </c>
       <c r="F278" s="14" t="s">
-        <v>1237</v>
+        <v>1240</v>
       </c>
       <c r="G278" s="14" t="s">
-        <v>1238</v>
+        <v>1241</v>
       </c>
       <c r="H278" s="15">
         <f t="shared" si="1"/>
@@ -11738,26 +12060,26 @@
       </c>
     </row>
     <row r="279">
-      <c r="A279" s="10" t="s">
+      <c r="A279" s="7" t="s">
         <v>485</v>
       </c>
       <c r="B279" s="11">
         <v>6.0</v>
       </c>
       <c r="C279" s="11" t="s">
-        <v>1239</v>
+        <v>1242</v>
       </c>
       <c r="D279" s="11" t="s">
-        <v>1240</v>
+        <v>1243</v>
       </c>
       <c r="E279" s="11" t="s">
-        <v>1241</v>
+        <v>1244</v>
       </c>
       <c r="F279" s="11" t="s">
-        <v>1242</v>
+        <v>1245</v>
       </c>
       <c r="G279" s="11" t="s">
-        <v>1243</v>
+        <v>1246</v>
       </c>
       <c r="H279" s="12">
         <f t="shared" si="1"/>
@@ -11765,26 +12087,26 @@
       </c>
     </row>
     <row r="280">
-      <c r="A280" s="13" t="s">
+      <c r="A280" s="4" t="s">
         <v>485</v>
       </c>
       <c r="B280" s="14">
         <v>6.0</v>
       </c>
       <c r="C280" s="14" t="s">
-        <v>1244</v>
+        <v>1247</v>
       </c>
       <c r="D280" s="14" t="s">
-        <v>1245</v>
+        <v>1248</v>
       </c>
       <c r="E280" s="14" t="s">
-        <v>1246</v>
+        <v>1249</v>
       </c>
       <c r="F280" s="14" t="s">
-        <v>1247</v>
+        <v>1250</v>
       </c>
       <c r="G280" s="14" t="s">
-        <v>1248</v>
+        <v>1251</v>
       </c>
       <c r="H280" s="15">
         <f t="shared" si="1"/>
@@ -11792,26 +12114,26 @@
       </c>
     </row>
     <row r="281">
-      <c r="A281" s="10" t="s">
+      <c r="A281" s="7" t="s">
         <v>485</v>
       </c>
       <c r="B281" s="11">
         <v>6.0</v>
       </c>
       <c r="C281" s="11" t="s">
-        <v>1249</v>
+        <v>1252</v>
       </c>
       <c r="D281" s="11" t="s">
-        <v>1250</v>
+        <v>1253</v>
       </c>
       <c r="E281" s="11" t="s">
-        <v>1251</v>
+        <v>1254</v>
       </c>
       <c r="F281" s="11" t="s">
-        <v>1252</v>
+        <v>1255</v>
       </c>
       <c r="G281" s="11" t="s">
-        <v>1253</v>
+        <v>1256</v>
       </c>
       <c r="H281" s="12">
         <f t="shared" si="1"/>
@@ -11819,30 +12141,597 @@
       </c>
     </row>
     <row r="282">
-      <c r="A282" s="20" t="s">
+      <c r="A282" s="13" t="s">
         <v>485</v>
       </c>
-      <c r="B282" s="21">
-        <v>6.0</v>
-      </c>
-      <c r="C282" s="21" t="s">
-        <v>1254</v>
-      </c>
-      <c r="D282" s="21" t="s">
-        <v>1255</v>
-      </c>
-      <c r="E282" s="21" t="s">
-        <v>1256</v>
-      </c>
-      <c r="F282" s="21" t="s">
+      <c r="B282" s="14">
+        <v>7.0</v>
+      </c>
+      <c r="C282" s="14" t="s">
         <v>1257</v>
       </c>
-      <c r="G282" s="21" t="s">
+      <c r="D282" s="14" t="s">
         <v>1258</v>
       </c>
-      <c r="H282" s="22">
+      <c r="E282" s="14" t="s">
+        <v>1259</v>
+      </c>
+      <c r="F282" s="14" t="s">
+        <v>1260</v>
+      </c>
+      <c r="G282" s="14" t="s">
+        <v>1261</v>
+      </c>
+      <c r="H282" s="15">
         <f t="shared" si="1"/>
         <v>282</v>
+      </c>
+    </row>
+    <row r="283">
+      <c r="A283" s="10" t="s">
+        <v>485</v>
+      </c>
+      <c r="B283" s="11">
+        <v>7.0</v>
+      </c>
+      <c r="C283" s="11" t="s">
+        <v>1262</v>
+      </c>
+      <c r="D283" s="11" t="s">
+        <v>1263</v>
+      </c>
+      <c r="E283" s="11" t="s">
+        <v>1264</v>
+      </c>
+      <c r="F283" s="11" t="s">
+        <v>1265</v>
+      </c>
+      <c r="G283" s="11" t="s">
+        <v>1266</v>
+      </c>
+      <c r="H283" s="12">
+        <f t="shared" si="1"/>
+        <v>283</v>
+      </c>
+    </row>
+    <row r="284">
+      <c r="A284" s="13" t="s">
+        <v>485</v>
+      </c>
+      <c r="B284" s="14">
+        <v>7.0</v>
+      </c>
+      <c r="C284" s="14" t="s">
+        <v>1267</v>
+      </c>
+      <c r="D284" s="14" t="s">
+        <v>1268</v>
+      </c>
+      <c r="E284" s="14" t="s">
+        <v>1269</v>
+      </c>
+      <c r="F284" s="14" t="s">
+        <v>1270</v>
+      </c>
+      <c r="G284" s="14" t="s">
+        <v>1271</v>
+      </c>
+      <c r="H284" s="15">
+        <f t="shared" si="1"/>
+        <v>284</v>
+      </c>
+    </row>
+    <row r="285">
+      <c r="A285" s="10" t="s">
+        <v>485</v>
+      </c>
+      <c r="B285" s="11">
+        <v>7.0</v>
+      </c>
+      <c r="C285" s="11" t="s">
+        <v>1272</v>
+      </c>
+      <c r="D285" s="11" t="s">
+        <v>1273</v>
+      </c>
+      <c r="E285" s="11" t="s">
+        <v>1274</v>
+      </c>
+      <c r="F285" s="11" t="s">
+        <v>1275</v>
+      </c>
+      <c r="G285" s="11" t="s">
+        <v>1276</v>
+      </c>
+      <c r="H285" s="12">
+        <f t="shared" si="1"/>
+        <v>285</v>
+      </c>
+    </row>
+    <row r="286">
+      <c r="A286" s="13" t="s">
+        <v>485</v>
+      </c>
+      <c r="B286" s="14">
+        <v>7.0</v>
+      </c>
+      <c r="C286" s="14" t="s">
+        <v>1277</v>
+      </c>
+      <c r="D286" s="14" t="s">
+        <v>1274</v>
+      </c>
+      <c r="E286" s="14" t="s">
+        <v>1273</v>
+      </c>
+      <c r="F286" s="14" t="s">
+        <v>1278</v>
+      </c>
+      <c r="G286" s="14" t="s">
+        <v>1275</v>
+      </c>
+      <c r="H286" s="15">
+        <f t="shared" si="1"/>
+        <v>286</v>
+      </c>
+    </row>
+    <row r="287">
+      <c r="A287" s="10" t="s">
+        <v>485</v>
+      </c>
+      <c r="B287" s="11">
+        <v>7.0</v>
+      </c>
+      <c r="C287" s="11" t="s">
+        <v>1279</v>
+      </c>
+      <c r="D287" s="11" t="s">
+        <v>1280</v>
+      </c>
+      <c r="E287" s="11" t="s">
+        <v>1281</v>
+      </c>
+      <c r="F287" s="11" t="s">
+        <v>1282</v>
+      </c>
+      <c r="G287" s="11" t="s">
+        <v>1283</v>
+      </c>
+      <c r="H287" s="12">
+        <f t="shared" si="1"/>
+        <v>287</v>
+      </c>
+    </row>
+    <row r="288">
+      <c r="A288" s="13" t="s">
+        <v>485</v>
+      </c>
+      <c r="B288" s="14">
+        <v>7.0</v>
+      </c>
+      <c r="C288" s="14" t="s">
+        <v>1284</v>
+      </c>
+      <c r="D288" s="14" t="s">
+        <v>1285</v>
+      </c>
+      <c r="E288" s="14" t="s">
+        <v>1286</v>
+      </c>
+      <c r="F288" s="14" t="s">
+        <v>1287</v>
+      </c>
+      <c r="G288" s="14" t="s">
+        <v>1288</v>
+      </c>
+      <c r="H288" s="15">
+        <f t="shared" si="1"/>
+        <v>288</v>
+      </c>
+    </row>
+    <row r="289">
+      <c r="A289" s="10" t="s">
+        <v>485</v>
+      </c>
+      <c r="B289" s="11">
+        <v>7.0</v>
+      </c>
+      <c r="C289" s="11" t="s">
+        <v>1289</v>
+      </c>
+      <c r="D289" s="11" t="s">
+        <v>1137</v>
+      </c>
+      <c r="E289" s="11" t="s">
+        <v>1290</v>
+      </c>
+      <c r="F289" s="11" t="s">
+        <v>1291</v>
+      </c>
+      <c r="G289" s="11" t="s">
+        <v>1292</v>
+      </c>
+      <c r="H289" s="12">
+        <f t="shared" si="1"/>
+        <v>289</v>
+      </c>
+    </row>
+    <row r="290">
+      <c r="A290" s="13" t="s">
+        <v>485</v>
+      </c>
+      <c r="B290" s="14">
+        <v>7.0</v>
+      </c>
+      <c r="C290" s="14" t="s">
+        <v>1293</v>
+      </c>
+      <c r="D290" s="14" t="s">
+        <v>1294</v>
+      </c>
+      <c r="E290" s="14" t="s">
+        <v>1295</v>
+      </c>
+      <c r="F290" s="14" t="s">
+        <v>1296</v>
+      </c>
+      <c r="G290" s="14" t="s">
+        <v>1297</v>
+      </c>
+      <c r="H290" s="15">
+        <f t="shared" si="1"/>
+        <v>290</v>
+      </c>
+    </row>
+    <row r="291">
+      <c r="A291" s="10" t="s">
+        <v>485</v>
+      </c>
+      <c r="B291" s="11">
+        <v>7.0</v>
+      </c>
+      <c r="C291" s="11" t="s">
+        <v>1298</v>
+      </c>
+      <c r="D291" s="11" t="s">
+        <v>1299</v>
+      </c>
+      <c r="E291" s="11" t="s">
+        <v>1300</v>
+      </c>
+      <c r="F291" s="11" t="s">
+        <v>1301</v>
+      </c>
+      <c r="G291" s="11" t="s">
+        <v>1302</v>
+      </c>
+      <c r="H291" s="12">
+        <f t="shared" si="1"/>
+        <v>291</v>
+      </c>
+    </row>
+    <row r="292">
+      <c r="A292" s="13" t="s">
+        <v>485</v>
+      </c>
+      <c r="B292" s="14">
+        <v>7.0</v>
+      </c>
+      <c r="C292" s="14" t="s">
+        <v>1303</v>
+      </c>
+      <c r="D292" s="14" t="s">
+        <v>1304</v>
+      </c>
+      <c r="E292" s="14" t="s">
+        <v>1305</v>
+      </c>
+      <c r="F292" s="14" t="s">
+        <v>1306</v>
+      </c>
+      <c r="G292" s="14" t="s">
+        <v>1307</v>
+      </c>
+      <c r="H292" s="15">
+        <f t="shared" si="1"/>
+        <v>292</v>
+      </c>
+    </row>
+    <row r="293">
+      <c r="A293" s="10" t="s">
+        <v>485</v>
+      </c>
+      <c r="B293" s="11">
+        <v>8.0</v>
+      </c>
+      <c r="C293" s="11" t="s">
+        <v>1308</v>
+      </c>
+      <c r="D293" s="11" t="s">
+        <v>1202</v>
+      </c>
+      <c r="E293" s="11" t="s">
+        <v>1309</v>
+      </c>
+      <c r="F293" s="11" t="s">
+        <v>1310</v>
+      </c>
+      <c r="G293" s="11" t="s">
+        <v>1311</v>
+      </c>
+      <c r="H293" s="12">
+        <f t="shared" si="1"/>
+        <v>293</v>
+      </c>
+    </row>
+    <row r="294">
+      <c r="A294" s="13" t="s">
+        <v>485</v>
+      </c>
+      <c r="B294" s="14">
+        <v>8.0</v>
+      </c>
+      <c r="C294" s="14" t="s">
+        <v>1312</v>
+      </c>
+      <c r="D294" s="14" t="s">
+        <v>1313</v>
+      </c>
+      <c r="E294" s="14" t="s">
+        <v>1204</v>
+      </c>
+      <c r="F294" s="14" t="s">
+        <v>1314</v>
+      </c>
+      <c r="G294" s="14" t="s">
+        <v>1315</v>
+      </c>
+      <c r="H294" s="15">
+        <f t="shared" si="1"/>
+        <v>294</v>
+      </c>
+    </row>
+    <row r="295">
+      <c r="A295" s="10" t="s">
+        <v>485</v>
+      </c>
+      <c r="B295" s="11">
+        <v>8.0</v>
+      </c>
+      <c r="C295" s="11" t="s">
+        <v>1316</v>
+      </c>
+      <c r="D295" s="11" t="s">
+        <v>1317</v>
+      </c>
+      <c r="E295" s="11" t="s">
+        <v>1318</v>
+      </c>
+      <c r="F295" s="11" t="s">
+        <v>1319</v>
+      </c>
+      <c r="G295" s="11" t="s">
+        <v>1320</v>
+      </c>
+      <c r="H295" s="12">
+        <f t="shared" si="1"/>
+        <v>295</v>
+      </c>
+    </row>
+    <row r="296">
+      <c r="A296" s="13" t="s">
+        <v>485</v>
+      </c>
+      <c r="B296" s="14">
+        <v>8.0</v>
+      </c>
+      <c r="C296" s="14" t="s">
+        <v>1321</v>
+      </c>
+      <c r="D296" s="14" t="s">
+        <v>1322</v>
+      </c>
+      <c r="E296" s="14" t="s">
+        <v>1323</v>
+      </c>
+      <c r="F296" s="14" t="s">
+        <v>1324</v>
+      </c>
+      <c r="G296" s="14" t="s">
+        <v>1325</v>
+      </c>
+      <c r="H296" s="15">
+        <f t="shared" si="1"/>
+        <v>296</v>
+      </c>
+    </row>
+    <row r="297">
+      <c r="A297" s="10" t="s">
+        <v>485</v>
+      </c>
+      <c r="B297" s="11">
+        <v>8.0</v>
+      </c>
+      <c r="C297" s="11" t="s">
+        <v>1326</v>
+      </c>
+      <c r="D297" s="11" t="s">
+        <v>1327</v>
+      </c>
+      <c r="E297" s="11" t="s">
+        <v>1328</v>
+      </c>
+      <c r="F297" s="11" t="s">
+        <v>1329</v>
+      </c>
+      <c r="G297" s="11" t="s">
+        <v>1330</v>
+      </c>
+      <c r="H297" s="12">
+        <f t="shared" si="1"/>
+        <v>297</v>
+      </c>
+    </row>
+    <row r="298">
+      <c r="A298" s="13" t="s">
+        <v>485</v>
+      </c>
+      <c r="B298" s="14">
+        <v>8.0</v>
+      </c>
+      <c r="C298" s="14" t="s">
+        <v>1331</v>
+      </c>
+      <c r="D298" s="14" t="s">
+        <v>1332</v>
+      </c>
+      <c r="E298" s="14" t="s">
+        <v>1333</v>
+      </c>
+      <c r="F298" s="14" t="s">
+        <v>1334</v>
+      </c>
+      <c r="G298" s="14" t="s">
+        <v>1335</v>
+      </c>
+      <c r="H298" s="15">
+        <f t="shared" si="1"/>
+        <v>298</v>
+      </c>
+    </row>
+    <row r="299">
+      <c r="A299" s="10" t="s">
+        <v>485</v>
+      </c>
+      <c r="B299" s="11">
+        <v>8.0</v>
+      </c>
+      <c r="C299" s="11" t="s">
+        <v>1336</v>
+      </c>
+      <c r="D299" s="11" t="s">
+        <v>1337</v>
+      </c>
+      <c r="E299" s="11" t="s">
+        <v>1338</v>
+      </c>
+      <c r="F299" s="11" t="s">
+        <v>1339</v>
+      </c>
+      <c r="G299" s="11" t="s">
+        <v>1340</v>
+      </c>
+      <c r="H299" s="12">
+        <f t="shared" si="1"/>
+        <v>299</v>
+      </c>
+    </row>
+    <row r="300">
+      <c r="A300" s="13" t="s">
+        <v>485</v>
+      </c>
+      <c r="B300" s="14">
+        <v>9.0</v>
+      </c>
+      <c r="C300" s="14" t="s">
+        <v>1341</v>
+      </c>
+      <c r="D300" s="14" t="s">
+        <v>1342</v>
+      </c>
+      <c r="E300" s="14" t="s">
+        <v>1343</v>
+      </c>
+      <c r="F300" s="14" t="s">
+        <v>1344</v>
+      </c>
+      <c r="G300" s="14" t="s">
+        <v>1345</v>
+      </c>
+      <c r="H300" s="15">
+        <f t="shared" si="1"/>
+        <v>300</v>
+      </c>
+    </row>
+    <row r="301">
+      <c r="A301" s="10" t="s">
+        <v>485</v>
+      </c>
+      <c r="B301" s="11">
+        <v>9.0</v>
+      </c>
+      <c r="C301" s="11" t="s">
+        <v>1346</v>
+      </c>
+      <c r="D301" s="11" t="s">
+        <v>1347</v>
+      </c>
+      <c r="E301" s="11" t="s">
+        <v>1348</v>
+      </c>
+      <c r="F301" s="11" t="s">
+        <v>1349</v>
+      </c>
+      <c r="G301" s="11" t="s">
+        <v>1350</v>
+      </c>
+      <c r="H301" s="12">
+        <f t="shared" si="1"/>
+        <v>301</v>
+      </c>
+    </row>
+    <row r="302">
+      <c r="A302" s="13" t="s">
+        <v>485</v>
+      </c>
+      <c r="B302" s="14">
+        <v>9.0</v>
+      </c>
+      <c r="C302" s="14" t="s">
+        <v>1351</v>
+      </c>
+      <c r="D302" s="14" t="s">
+        <v>1352</v>
+      </c>
+      <c r="E302" s="14" t="s">
+        <v>1353</v>
+      </c>
+      <c r="F302" s="14" t="s">
+        <v>1354</v>
+      </c>
+      <c r="G302" s="14" t="s">
+        <v>1355</v>
+      </c>
+      <c r="H302" s="15">
+        <f t="shared" si="1"/>
+        <v>302</v>
+      </c>
+    </row>
+    <row r="303">
+      <c r="A303" s="20" t="s">
+        <v>485</v>
+      </c>
+      <c r="B303" s="21">
+        <v>9.0</v>
+      </c>
+      <c r="C303" s="21" t="s">
+        <v>1356</v>
+      </c>
+      <c r="D303" s="21" t="s">
+        <v>1357</v>
+      </c>
+      <c r="E303" s="21" t="s">
+        <v>1358</v>
+      </c>
+      <c r="F303" s="21" t="s">
+        <v>1359</v>
+      </c>
+      <c r="G303" s="21" t="s">
+        <v>1360</v>
+      </c>
+      <c r="H303" s="22">
+        <f t="shared" si="1"/>
+        <v>303</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Added weather, weather figure buttons, and questions download button
</commit_message>
<xml_diff>
--- a/public/questions.xlsx
+++ b/public/questions.xlsx
@@ -6,14 +6,14 @@
     <sheet state="visible" name="Sheet1" sheetId="1" r:id="rId4"/>
   </sheets>
   <definedNames>
-    <definedName hidden="1" localSheetId="0" name="_xlnm._FilterDatabase">Sheet1!$A$1:$H$349</definedName>
+    <definedName hidden="1" localSheetId="0" name="_xlnm._FilterDatabase">Sheet1!$A$1:$H$403</definedName>
   </definedNames>
   <calcPr/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2069" uniqueCount="1568">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2389" uniqueCount="1825">
   <si>
     <t>Topic</t>
   </si>
@@ -4605,7 +4605,7 @@
     <t>Cirrus</t>
   </si>
   <si>
-    <t>Throughout your flight the winds you are experiencing have been consistent and predictable. What kind of airmass would you expect to be in?</t>
+    <t>Throughout your flight the winds you are experiencing have been consistent and predictable. What kind of air mass would you expect to be in?</t>
   </si>
   <si>
     <t>Warm</t>
@@ -4717,6 +4717,778 @@
   </si>
   <si>
     <t>Tropical Wave</t>
+  </si>
+  <si>
+    <t>Steady precipitation preceding a front is an indication of</t>
+  </si>
+  <si>
+    <t>Stratiform clouds with little or no turbulence</t>
+  </si>
+  <si>
+    <t>Stratiform clouds with moderate turbulence</t>
+  </si>
+  <si>
+    <t>Cumuliform clouds with little or no turbulence</t>
+  </si>
+  <si>
+    <t>Cumuliform clouds with moderate turbulence</t>
+  </si>
+  <si>
+    <t>What are characteristics of a moist, unstable air mass?</t>
+  </si>
+  <si>
+    <t>Cumuliform clouds and showery precipitation</t>
+  </si>
+  <si>
+    <t>Stratiform clouds and showery precipitation</t>
+  </si>
+  <si>
+    <t>Poor visibility and smooth air</t>
+  </si>
+  <si>
+    <t>Gusty winds and rime icing</t>
+  </si>
+  <si>
+    <t>At approximately what altitude above the surface would the pilot expect the base of cumuliform clouds if the surface air temperature is 27° C and the dewpoint is 3° C?</t>
+  </si>
+  <si>
+    <t>11000 AGL</t>
+  </si>
+  <si>
+    <t>10000 AGL</t>
+  </si>
+  <si>
+    <t>9000 AGL</t>
+  </si>
+  <si>
+    <t>12000 AGL</t>
+  </si>
+  <si>
+    <t>A TAF includes:</t>
+  </si>
+  <si>
+    <t>Wind, visibility, weather phenomena, obstructions to vision, and cloud coverage</t>
+  </si>
+  <si>
+    <t>Wind, visibility, cloud coverage, and cloud tops in feet MSL</t>
+  </si>
+  <si>
+    <t>Wind, obstructions to vision, and cloud tops in feet MSL</t>
+  </si>
+  <si>
+    <t>Wind, visibility, weather phenomena, obstructions to vision, cloud coverage, and cloud tops in feet MSL</t>
+  </si>
+  <si>
+    <t>While flying over mountainous terrain you see clouds with extensive vertical development. What does this indicate?</t>
+  </si>
+  <si>
+    <t>An unstable air mass over the mountains</t>
+  </si>
+  <si>
+    <t>You are in a stable air mass</t>
+  </si>
+  <si>
+    <t>Dry air</t>
+  </si>
+  <si>
+    <t>You are flying in are colder than the ground</t>
+  </si>
+  <si>
+    <t>Frost on the wing of an airplane:</t>
+  </si>
+  <si>
+    <t>Shall always be removed before flying</t>
+  </si>
+  <si>
+    <t>Causes no problem due to its smooth surface</t>
+  </si>
+  <si>
+    <t>Should only be removed if it has an extremely rough texture</t>
+  </si>
+  <si>
+    <t>Should be scrapped off before flying</t>
+  </si>
+  <si>
+    <t>The amount of water vapor which air can hold depends on the</t>
+  </si>
+  <si>
+    <t>air temperature</t>
+  </si>
+  <si>
+    <t>stability of the air</t>
+  </si>
+  <si>
+    <t>dewpoint</t>
+  </si>
+  <si>
+    <t>relative humidity</t>
+  </si>
+  <si>
+    <t>A nonfrontal, narrow band of active thunderstorms that often develop ahead of a cold front is a known as a</t>
+  </si>
+  <si>
+    <t>Prefrontal System</t>
+  </si>
+  <si>
+    <t>Dry line</t>
+  </si>
+  <si>
+    <t>One in-flight condition necessary for structural icing to form is</t>
+  </si>
+  <si>
+    <t>visible moisture</t>
+  </si>
+  <si>
+    <t>small temperature/dewpoint spread</t>
+  </si>
+  <si>
+    <t>stratiform clouds</t>
+  </si>
+  <si>
+    <t>ground temperature below freezing</t>
+  </si>
+  <si>
+    <t>Clouds are divided into four families according to their</t>
+  </si>
+  <si>
+    <t>height range</t>
+  </si>
+  <si>
+    <t>outward shape</t>
+  </si>
+  <si>
+    <t>composition</t>
+  </si>
+  <si>
+    <t>stability</t>
+  </si>
+  <si>
+    <t>One weather phenomenon which will always occur when flying across a front is a change in the</t>
+  </si>
+  <si>
+    <t>wind direction</t>
+  </si>
+  <si>
+    <t>stability of the air mass</t>
+  </si>
+  <si>
+    <t>type of precipitation</t>
+  </si>
+  <si>
+    <t>cloud type</t>
+  </si>
+  <si>
+    <t>What is meant by the term 'dewpoint'?</t>
+  </si>
+  <si>
+    <t>The temperature to which air must be cooled to become saturated</t>
+  </si>
+  <si>
+    <t>The temperature at which dew will always form</t>
+  </si>
+  <si>
+    <t>The temperature at which condensation and evaporation are equal</t>
+  </si>
+  <si>
+    <t>The temperature at which clouds begin to form</t>
+  </si>
+  <si>
+    <t>Upon encountering severe turbulence, which flight condition should the pilot attempt to maintain?</t>
+  </si>
+  <si>
+    <t>Pitch and bank and keep level attitude</t>
+  </si>
+  <si>
+    <t>Constant altitude and airspeed</t>
+  </si>
+  <si>
+    <t>Constant angle of attack</t>
+  </si>
+  <si>
+    <t>Current airplane attitude</t>
+  </si>
+  <si>
+    <t>Aviation Routine Weather reports (METARs) contain</t>
+  </si>
+  <si>
+    <t>Wind, visibility, precipitation, cloud coverage, temperature, and altimeter setting</t>
+  </si>
+  <si>
+    <t>Wind, visibility, and precipitation</t>
+  </si>
+  <si>
+    <t>Wind, visibility, precipitation, and temperature</t>
+  </si>
+  <si>
+    <t>Wind, visibility, precipitation, cloud coverage, temperature, humidity, and altimeter setting</t>
+  </si>
+  <si>
+    <t>Inland fog is most likely</t>
+  </si>
+  <si>
+    <t>Radiation fog</t>
+  </si>
+  <si>
+    <t>Advection fog</t>
+  </si>
+  <si>
+    <t>Upslope fog</t>
+  </si>
+  <si>
+    <t>Precipitation Induced fog</t>
+  </si>
+  <si>
+    <t>You define an air mass as</t>
+  </si>
+  <si>
+    <t>Large bodies of air with a uniform temperature and moisture.</t>
+  </si>
+  <si>
+    <t>Low pressure areas</t>
+  </si>
+  <si>
+    <t>High pressure areas</t>
+  </si>
+  <si>
+    <t>Large bodies of air with a uniform temperature</t>
+  </si>
+  <si>
+    <t>In which situation is advection fog most likely to form</t>
+  </si>
+  <si>
+    <t>An air mass moving inland from the coast in winter</t>
+  </si>
+  <si>
+    <t>A warm, moist air mass on the windward side of mountains</t>
+  </si>
+  <si>
+    <t>A light breeze blowing colder air out to sea</t>
+  </si>
+  <si>
+    <t>At night on clear, calm evenings after the sun has set</t>
+  </si>
+  <si>
+    <t>If an unstable air mass is forced upward, what type clouds can be expected?</t>
+  </si>
+  <si>
+    <t>Clouds with considerable vertical development and associated turbulence</t>
+  </si>
+  <si>
+    <t>Stratus clouds with little vertical development</t>
+  </si>
+  <si>
+    <t>Stratus clouds with considerable associated turbulence</t>
+  </si>
+  <si>
+    <t>Cumulus clouds with rime icing risk</t>
+  </si>
+  <si>
+    <t>On a TAF, the broken cloud layer written as, BKN250 indicates:</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> A broken cloud layer at 25,000 feet AGL</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> A broken cloud layer at 2,500 feet AGL</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> A broken cloud layer at 250 feet AGL</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> A broken cloud layer at 2,500 feet MSL</t>
+  </si>
+  <si>
+    <t>Every physical process of weather is accompanied by, or is the result of, a:</t>
+  </si>
+  <si>
+    <t>heat exchange</t>
+  </si>
+  <si>
+    <t>movement of air</t>
+  </si>
+  <si>
+    <t>pressure differential</t>
+  </si>
+  <si>
+    <t>temperature inversion</t>
+  </si>
+  <si>
+    <t>Which is true with respect to a high - or low-pressure system</t>
+  </si>
+  <si>
+    <t>A high-pressure area or ridge is an area of descending air</t>
+  </si>
+  <si>
+    <t>A low-pressure area or trough is an area of descending air</t>
+  </si>
+  <si>
+    <t>A high-pressure area or ridge is an area of rising air</t>
+  </si>
+  <si>
+    <t>A low-pressure area or trough is an area of hot air</t>
+  </si>
+  <si>
+    <t>What situation is most conducive to the formation of radiation fog?</t>
+  </si>
+  <si>
+    <t>Warm, moist air over low, flatland areas on clear, calm nights</t>
+  </si>
+  <si>
+    <t>The movement of cold air over much warmer water</t>
+  </si>
+  <si>
+    <t>Moist, tropical air moving over cold, offshore water</t>
+  </si>
+  <si>
+    <t>What is the approximate base of the cumulus clouds if the surface air temperature at 1,000' MSL is 21° C and the dewpoint is 9° C?</t>
+  </si>
+  <si>
+    <t>6,000' MSL</t>
+  </si>
+  <si>
+    <t>5,000' MSL</t>
+  </si>
+  <si>
+    <t>7,000' MSL</t>
+  </si>
+  <si>
+    <t>8,000' MSL</t>
+  </si>
+  <si>
+    <t>The most frequent type of ground or surface-based temperature inversion is that which is produced by</t>
+  </si>
+  <si>
+    <t>terrestrial radiation on a clear, relatively still night</t>
+  </si>
+  <si>
+    <t>warm air being lifted rapidly aloft in the vicinity of mountainous terrain</t>
+  </si>
+  <si>
+    <t>the movement of colder air under warm air, or the movement of warm air over cold air</t>
+  </si>
+  <si>
+    <t>surface air remaining cool under the shade of clouds</t>
+  </si>
+  <si>
+    <t>When avoiding a thunderstorm, which of the following course of action would you select first?</t>
+  </si>
+  <si>
+    <t>Flying over the thunderstorm at 1000' over the top per 10 kt wind speed at top</t>
+  </si>
+  <si>
+    <t>Flying under the thunderstorm within the lower 1/3 of the distance between the ground and the cloud base</t>
+  </si>
+  <si>
+    <t>Flying through the thunderstorm by penetrating the lower 1/3 of the storm straight in</t>
+  </si>
+  <si>
+    <t>Flying under the thunderstorm at 1000' below the base per 10 kt wind speed at base as able</t>
+  </si>
+  <si>
+    <t>Fog occurs when:</t>
+  </si>
+  <si>
+    <t>cloud base is within 50' of the ground, greater than 20' thick, and visibility is less than 5/8 sm</t>
+  </si>
+  <si>
+    <t>cloud base is within 50' of the ground, greater than 20' thick, and visibility is less than 5/8 nm</t>
+  </si>
+  <si>
+    <t>cloud base is within 50' of the ground and visibility is less than 5/8 sm</t>
+  </si>
+  <si>
+    <t>cloud base is on the surface, greater than 20' thick, and visibility is less than 1/2 sm</t>
+  </si>
+  <si>
+    <t>For fog to form, what is required?</t>
+  </si>
+  <si>
+    <t>Condensation nuclei, low temp/dew point spread, and light surface winds</t>
+  </si>
+  <si>
+    <t>Warm moist air flowing over cold ground which causes condensation</t>
+  </si>
+  <si>
+    <t>Visible moisture, free air temp below freezing, and light surface winds</t>
+  </si>
+  <si>
+    <t>High relative humidity, unstable air, and strong surface winds</t>
+  </si>
+  <si>
+    <t>Thermal turbulence results from</t>
+  </si>
+  <si>
+    <t>Air heated from below</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Frontal lifting that is associated with the passage of a cold front
+</t>
+  </si>
+  <si>
+    <t>A warm front passing over an area</t>
+  </si>
+  <si>
+    <t>The most hazardous aspect of structural icing is</t>
+  </si>
+  <si>
+    <t>Its aerodynamic effects on the airfoil, decreasing lift, thrust and range while increasing drag, weight, fuel consumption, and stall speed</t>
+  </si>
+  <si>
+    <t>Its aerodynamic effects on the airfoil, decreasing lift, drag, and thrust while increasing range, weight, fuel consumption, and stall speed</t>
+  </si>
+  <si>
+    <t>The structural damage is can cause on the airfoil and control surfaces</t>
+  </si>
+  <si>
+    <t>The decreases in reliability it can cause on instruments via pitot tube blockage, static port blockage, and carburetor icing</t>
+  </si>
+  <si>
+    <t>Gust fronts occur ______ miles in front of an approaching _____</t>
+  </si>
+  <si>
+    <t>5-20, thunderstorm</t>
+  </si>
+  <si>
+    <t>50-300, thunderstorm</t>
+  </si>
+  <si>
+    <t>5-20, cold front</t>
+  </si>
+  <si>
+    <t>50-300, cold front</t>
+  </si>
+  <si>
+    <t>How are Prognostic Charts best used by a pilot?</t>
+  </si>
+  <si>
+    <t>For big picture planning and general areas to avoid</t>
+  </si>
+  <si>
+    <t>For analyzing current frontal activity and cloud coverage</t>
+  </si>
+  <si>
+    <t>For overall planning at all altitudes</t>
+  </si>
+  <si>
+    <t>To anticipate arrival and departure weather at the intended airports</t>
+  </si>
+  <si>
+    <t>What could be indicated when a current CONVECTIVE SIGMET forecasts thunderstorms?</t>
+  </si>
+  <si>
+    <t>Severe or embedded storms for more than 30 mins</t>
+  </si>
+  <si>
+    <t>Moderate thunderstorms with very high radar reflectivity covering 30% of the area.</t>
+  </si>
+  <si>
+    <t>Moderate or severe turbulence</t>
+  </si>
+  <si>
+    <t>50 miles long line with storms affecting 40% of its length</t>
+  </si>
+  <si>
+    <t>For which of these is a convective SIGMET issued?</t>
+  </si>
+  <si>
+    <t>Line of thunderstorms 60 miles long line with thunderstorms affecting 40% of its length</t>
+  </si>
+  <si>
+    <t>Volcanic ash</t>
+  </si>
+  <si>
+    <t>Dust storms and/or sandstorms lowering visibility to less than 3 miles</t>
+  </si>
+  <si>
+    <t>Severe/Extreme turbulence or severe icing not associated with thunderstorms</t>
+  </si>
+  <si>
+    <t>For which of these is an AIRMET issued?</t>
+  </si>
+  <si>
+    <t>Moderate turbulence, strong surface winds above 30 kts, moderate structural icing</t>
+  </si>
+  <si>
+    <t>Severe icing and severe/extreme turbulence</t>
+  </si>
+  <si>
+    <t>Area of severe thunderstorms covering at least 40% of the are concerned</t>
+  </si>
+  <si>
+    <t>For conditions associated with hurricanes, how long are non-convective SIGMETs issued for?</t>
+  </si>
+  <si>
+    <t>6 hours</t>
+  </si>
+  <si>
+    <t>2 hours</t>
+  </si>
+  <si>
+    <t>4 hours</t>
+  </si>
+  <si>
+    <t>1 hour</t>
+  </si>
+  <si>
+    <t>If severe low level wind shear is detected, specifically wind shifts over 20 kts below 2,000' AGL, what do you expect to be issued?</t>
+  </si>
+  <si>
+    <t>AIRMET</t>
+  </si>
+  <si>
+    <t>Non-convective SIGMET</t>
+  </si>
+  <si>
+    <t>SIGMET</t>
+  </si>
+  <si>
+    <t>If fog is present, which of these would you most expect to see on a METAR?</t>
+  </si>
+  <si>
+    <t>VV002</t>
+  </si>
+  <si>
+    <t>OVC002</t>
+  </si>
+  <si>
+    <t>BKN004</t>
+  </si>
+  <si>
+    <t>OVC001</t>
+  </si>
+  <si>
+    <t>What kinds of visibility can be present on METARS/TAFS?</t>
+  </si>
+  <si>
+    <t>Prevailing visibility and runway visual range</t>
+  </si>
+  <si>
+    <t>Prevailing visibility and flight visibility</t>
+  </si>
+  <si>
+    <t>Flight visibility and runway visual range</t>
+  </si>
+  <si>
+    <t>Flight visibility and slant range visibility</t>
+  </si>
+  <si>
+    <t>Prevailing visibility is defined as:</t>
+  </si>
+  <si>
+    <t>The greatest horizontal visibility through at least half of the horizon circle</t>
+  </si>
+  <si>
+    <t>The minimum horizontal visibility anywhere on the horizon circle</t>
+  </si>
+  <si>
+    <t>The average horizontal visibility across the horizon circle</t>
+  </si>
+  <si>
+    <t>The maximum horizontal visibility anywhere on the horizon circle</t>
+  </si>
+  <si>
+    <t>(Refer to figure 17.) What wind is forecast for AMA at 12,000 feet?</t>
+  </si>
+  <si>
+    <t>260° true at 25 knots.</t>
+  </si>
+  <si>
+    <t>260° magnetic at 25 knots.</t>
+  </si>
+  <si>
+    <t>250° true at 26 knots.</t>
+  </si>
+  <si>
+    <t>250° magnetic at 26 knots.</t>
+  </si>
+  <si>
+    <t>(Refer to figure 17.) Determine the wind and temperature aloft forecast for STL at 34,000 feet.</t>
+  </si>
+  <si>
+    <t>230° true at 119 knots, temperature -60°C.</t>
+  </si>
+  <si>
+    <t>230° true at 19 knots, temperature 60°C.</t>
+  </si>
+  <si>
+    <t>730° true at 19 knots, temperature -60°C.</t>
+  </si>
+  <si>
+    <t>230° magnetic at 19 knots, temperature -60°C.</t>
+  </si>
+  <si>
+    <t>(Refer to figure 15.) What is the valid period for the TAF for KMEM?</t>
+  </si>
+  <si>
+    <t>1800Z on the 12th to 2400Z on the 13th</t>
+  </si>
+  <si>
+    <t>1200Z to 1800Z</t>
+  </si>
+  <si>
+    <t>1218Z to 1324Z</t>
+  </si>
+  <si>
+    <t>121720Z to 131720Z</t>
+  </si>
+  <si>
+    <t>(Refer to figure 15.) Between 1000Z and 1200Z the visibility at KMEM is forecast to be?</t>
+  </si>
+  <si>
+    <t>3 sm</t>
+  </si>
+  <si>
+    <t>6 sm</t>
+  </si>
+  <si>
+    <t>1/2 sm</t>
+  </si>
+  <si>
+    <t>5 sm</t>
+  </si>
+  <si>
+    <t>(Refer to figure 15.) In the TAF from KOKC, the clear sky becomes</t>
+  </si>
+  <si>
+    <t>overcast at 2,000 feet during the forecast period between 2200Z and 2400Z</t>
+  </si>
+  <si>
+    <t>overcast at 200 feet with a 40 percent probability of becoming overcast at 600 feet during the forecast period between 2200Z and 2400Z</t>
+  </si>
+  <si>
+    <t>overcast at 200 feet with the probability of becoming overcast at 400 feet during the forecast period between 2200Z and 2400Z</t>
+  </si>
+  <si>
+    <t>with a 40 percent probability of overcast at 800 feet during the forecast period between 0000Z and 0600Z</t>
+  </si>
+  <si>
+    <t>(Refer to figure 15.) In the TAF from KOKC, the 'FM (FROM) Group' is forecast for the hours from 1600Z to 2200Z with the wind from</t>
+  </si>
+  <si>
+    <t>180° at 10 knots.</t>
+  </si>
+  <si>
+    <t>160° at 10 knots.</t>
+  </si>
+  <si>
+    <t>180° at 10 knots, becoming 200° at 13 knots.</t>
+  </si>
+  <si>
+    <t>140° at 8 knots.</t>
+  </si>
+  <si>
+    <t>(Refer to figure 15.) In the TAF for KMEM, from 2000Z to 2200Z what kind of condition could happen?</t>
+  </si>
+  <si>
+    <t>Rain showers and thunderstorms</t>
+  </si>
+  <si>
+    <t>Mist</t>
+  </si>
+  <si>
+    <t>Haze</t>
+  </si>
+  <si>
+    <t>Fog</t>
+  </si>
+  <si>
+    <t>(Refer to figure 15.) In the TAF for KMEM, what is the prevailing visibility at 1500Z?</t>
+  </si>
+  <si>
+    <t>Greater than 6 sm</t>
+  </si>
+  <si>
+    <t>(Refer to figure 12.) What are the wind conditions at Wink, Texas (KINK)?</t>
+  </si>
+  <si>
+    <t>110° true at 12 knots, gusts 18 knots.</t>
+  </si>
+  <si>
+    <t>110° magnetic at 12 knots, gusts 18 knots.</t>
+  </si>
+  <si>
+    <t>Calm</t>
+  </si>
+  <si>
+    <t>110° magnetic at 12 knots, up to greater than 18 knots.</t>
+  </si>
+  <si>
+    <t>(Refer to figure 12.) What are the current conditions depicted for Chicago Midway Airport (KMDW)?</t>
+  </si>
+  <si>
+    <t>Sky 700 feet overcast, visibility 1-1/2SM, moderate rain.</t>
+  </si>
+  <si>
+    <t>Sky 7000 feet overcast, visibility 1-1/2SM, heavy rain</t>
+  </si>
+  <si>
+    <t>Sky 700 feet overcast, visibility 11, occasionally 2SM, with light rain</t>
+  </si>
+  <si>
+    <t>Sky 700 feet overcast, visibility 1-1/2SM, dewpoint 17°C</t>
+  </si>
+  <si>
+    <t>(Refer to figure 4.) Which of these is true according to the Houston TAF?</t>
+  </si>
+  <si>
+    <t>At 0100Z there is light showering rain</t>
+  </si>
+  <si>
+    <t>At 0000Z, light thunderstorms with rain can be expected</t>
+  </si>
+  <si>
+    <t>Visibility is greater than 9999 feet at 1600Z</t>
+  </si>
+  <si>
+    <t>The clouding ceiling is at 1,500' AGL at 1700Z</t>
+  </si>
+  <si>
+    <t>(Refer to figure 4.) What is the ceiling at 2000Z according to the Houston TAF?</t>
+  </si>
+  <si>
+    <t>BKN at 1000' AGL with cumulonimbus clouds</t>
+  </si>
+  <si>
+    <t>BKN at 1000' MSL</t>
+  </si>
+  <si>
+    <t>There is no ceiling</t>
+  </si>
+  <si>
+    <t>OVC at 800' AGL</t>
+  </si>
+  <si>
+    <t>(Refer to figure 5.) What are the wind conditions at KJKA?</t>
+  </si>
+  <si>
+    <t>Winds from the Southeast at 10 kts gusting to 16 kts</t>
+  </si>
+  <si>
+    <t>Winds from the Southeast at 5 kts gusting to 16 kts</t>
+  </si>
+  <si>
+    <t>Winds to the Southeast at 10 kts gusting to 16 kts</t>
+  </si>
+  <si>
+    <t>Winds to the Southeast at 5 kts gusting to 16 kts</t>
+  </si>
+  <si>
+    <t>(Refer to figure 5.) What is the current altimeter setting at KJKA?</t>
+  </si>
+  <si>
+    <t>(Refer to figure 5.) What is the current dew point spread at KJKA?</t>
+  </si>
+  <si>
+    <t>25° F</t>
+  </si>
+  <si>
+    <t>25° C</t>
+  </si>
+  <si>
+    <t>10° C</t>
+  </si>
+  <si>
+    <t>6° C</t>
   </si>
 </sst>
 </file>
@@ -4925,7 +5697,7 @@
   <cellStyleXfs count="1">
     <xf borderId="0" fillId="0" fontId="0" numFmtId="0" applyAlignment="1" applyFont="1"/>
   </cellStyleXfs>
-  <cellXfs count="28">
+  <cellXfs count="30">
     <xf borderId="0" fillId="0" fontId="0" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
       <alignment readingOrder="0" shrinkToFit="0" vertical="bottom" wrapText="0"/>
     </xf>
@@ -5001,6 +5773,12 @@
     <xf borderId="8" fillId="0" fontId="2" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
       <alignment readingOrder="0" shrinkToFit="0" vertical="bottom" wrapText="0"/>
     </xf>
+    <xf borderId="5" fillId="0" fontId="1" numFmtId="3" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1" applyNumberFormat="1">
+      <alignment readingOrder="0" shrinkToFit="0" vertical="center" wrapText="0"/>
+    </xf>
+    <xf borderId="8" fillId="0" fontId="1" numFmtId="3" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1" applyNumberFormat="1">
+      <alignment readingOrder="0" shrinkToFit="0" vertical="center" wrapText="0"/>
+    </xf>
     <xf borderId="10" fillId="0" fontId="1" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
       <alignment readingOrder="0" shrinkToFit="0" vertical="center" wrapText="0"/>
     </xf>
@@ -5068,8 +5846,8 @@
 </file>
 
 <file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" ref="A1:H349" displayName="Table1" name="Table1" id="1">
-  <autoFilter ref="$A$1:$H$349"/>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" ref="A1:H403" displayName="Table1" name="Table1" id="1">
+  <autoFilter ref="$A$1:$H$403"/>
   <tableColumns count="8">
     <tableColumn name="Topic" id="1"/>
     <tableColumn name="Lecture" id="2"/>
@@ -5345,7 +6123,7 @@
         <v>13</v>
       </c>
       <c r="H2" s="6">
-        <f t="shared" ref="H2:H349" si="1">ROW()</f>
+        <f t="shared" ref="H2:H403" si="1">ROW()</f>
         <v>2</v>
       </c>
     </row>
@@ -13365,7 +14143,7 @@
       </c>
     </row>
     <row r="304">
-      <c r="A304" s="20" t="s">
+      <c r="A304" s="4" t="s">
         <v>1340</v>
       </c>
       <c r="B304" s="10">
@@ -13392,7 +14170,7 @@
       </c>
     </row>
     <row r="305">
-      <c r="A305" s="23" t="s">
+      <c r="A305" s="7" t="s">
         <v>1340</v>
       </c>
       <c r="B305" s="12">
@@ -13419,7 +14197,7 @@
       </c>
     </row>
     <row r="306">
-      <c r="A306" s="20" t="s">
+      <c r="A306" s="4" t="s">
         <v>1340</v>
       </c>
       <c r="B306" s="10">
@@ -13446,7 +14224,7 @@
       </c>
     </row>
     <row r="307">
-      <c r="A307" s="23" t="s">
+      <c r="A307" s="7" t="s">
         <v>1340</v>
       </c>
       <c r="B307" s="12">
@@ -13473,7 +14251,7 @@
       </c>
     </row>
     <row r="308">
-      <c r="A308" s="20" t="s">
+      <c r="A308" s="4" t="s">
         <v>1340</v>
       </c>
       <c r="B308" s="10">
@@ -13500,7 +14278,7 @@
       </c>
     </row>
     <row r="309">
-      <c r="A309" s="23" t="s">
+      <c r="A309" s="7" t="s">
         <v>1340</v>
       </c>
       <c r="B309" s="12">
@@ -13527,7 +14305,7 @@
       </c>
     </row>
     <row r="310">
-      <c r="A310" s="20" t="s">
+      <c r="A310" s="4" t="s">
         <v>1340</v>
       </c>
       <c r="B310" s="10">
@@ -13554,7 +14332,7 @@
       </c>
     </row>
     <row r="311">
-      <c r="A311" s="23" t="s">
+      <c r="A311" s="7" t="s">
         <v>1340</v>
       </c>
       <c r="B311" s="12">
@@ -13581,7 +14359,7 @@
       </c>
     </row>
     <row r="312">
-      <c r="A312" s="20" t="s">
+      <c r="A312" s="4" t="s">
         <v>1340</v>
       </c>
       <c r="B312" s="10">
@@ -13608,7 +14386,7 @@
       </c>
     </row>
     <row r="313">
-      <c r="A313" s="23" t="s">
+      <c r="A313" s="7" t="s">
         <v>1340</v>
       </c>
       <c r="B313" s="12">
@@ -13635,7 +14413,7 @@
       </c>
     </row>
     <row r="314">
-      <c r="A314" s="20" t="s">
+      <c r="A314" s="4" t="s">
         <v>1340</v>
       </c>
       <c r="B314" s="10">
@@ -13662,7 +14440,7 @@
       </c>
     </row>
     <row r="315">
-      <c r="A315" s="23" t="s">
+      <c r="A315" s="7" t="s">
         <v>1340</v>
       </c>
       <c r="B315" s="12">
@@ -13689,7 +14467,7 @@
       </c>
     </row>
     <row r="316">
-      <c r="A316" s="20" t="s">
+      <c r="A316" s="4" t="s">
         <v>1340</v>
       </c>
       <c r="B316" s="10">
@@ -13716,7 +14494,7 @@
       </c>
     </row>
     <row r="317">
-      <c r="A317" s="23" t="s">
+      <c r="A317" s="7" t="s">
         <v>1340</v>
       </c>
       <c r="B317" s="12">
@@ -13743,7 +14521,7 @@
       </c>
     </row>
     <row r="318">
-      <c r="A318" s="20" t="s">
+      <c r="A318" s="4" t="s">
         <v>1340</v>
       </c>
       <c r="B318" s="10">
@@ -13797,7 +14575,7 @@
       </c>
     </row>
     <row r="320">
-      <c r="A320" s="20" t="s">
+      <c r="A320" s="4" t="s">
         <v>1340</v>
       </c>
       <c r="B320" s="10">
@@ -13824,7 +14602,7 @@
       </c>
     </row>
     <row r="321">
-      <c r="A321" s="23" t="s">
+      <c r="A321" s="7" t="s">
         <v>1340</v>
       </c>
       <c r="B321" s="12">
@@ -13851,7 +14629,7 @@
       </c>
     </row>
     <row r="322">
-      <c r="A322" s="20" t="s">
+      <c r="A322" s="4" t="s">
         <v>1340</v>
       </c>
       <c r="B322" s="10">
@@ -13878,7 +14656,7 @@
       </c>
     </row>
     <row r="323">
-      <c r="A323" s="23" t="s">
+      <c r="A323" s="7" t="s">
         <v>1340</v>
       </c>
       <c r="B323" s="12">
@@ -13905,7 +14683,7 @@
       </c>
     </row>
     <row r="324">
-      <c r="A324" s="20" t="s">
+      <c r="A324" s="4" t="s">
         <v>1340</v>
       </c>
       <c r="B324" s="10">
@@ -13932,7 +14710,7 @@
       </c>
     </row>
     <row r="325">
-      <c r="A325" s="23" t="s">
+      <c r="A325" s="7" t="s">
         <v>1340</v>
       </c>
       <c r="B325" s="12">
@@ -13959,7 +14737,7 @@
       </c>
     </row>
     <row r="326">
-      <c r="A326" s="20" t="s">
+      <c r="A326" s="4" t="s">
         <v>1340</v>
       </c>
       <c r="B326" s="10">
@@ -13986,7 +14764,7 @@
       </c>
     </row>
     <row r="327">
-      <c r="A327" s="23" t="s">
+      <c r="A327" s="7" t="s">
         <v>1340</v>
       </c>
       <c r="B327" s="12">
@@ -14013,7 +14791,7 @@
       </c>
     </row>
     <row r="328">
-      <c r="A328" s="20" t="s">
+      <c r="A328" s="4" t="s">
         <v>1340</v>
       </c>
       <c r="B328" s="10">
@@ -14040,7 +14818,7 @@
       </c>
     </row>
     <row r="329">
-      <c r="A329" s="23" t="s">
+      <c r="A329" s="7" t="s">
         <v>1340</v>
       </c>
       <c r="B329" s="12">
@@ -14067,7 +14845,7 @@
       </c>
     </row>
     <row r="330">
-      <c r="A330" s="20" t="s">
+      <c r="A330" s="4" t="s">
         <v>1340</v>
       </c>
       <c r="B330" s="10">
@@ -14094,7 +14872,7 @@
       </c>
     </row>
     <row r="331">
-      <c r="A331" s="23" t="s">
+      <c r="A331" s="7" t="s">
         <v>1340</v>
       </c>
       <c r="B331" s="12">
@@ -14121,7 +14899,7 @@
       </c>
     </row>
     <row r="332">
-      <c r="A332" s="20" t="s">
+      <c r="A332" s="4" t="s">
         <v>1340</v>
       </c>
       <c r="B332" s="10">
@@ -14148,7 +14926,7 @@
       </c>
     </row>
     <row r="333">
-      <c r="A333" s="23" t="s">
+      <c r="A333" s="7" t="s">
         <v>1340</v>
       </c>
       <c r="B333" s="12">
@@ -14175,7 +14953,7 @@
       </c>
     </row>
     <row r="334">
-      <c r="A334" s="20" t="s">
+      <c r="A334" s="4" t="s">
         <v>1340</v>
       </c>
       <c r="B334" s="10">
@@ -14202,7 +14980,7 @@
       </c>
     </row>
     <row r="335">
-      <c r="A335" s="23" t="s">
+      <c r="A335" s="7" t="s">
         <v>1340</v>
       </c>
       <c r="B335" s="12">
@@ -14229,7 +15007,7 @@
       </c>
     </row>
     <row r="336">
-      <c r="A336" s="20" t="s">
+      <c r="A336" s="4" t="s">
         <v>1340</v>
       </c>
       <c r="B336" s="10">
@@ -14256,7 +15034,7 @@
       </c>
     </row>
     <row r="337">
-      <c r="A337" s="23" t="s">
+      <c r="A337" s="7" t="s">
         <v>1340</v>
       </c>
       <c r="B337" s="12">
@@ -14283,7 +15061,7 @@
       </c>
     </row>
     <row r="338">
-      <c r="A338" s="20" t="s">
+      <c r="A338" s="4" t="s">
         <v>1340</v>
       </c>
       <c r="B338" s="10">
@@ -14310,7 +15088,7 @@
       </c>
     </row>
     <row r="339">
-      <c r="A339" s="23" t="s">
+      <c r="A339" s="7" t="s">
         <v>1340</v>
       </c>
       <c r="B339" s="12">
@@ -14337,7 +15115,7 @@
       </c>
     </row>
     <row r="340">
-      <c r="A340" s="20" t="s">
+      <c r="A340" s="4" t="s">
         <v>1340</v>
       </c>
       <c r="B340" s="10">
@@ -14364,7 +15142,7 @@
       </c>
     </row>
     <row r="341">
-      <c r="A341" s="23" t="s">
+      <c r="A341" s="7" t="s">
         <v>1340</v>
       </c>
       <c r="B341" s="12">
@@ -14391,7 +15169,7 @@
       </c>
     </row>
     <row r="342">
-      <c r="A342" s="20" t="s">
+      <c r="A342" s="4" t="s">
         <v>1340</v>
       </c>
       <c r="B342" s="10">
@@ -14418,7 +15196,7 @@
       </c>
     </row>
     <row r="343">
-      <c r="A343" s="23" t="s">
+      <c r="A343" s="7" t="s">
         <v>1340</v>
       </c>
       <c r="B343" s="12">
@@ -14445,7 +15223,7 @@
       </c>
     </row>
     <row r="344">
-      <c r="A344" s="20" t="s">
+      <c r="A344" s="4" t="s">
         <v>1340</v>
       </c>
       <c r="B344" s="10">
@@ -14472,7 +15250,7 @@
       </c>
     </row>
     <row r="345">
-      <c r="A345" s="23" t="s">
+      <c r="A345" s="7" t="s">
         <v>1340</v>
       </c>
       <c r="B345" s="12">
@@ -14499,7 +15277,7 @@
       </c>
     </row>
     <row r="346">
-      <c r="A346" s="20" t="s">
+      <c r="A346" s="4" t="s">
         <v>1340</v>
       </c>
       <c r="B346" s="10">
@@ -14526,7 +15304,7 @@
       </c>
     </row>
     <row r="347">
-      <c r="A347" s="23" t="s">
+      <c r="A347" s="7" t="s">
         <v>1340</v>
       </c>
       <c r="B347" s="12">
@@ -14580,30 +15358,1488 @@
       </c>
     </row>
     <row r="349">
-      <c r="A349" s="25" t="s">
+      <c r="A349" s="7" t="s">
         <v>1340</v>
       </c>
-      <c r="B349" s="26">
+      <c r="B349" s="12">
+        <v>2.0</v>
+      </c>
+      <c r="C349" s="12" t="s">
+        <v>1563</v>
+      </c>
+      <c r="D349" s="12" t="s">
+        <v>1564</v>
+      </c>
+      <c r="E349" s="12" t="s">
+        <v>1565</v>
+      </c>
+      <c r="F349" s="12" t="s">
+        <v>1566</v>
+      </c>
+      <c r="G349" s="12" t="s">
+        <v>1567</v>
+      </c>
+      <c r="H349" s="13">
+        <f t="shared" si="1"/>
+        <v>349</v>
+      </c>
+    </row>
+    <row r="350">
+      <c r="A350" s="4" t="s">
+        <v>1340</v>
+      </c>
+      <c r="B350" s="10">
+        <v>2.0</v>
+      </c>
+      <c r="C350" s="10" t="s">
+        <v>1568</v>
+      </c>
+      <c r="D350" s="10" t="s">
+        <v>1569</v>
+      </c>
+      <c r="E350" s="10" t="s">
+        <v>1570</v>
+      </c>
+      <c r="F350" s="10" t="s">
+        <v>1571</v>
+      </c>
+      <c r="G350" s="10" t="s">
+        <v>1572</v>
+      </c>
+      <c r="H350" s="11">
+        <f t="shared" si="1"/>
+        <v>350</v>
+      </c>
+    </row>
+    <row r="351">
+      <c r="A351" s="7" t="s">
+        <v>1340</v>
+      </c>
+      <c r="B351" s="12">
+        <v>2.0</v>
+      </c>
+      <c r="C351" s="12" t="s">
+        <v>1573</v>
+      </c>
+      <c r="D351" s="12" t="s">
+        <v>1574</v>
+      </c>
+      <c r="E351" s="12" t="s">
+        <v>1575</v>
+      </c>
+      <c r="F351" s="12" t="s">
+        <v>1576</v>
+      </c>
+      <c r="G351" s="12" t="s">
+        <v>1577</v>
+      </c>
+      <c r="H351" s="13">
+        <f t="shared" si="1"/>
+        <v>351</v>
+      </c>
+    </row>
+    <row r="352">
+      <c r="A352" s="4" t="s">
+        <v>1340</v>
+      </c>
+      <c r="B352" s="10">
+        <v>2.0</v>
+      </c>
+      <c r="C352" s="10" t="s">
+        <v>1578</v>
+      </c>
+      <c r="D352" s="25" t="s">
+        <v>1579</v>
+      </c>
+      <c r="E352" s="25" t="s">
+        <v>1580</v>
+      </c>
+      <c r="F352" s="25" t="s">
+        <v>1581</v>
+      </c>
+      <c r="G352" s="10" t="s">
+        <v>1582</v>
+      </c>
+      <c r="H352" s="11">
+        <f t="shared" si="1"/>
+        <v>352</v>
+      </c>
+    </row>
+    <row r="353">
+      <c r="A353" s="7" t="s">
+        <v>1340</v>
+      </c>
+      <c r="B353" s="12">
         <v>4.0</v>
       </c>
-      <c r="C349" s="26" t="s">
-        <v>1563</v>
-      </c>
-      <c r="D349" s="26" t="s">
+      <c r="C353" s="12" t="s">
+        <v>1583</v>
+      </c>
+      <c r="D353" s="26" t="s">
+        <v>1584</v>
+      </c>
+      <c r="E353" s="26" t="s">
+        <v>1585</v>
+      </c>
+      <c r="F353" s="26" t="s">
+        <v>1586</v>
+      </c>
+      <c r="G353" s="26" t="s">
+        <v>1587</v>
+      </c>
+      <c r="H353" s="13">
+        <f t="shared" si="1"/>
+        <v>353</v>
+      </c>
+    </row>
+    <row r="354">
+      <c r="A354" s="4" t="s">
+        <v>1340</v>
+      </c>
+      <c r="B354" s="10">
+        <v>2.0</v>
+      </c>
+      <c r="C354" s="10" t="s">
+        <v>1588</v>
+      </c>
+      <c r="D354" s="25" t="s">
+        <v>1589</v>
+      </c>
+      <c r="E354" s="25" t="s">
+        <v>1590</v>
+      </c>
+      <c r="F354" s="25" t="s">
+        <v>1591</v>
+      </c>
+      <c r="G354" s="25" t="s">
+        <v>1592</v>
+      </c>
+      <c r="H354" s="11">
+        <f t="shared" si="1"/>
+        <v>354</v>
+      </c>
+    </row>
+    <row r="355">
+      <c r="A355" s="7" t="s">
+        <v>1340</v>
+      </c>
+      <c r="B355" s="12">
+        <v>3.0</v>
+      </c>
+      <c r="C355" s="12" t="s">
+        <v>1593</v>
+      </c>
+      <c r="D355" s="26" t="s">
+        <v>1594</v>
+      </c>
+      <c r="E355" s="26" t="s">
+        <v>1595</v>
+      </c>
+      <c r="F355" s="26" t="s">
+        <v>1596</v>
+      </c>
+      <c r="G355" s="26" t="s">
+        <v>1597</v>
+      </c>
+      <c r="H355" s="13">
+        <f t="shared" si="1"/>
+        <v>355</v>
+      </c>
+    </row>
+    <row r="356">
+      <c r="A356" s="4" t="s">
+        <v>1340</v>
+      </c>
+      <c r="B356" s="10">
+        <v>1.0</v>
+      </c>
+      <c r="C356" s="10" t="s">
+        <v>1598</v>
+      </c>
+      <c r="D356" s="25" t="s">
+        <v>1599</v>
+      </c>
+      <c r="E356" s="25" t="s">
+        <v>1600</v>
+      </c>
+      <c r="F356" s="25" t="s">
+        <v>1601</v>
+      </c>
+      <c r="G356" s="25" t="s">
+        <v>1602</v>
+      </c>
+      <c r="H356" s="11">
+        <f t="shared" si="1"/>
+        <v>356</v>
+      </c>
+    </row>
+    <row r="357">
+      <c r="A357" s="7" t="s">
+        <v>1340</v>
+      </c>
+      <c r="B357" s="12">
+        <v>2.0</v>
+      </c>
+      <c r="C357" s="12" t="s">
+        <v>1603</v>
+      </c>
+      <c r="D357" s="26" t="s">
         <v>1564</v>
       </c>
-      <c r="E349" s="26" t="s">
-        <v>1565</v>
-      </c>
-      <c r="F349" s="26" t="s">
-        <v>1566</v>
-      </c>
-      <c r="G349" s="26" t="s">
-        <v>1567</v>
-      </c>
-      <c r="H349" s="27">
-        <f t="shared" si="1"/>
-        <v>349</v>
+      <c r="E357" s="26" t="s">
+        <v>1604</v>
+      </c>
+      <c r="F357" s="26" t="s">
+        <v>1605</v>
+      </c>
+      <c r="G357" s="26" t="s">
+        <v>1479</v>
+      </c>
+      <c r="H357" s="13">
+        <f t="shared" si="1"/>
+        <v>357</v>
+      </c>
+    </row>
+    <row r="358">
+      <c r="A358" s="4" t="s">
+        <v>1340</v>
+      </c>
+      <c r="B358" s="10">
+        <v>3.0</v>
+      </c>
+      <c r="C358" s="10" t="s">
+        <v>1606</v>
+      </c>
+      <c r="D358" s="25" t="s">
+        <v>1607</v>
+      </c>
+      <c r="E358" s="25" t="s">
+        <v>1608</v>
+      </c>
+      <c r="F358" s="25" t="s">
+        <v>1609</v>
+      </c>
+      <c r="G358" s="25" t="s">
+        <v>1610</v>
+      </c>
+      <c r="H358" s="11">
+        <f t="shared" si="1"/>
+        <v>358</v>
+      </c>
+    </row>
+    <row r="359">
+      <c r="A359" s="7" t="s">
+        <v>1340</v>
+      </c>
+      <c r="B359" s="12">
+        <v>1.0</v>
+      </c>
+      <c r="C359" s="12" t="s">
+        <v>1611</v>
+      </c>
+      <c r="D359" s="26" t="s">
+        <v>1612</v>
+      </c>
+      <c r="E359" s="26" t="s">
+        <v>1613</v>
+      </c>
+      <c r="F359" s="26" t="s">
+        <v>1614</v>
+      </c>
+      <c r="G359" s="26" t="s">
+        <v>1615</v>
+      </c>
+      <c r="H359" s="13">
+        <f t="shared" si="1"/>
+        <v>359</v>
+      </c>
+    </row>
+    <row r="360">
+      <c r="A360" s="4" t="s">
+        <v>1340</v>
+      </c>
+      <c r="B360" s="10">
+        <v>2.0</v>
+      </c>
+      <c r="C360" s="10" t="s">
+        <v>1616</v>
+      </c>
+      <c r="D360" s="25" t="s">
+        <v>1617</v>
+      </c>
+      <c r="E360" s="25" t="s">
+        <v>1618</v>
+      </c>
+      <c r="F360" s="25" t="s">
+        <v>1619</v>
+      </c>
+      <c r="G360" s="25" t="s">
+        <v>1620</v>
+      </c>
+      <c r="H360" s="11">
+        <f t="shared" si="1"/>
+        <v>360</v>
+      </c>
+    </row>
+    <row r="361">
+      <c r="A361" s="7" t="s">
+        <v>1340</v>
+      </c>
+      <c r="B361" s="12">
+        <v>1.0</v>
+      </c>
+      <c r="C361" s="12" t="s">
+        <v>1621</v>
+      </c>
+      <c r="D361" s="26" t="s">
+        <v>1622</v>
+      </c>
+      <c r="E361" s="26" t="s">
+        <v>1623</v>
+      </c>
+      <c r="F361" s="26" t="s">
+        <v>1624</v>
+      </c>
+      <c r="G361" s="26" t="s">
+        <v>1625</v>
+      </c>
+      <c r="H361" s="13">
+        <f t="shared" si="1"/>
+        <v>361</v>
+      </c>
+    </row>
+    <row r="362">
+      <c r="A362" s="4" t="s">
+        <v>1340</v>
+      </c>
+      <c r="B362" s="10">
+        <v>3.0</v>
+      </c>
+      <c r="C362" s="10" t="s">
+        <v>1626</v>
+      </c>
+      <c r="D362" s="25" t="s">
+        <v>1627</v>
+      </c>
+      <c r="E362" s="25" t="s">
+        <v>1628</v>
+      </c>
+      <c r="F362" s="25" t="s">
+        <v>1629</v>
+      </c>
+      <c r="G362" s="25" t="s">
+        <v>1630</v>
+      </c>
+      <c r="H362" s="11">
+        <f t="shared" si="1"/>
+        <v>362</v>
+      </c>
+    </row>
+    <row r="363">
+      <c r="A363" s="7" t="s">
+        <v>1340</v>
+      </c>
+      <c r="B363" s="12">
+        <v>4.0</v>
+      </c>
+      <c r="C363" s="12" t="s">
+        <v>1631</v>
+      </c>
+      <c r="D363" s="26" t="s">
+        <v>1632</v>
+      </c>
+      <c r="E363" s="26" t="s">
+        <v>1633</v>
+      </c>
+      <c r="F363" s="26" t="s">
+        <v>1634</v>
+      </c>
+      <c r="G363" s="26" t="s">
+        <v>1635</v>
+      </c>
+      <c r="H363" s="13">
+        <f t="shared" si="1"/>
+        <v>363</v>
+      </c>
+    </row>
+    <row r="364">
+      <c r="A364" s="4" t="s">
+        <v>1340</v>
+      </c>
+      <c r="B364" s="10">
+        <v>3.0</v>
+      </c>
+      <c r="C364" s="10" t="s">
+        <v>1636</v>
+      </c>
+      <c r="D364" s="25" t="s">
+        <v>1637</v>
+      </c>
+      <c r="E364" s="25" t="s">
+        <v>1638</v>
+      </c>
+      <c r="F364" s="25" t="s">
+        <v>1639</v>
+      </c>
+      <c r="G364" s="25" t="s">
+        <v>1640</v>
+      </c>
+      <c r="H364" s="11">
+        <f t="shared" si="1"/>
+        <v>364</v>
+      </c>
+    </row>
+    <row r="365">
+      <c r="A365" s="7" t="s">
+        <v>1340</v>
+      </c>
+      <c r="B365" s="12">
+        <v>1.0</v>
+      </c>
+      <c r="C365" s="12" t="s">
+        <v>1641</v>
+      </c>
+      <c r="D365" s="26" t="s">
+        <v>1642</v>
+      </c>
+      <c r="E365" s="26" t="s">
+        <v>1643</v>
+      </c>
+      <c r="F365" s="26" t="s">
+        <v>1644</v>
+      </c>
+      <c r="G365" s="26" t="s">
+        <v>1645</v>
+      </c>
+      <c r="H365" s="13">
+        <f t="shared" si="1"/>
+        <v>365</v>
+      </c>
+    </row>
+    <row r="366">
+      <c r="A366" s="4" t="s">
+        <v>1340</v>
+      </c>
+      <c r="B366" s="10">
+        <v>3.0</v>
+      </c>
+      <c r="C366" s="10" t="s">
+        <v>1646</v>
+      </c>
+      <c r="D366" s="25" t="s">
+        <v>1647</v>
+      </c>
+      <c r="E366" s="25" t="s">
+        <v>1648</v>
+      </c>
+      <c r="F366" s="25" t="s">
+        <v>1649</v>
+      </c>
+      <c r="G366" s="25" t="s">
+        <v>1650</v>
+      </c>
+      <c r="H366" s="11">
+        <f t="shared" si="1"/>
+        <v>366</v>
+      </c>
+    </row>
+    <row r="367">
+      <c r="A367" s="7" t="s">
+        <v>1340</v>
+      </c>
+      <c r="B367" s="12">
+        <v>2.0</v>
+      </c>
+      <c r="C367" s="12" t="s">
+        <v>1651</v>
+      </c>
+      <c r="D367" s="26" t="s">
+        <v>1652</v>
+      </c>
+      <c r="E367" s="26" t="s">
+        <v>1653</v>
+      </c>
+      <c r="F367" s="26" t="s">
+        <v>1654</v>
+      </c>
+      <c r="G367" s="26" t="s">
+        <v>1655</v>
+      </c>
+      <c r="H367" s="13">
+        <f t="shared" si="1"/>
+        <v>367</v>
+      </c>
+    </row>
+    <row r="368">
+      <c r="A368" s="4" t="s">
+        <v>1340</v>
+      </c>
+      <c r="B368" s="10">
+        <v>4.0</v>
+      </c>
+      <c r="C368" s="10" t="s">
+        <v>1656</v>
+      </c>
+      <c r="D368" s="25" t="s">
+        <v>1657</v>
+      </c>
+      <c r="E368" s="25" t="s">
+        <v>1658</v>
+      </c>
+      <c r="F368" s="25" t="s">
+        <v>1659</v>
+      </c>
+      <c r="G368" s="25" t="s">
+        <v>1660</v>
+      </c>
+      <c r="H368" s="11">
+        <f t="shared" si="1"/>
+        <v>368</v>
+      </c>
+    </row>
+    <row r="369">
+      <c r="A369" s="7" t="s">
+        <v>1340</v>
+      </c>
+      <c r="B369" s="12">
+        <v>1.0</v>
+      </c>
+      <c r="C369" s="12" t="s">
+        <v>1661</v>
+      </c>
+      <c r="D369" s="26" t="s">
+        <v>1662</v>
+      </c>
+      <c r="E369" s="26" t="s">
+        <v>1663</v>
+      </c>
+      <c r="F369" s="26" t="s">
+        <v>1664</v>
+      </c>
+      <c r="G369" s="26" t="s">
+        <v>1665</v>
+      </c>
+      <c r="H369" s="13">
+        <f t="shared" si="1"/>
+        <v>369</v>
+      </c>
+    </row>
+    <row r="370">
+      <c r="A370" s="4" t="s">
+        <v>1340</v>
+      </c>
+      <c r="B370" s="10">
+        <v>2.0</v>
+      </c>
+      <c r="C370" s="10" t="s">
+        <v>1666</v>
+      </c>
+      <c r="D370" s="25" t="s">
+        <v>1667</v>
+      </c>
+      <c r="E370" s="25" t="s">
+        <v>1668</v>
+      </c>
+      <c r="F370" s="25" t="s">
+        <v>1669</v>
+      </c>
+      <c r="G370" s="25" t="s">
+        <v>1670</v>
+      </c>
+      <c r="H370" s="11">
+        <f t="shared" si="1"/>
+        <v>370</v>
+      </c>
+    </row>
+    <row r="371">
+      <c r="A371" s="7" t="s">
+        <v>1340</v>
+      </c>
+      <c r="B371" s="12">
+        <v>3.0</v>
+      </c>
+      <c r="C371" s="12" t="s">
+        <v>1671</v>
+      </c>
+      <c r="D371" s="26" t="s">
+        <v>1672</v>
+      </c>
+      <c r="E371" s="26" t="s">
+        <v>1673</v>
+      </c>
+      <c r="F371" s="26" t="s">
+        <v>1674</v>
+      </c>
+      <c r="G371" s="26" t="s">
+        <v>1648</v>
+      </c>
+      <c r="H371" s="13">
+        <f t="shared" si="1"/>
+        <v>371</v>
+      </c>
+    </row>
+    <row r="372">
+      <c r="A372" s="4" t="s">
+        <v>1340</v>
+      </c>
+      <c r="B372" s="10">
+        <v>2.0</v>
+      </c>
+      <c r="C372" s="10" t="s">
+        <v>1675</v>
+      </c>
+      <c r="D372" s="25" t="s">
+        <v>1676</v>
+      </c>
+      <c r="E372" s="25" t="s">
+        <v>1677</v>
+      </c>
+      <c r="F372" s="25" t="s">
+        <v>1678</v>
+      </c>
+      <c r="G372" s="25" t="s">
+        <v>1679</v>
+      </c>
+      <c r="H372" s="11">
+        <f t="shared" si="1"/>
+        <v>372</v>
+      </c>
+    </row>
+    <row r="373">
+      <c r="A373" s="7" t="s">
+        <v>1340</v>
+      </c>
+      <c r="B373" s="12">
+        <v>3.0</v>
+      </c>
+      <c r="C373" s="12" t="s">
+        <v>1680</v>
+      </c>
+      <c r="D373" s="26" t="s">
+        <v>1681</v>
+      </c>
+      <c r="E373" s="26" t="s">
+        <v>1682</v>
+      </c>
+      <c r="F373" s="26" t="s">
+        <v>1683</v>
+      </c>
+      <c r="G373" s="26" t="s">
+        <v>1684</v>
+      </c>
+      <c r="H373" s="13">
+        <f t="shared" si="1"/>
+        <v>373</v>
+      </c>
+    </row>
+    <row r="374">
+      <c r="A374" s="4" t="s">
+        <v>1340</v>
+      </c>
+      <c r="B374" s="10">
+        <v>3.0</v>
+      </c>
+      <c r="C374" s="10" t="s">
+        <v>1685</v>
+      </c>
+      <c r="D374" s="25" t="s">
+        <v>1686</v>
+      </c>
+      <c r="E374" s="25" t="s">
+        <v>1687</v>
+      </c>
+      <c r="F374" s="25" t="s">
+        <v>1688</v>
+      </c>
+      <c r="G374" s="25" t="s">
+        <v>1689</v>
+      </c>
+      <c r="H374" s="11">
+        <f t="shared" si="1"/>
+        <v>374</v>
+      </c>
+    </row>
+    <row r="375">
+      <c r="A375" s="7" t="s">
+        <v>1340</v>
+      </c>
+      <c r="B375" s="12">
+        <v>3.0</v>
+      </c>
+      <c r="C375" s="12" t="s">
+        <v>1690</v>
+      </c>
+      <c r="D375" s="26" t="s">
+        <v>1691</v>
+      </c>
+      <c r="E375" s="26" t="s">
+        <v>1692</v>
+      </c>
+      <c r="F375" s="26" t="s">
+        <v>1693</v>
+      </c>
+      <c r="G375" s="26" t="s">
+        <v>1694</v>
+      </c>
+      <c r="H375" s="13">
+        <f t="shared" si="1"/>
+        <v>375</v>
+      </c>
+    </row>
+    <row r="376">
+      <c r="A376" s="4" t="s">
+        <v>1340</v>
+      </c>
+      <c r="B376" s="10">
+        <v>3.0</v>
+      </c>
+      <c r="C376" s="10" t="s">
+        <v>1695</v>
+      </c>
+      <c r="D376" s="25" t="s">
+        <v>1696</v>
+      </c>
+      <c r="E376" s="25" t="s">
+        <v>1697</v>
+      </c>
+      <c r="F376" s="25" t="s">
+        <v>1698</v>
+      </c>
+      <c r="G376" s="25" t="s">
+        <v>1699</v>
+      </c>
+      <c r="H376" s="11">
+        <f t="shared" si="1"/>
+        <v>376</v>
+      </c>
+    </row>
+    <row r="377">
+      <c r="A377" s="7" t="s">
+        <v>1340</v>
+      </c>
+      <c r="B377" s="12">
+        <v>3.0</v>
+      </c>
+      <c r="C377" s="12" t="s">
+        <v>1700</v>
+      </c>
+      <c r="D377" s="26" t="s">
+        <v>1701</v>
+      </c>
+      <c r="E377" s="26" t="s">
+        <v>1702</v>
+      </c>
+      <c r="F377" s="26" t="s">
+        <v>1703</v>
+      </c>
+      <c r="G377" s="26" t="s">
+        <v>1415</v>
+      </c>
+      <c r="H377" s="13">
+        <f t="shared" si="1"/>
+        <v>377</v>
+      </c>
+    </row>
+    <row r="378">
+      <c r="A378" s="4" t="s">
+        <v>1340</v>
+      </c>
+      <c r="B378" s="10">
+        <v>3.0</v>
+      </c>
+      <c r="C378" s="10" t="s">
+        <v>1704</v>
+      </c>
+      <c r="D378" s="25" t="s">
+        <v>1705</v>
+      </c>
+      <c r="E378" s="25" t="s">
+        <v>1706</v>
+      </c>
+      <c r="F378" s="25" t="s">
+        <v>1707</v>
+      </c>
+      <c r="G378" s="25" t="s">
+        <v>1708</v>
+      </c>
+      <c r="H378" s="11">
+        <f t="shared" si="1"/>
+        <v>378</v>
+      </c>
+    </row>
+    <row r="379">
+      <c r="A379" s="7" t="s">
+        <v>1340</v>
+      </c>
+      <c r="B379" s="12">
+        <v>3.0</v>
+      </c>
+      <c r="C379" s="12" t="s">
+        <v>1709</v>
+      </c>
+      <c r="D379" s="26" t="s">
+        <v>1710</v>
+      </c>
+      <c r="E379" s="26" t="s">
+        <v>1711</v>
+      </c>
+      <c r="F379" s="26" t="s">
+        <v>1712</v>
+      </c>
+      <c r="G379" s="26" t="s">
+        <v>1713</v>
+      </c>
+      <c r="H379" s="13">
+        <f t="shared" si="1"/>
+        <v>379</v>
+      </c>
+    </row>
+    <row r="380">
+      <c r="A380" s="4" t="s">
+        <v>1340</v>
+      </c>
+      <c r="B380" s="10">
+        <v>4.0</v>
+      </c>
+      <c r="C380" s="10" t="s">
+        <v>1714</v>
+      </c>
+      <c r="D380" s="25" t="s">
+        <v>1715</v>
+      </c>
+      <c r="E380" s="25" t="s">
+        <v>1716</v>
+      </c>
+      <c r="F380" s="25" t="s">
+        <v>1717</v>
+      </c>
+      <c r="G380" s="25" t="s">
+        <v>1718</v>
+      </c>
+      <c r="H380" s="11">
+        <f t="shared" si="1"/>
+        <v>380</v>
+      </c>
+    </row>
+    <row r="381">
+      <c r="A381" s="7" t="s">
+        <v>1340</v>
+      </c>
+      <c r="B381" s="12">
+        <v>4.0</v>
+      </c>
+      <c r="C381" s="12" t="s">
+        <v>1719</v>
+      </c>
+      <c r="D381" s="8" t="s">
+        <v>1720</v>
+      </c>
+      <c r="E381" s="26" t="s">
+        <v>1721</v>
+      </c>
+      <c r="F381" s="26" t="s">
+        <v>1722</v>
+      </c>
+      <c r="G381" s="26" t="s">
+        <v>1723</v>
+      </c>
+      <c r="H381" s="13">
+        <f t="shared" si="1"/>
+        <v>381</v>
+      </c>
+    </row>
+    <row r="382">
+      <c r="A382" s="4" t="s">
+        <v>1340</v>
+      </c>
+      <c r="B382" s="10">
+        <v>4.0</v>
+      </c>
+      <c r="C382" s="10" t="s">
+        <v>1724</v>
+      </c>
+      <c r="D382" s="25" t="s">
+        <v>1725</v>
+      </c>
+      <c r="E382" s="25" t="s">
+        <v>1726</v>
+      </c>
+      <c r="F382" s="25" t="s">
+        <v>1727</v>
+      </c>
+      <c r="G382" s="25" t="s">
+        <v>1728</v>
+      </c>
+      <c r="H382" s="11">
+        <f t="shared" si="1"/>
+        <v>382</v>
+      </c>
+    </row>
+    <row r="383">
+      <c r="A383" s="7" t="s">
+        <v>1340</v>
+      </c>
+      <c r="B383" s="12">
+        <v>4.0</v>
+      </c>
+      <c r="C383" s="12" t="s">
+        <v>1729</v>
+      </c>
+      <c r="D383" s="26" t="s">
+        <v>1730</v>
+      </c>
+      <c r="E383" s="26" t="s">
+        <v>1731</v>
+      </c>
+      <c r="F383" s="26" t="s">
+        <v>1726</v>
+      </c>
+      <c r="G383" s="26" t="s">
+        <v>1732</v>
+      </c>
+      <c r="H383" s="13">
+        <f t="shared" si="1"/>
+        <v>383</v>
+      </c>
+    </row>
+    <row r="384">
+      <c r="A384" s="4" t="s">
+        <v>1340</v>
+      </c>
+      <c r="B384" s="10">
+        <v>4.0</v>
+      </c>
+      <c r="C384" s="10" t="s">
+        <v>1733</v>
+      </c>
+      <c r="D384" s="25" t="s">
+        <v>1734</v>
+      </c>
+      <c r="E384" s="25" t="s">
+        <v>1735</v>
+      </c>
+      <c r="F384" s="25" t="s">
+        <v>1736</v>
+      </c>
+      <c r="G384" s="25" t="s">
+        <v>1737</v>
+      </c>
+      <c r="H384" s="11">
+        <f t="shared" si="1"/>
+        <v>384</v>
+      </c>
+    </row>
+    <row r="385">
+      <c r="A385" s="7" t="s">
+        <v>1340</v>
+      </c>
+      <c r="B385" s="12">
+        <v>4.0</v>
+      </c>
+      <c r="C385" s="12" t="s">
+        <v>1738</v>
+      </c>
+      <c r="D385" s="26" t="s">
+        <v>1739</v>
+      </c>
+      <c r="E385" s="26" t="s">
+        <v>1740</v>
+      </c>
+      <c r="F385" s="26" t="s">
+        <v>1741</v>
+      </c>
+      <c r="G385" s="26" t="s">
+        <v>64</v>
+      </c>
+      <c r="H385" s="13">
+        <f t="shared" si="1"/>
+        <v>385</v>
+      </c>
+    </row>
+    <row r="386">
+      <c r="A386" s="4" t="s">
+        <v>1340</v>
+      </c>
+      <c r="B386" s="10">
+        <v>4.0</v>
+      </c>
+      <c r="C386" s="10" t="s">
+        <v>1742</v>
+      </c>
+      <c r="D386" s="25" t="s">
+        <v>1743</v>
+      </c>
+      <c r="E386" s="25" t="s">
+        <v>1744</v>
+      </c>
+      <c r="F386" s="25" t="s">
+        <v>1745</v>
+      </c>
+      <c r="G386" s="25" t="s">
+        <v>1746</v>
+      </c>
+      <c r="H386" s="11">
+        <f t="shared" si="1"/>
+        <v>386</v>
+      </c>
+    </row>
+    <row r="387">
+      <c r="A387" s="7" t="s">
+        <v>1340</v>
+      </c>
+      <c r="B387" s="12">
+        <v>4.0</v>
+      </c>
+      <c r="C387" s="12" t="s">
+        <v>1747</v>
+      </c>
+      <c r="D387" s="26" t="s">
+        <v>1748</v>
+      </c>
+      <c r="E387" s="26" t="s">
+        <v>1749</v>
+      </c>
+      <c r="F387" s="26" t="s">
+        <v>1750</v>
+      </c>
+      <c r="G387" s="26" t="s">
+        <v>1751</v>
+      </c>
+      <c r="H387" s="13">
+        <f t="shared" si="1"/>
+        <v>387</v>
+      </c>
+    </row>
+    <row r="388">
+      <c r="A388" s="4" t="s">
+        <v>1340</v>
+      </c>
+      <c r="B388" s="10">
+        <v>4.0</v>
+      </c>
+      <c r="C388" s="10" t="s">
+        <v>1752</v>
+      </c>
+      <c r="D388" s="25" t="s">
+        <v>1753</v>
+      </c>
+      <c r="E388" s="25" t="s">
+        <v>1754</v>
+      </c>
+      <c r="F388" s="25" t="s">
+        <v>1755</v>
+      </c>
+      <c r="G388" s="25" t="s">
+        <v>1756</v>
+      </c>
+      <c r="H388" s="11">
+        <f t="shared" si="1"/>
+        <v>388</v>
+      </c>
+    </row>
+    <row r="389">
+      <c r="A389" s="7" t="s">
+        <v>1340</v>
+      </c>
+      <c r="B389" s="12">
+        <v>4.0</v>
+      </c>
+      <c r="C389" s="12" t="s">
+        <v>1757</v>
+      </c>
+      <c r="D389" s="26" t="s">
+        <v>1758</v>
+      </c>
+      <c r="E389" s="26" t="s">
+        <v>1759</v>
+      </c>
+      <c r="F389" s="26" t="s">
+        <v>1760</v>
+      </c>
+      <c r="G389" s="26" t="s">
+        <v>1761</v>
+      </c>
+      <c r="H389" s="13">
+        <f t="shared" si="1"/>
+        <v>389</v>
+      </c>
+    </row>
+    <row r="390">
+      <c r="A390" s="4" t="s">
+        <v>1340</v>
+      </c>
+      <c r="B390" s="10">
+        <v>4.0</v>
+      </c>
+      <c r="C390" s="10" t="s">
+        <v>1762</v>
+      </c>
+      <c r="D390" s="25" t="s">
+        <v>1763</v>
+      </c>
+      <c r="E390" s="25" t="s">
+        <v>1764</v>
+      </c>
+      <c r="F390" s="25" t="s">
+        <v>1765</v>
+      </c>
+      <c r="G390" s="25" t="s">
+        <v>1766</v>
+      </c>
+      <c r="H390" s="11">
+        <f t="shared" si="1"/>
+        <v>390</v>
+      </c>
+    </row>
+    <row r="391">
+      <c r="A391" s="7" t="s">
+        <v>1340</v>
+      </c>
+      <c r="B391" s="12">
+        <v>4.0</v>
+      </c>
+      <c r="C391" s="12" t="s">
+        <v>1767</v>
+      </c>
+      <c r="D391" s="26" t="s">
+        <v>1768</v>
+      </c>
+      <c r="E391" s="26" t="s">
+        <v>1769</v>
+      </c>
+      <c r="F391" s="26" t="s">
+        <v>1770</v>
+      </c>
+      <c r="G391" s="26" t="s">
+        <v>1771</v>
+      </c>
+      <c r="H391" s="13">
+        <f t="shared" si="1"/>
+        <v>391</v>
+      </c>
+    </row>
+    <row r="392">
+      <c r="A392" s="4" t="s">
+        <v>1340</v>
+      </c>
+      <c r="B392" s="10">
+        <v>4.0</v>
+      </c>
+      <c r="C392" s="10" t="s">
+        <v>1772</v>
+      </c>
+      <c r="D392" s="25" t="s">
+        <v>1773</v>
+      </c>
+      <c r="E392" s="25" t="s">
+        <v>1774</v>
+      </c>
+      <c r="F392" s="25" t="s">
+        <v>1775</v>
+      </c>
+      <c r="G392" s="25" t="s">
+        <v>1776</v>
+      </c>
+      <c r="H392" s="11">
+        <f t="shared" si="1"/>
+        <v>392</v>
+      </c>
+    </row>
+    <row r="393">
+      <c r="A393" s="7" t="s">
+        <v>1340</v>
+      </c>
+      <c r="B393" s="12">
+        <v>4.0</v>
+      </c>
+      <c r="C393" s="12" t="s">
+        <v>1777</v>
+      </c>
+      <c r="D393" s="26" t="s">
+        <v>1778</v>
+      </c>
+      <c r="E393" s="26" t="s">
+        <v>1779</v>
+      </c>
+      <c r="F393" s="26" t="s">
+        <v>1780</v>
+      </c>
+      <c r="G393" s="26" t="s">
+        <v>1781</v>
+      </c>
+      <c r="H393" s="13">
+        <f t="shared" si="1"/>
+        <v>393</v>
+      </c>
+    </row>
+    <row r="394">
+      <c r="A394" s="4" t="s">
+        <v>1340</v>
+      </c>
+      <c r="B394" s="10">
+        <v>4.0</v>
+      </c>
+      <c r="C394" s="10" t="s">
+        <v>1782</v>
+      </c>
+      <c r="D394" s="25" t="s">
+        <v>1783</v>
+      </c>
+      <c r="E394" s="25" t="s">
+        <v>1784</v>
+      </c>
+      <c r="F394" s="25" t="s">
+        <v>1785</v>
+      </c>
+      <c r="G394" s="25" t="s">
+        <v>1786</v>
+      </c>
+      <c r="H394" s="11">
+        <f t="shared" si="1"/>
+        <v>394</v>
+      </c>
+    </row>
+    <row r="395">
+      <c r="A395" s="7" t="s">
+        <v>1340</v>
+      </c>
+      <c r="B395" s="12">
+        <v>4.0</v>
+      </c>
+      <c r="C395" s="12" t="s">
+        <v>1787</v>
+      </c>
+      <c r="D395" s="26" t="s">
+        <v>1788</v>
+      </c>
+      <c r="E395" s="26" t="s">
+        <v>1789</v>
+      </c>
+      <c r="F395" s="26" t="s">
+        <v>1790</v>
+      </c>
+      <c r="G395" s="26" t="s">
+        <v>1791</v>
+      </c>
+      <c r="H395" s="13">
+        <f t="shared" si="1"/>
+        <v>395</v>
+      </c>
+    </row>
+    <row r="396">
+      <c r="A396" s="4" t="s">
+        <v>1340</v>
+      </c>
+      <c r="B396" s="10">
+        <v>4.0</v>
+      </c>
+      <c r="C396" s="10" t="s">
+        <v>1792</v>
+      </c>
+      <c r="D396" s="25" t="s">
+        <v>1773</v>
+      </c>
+      <c r="E396" s="25" t="s">
+        <v>1793</v>
+      </c>
+      <c r="F396" s="25" t="s">
+        <v>1775</v>
+      </c>
+      <c r="G396" s="25" t="s">
+        <v>1776</v>
+      </c>
+      <c r="H396" s="11">
+        <f t="shared" si="1"/>
+        <v>396</v>
+      </c>
+    </row>
+    <row r="397">
+      <c r="A397" s="7" t="s">
+        <v>1340</v>
+      </c>
+      <c r="B397" s="12">
+        <v>4.0</v>
+      </c>
+      <c r="C397" s="12" t="s">
+        <v>1794</v>
+      </c>
+      <c r="D397" s="26" t="s">
+        <v>1795</v>
+      </c>
+      <c r="E397" s="26" t="s">
+        <v>1796</v>
+      </c>
+      <c r="F397" s="26" t="s">
+        <v>1797</v>
+      </c>
+      <c r="G397" s="26" t="s">
+        <v>1798</v>
+      </c>
+      <c r="H397" s="13">
+        <f t="shared" si="1"/>
+        <v>397</v>
+      </c>
+    </row>
+    <row r="398">
+      <c r="A398" s="4" t="s">
+        <v>1340</v>
+      </c>
+      <c r="B398" s="10">
+        <v>4.0</v>
+      </c>
+      <c r="C398" s="10" t="s">
+        <v>1799</v>
+      </c>
+      <c r="D398" s="25" t="s">
+        <v>1800</v>
+      </c>
+      <c r="E398" s="25" t="s">
+        <v>1801</v>
+      </c>
+      <c r="F398" s="25" t="s">
+        <v>1802</v>
+      </c>
+      <c r="G398" s="25" t="s">
+        <v>1803</v>
+      </c>
+      <c r="H398" s="11">
+        <f t="shared" si="1"/>
+        <v>398</v>
+      </c>
+    </row>
+    <row r="399">
+      <c r="A399" s="7" t="s">
+        <v>1340</v>
+      </c>
+      <c r="B399" s="12">
+        <v>4.0</v>
+      </c>
+      <c r="C399" s="12" t="s">
+        <v>1804</v>
+      </c>
+      <c r="D399" s="8" t="s">
+        <v>1805</v>
+      </c>
+      <c r="E399" s="26" t="s">
+        <v>1806</v>
+      </c>
+      <c r="F399" s="26" t="s">
+        <v>1807</v>
+      </c>
+      <c r="G399" s="26" t="s">
+        <v>1808</v>
+      </c>
+      <c r="H399" s="13">
+        <f t="shared" si="1"/>
+        <v>399</v>
+      </c>
+    </row>
+    <row r="400">
+      <c r="A400" s="4" t="s">
+        <v>1340</v>
+      </c>
+      <c r="B400" s="10">
+        <v>4.0</v>
+      </c>
+      <c r="C400" s="10" t="s">
+        <v>1809</v>
+      </c>
+      <c r="D400" s="10" t="s">
+        <v>1810</v>
+      </c>
+      <c r="E400" s="10" t="s">
+        <v>1811</v>
+      </c>
+      <c r="F400" s="25" t="s">
+        <v>1812</v>
+      </c>
+      <c r="G400" s="25" t="s">
+        <v>1813</v>
+      </c>
+      <c r="H400" s="11">
+        <f t="shared" si="1"/>
+        <v>400</v>
+      </c>
+    </row>
+    <row r="401">
+      <c r="A401" s="7" t="s">
+        <v>1340</v>
+      </c>
+      <c r="B401" s="12">
+        <v>4.0</v>
+      </c>
+      <c r="C401" s="12" t="s">
+        <v>1814</v>
+      </c>
+      <c r="D401" s="12" t="s">
+        <v>1815</v>
+      </c>
+      <c r="E401" s="12" t="s">
+        <v>1816</v>
+      </c>
+      <c r="F401" s="12" t="s">
+        <v>1817</v>
+      </c>
+      <c r="G401" s="12" t="s">
+        <v>1818</v>
+      </c>
+      <c r="H401" s="13">
+        <f t="shared" si="1"/>
+        <v>401</v>
+      </c>
+    </row>
+    <row r="402">
+      <c r="A402" s="4" t="s">
+        <v>1340</v>
+      </c>
+      <c r="B402" s="10">
+        <v>4.0</v>
+      </c>
+      <c r="C402" s="10" t="s">
+        <v>1819</v>
+      </c>
+      <c r="D402" s="10">
+        <v>30.06</v>
+      </c>
+      <c r="E402" s="10">
+        <v>29.86</v>
+      </c>
+      <c r="F402" s="10">
+        <v>29.61</v>
+      </c>
+      <c r="G402" s="10">
+        <v>30.86</v>
+      </c>
+      <c r="H402" s="11">
+        <f t="shared" si="1"/>
+        <v>402</v>
+      </c>
+    </row>
+    <row r="403">
+      <c r="A403" s="27" t="s">
+        <v>1340</v>
+      </c>
+      <c r="B403" s="28">
+        <v>4.0</v>
+      </c>
+      <c r="C403" s="28" t="s">
+        <v>1820</v>
+      </c>
+      <c r="D403" s="28" t="s">
+        <v>1821</v>
+      </c>
+      <c r="E403" s="28" t="s">
+        <v>1822</v>
+      </c>
+      <c r="F403" s="28" t="s">
+        <v>1823</v>
+      </c>
+      <c r="G403" s="28" t="s">
+        <v>1824</v>
+      </c>
+      <c r="H403" s="29">
+        <f t="shared" si="1"/>
+        <v>403</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Added and updated weather questions
</commit_message>
<xml_diff>
--- a/public/questions.xlsx
+++ b/public/questions.xlsx
@@ -6,14 +6,14 @@
     <sheet state="visible" name="Sheet1" sheetId="1" r:id="rId4"/>
   </sheets>
   <definedNames>
-    <definedName hidden="1" localSheetId="0" name="_xlnm._FilterDatabase">Sheet1!$A$1:$H$403</definedName>
+    <definedName hidden="1" localSheetId="0" name="_xlnm._FilterDatabase">Sheet1!$A$1:$H$407</definedName>
   </definedNames>
   <calcPr/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2389" uniqueCount="1825">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2413" uniqueCount="1840">
   <si>
     <t>Topic</t>
   </si>
@@ -4317,6 +4317,81 @@
     <t>5° C or less</t>
   </si>
   <si>
+    <t>The amount of water vapor which air can hold depends on the</t>
+  </si>
+  <si>
+    <t>air temperature</t>
+  </si>
+  <si>
+    <t>stability of the air</t>
+  </si>
+  <si>
+    <t>dewpoint</t>
+  </si>
+  <si>
+    <t>relative humidity</t>
+  </si>
+  <si>
+    <t>Clouds are divided into four families according to their</t>
+  </si>
+  <si>
+    <t>height range</t>
+  </si>
+  <si>
+    <t>outward shape</t>
+  </si>
+  <si>
+    <t>composition</t>
+  </si>
+  <si>
+    <t>stability</t>
+  </si>
+  <si>
+    <t>What is meant by the term 'dewpoint'?</t>
+  </si>
+  <si>
+    <t>The temperature to which air must be cooled to become saturated</t>
+  </si>
+  <si>
+    <t>The temperature at which dew will always form</t>
+  </si>
+  <si>
+    <t>The temperature at which condensation and evaporation are equal</t>
+  </si>
+  <si>
+    <t>The temperature at which clouds begin to form</t>
+  </si>
+  <si>
+    <t>You define an air mass as</t>
+  </si>
+  <si>
+    <t>Large bodies of air with a uniform temperature and moisture.</t>
+  </si>
+  <si>
+    <t>Low pressure areas</t>
+  </si>
+  <si>
+    <t>High pressure areas</t>
+  </si>
+  <si>
+    <t>Large bodies of air with a uniform temperature</t>
+  </si>
+  <si>
+    <t>Every physical process of weather is accompanied by, or is the result of, a:</t>
+  </si>
+  <si>
+    <t>heat exchange</t>
+  </si>
+  <si>
+    <t>movement of air</t>
+  </si>
+  <si>
+    <t>pressure differential</t>
+  </si>
+  <si>
+    <t>temperature inversion</t>
+  </si>
+  <si>
     <t>Low clouds range from the surface to _____ ft AGL and have the prefix _____</t>
   </si>
   <si>
@@ -4662,6 +4737,150 @@
     <t>From a left crosswind to a right crosswind</t>
   </si>
   <si>
+    <t>On a prognostic chart, a red line with a repeated pattern of one dash and two dots signifies what?</t>
+  </si>
+  <si>
+    <t>Squall line</t>
+  </si>
+  <si>
+    <t>Trough</t>
+  </si>
+  <si>
+    <t>Warm Front</t>
+  </si>
+  <si>
+    <t>Tropical Wave</t>
+  </si>
+  <si>
+    <t>Steady precipitation preceding a front is an indication of</t>
+  </si>
+  <si>
+    <t>Stratiform clouds with little or no turbulence</t>
+  </si>
+  <si>
+    <t>Stratiform clouds with moderate turbulence</t>
+  </si>
+  <si>
+    <t>Cumuliform clouds with little or no turbulence</t>
+  </si>
+  <si>
+    <t>Cumuliform clouds with moderate turbulence</t>
+  </si>
+  <si>
+    <t>What are characteristics of a moist, unstable air mass?</t>
+  </si>
+  <si>
+    <t>Cumuliform clouds and showery precipitation</t>
+  </si>
+  <si>
+    <t>Stratiform clouds and showery precipitation</t>
+  </si>
+  <si>
+    <t>Poor visibility and smooth air</t>
+  </si>
+  <si>
+    <t>Gusty winds and rime icing</t>
+  </si>
+  <si>
+    <t>At approximately what altitude above the surface would the pilot expect the base of cumuliform clouds if the surface air temperature is 27° C and the dewpoint is 3° C?</t>
+  </si>
+  <si>
+    <t>11000 AGL</t>
+  </si>
+  <si>
+    <t>10000 AGL</t>
+  </si>
+  <si>
+    <t>9000 AGL</t>
+  </si>
+  <si>
+    <t>12000 AGL</t>
+  </si>
+  <si>
+    <t>While flying over mountainous terrain you see clouds with extensive vertical development. What does this indicate?</t>
+  </si>
+  <si>
+    <t>An unstable air mass over the mountains</t>
+  </si>
+  <si>
+    <t>You are in a stable air mass</t>
+  </si>
+  <si>
+    <t>Dry air</t>
+  </si>
+  <si>
+    <t>You are flying in are colder than the ground</t>
+  </si>
+  <si>
+    <t>A nonfrontal, narrow band of active thunderstorms that often develop ahead of a cold front is a known as a</t>
+  </si>
+  <si>
+    <t>Prefrontal System</t>
+  </si>
+  <si>
+    <t>Dry line</t>
+  </si>
+  <si>
+    <t>One weather phenomenon which will always occur when flying across a front is a change in the</t>
+  </si>
+  <si>
+    <t>wind direction</t>
+  </si>
+  <si>
+    <t>stability of the air mass</t>
+  </si>
+  <si>
+    <t>type of precipitation</t>
+  </si>
+  <si>
+    <t>cloud type</t>
+  </si>
+  <si>
+    <t>If an unstable air mass is forced upward, what type clouds can be expected?</t>
+  </si>
+  <si>
+    <t>Clouds with considerable vertical development and associated turbulence</t>
+  </si>
+  <si>
+    <t>Stratus clouds with little vertical development</t>
+  </si>
+  <si>
+    <t>Stratus clouds with considerable associated turbulence</t>
+  </si>
+  <si>
+    <t>Cumulus clouds with rime icing risk</t>
+  </si>
+  <si>
+    <t>Which is true with respect to a high - or low-pressure system</t>
+  </si>
+  <si>
+    <t>A high-pressure area or ridge is an area of descending air</t>
+  </si>
+  <si>
+    <t>A low-pressure area or trough is an area of descending air</t>
+  </si>
+  <si>
+    <t>A high-pressure area or ridge is an area of rising air</t>
+  </si>
+  <si>
+    <t>A low-pressure area or trough is an area of hot air</t>
+  </si>
+  <si>
+    <t>What is the approximate base of the cumulus clouds if the surface air temperature at 1,000' MSL is 21° C and the dewpoint is 9° C?</t>
+  </si>
+  <si>
+    <t>6,000' MSL</t>
+  </si>
+  <si>
+    <t>5,000' MSL</t>
+  </si>
+  <si>
+    <t>7,000' MSL</t>
+  </si>
+  <si>
+    <t>8,000' MSL</t>
+  </si>
+  <si>
     <t>If you are experiencing turbulence 60% of the time, how would you report the duration?</t>
   </si>
   <si>
@@ -4692,108 +4911,6 @@
     <t>Temperature inversion turbulence, because it subverts pilot expectations for performance, causing a large chance for disorientation and loss of control</t>
   </si>
   <si>
-    <t>The FAA defines a ceiling as</t>
-  </si>
-  <si>
-    <t xml:space="preserve">The height of the lowest layer of clouds above the surface that are either broken or overcast, but not thin. </t>
-  </si>
-  <si>
-    <t>The base of the highest scattered (or denser) cloud above the surface AGL</t>
-  </si>
-  <si>
-    <t>The top of the lowest broken or overcast cloud in the celestial dome</t>
-  </si>
-  <si>
-    <t>On a prognostic chart, a red line with a repeated pattern of one dash and two dots signifies what?</t>
-  </si>
-  <si>
-    <t>Squall line</t>
-  </si>
-  <si>
-    <t>Trough</t>
-  </si>
-  <si>
-    <t>Warm Front</t>
-  </si>
-  <si>
-    <t>Tropical Wave</t>
-  </si>
-  <si>
-    <t>Steady precipitation preceding a front is an indication of</t>
-  </si>
-  <si>
-    <t>Stratiform clouds with little or no turbulence</t>
-  </si>
-  <si>
-    <t>Stratiform clouds with moderate turbulence</t>
-  </si>
-  <si>
-    <t>Cumuliform clouds with little or no turbulence</t>
-  </si>
-  <si>
-    <t>Cumuliform clouds with moderate turbulence</t>
-  </si>
-  <si>
-    <t>What are characteristics of a moist, unstable air mass?</t>
-  </si>
-  <si>
-    <t>Cumuliform clouds and showery precipitation</t>
-  </si>
-  <si>
-    <t>Stratiform clouds and showery precipitation</t>
-  </si>
-  <si>
-    <t>Poor visibility and smooth air</t>
-  </si>
-  <si>
-    <t>Gusty winds and rime icing</t>
-  </si>
-  <si>
-    <t>At approximately what altitude above the surface would the pilot expect the base of cumuliform clouds if the surface air temperature is 27° C and the dewpoint is 3° C?</t>
-  </si>
-  <si>
-    <t>11000 AGL</t>
-  </si>
-  <si>
-    <t>10000 AGL</t>
-  </si>
-  <si>
-    <t>9000 AGL</t>
-  </si>
-  <si>
-    <t>12000 AGL</t>
-  </si>
-  <si>
-    <t>A TAF includes:</t>
-  </si>
-  <si>
-    <t>Wind, visibility, weather phenomena, obstructions to vision, and cloud coverage</t>
-  </si>
-  <si>
-    <t>Wind, visibility, cloud coverage, and cloud tops in feet MSL</t>
-  </si>
-  <si>
-    <t>Wind, obstructions to vision, and cloud tops in feet MSL</t>
-  </si>
-  <si>
-    <t>Wind, visibility, weather phenomena, obstructions to vision, cloud coverage, and cloud tops in feet MSL</t>
-  </si>
-  <si>
-    <t>While flying over mountainous terrain you see clouds with extensive vertical development. What does this indicate?</t>
-  </si>
-  <si>
-    <t>An unstable air mass over the mountains</t>
-  </si>
-  <si>
-    <t>You are in a stable air mass</t>
-  </si>
-  <si>
-    <t>Dry air</t>
-  </si>
-  <si>
-    <t>You are flying in are colder than the ground</t>
-  </si>
-  <si>
     <t>Frost on the wing of an airplane:</t>
   </si>
   <si>
@@ -4809,30 +4926,6 @@
     <t>Should be scrapped off before flying</t>
   </si>
   <si>
-    <t>The amount of water vapor which air can hold depends on the</t>
-  </si>
-  <si>
-    <t>air temperature</t>
-  </si>
-  <si>
-    <t>stability of the air</t>
-  </si>
-  <si>
-    <t>dewpoint</t>
-  </si>
-  <si>
-    <t>relative humidity</t>
-  </si>
-  <si>
-    <t>A nonfrontal, narrow band of active thunderstorms that often develop ahead of a cold front is a known as a</t>
-  </si>
-  <si>
-    <t>Prefrontal System</t>
-  </si>
-  <si>
-    <t>Dry line</t>
-  </si>
-  <si>
     <t>One in-flight condition necessary for structural icing to form is</t>
   </si>
   <si>
@@ -4848,51 +4941,6 @@
     <t>ground temperature below freezing</t>
   </si>
   <si>
-    <t>Clouds are divided into four families according to their</t>
-  </si>
-  <si>
-    <t>height range</t>
-  </si>
-  <si>
-    <t>outward shape</t>
-  </si>
-  <si>
-    <t>composition</t>
-  </si>
-  <si>
-    <t>stability</t>
-  </si>
-  <si>
-    <t>One weather phenomenon which will always occur when flying across a front is a change in the</t>
-  </si>
-  <si>
-    <t>wind direction</t>
-  </si>
-  <si>
-    <t>stability of the air mass</t>
-  </si>
-  <si>
-    <t>type of precipitation</t>
-  </si>
-  <si>
-    <t>cloud type</t>
-  </si>
-  <si>
-    <t>What is meant by the term 'dewpoint'?</t>
-  </si>
-  <si>
-    <t>The temperature to which air must be cooled to become saturated</t>
-  </si>
-  <si>
-    <t>The temperature at which dew will always form</t>
-  </si>
-  <si>
-    <t>The temperature at which condensation and evaporation are equal</t>
-  </si>
-  <si>
-    <t>The temperature at which clouds begin to form</t>
-  </si>
-  <si>
     <t>Upon encountering severe turbulence, which flight condition should the pilot attempt to maintain?</t>
   </si>
   <si>
@@ -4908,21 +4956,6 @@
     <t>Current airplane attitude</t>
   </si>
   <si>
-    <t>Aviation Routine Weather reports (METARs) contain</t>
-  </si>
-  <si>
-    <t>Wind, visibility, precipitation, cloud coverage, temperature, and altimeter setting</t>
-  </si>
-  <si>
-    <t>Wind, visibility, and precipitation</t>
-  </si>
-  <si>
-    <t>Wind, visibility, precipitation, and temperature</t>
-  </si>
-  <si>
-    <t>Wind, visibility, precipitation, cloud coverage, temperature, humidity, and altimeter setting</t>
-  </si>
-  <si>
     <t>Inland fog is most likely</t>
   </si>
   <si>
@@ -4938,21 +4971,6 @@
     <t>Precipitation Induced fog</t>
   </si>
   <si>
-    <t>You define an air mass as</t>
-  </si>
-  <si>
-    <t>Large bodies of air with a uniform temperature and moisture.</t>
-  </si>
-  <si>
-    <t>Low pressure areas</t>
-  </si>
-  <si>
-    <t>High pressure areas</t>
-  </si>
-  <si>
-    <t>Large bodies of air with a uniform temperature</t>
-  </si>
-  <si>
     <t>In which situation is advection fog most likely to form</t>
   </si>
   <si>
@@ -4968,66 +4986,6 @@
     <t>At night on clear, calm evenings after the sun has set</t>
   </si>
   <si>
-    <t>If an unstable air mass is forced upward, what type clouds can be expected?</t>
-  </si>
-  <si>
-    <t>Clouds with considerable vertical development and associated turbulence</t>
-  </si>
-  <si>
-    <t>Stratus clouds with little vertical development</t>
-  </si>
-  <si>
-    <t>Stratus clouds with considerable associated turbulence</t>
-  </si>
-  <si>
-    <t>Cumulus clouds with rime icing risk</t>
-  </si>
-  <si>
-    <t>On a TAF, the broken cloud layer written as, BKN250 indicates:</t>
-  </si>
-  <si>
-    <t xml:space="preserve"> A broken cloud layer at 25,000 feet AGL</t>
-  </si>
-  <si>
-    <t xml:space="preserve"> A broken cloud layer at 2,500 feet AGL</t>
-  </si>
-  <si>
-    <t xml:space="preserve"> A broken cloud layer at 250 feet AGL</t>
-  </si>
-  <si>
-    <t xml:space="preserve"> A broken cloud layer at 2,500 feet MSL</t>
-  </si>
-  <si>
-    <t>Every physical process of weather is accompanied by, or is the result of, a:</t>
-  </si>
-  <si>
-    <t>heat exchange</t>
-  </si>
-  <si>
-    <t>movement of air</t>
-  </si>
-  <si>
-    <t>pressure differential</t>
-  </si>
-  <si>
-    <t>temperature inversion</t>
-  </si>
-  <si>
-    <t>Which is true with respect to a high - or low-pressure system</t>
-  </si>
-  <si>
-    <t>A high-pressure area or ridge is an area of descending air</t>
-  </si>
-  <si>
-    <t>A low-pressure area or trough is an area of descending air</t>
-  </si>
-  <si>
-    <t>A high-pressure area or ridge is an area of rising air</t>
-  </si>
-  <si>
-    <t>A low-pressure area or trough is an area of hot air</t>
-  </si>
-  <si>
     <t>What situation is most conducive to the formation of radiation fog?</t>
   </si>
   <si>
@@ -5038,21 +4996,6 @@
   </si>
   <si>
     <t>Moist, tropical air moving over cold, offshore water</t>
-  </si>
-  <si>
-    <t>What is the approximate base of the cumulus clouds if the surface air temperature at 1,000' MSL is 21° C and the dewpoint is 9° C?</t>
-  </si>
-  <si>
-    <t>6,000' MSL</t>
-  </si>
-  <si>
-    <t>5,000' MSL</t>
-  </si>
-  <si>
-    <t>7,000' MSL</t>
-  </si>
-  <si>
-    <t>8,000' MSL</t>
   </si>
   <si>
     <t>The most frequent type of ground or surface-based temperature inversion is that which is produced by</t>
@@ -5158,6 +5101,108 @@
     <t>50-300, cold front</t>
   </si>
   <si>
+    <t>Going under a thunderstorm is the ______ option just after ______</t>
+  </si>
+  <si>
+    <t>3rd, going over</t>
+  </si>
+  <si>
+    <t>2nd, circumnavigating</t>
+  </si>
+  <si>
+    <t>1st, none</t>
+  </si>
+  <si>
+    <t>4th, going through it</t>
+  </si>
+  <si>
+    <t>What kind of fog can the sun dissipate</t>
+  </si>
+  <si>
+    <t>Convection fog</t>
+  </si>
+  <si>
+    <t>What are the intensity levels of turbulence</t>
+  </si>
+  <si>
+    <t>Light, moderate, severe, and extreme</t>
+  </si>
+  <si>
+    <t>Trace, light, moderate, and severe</t>
+  </si>
+  <si>
+    <t>Light, moderate, and heavy</t>
+  </si>
+  <si>
+    <t>Light, moderate, heavy, and extreme</t>
+  </si>
+  <si>
+    <t>What are the intensity levels of icing</t>
+  </si>
+  <si>
+    <t>Light, moderate, and severe</t>
+  </si>
+  <si>
+    <t>Trace, moderate, and severe</t>
+  </si>
+  <si>
+    <t>The FAA defines a ceiling as</t>
+  </si>
+  <si>
+    <t xml:space="preserve">The height of the lowest layer of clouds above the surface that are either broken or overcast, but not thin. </t>
+  </si>
+  <si>
+    <t>The base of the highest scattered (or denser) cloud above the surface AGL</t>
+  </si>
+  <si>
+    <t>The top of the lowest broken or overcast cloud in the celestial dome</t>
+  </si>
+  <si>
+    <t>A TAF includes:</t>
+  </si>
+  <si>
+    <t>Wind, visibility, weather phenomena, obstructions to vision, and cloud coverage</t>
+  </si>
+  <si>
+    <t>Wind, visibility, cloud coverage, and cloud tops in feet MSL</t>
+  </si>
+  <si>
+    <t>Wind, obstructions to vision, and cloud tops in feet MSL</t>
+  </si>
+  <si>
+    <t>Wind, visibility, weather phenomena, obstructions to vision, cloud coverage, and cloud tops in feet MSL</t>
+  </si>
+  <si>
+    <t>Aviation Routine Weather reports (METARs) contain</t>
+  </si>
+  <si>
+    <t>Wind, visibility, precipitation, cloud coverage, temperature, and altimeter setting</t>
+  </si>
+  <si>
+    <t>Wind, visibility, and precipitation</t>
+  </si>
+  <si>
+    <t>Wind, visibility, precipitation, and temperature</t>
+  </si>
+  <si>
+    <t>Wind, visibility, precipitation, cloud coverage, temperature, humidity, and altimeter setting</t>
+  </si>
+  <si>
+    <t>On a TAF, the broken cloud layer written as, BKN250 indicates:</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> A broken cloud layer at 25,000 feet AGL</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> A broken cloud layer at 2,500 feet AGL</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> A broken cloud layer at 250 feet AGL</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> A broken cloud layer at 2,500 feet MSL</t>
+  </si>
+  <si>
     <t>How are Prognostic Charts best used by a pilot?</t>
   </si>
   <si>
@@ -5284,7 +5329,7 @@
     <t>The average horizontal visibility across the horizon circle</t>
   </si>
   <si>
-    <t>The maximum horizontal visibility anywhere on the horizon circle</t>
+    <t>The greatest horizontal visibility through a continuous arc that is at least half of the horizon circle</t>
   </si>
   <si>
     <t>(Refer to figure 17.) What wind is forecast for AMA at 12,000 feet?</t>
@@ -5773,10 +5818,10 @@
     <xf borderId="8" fillId="0" fontId="2" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
       <alignment readingOrder="0" shrinkToFit="0" vertical="bottom" wrapText="0"/>
     </xf>
-    <xf borderId="5" fillId="0" fontId="1" numFmtId="3" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1" applyNumberFormat="1">
+    <xf borderId="8" fillId="0" fontId="1" numFmtId="3" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1" applyNumberFormat="1">
       <alignment readingOrder="0" shrinkToFit="0" vertical="center" wrapText="0"/>
     </xf>
-    <xf borderId="8" fillId="0" fontId="1" numFmtId="3" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1" applyNumberFormat="1">
+    <xf borderId="5" fillId="0" fontId="1" numFmtId="3" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1" applyNumberFormat="1">
       <alignment readingOrder="0" shrinkToFit="0" vertical="center" wrapText="0"/>
     </xf>
     <xf borderId="10" fillId="0" fontId="1" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
@@ -5846,8 +5891,8 @@
 </file>
 
 <file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" ref="A1:H403" displayName="Table1" name="Table1" id="1">
-  <autoFilter ref="$A$1:$H$403"/>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" ref="A1:H407" displayName="Table1" name="Table1" id="1">
+  <autoFilter ref="$A$1:$H$407"/>
   <tableColumns count="8">
     <tableColumn name="Topic" id="1"/>
     <tableColumn name="Lecture" id="2"/>
@@ -6123,7 +6168,7 @@
         <v>13</v>
       </c>
       <c r="H2" s="6">
-        <f t="shared" ref="H2:H403" si="1">ROW()</f>
+        <f t="shared" ref="H2:H407" si="1">ROW()</f>
         <v>2</v>
       </c>
     </row>
@@ -14551,25 +14596,25 @@
       <c r="A319" s="7" t="s">
         <v>1340</v>
       </c>
-      <c r="B319" s="8">
-        <v>2.0</v>
-      </c>
-      <c r="C319" s="8" t="s">
+      <c r="B319" s="12">
+        <v>1.0</v>
+      </c>
+      <c r="C319" s="12" t="s">
         <v>1434</v>
       </c>
-      <c r="D319" s="8" t="s">
+      <c r="D319" s="25" t="s">
         <v>1435</v>
       </c>
-      <c r="E319" s="8" t="s">
+      <c r="E319" s="25" t="s">
         <v>1436</v>
       </c>
-      <c r="F319" s="8" t="s">
+      <c r="F319" s="25" t="s">
         <v>1437</v>
       </c>
-      <c r="G319" s="8" t="s">
+      <c r="G319" s="25" t="s">
         <v>1438</v>
       </c>
-      <c r="H319" s="9">
+      <c r="H319" s="13">
         <f t="shared" si="1"/>
         <v>319</v>
       </c>
@@ -14579,21 +14624,21 @@
         <v>1340</v>
       </c>
       <c r="B320" s="10">
-        <v>2.0</v>
+        <v>1.0</v>
       </c>
       <c r="C320" s="10" t="s">
         <v>1439</v>
       </c>
-      <c r="D320" s="10" t="s">
+      <c r="D320" s="26" t="s">
         <v>1440</v>
       </c>
-      <c r="E320" s="10" t="s">
+      <c r="E320" s="26" t="s">
         <v>1441</v>
       </c>
-      <c r="F320" s="10" t="s">
+      <c r="F320" s="26" t="s">
         <v>1442</v>
       </c>
-      <c r="G320" s="10" t="s">
+      <c r="G320" s="26" t="s">
         <v>1443</v>
       </c>
       <c r="H320" s="11">
@@ -14606,22 +14651,22 @@
         <v>1340</v>
       </c>
       <c r="B321" s="12">
-        <v>2.0</v>
+        <v>1.0</v>
       </c>
       <c r="C321" s="12" t="s">
         <v>1444</v>
       </c>
-      <c r="D321" s="12" t="s">
-        <v>1440</v>
-      </c>
-      <c r="E321" s="12" t="s">
-        <v>1441</v>
-      </c>
-      <c r="F321" s="12" t="s">
-        <v>1442</v>
-      </c>
-      <c r="G321" s="12" t="s">
-        <v>1443</v>
+      <c r="D321" s="25" t="s">
+        <v>1445</v>
+      </c>
+      <c r="E321" s="25" t="s">
+        <v>1446</v>
+      </c>
+      <c r="F321" s="25" t="s">
+        <v>1447</v>
+      </c>
+      <c r="G321" s="25" t="s">
+        <v>1448</v>
       </c>
       <c r="H321" s="13">
         <f t="shared" si="1"/>
@@ -14633,22 +14678,22 @@
         <v>1340</v>
       </c>
       <c r="B322" s="10">
-        <v>2.0</v>
+        <v>1.0</v>
       </c>
       <c r="C322" s="10" t="s">
-        <v>1445</v>
-      </c>
-      <c r="D322" s="10" t="s">
-        <v>1446</v>
-      </c>
-      <c r="E322" s="10" t="s">
-        <v>1447</v>
-      </c>
-      <c r="F322" s="10" t="s">
-        <v>1448</v>
-      </c>
-      <c r="G322" s="10" t="s">
         <v>1449</v>
+      </c>
+      <c r="D322" s="26" t="s">
+        <v>1450</v>
+      </c>
+      <c r="E322" s="26" t="s">
+        <v>1451</v>
+      </c>
+      <c r="F322" s="26" t="s">
+        <v>1452</v>
+      </c>
+      <c r="G322" s="26" t="s">
+        <v>1453</v>
       </c>
       <c r="H322" s="11">
         <f t="shared" si="1"/>
@@ -14660,22 +14705,22 @@
         <v>1340</v>
       </c>
       <c r="B323" s="12">
-        <v>2.0</v>
+        <v>1.0</v>
       </c>
       <c r="C323" s="12" t="s">
-        <v>1450</v>
-      </c>
-      <c r="D323" s="12" t="s">
-        <v>1451</v>
-      </c>
-      <c r="E323" s="12" t="s">
-        <v>1452</v>
-      </c>
-      <c r="F323" s="12" t="s">
-        <v>1453</v>
-      </c>
-      <c r="G323" s="12" t="s">
         <v>1454</v>
+      </c>
+      <c r="D323" s="25" t="s">
+        <v>1455</v>
+      </c>
+      <c r="E323" s="25" t="s">
+        <v>1456</v>
+      </c>
+      <c r="F323" s="25" t="s">
+        <v>1457</v>
+      </c>
+      <c r="G323" s="25" t="s">
+        <v>1458</v>
       </c>
       <c r="H323" s="13">
         <f t="shared" si="1"/>
@@ -14686,25 +14731,25 @@
       <c r="A324" s="4" t="s">
         <v>1340</v>
       </c>
-      <c r="B324" s="10">
+      <c r="B324" s="5">
         <v>2.0</v>
       </c>
-      <c r="C324" s="10" t="s">
-        <v>1455</v>
-      </c>
-      <c r="D324" s="10" t="s">
-        <v>1456</v>
-      </c>
-      <c r="E324" s="10" t="s">
-        <v>1441</v>
-      </c>
-      <c r="F324" s="10" t="s">
-        <v>1457</v>
-      </c>
-      <c r="G324" s="10" t="s">
-        <v>1458</v>
-      </c>
-      <c r="H324" s="11">
+      <c r="C324" s="5" t="s">
+        <v>1459</v>
+      </c>
+      <c r="D324" s="5" t="s">
+        <v>1460</v>
+      </c>
+      <c r="E324" s="5" t="s">
+        <v>1461</v>
+      </c>
+      <c r="F324" s="5" t="s">
+        <v>1462</v>
+      </c>
+      <c r="G324" s="5" t="s">
+        <v>1463</v>
+      </c>
+      <c r="H324" s="6">
         <f t="shared" si="1"/>
         <v>324</v>
       </c>
@@ -14717,19 +14762,19 @@
         <v>2.0</v>
       </c>
       <c r="C325" s="12" t="s">
-        <v>1459</v>
+        <v>1464</v>
       </c>
       <c r="D325" s="12" t="s">
-        <v>1460</v>
+        <v>1465</v>
       </c>
       <c r="E325" s="12" t="s">
-        <v>1461</v>
+        <v>1466</v>
       </c>
       <c r="F325" s="12" t="s">
-        <v>1462</v>
+        <v>1467</v>
       </c>
       <c r="G325" s="12" t="s">
-        <v>1463</v>
+        <v>1468</v>
       </c>
       <c r="H325" s="13">
         <f t="shared" si="1"/>
@@ -14744,7 +14789,7 @@
         <v>2.0</v>
       </c>
       <c r="C326" s="10" t="s">
-        <v>1464</v>
+        <v>1469</v>
       </c>
       <c r="D326" s="10" t="s">
         <v>1465</v>
@@ -14753,10 +14798,10 @@
         <v>1466</v>
       </c>
       <c r="F326" s="10" t="s">
-        <v>1461</v>
+        <v>1467</v>
       </c>
       <c r="G326" s="10" t="s">
-        <v>1462</v>
+        <v>1468</v>
       </c>
       <c r="H326" s="11">
         <f t="shared" si="1"/>
@@ -14771,19 +14816,19 @@
         <v>2.0</v>
       </c>
       <c r="C327" s="12" t="s">
-        <v>1467</v>
+        <v>1470</v>
       </c>
       <c r="D327" s="12" t="s">
-        <v>1468</v>
+        <v>1471</v>
       </c>
       <c r="E327" s="12" t="s">
-        <v>1469</v>
+        <v>1472</v>
       </c>
       <c r="F327" s="12" t="s">
-        <v>1470</v>
+        <v>1473</v>
       </c>
       <c r="G327" s="12" t="s">
-        <v>1471</v>
+        <v>1474</v>
       </c>
       <c r="H327" s="13">
         <f t="shared" si="1"/>
@@ -14798,19 +14843,19 @@
         <v>2.0</v>
       </c>
       <c r="C328" s="10" t="s">
-        <v>1472</v>
+        <v>1475</v>
       </c>
       <c r="D328" s="10" t="s">
-        <v>1473</v>
+        <v>1476</v>
       </c>
       <c r="E328" s="10" t="s">
-        <v>1474</v>
+        <v>1477</v>
       </c>
       <c r="F328" s="10" t="s">
-        <v>1475</v>
+        <v>1478</v>
       </c>
       <c r="G328" s="10" t="s">
-        <v>1476</v>
+        <v>1479</v>
       </c>
       <c r="H328" s="11">
         <f t="shared" si="1"/>
@@ -14825,19 +14870,19 @@
         <v>2.0</v>
       </c>
       <c r="C329" s="12" t="s">
-        <v>1477</v>
+        <v>1480</v>
       </c>
       <c r="D329" s="12" t="s">
-        <v>1478</v>
+        <v>1481</v>
       </c>
       <c r="E329" s="12" t="s">
-        <v>1479</v>
+        <v>1466</v>
       </c>
       <c r="F329" s="12" t="s">
-        <v>1480</v>
+        <v>1482</v>
       </c>
       <c r="G329" s="12" t="s">
-        <v>1481</v>
+        <v>1483</v>
       </c>
       <c r="H329" s="13">
         <f t="shared" si="1"/>
@@ -14852,19 +14897,19 @@
         <v>2.0</v>
       </c>
       <c r="C330" s="10" t="s">
-        <v>1482</v>
+        <v>1484</v>
       </c>
       <c r="D330" s="10" t="s">
-        <v>1483</v>
+        <v>1485</v>
       </c>
       <c r="E330" s="10" t="s">
-        <v>1484</v>
+        <v>1486</v>
       </c>
       <c r="F330" s="10" t="s">
-        <v>1485</v>
+        <v>1487</v>
       </c>
       <c r="G330" s="10" t="s">
-        <v>1486</v>
+        <v>1488</v>
       </c>
       <c r="H330" s="11">
         <f t="shared" si="1"/>
@@ -14879,19 +14924,19 @@
         <v>2.0</v>
       </c>
       <c r="C331" s="12" t="s">
+        <v>1489</v>
+      </c>
+      <c r="D331" s="12" t="s">
+        <v>1490</v>
+      </c>
+      <c r="E331" s="12" t="s">
+        <v>1491</v>
+      </c>
+      <c r="F331" s="12" t="s">
+        <v>1486</v>
+      </c>
+      <c r="G331" s="12" t="s">
         <v>1487</v>
-      </c>
-      <c r="D331" s="12" t="s">
-        <v>1479</v>
-      </c>
-      <c r="E331" s="12" t="s">
-        <v>1478</v>
-      </c>
-      <c r="F331" s="12" t="s">
-        <v>1480</v>
-      </c>
-      <c r="G331" s="12" t="s">
-        <v>1481</v>
       </c>
       <c r="H331" s="13">
         <f t="shared" si="1"/>
@@ -14906,19 +14951,19 @@
         <v>2.0</v>
       </c>
       <c r="C332" s="10" t="s">
-        <v>1488</v>
+        <v>1492</v>
       </c>
       <c r="D332" s="10" t="s">
-        <v>1489</v>
+        <v>1493</v>
       </c>
       <c r="E332" s="10" t="s">
-        <v>1490</v>
+        <v>1494</v>
       </c>
       <c r="F332" s="10" t="s">
-        <v>1491</v>
+        <v>1495</v>
       </c>
       <c r="G332" s="10" t="s">
-        <v>1492</v>
+        <v>1496</v>
       </c>
       <c r="H332" s="11">
         <f t="shared" si="1"/>
@@ -14933,19 +14978,19 @@
         <v>2.0</v>
       </c>
       <c r="C333" s="12" t="s">
-        <v>1493</v>
+        <v>1497</v>
       </c>
       <c r="D333" s="12" t="s">
-        <v>1494</v>
+        <v>1498</v>
       </c>
       <c r="E333" s="12" t="s">
-        <v>1480</v>
+        <v>1499</v>
       </c>
       <c r="F333" s="12" t="s">
-        <v>1481</v>
+        <v>1500</v>
       </c>
       <c r="G333" s="12" t="s">
-        <v>1495</v>
+        <v>1501</v>
       </c>
       <c r="H333" s="13">
         <f t="shared" si="1"/>
@@ -14960,19 +15005,19 @@
         <v>2.0</v>
       </c>
       <c r="C334" s="10" t="s">
-        <v>1496</v>
+        <v>1502</v>
       </c>
       <c r="D334" s="10" t="s">
-        <v>1497</v>
+        <v>1503</v>
       </c>
       <c r="E334" s="10" t="s">
-        <v>1498</v>
+        <v>1504</v>
       </c>
       <c r="F334" s="10" t="s">
-        <v>1499</v>
+        <v>1505</v>
       </c>
       <c r="G334" s="10" t="s">
-        <v>1500</v>
+        <v>1506</v>
       </c>
       <c r="H334" s="11">
         <f t="shared" si="1"/>
@@ -14987,19 +15032,19 @@
         <v>2.0</v>
       </c>
       <c r="C335" s="12" t="s">
-        <v>1501</v>
+        <v>1507</v>
       </c>
       <c r="D335" s="12" t="s">
-        <v>1502</v>
+        <v>1508</v>
       </c>
       <c r="E335" s="12" t="s">
-        <v>1503</v>
+        <v>1509</v>
       </c>
       <c r="F335" s="12" t="s">
-        <v>1504</v>
+        <v>1510</v>
       </c>
       <c r="G335" s="12" t="s">
-        <v>1505</v>
+        <v>1511</v>
       </c>
       <c r="H335" s="13">
         <f t="shared" si="1"/>
@@ -15014,19 +15059,19 @@
         <v>2.0</v>
       </c>
       <c r="C336" s="10" t="s">
+        <v>1512</v>
+      </c>
+      <c r="D336" s="10" t="s">
+        <v>1504</v>
+      </c>
+      <c r="E336" s="10" t="s">
+        <v>1503</v>
+      </c>
+      <c r="F336" s="10" t="s">
+        <v>1505</v>
+      </c>
+      <c r="G336" s="10" t="s">
         <v>1506</v>
-      </c>
-      <c r="D336" s="10" t="s">
-        <v>1507</v>
-      </c>
-      <c r="E336" s="10" t="s">
-        <v>1508</v>
-      </c>
-      <c r="F336" s="10" t="s">
-        <v>1509</v>
-      </c>
-      <c r="G336" s="10" t="s">
-        <v>1510</v>
       </c>
       <c r="H336" s="11">
         <f t="shared" si="1"/>
@@ -15041,19 +15086,19 @@
         <v>2.0</v>
       </c>
       <c r="C337" s="12" t="s">
-        <v>1511</v>
+        <v>1513</v>
       </c>
       <c r="D337" s="12" t="s">
-        <v>1512</v>
+        <v>1514</v>
       </c>
       <c r="E337" s="12" t="s">
-        <v>1513</v>
+        <v>1515</v>
       </c>
       <c r="F337" s="12" t="s">
-        <v>1513</v>
+        <v>1516</v>
       </c>
       <c r="G337" s="12" t="s">
-        <v>1514</v>
+        <v>1517</v>
       </c>
       <c r="H337" s="13">
         <f t="shared" si="1"/>
@@ -15068,19 +15113,19 @@
         <v>2.0</v>
       </c>
       <c r="C338" s="10" t="s">
-        <v>1515</v>
+        <v>1518</v>
       </c>
       <c r="D338" s="10" t="s">
-        <v>1516</v>
+        <v>1519</v>
       </c>
       <c r="E338" s="10" t="s">
-        <v>1517</v>
+        <v>1505</v>
       </c>
       <c r="F338" s="10" t="s">
-        <v>1518</v>
+        <v>1506</v>
       </c>
       <c r="G338" s="10" t="s">
-        <v>169</v>
+        <v>1520</v>
       </c>
       <c r="H338" s="11">
         <f t="shared" si="1"/>
@@ -15095,19 +15140,19 @@
         <v>2.0</v>
       </c>
       <c r="C339" s="12" t="s">
-        <v>1519</v>
+        <v>1521</v>
       </c>
       <c r="D339" s="12" t="s">
-        <v>1520</v>
+        <v>1522</v>
       </c>
       <c r="E339" s="12" t="s">
-        <v>1521</v>
+        <v>1523</v>
       </c>
       <c r="F339" s="12" t="s">
-        <v>1520</v>
+        <v>1524</v>
       </c>
       <c r="G339" s="12" t="s">
-        <v>1522</v>
+        <v>1525</v>
       </c>
       <c r="H339" s="13">
         <f t="shared" si="1"/>
@@ -15122,19 +15167,19 @@
         <v>2.0</v>
       </c>
       <c r="C340" s="10" t="s">
-        <v>1523</v>
+        <v>1526</v>
       </c>
       <c r="D340" s="10" t="s">
-        <v>1524</v>
+        <v>1527</v>
       </c>
       <c r="E340" s="10" t="s">
-        <v>1525</v>
+        <v>1528</v>
       </c>
       <c r="F340" s="10" t="s">
-        <v>1526</v>
+        <v>1529</v>
       </c>
       <c r="G340" s="10" t="s">
-        <v>1527</v>
+        <v>1530</v>
       </c>
       <c r="H340" s="11">
         <f t="shared" si="1"/>
@@ -15149,19 +15194,19 @@
         <v>2.0</v>
       </c>
       <c r="C341" s="12" t="s">
-        <v>1528</v>
+        <v>1531</v>
       </c>
       <c r="D341" s="12" t="s">
-        <v>1480</v>
+        <v>1532</v>
       </c>
       <c r="E341" s="12" t="s">
-        <v>1529</v>
+        <v>1533</v>
       </c>
       <c r="F341" s="12" t="s">
-        <v>1481</v>
+        <v>1534</v>
       </c>
       <c r="G341" s="12" t="s">
-        <v>1478</v>
+        <v>1535</v>
       </c>
       <c r="H341" s="13">
         <f t="shared" si="1"/>
@@ -15176,19 +15221,19 @@
         <v>2.0</v>
       </c>
       <c r="C342" s="10" t="s">
-        <v>1530</v>
+        <v>1536</v>
       </c>
       <c r="D342" s="10" t="s">
-        <v>1531</v>
+        <v>1537</v>
       </c>
       <c r="E342" s="10" t="s">
-        <v>1532</v>
+        <v>1538</v>
       </c>
       <c r="F342" s="10" t="s">
-        <v>1533</v>
+        <v>1538</v>
       </c>
       <c r="G342" s="10" t="s">
-        <v>169</v>
+        <v>1539</v>
       </c>
       <c r="H342" s="11">
         <f t="shared" si="1"/>
@@ -15203,19 +15248,19 @@
         <v>2.0</v>
       </c>
       <c r="C343" s="12" t="s">
-        <v>1534</v>
+        <v>1540</v>
       </c>
       <c r="D343" s="12" t="s">
-        <v>1535</v>
+        <v>1541</v>
       </c>
       <c r="E343" s="12" t="s">
-        <v>1536</v>
+        <v>1542</v>
       </c>
       <c r="F343" s="12" t="s">
-        <v>1537</v>
+        <v>1543</v>
       </c>
       <c r="G343" s="12" t="s">
-        <v>1538</v>
+        <v>169</v>
       </c>
       <c r="H343" s="13">
         <f t="shared" si="1"/>
@@ -15230,19 +15275,19 @@
         <v>2.0</v>
       </c>
       <c r="C344" s="10" t="s">
-        <v>1539</v>
+        <v>1544</v>
       </c>
       <c r="D344" s="10" t="s">
-        <v>1540</v>
+        <v>1545</v>
       </c>
       <c r="E344" s="10" t="s">
-        <v>1541</v>
+        <v>1546</v>
       </c>
       <c r="F344" s="10" t="s">
-        <v>1542</v>
+        <v>1545</v>
       </c>
       <c r="G344" s="10" t="s">
-        <v>1543</v>
+        <v>1547</v>
       </c>
       <c r="H344" s="11">
         <f t="shared" si="1"/>
@@ -15257,19 +15302,19 @@
         <v>2.0</v>
       </c>
       <c r="C345" s="12" t="s">
-        <v>1544</v>
+        <v>1548</v>
       </c>
       <c r="D345" s="12" t="s">
-        <v>1545</v>
+        <v>1549</v>
       </c>
       <c r="E345" s="12" t="s">
-        <v>1546</v>
+        <v>1550</v>
       </c>
       <c r="F345" s="12" t="s">
-        <v>1547</v>
+        <v>1551</v>
       </c>
       <c r="G345" s="12" t="s">
-        <v>1548</v>
+        <v>1552</v>
       </c>
       <c r="H345" s="13">
         <f t="shared" si="1"/>
@@ -15281,22 +15326,22 @@
         <v>1340</v>
       </c>
       <c r="B346" s="10">
-        <v>3.0</v>
+        <v>2.0</v>
       </c>
       <c r="C346" s="10" t="s">
-        <v>1549</v>
+        <v>1553</v>
       </c>
       <c r="D346" s="10" t="s">
-        <v>1550</v>
+        <v>1505</v>
       </c>
       <c r="E346" s="10" t="s">
-        <v>1551</v>
+        <v>1554</v>
       </c>
       <c r="F346" s="10" t="s">
-        <v>1552</v>
+        <v>1506</v>
       </c>
       <c r="G346" s="10" t="s">
-        <v>1553</v>
+        <v>1503</v>
       </c>
       <c r="H346" s="11">
         <f t="shared" si="1"/>
@@ -15308,22 +15353,22 @@
         <v>1340</v>
       </c>
       <c r="B347" s="12">
-        <v>3.0</v>
+        <v>2.0</v>
       </c>
       <c r="C347" s="12" t="s">
-        <v>1554</v>
+        <v>1555</v>
       </c>
       <c r="D347" s="12" t="s">
-        <v>1555</v>
+        <v>1556</v>
       </c>
       <c r="E347" s="12" t="s">
-        <v>1556</v>
+        <v>1557</v>
       </c>
       <c r="F347" s="12" t="s">
-        <v>1557</v>
+        <v>1558</v>
       </c>
       <c r="G347" s="12" t="s">
-        <v>1558</v>
+        <v>169</v>
       </c>
       <c r="H347" s="13">
         <f t="shared" si="1"/>
@@ -15334,25 +15379,25 @@
       <c r="A348" s="4" t="s">
         <v>1340</v>
       </c>
-      <c r="B348" s="5">
-        <v>4.0</v>
-      </c>
-      <c r="C348" s="5" t="s">
+      <c r="B348" s="10">
+        <v>2.0</v>
+      </c>
+      <c r="C348" s="10" t="s">
         <v>1559</v>
       </c>
-      <c r="D348" s="5" t="s">
+      <c r="D348" s="10" t="s">
         <v>1560</v>
       </c>
-      <c r="E348" s="5" t="s">
+      <c r="E348" s="10" t="s">
         <v>1561</v>
       </c>
-      <c r="F348" s="5" t="s">
+      <c r="F348" s="10" t="s">
         <v>1562</v>
       </c>
-      <c r="G348" s="5" t="s">
-        <v>828</v>
-      </c>
-      <c r="H348" s="6">
+      <c r="G348" s="10" t="s">
+        <v>1563</v>
+      </c>
+      <c r="H348" s="11">
         <f t="shared" si="1"/>
         <v>348</v>
       </c>
@@ -15365,19 +15410,19 @@
         <v>2.0</v>
       </c>
       <c r="C349" s="12" t="s">
-        <v>1563</v>
+        <v>1564</v>
       </c>
       <c r="D349" s="12" t="s">
-        <v>1564</v>
+        <v>1565</v>
       </c>
       <c r="E349" s="12" t="s">
-        <v>1565</v>
+        <v>1566</v>
       </c>
       <c r="F349" s="12" t="s">
-        <v>1566</v>
+        <v>1567</v>
       </c>
       <c r="G349" s="12" t="s">
-        <v>1567</v>
+        <v>1568</v>
       </c>
       <c r="H349" s="13">
         <f t="shared" si="1"/>
@@ -15392,19 +15437,19 @@
         <v>2.0</v>
       </c>
       <c r="C350" s="10" t="s">
-        <v>1568</v>
+        <v>1569</v>
       </c>
       <c r="D350" s="10" t="s">
-        <v>1569</v>
+        <v>1570</v>
       </c>
       <c r="E350" s="10" t="s">
-        <v>1570</v>
+        <v>1571</v>
       </c>
       <c r="F350" s="10" t="s">
-        <v>1571</v>
+        <v>1572</v>
       </c>
       <c r="G350" s="10" t="s">
-        <v>1572</v>
+        <v>1573</v>
       </c>
       <c r="H350" s="11">
         <f t="shared" si="1"/>
@@ -15419,19 +15464,19 @@
         <v>2.0</v>
       </c>
       <c r="C351" s="12" t="s">
-        <v>1573</v>
+        <v>1574</v>
       </c>
       <c r="D351" s="12" t="s">
-        <v>1574</v>
+        <v>1575</v>
       </c>
       <c r="E351" s="12" t="s">
-        <v>1575</v>
+        <v>1576</v>
       </c>
       <c r="F351" s="12" t="s">
-        <v>1576</v>
+        <v>1577</v>
       </c>
       <c r="G351" s="12" t="s">
-        <v>1577</v>
+        <v>1578</v>
       </c>
       <c r="H351" s="13">
         <f t="shared" si="1"/>
@@ -15446,19 +15491,19 @@
         <v>2.0</v>
       </c>
       <c r="C352" s="10" t="s">
-        <v>1578</v>
-      </c>
-      <c r="D352" s="25" t="s">
         <v>1579</v>
       </c>
-      <c r="E352" s="25" t="s">
+      <c r="D352" s="10" t="s">
         <v>1580</v>
       </c>
-      <c r="F352" s="25" t="s">
+      <c r="E352" s="10" t="s">
         <v>1581</v>
       </c>
+      <c r="F352" s="10" t="s">
+        <v>1582</v>
+      </c>
       <c r="G352" s="10" t="s">
-        <v>1582</v>
+        <v>1583</v>
       </c>
       <c r="H352" s="11">
         <f t="shared" si="1"/>
@@ -15470,22 +15515,22 @@
         <v>1340</v>
       </c>
       <c r="B353" s="12">
-        <v>4.0</v>
+        <v>2.0</v>
       </c>
       <c r="C353" s="12" t="s">
-        <v>1583</v>
-      </c>
-      <c r="D353" s="26" t="s">
         <v>1584</v>
       </c>
-      <c r="E353" s="26" t="s">
+      <c r="D353" s="12" t="s">
         <v>1585</v>
       </c>
-      <c r="F353" s="26" t="s">
+      <c r="E353" s="12" t="s">
         <v>1586</v>
       </c>
-      <c r="G353" s="26" t="s">
+      <c r="F353" s="12" t="s">
         <v>1587</v>
+      </c>
+      <c r="G353" s="12" t="s">
+        <v>1588</v>
       </c>
       <c r="H353" s="13">
         <f t="shared" si="1"/>
@@ -15500,19 +15545,19 @@
         <v>2.0</v>
       </c>
       <c r="C354" s="10" t="s">
-        <v>1588</v>
-      </c>
-      <c r="D354" s="25" t="s">
         <v>1589</v>
       </c>
-      <c r="E354" s="25" t="s">
+      <c r="D354" s="26" t="s">
         <v>1590</v>
       </c>
-      <c r="F354" s="25" t="s">
+      <c r="E354" s="26" t="s">
         <v>1591</v>
       </c>
-      <c r="G354" s="25" t="s">
+      <c r="F354" s="26" t="s">
         <v>1592</v>
+      </c>
+      <c r="G354" s="10" t="s">
+        <v>1593</v>
       </c>
       <c r="H354" s="11">
         <f t="shared" si="1"/>
@@ -15524,22 +15569,22 @@
         <v>1340</v>
       </c>
       <c r="B355" s="12">
-        <v>3.0</v>
+        <v>2.0</v>
       </c>
       <c r="C355" s="12" t="s">
-        <v>1593</v>
-      </c>
-      <c r="D355" s="26" t="s">
         <v>1594</v>
       </c>
-      <c r="E355" s="26" t="s">
+      <c r="D355" s="25" t="s">
         <v>1595</v>
       </c>
-      <c r="F355" s="26" t="s">
+      <c r="E355" s="25" t="s">
         <v>1596</v>
       </c>
-      <c r="G355" s="26" t="s">
+      <c r="F355" s="25" t="s">
         <v>1597</v>
+      </c>
+      <c r="G355" s="25" t="s">
+        <v>1598</v>
       </c>
       <c r="H355" s="13">
         <f t="shared" si="1"/>
@@ -15551,22 +15596,22 @@
         <v>1340</v>
       </c>
       <c r="B356" s="10">
-        <v>1.0</v>
+        <v>2.0</v>
       </c>
       <c r="C356" s="10" t="s">
-        <v>1598</v>
-      </c>
-      <c r="D356" s="25" t="s">
         <v>1599</v>
       </c>
-      <c r="E356" s="25" t="s">
+      <c r="D356" s="26" t="s">
+        <v>1575</v>
+      </c>
+      <c r="E356" s="26" t="s">
         <v>1600</v>
       </c>
-      <c r="F356" s="25" t="s">
+      <c r="F356" s="26" t="s">
         <v>1601</v>
       </c>
-      <c r="G356" s="25" t="s">
-        <v>1602</v>
+      <c r="G356" s="26" t="s">
+        <v>1504</v>
       </c>
       <c r="H356" s="11">
         <f t="shared" si="1"/>
@@ -15581,19 +15626,19 @@
         <v>2.0</v>
       </c>
       <c r="C357" s="12" t="s">
+        <v>1602</v>
+      </c>
+      <c r="D357" s="25" t="s">
         <v>1603</v>
       </c>
-      <c r="D357" s="26" t="s">
-        <v>1564</v>
-      </c>
-      <c r="E357" s="26" t="s">
+      <c r="E357" s="25" t="s">
         <v>1604</v>
       </c>
-      <c r="F357" s="26" t="s">
+      <c r="F357" s="25" t="s">
         <v>1605</v>
       </c>
-      <c r="G357" s="26" t="s">
-        <v>1479</v>
+      <c r="G357" s="25" t="s">
+        <v>1606</v>
       </c>
       <c r="H357" s="13">
         <f t="shared" si="1"/>
@@ -15605,22 +15650,22 @@
         <v>1340</v>
       </c>
       <c r="B358" s="10">
-        <v>3.0</v>
+        <v>2.0</v>
       </c>
       <c r="C358" s="10" t="s">
-        <v>1606</v>
-      </c>
-      <c r="D358" s="25" t="s">
         <v>1607</v>
       </c>
-      <c r="E358" s="25" t="s">
+      <c r="D358" s="26" t="s">
         <v>1608</v>
       </c>
-      <c r="F358" s="25" t="s">
+      <c r="E358" s="26" t="s">
         <v>1609</v>
       </c>
-      <c r="G358" s="25" t="s">
+      <c r="F358" s="26" t="s">
         <v>1610</v>
+      </c>
+      <c r="G358" s="26" t="s">
+        <v>1611</v>
       </c>
       <c r="H358" s="11">
         <f t="shared" si="1"/>
@@ -15632,22 +15677,22 @@
         <v>1340</v>
       </c>
       <c r="B359" s="12">
-        <v>1.0</v>
+        <v>2.0</v>
       </c>
       <c r="C359" s="12" t="s">
-        <v>1611</v>
-      </c>
-      <c r="D359" s="26" t="s">
         <v>1612</v>
       </c>
-      <c r="E359" s="26" t="s">
+      <c r="D359" s="25" t="s">
         <v>1613</v>
       </c>
-      <c r="F359" s="26" t="s">
+      <c r="E359" s="25" t="s">
         <v>1614</v>
       </c>
-      <c r="G359" s="26" t="s">
+      <c r="F359" s="25" t="s">
         <v>1615</v>
+      </c>
+      <c r="G359" s="25" t="s">
+        <v>1616</v>
       </c>
       <c r="H359" s="13">
         <f t="shared" si="1"/>
@@ -15662,19 +15707,19 @@
         <v>2.0</v>
       </c>
       <c r="C360" s="10" t="s">
-        <v>1616</v>
-      </c>
-      <c r="D360" s="25" t="s">
         <v>1617</v>
       </c>
-      <c r="E360" s="25" t="s">
+      <c r="D360" s="26" t="s">
         <v>1618</v>
       </c>
-      <c r="F360" s="25" t="s">
+      <c r="E360" s="26" t="s">
         <v>1619</v>
       </c>
-      <c r="G360" s="25" t="s">
+      <c r="F360" s="26" t="s">
         <v>1620</v>
+      </c>
+      <c r="G360" s="26" t="s">
+        <v>1621</v>
       </c>
       <c r="H360" s="11">
         <f t="shared" si="1"/>
@@ -15686,22 +15731,22 @@
         <v>1340</v>
       </c>
       <c r="B361" s="12">
-        <v>1.0</v>
+        <v>3.0</v>
       </c>
       <c r="C361" s="12" t="s">
-        <v>1621</v>
-      </c>
-      <c r="D361" s="26" t="s">
         <v>1622</v>
       </c>
-      <c r="E361" s="26" t="s">
+      <c r="D361" s="12" t="s">
         <v>1623</v>
       </c>
-      <c r="F361" s="26" t="s">
+      <c r="E361" s="12" t="s">
         <v>1624</v>
       </c>
-      <c r="G361" s="26" t="s">
+      <c r="F361" s="12" t="s">
         <v>1625</v>
+      </c>
+      <c r="G361" s="12" t="s">
+        <v>1626</v>
       </c>
       <c r="H361" s="13">
         <f t="shared" si="1"/>
@@ -15716,19 +15761,19 @@
         <v>3.0</v>
       </c>
       <c r="C362" s="10" t="s">
-        <v>1626</v>
-      </c>
-      <c r="D362" s="25" t="s">
         <v>1627</v>
       </c>
-      <c r="E362" s="25" t="s">
+      <c r="D362" s="10" t="s">
         <v>1628</v>
       </c>
-      <c r="F362" s="25" t="s">
+      <c r="E362" s="10" t="s">
         <v>1629</v>
       </c>
-      <c r="G362" s="25" t="s">
+      <c r="F362" s="10" t="s">
         <v>1630</v>
+      </c>
+      <c r="G362" s="10" t="s">
+        <v>1631</v>
       </c>
       <c r="H362" s="11">
         <f t="shared" si="1"/>
@@ -15740,22 +15785,22 @@
         <v>1340</v>
       </c>
       <c r="B363" s="12">
-        <v>4.0</v>
+        <v>3.0</v>
       </c>
       <c r="C363" s="12" t="s">
-        <v>1631</v>
-      </c>
-      <c r="D363" s="26" t="s">
         <v>1632</v>
       </c>
-      <c r="E363" s="26" t="s">
+      <c r="D363" s="25" t="s">
         <v>1633</v>
       </c>
-      <c r="F363" s="26" t="s">
+      <c r="E363" s="25" t="s">
         <v>1634</v>
       </c>
-      <c r="G363" s="26" t="s">
+      <c r="F363" s="25" t="s">
         <v>1635</v>
+      </c>
+      <c r="G363" s="25" t="s">
+        <v>1636</v>
       </c>
       <c r="H363" s="13">
         <f t="shared" si="1"/>
@@ -15770,19 +15815,19 @@
         <v>3.0</v>
       </c>
       <c r="C364" s="10" t="s">
-        <v>1636</v>
-      </c>
-      <c r="D364" s="25" t="s">
         <v>1637</v>
       </c>
-      <c r="E364" s="25" t="s">
+      <c r="D364" s="26" t="s">
         <v>1638</v>
       </c>
-      <c r="F364" s="25" t="s">
+      <c r="E364" s="26" t="s">
         <v>1639</v>
       </c>
-      <c r="G364" s="25" t="s">
+      <c r="F364" s="26" t="s">
         <v>1640</v>
+      </c>
+      <c r="G364" s="26" t="s">
+        <v>1641</v>
       </c>
       <c r="H364" s="11">
         <f t="shared" si="1"/>
@@ -15794,22 +15839,22 @@
         <v>1340</v>
       </c>
       <c r="B365" s="12">
-        <v>1.0</v>
+        <v>3.0</v>
       </c>
       <c r="C365" s="12" t="s">
-        <v>1641</v>
-      </c>
-      <c r="D365" s="26" t="s">
         <v>1642</v>
       </c>
-      <c r="E365" s="26" t="s">
+      <c r="D365" s="25" t="s">
         <v>1643</v>
       </c>
-      <c r="F365" s="26" t="s">
+      <c r="E365" s="25" t="s">
         <v>1644</v>
       </c>
-      <c r="G365" s="26" t="s">
+      <c r="F365" s="25" t="s">
         <v>1645</v>
+      </c>
+      <c r="G365" s="25" t="s">
+        <v>1646</v>
       </c>
       <c r="H365" s="13">
         <f t="shared" si="1"/>
@@ -15824,19 +15869,19 @@
         <v>3.0</v>
       </c>
       <c r="C366" s="10" t="s">
-        <v>1646</v>
-      </c>
-      <c r="D366" s="25" t="s">
         <v>1647</v>
       </c>
-      <c r="E366" s="25" t="s">
+      <c r="D366" s="26" t="s">
         <v>1648</v>
       </c>
-      <c r="F366" s="25" t="s">
+      <c r="E366" s="26" t="s">
         <v>1649</v>
       </c>
-      <c r="G366" s="25" t="s">
+      <c r="F366" s="26" t="s">
         <v>1650</v>
+      </c>
+      <c r="G366" s="26" t="s">
+        <v>1651</v>
       </c>
       <c r="H366" s="11">
         <f t="shared" si="1"/>
@@ -15848,22 +15893,22 @@
         <v>1340</v>
       </c>
       <c r="B367" s="12">
-        <v>2.0</v>
+        <v>3.0</v>
       </c>
       <c r="C367" s="12" t="s">
-        <v>1651</v>
-      </c>
-      <c r="D367" s="26" t="s">
         <v>1652</v>
       </c>
-      <c r="E367" s="26" t="s">
+      <c r="D367" s="25" t="s">
         <v>1653</v>
       </c>
-      <c r="F367" s="26" t="s">
+      <c r="E367" s="25" t="s">
         <v>1654</v>
       </c>
-      <c r="G367" s="26" t="s">
+      <c r="F367" s="25" t="s">
         <v>1655</v>
+      </c>
+      <c r="G367" s="25" t="s">
+        <v>1656</v>
       </c>
       <c r="H367" s="13">
         <f t="shared" si="1"/>
@@ -15875,22 +15920,22 @@
         <v>1340</v>
       </c>
       <c r="B368" s="10">
-        <v>4.0</v>
+        <v>3.0</v>
       </c>
       <c r="C368" s="10" t="s">
-        <v>1656</v>
-      </c>
-      <c r="D368" s="25" t="s">
         <v>1657</v>
       </c>
-      <c r="E368" s="25" t="s">
+      <c r="D368" s="26" t="s">
         <v>1658</v>
       </c>
-      <c r="F368" s="25" t="s">
+      <c r="E368" s="26" t="s">
         <v>1659</v>
       </c>
-      <c r="G368" s="25" t="s">
+      <c r="F368" s="26" t="s">
         <v>1660</v>
+      </c>
+      <c r="G368" s="26" t="s">
+        <v>1654</v>
       </c>
       <c r="H368" s="11">
         <f t="shared" si="1"/>
@@ -15902,21 +15947,21 @@
         <v>1340</v>
       </c>
       <c r="B369" s="12">
-        <v>1.0</v>
+        <v>3.0</v>
       </c>
       <c r="C369" s="12" t="s">
         <v>1661</v>
       </c>
-      <c r="D369" s="26" t="s">
+      <c r="D369" s="25" t="s">
         <v>1662</v>
       </c>
-      <c r="E369" s="26" t="s">
+      <c r="E369" s="25" t="s">
         <v>1663</v>
       </c>
-      <c r="F369" s="26" t="s">
+      <c r="F369" s="25" t="s">
         <v>1664</v>
       </c>
-      <c r="G369" s="26" t="s">
+      <c r="G369" s="25" t="s">
         <v>1665</v>
       </c>
       <c r="H369" s="13">
@@ -15929,21 +15974,21 @@
         <v>1340</v>
       </c>
       <c r="B370" s="10">
-        <v>2.0</v>
+        <v>3.0</v>
       </c>
       <c r="C370" s="10" t="s">
         <v>1666</v>
       </c>
-      <c r="D370" s="25" t="s">
+      <c r="D370" s="26" t="s">
         <v>1667</v>
       </c>
-      <c r="E370" s="25" t="s">
+      <c r="E370" s="26" t="s">
         <v>1668</v>
       </c>
-      <c r="F370" s="25" t="s">
+      <c r="F370" s="26" t="s">
         <v>1669</v>
       </c>
-      <c r="G370" s="25" t="s">
+      <c r="G370" s="26" t="s">
         <v>1670</v>
       </c>
       <c r="H370" s="11">
@@ -15961,17 +16006,17 @@
       <c r="C371" s="12" t="s">
         <v>1671</v>
       </c>
-      <c r="D371" s="26" t="s">
+      <c r="D371" s="25" t="s">
         <v>1672</v>
       </c>
-      <c r="E371" s="26" t="s">
+      <c r="E371" s="25" t="s">
         <v>1673</v>
       </c>
-      <c r="F371" s="26" t="s">
+      <c r="F371" s="25" t="s">
         <v>1674</v>
       </c>
-      <c r="G371" s="26" t="s">
-        <v>1648</v>
+      <c r="G371" s="25" t="s">
+        <v>1675</v>
       </c>
       <c r="H371" s="13">
         <f t="shared" si="1"/>
@@ -15983,22 +16028,22 @@
         <v>1340</v>
       </c>
       <c r="B372" s="10">
-        <v>2.0</v>
+        <v>3.0</v>
       </c>
       <c r="C372" s="10" t="s">
-        <v>1675</v>
-      </c>
-      <c r="D372" s="25" t="s">
         <v>1676</v>
       </c>
-      <c r="E372" s="25" t="s">
+      <c r="D372" s="26" t="s">
         <v>1677</v>
       </c>
-      <c r="F372" s="25" t="s">
+      <c r="E372" s="26" t="s">
         <v>1678</v>
       </c>
-      <c r="G372" s="25" t="s">
+      <c r="F372" s="26" t="s">
         <v>1679</v>
+      </c>
+      <c r="G372" s="26" t="s">
+        <v>1680</v>
       </c>
       <c r="H372" s="11">
         <f t="shared" si="1"/>
@@ -16013,19 +16058,19 @@
         <v>3.0</v>
       </c>
       <c r="C373" s="12" t="s">
-        <v>1680</v>
-      </c>
-      <c r="D373" s="26" t="s">
         <v>1681</v>
       </c>
-      <c r="E373" s="26" t="s">
+      <c r="D373" s="25" t="s">
         <v>1682</v>
       </c>
-      <c r="F373" s="26" t="s">
+      <c r="E373" s="25" t="s">
         <v>1683</v>
       </c>
-      <c r="G373" s="26" t="s">
+      <c r="F373" s="25" t="s">
         <v>1684</v>
+      </c>
+      <c r="G373" s="25" t="s">
+        <v>1415</v>
       </c>
       <c r="H373" s="13">
         <f t="shared" si="1"/>
@@ -16042,16 +16087,16 @@
       <c r="C374" s="10" t="s">
         <v>1685</v>
       </c>
-      <c r="D374" s="25" t="s">
+      <c r="D374" s="26" t="s">
         <v>1686</v>
       </c>
-      <c r="E374" s="25" t="s">
+      <c r="E374" s="26" t="s">
         <v>1687</v>
       </c>
-      <c r="F374" s="25" t="s">
+      <c r="F374" s="26" t="s">
         <v>1688</v>
       </c>
-      <c r="G374" s="25" t="s">
+      <c r="G374" s="26" t="s">
         <v>1689</v>
       </c>
       <c r="H374" s="11">
@@ -16069,16 +16114,16 @@
       <c r="C375" s="12" t="s">
         <v>1690</v>
       </c>
-      <c r="D375" s="26" t="s">
+      <c r="D375" s="25" t="s">
         <v>1691</v>
       </c>
-      <c r="E375" s="26" t="s">
+      <c r="E375" s="25" t="s">
         <v>1692</v>
       </c>
-      <c r="F375" s="26" t="s">
+      <c r="F375" s="25" t="s">
         <v>1693</v>
       </c>
-      <c r="G375" s="26" t="s">
+      <c r="G375" s="25" t="s">
         <v>1694</v>
       </c>
       <c r="H375" s="13">
@@ -16087,7 +16132,7 @@
       </c>
     </row>
     <row r="376">
-      <c r="A376" s="4" t="s">
+      <c r="A376" s="20" t="s">
         <v>1340</v>
       </c>
       <c r="B376" s="10">
@@ -16096,16 +16141,16 @@
       <c r="C376" s="10" t="s">
         <v>1695</v>
       </c>
-      <c r="D376" s="25" t="s">
+      <c r="D376" s="10" t="s">
         <v>1696</v>
       </c>
-      <c r="E376" s="25" t="s">
+      <c r="E376" s="10" t="s">
         <v>1697</v>
       </c>
-      <c r="F376" s="25" t="s">
+      <c r="F376" s="10" t="s">
         <v>1698</v>
       </c>
-      <c r="G376" s="25" t="s">
+      <c r="G376" s="10" t="s">
         <v>1699</v>
       </c>
       <c r="H376" s="11">
@@ -16114,7 +16159,7 @@
       </c>
     </row>
     <row r="377">
-      <c r="A377" s="7" t="s">
+      <c r="A377" s="23" t="s">
         <v>1340</v>
       </c>
       <c r="B377" s="12">
@@ -16123,17 +16168,17 @@
       <c r="C377" s="12" t="s">
         <v>1700</v>
       </c>
-      <c r="D377" s="26" t="s">
+      <c r="D377" s="12" t="s">
+        <v>1648</v>
+      </c>
+      <c r="E377" s="12" t="s">
+        <v>1649</v>
+      </c>
+      <c r="F377" s="12" t="s">
         <v>1701</v>
       </c>
-      <c r="E377" s="26" t="s">
-        <v>1702</v>
-      </c>
-      <c r="F377" s="26" t="s">
-        <v>1703</v>
-      </c>
-      <c r="G377" s="26" t="s">
-        <v>1415</v>
+      <c r="G377" s="12" t="s">
+        <v>1650</v>
       </c>
       <c r="H377" s="13">
         <f t="shared" si="1"/>
@@ -16141,53 +16186,53 @@
       </c>
     </row>
     <row r="378">
-      <c r="A378" s="4" t="s">
+      <c r="A378" s="20" t="s">
         <v>1340</v>
       </c>
       <c r="B378" s="10">
         <v>3.0</v>
       </c>
       <c r="C378" s="10" t="s">
+        <v>1702</v>
+      </c>
+      <c r="D378" s="10" t="s">
+        <v>1703</v>
+      </c>
+      <c r="E378" s="10" t="s">
         <v>1704</v>
       </c>
-      <c r="D378" s="25" t="s">
+      <c r="F378" s="10" t="s">
         <v>1705</v>
       </c>
-      <c r="E378" s="25" t="s">
+      <c r="G378" s="10" t="s">
         <v>1706</v>
       </c>
-      <c r="F378" s="25" t="s">
-        <v>1707</v>
-      </c>
-      <c r="G378" s="25" t="s">
-        <v>1708</v>
-      </c>
       <c r="H378" s="11">
         <f t="shared" si="1"/>
         <v>378</v>
       </c>
     </row>
     <row r="379">
-      <c r="A379" s="7" t="s">
+      <c r="A379" s="23" t="s">
         <v>1340</v>
       </c>
       <c r="B379" s="12">
         <v>3.0</v>
       </c>
       <c r="C379" s="12" t="s">
+        <v>1707</v>
+      </c>
+      <c r="D379" s="12" t="s">
+        <v>1704</v>
+      </c>
+      <c r="E379" s="12" t="s">
+        <v>1703</v>
+      </c>
+      <c r="F379" s="12" t="s">
+        <v>1708</v>
+      </c>
+      <c r="G379" s="12" t="s">
         <v>1709</v>
-      </c>
-      <c r="D379" s="26" t="s">
-        <v>1710</v>
-      </c>
-      <c r="E379" s="26" t="s">
-        <v>1711</v>
-      </c>
-      <c r="F379" s="26" t="s">
-        <v>1712</v>
-      </c>
-      <c r="G379" s="26" t="s">
-        <v>1713</v>
       </c>
       <c r="H379" s="13">
         <f t="shared" si="1"/>
@@ -16198,25 +16243,25 @@
       <c r="A380" s="4" t="s">
         <v>1340</v>
       </c>
-      <c r="B380" s="10">
+      <c r="B380" s="5">
         <v>4.0</v>
       </c>
-      <c r="C380" s="10" t="s">
-        <v>1714</v>
-      </c>
-      <c r="D380" s="25" t="s">
-        <v>1715</v>
-      </c>
-      <c r="E380" s="25" t="s">
-        <v>1716</v>
-      </c>
-      <c r="F380" s="25" t="s">
-        <v>1717</v>
-      </c>
-      <c r="G380" s="25" t="s">
-        <v>1718</v>
-      </c>
-      <c r="H380" s="11">
+      <c r="C380" s="5" t="s">
+        <v>1710</v>
+      </c>
+      <c r="D380" s="5" t="s">
+        <v>1711</v>
+      </c>
+      <c r="E380" s="5" t="s">
+        <v>1712</v>
+      </c>
+      <c r="F380" s="5" t="s">
+        <v>1713</v>
+      </c>
+      <c r="G380" s="5" t="s">
+        <v>828</v>
+      </c>
+      <c r="H380" s="6">
         <f t="shared" si="1"/>
         <v>380</v>
       </c>
@@ -16229,19 +16274,19 @@
         <v>4.0</v>
       </c>
       <c r="C381" s="12" t="s">
-        <v>1719</v>
-      </c>
-      <c r="D381" s="8" t="s">
-        <v>1720</v>
-      </c>
-      <c r="E381" s="26" t="s">
-        <v>1721</v>
-      </c>
-      <c r="F381" s="26" t="s">
-        <v>1722</v>
-      </c>
-      <c r="G381" s="26" t="s">
-        <v>1723</v>
+        <v>1714</v>
+      </c>
+      <c r="D381" s="25" t="s">
+        <v>1715</v>
+      </c>
+      <c r="E381" s="25" t="s">
+        <v>1716</v>
+      </c>
+      <c r="F381" s="25" t="s">
+        <v>1717</v>
+      </c>
+      <c r="G381" s="25" t="s">
+        <v>1718</v>
       </c>
       <c r="H381" s="13">
         <f t="shared" si="1"/>
@@ -16256,19 +16301,19 @@
         <v>4.0</v>
       </c>
       <c r="C382" s="10" t="s">
-        <v>1724</v>
-      </c>
-      <c r="D382" s="25" t="s">
-        <v>1725</v>
-      </c>
-      <c r="E382" s="25" t="s">
-        <v>1726</v>
-      </c>
-      <c r="F382" s="25" t="s">
-        <v>1727</v>
-      </c>
-      <c r="G382" s="25" t="s">
-        <v>1728</v>
+        <v>1719</v>
+      </c>
+      <c r="D382" s="26" t="s">
+        <v>1720</v>
+      </c>
+      <c r="E382" s="26" t="s">
+        <v>1721</v>
+      </c>
+      <c r="F382" s="26" t="s">
+        <v>1722</v>
+      </c>
+      <c r="G382" s="26" t="s">
+        <v>1723</v>
       </c>
       <c r="H382" s="11">
         <f t="shared" si="1"/>
@@ -16283,19 +16328,19 @@
         <v>4.0</v>
       </c>
       <c r="C383" s="12" t="s">
-        <v>1729</v>
-      </c>
-      <c r="D383" s="26" t="s">
-        <v>1730</v>
-      </c>
-      <c r="E383" s="26" t="s">
-        <v>1731</v>
-      </c>
-      <c r="F383" s="26" t="s">
+        <v>1724</v>
+      </c>
+      <c r="D383" s="25" t="s">
+        <v>1725</v>
+      </c>
+      <c r="E383" s="25" t="s">
         <v>1726</v>
       </c>
-      <c r="G383" s="26" t="s">
-        <v>1732</v>
+      <c r="F383" s="25" t="s">
+        <v>1727</v>
+      </c>
+      <c r="G383" s="25" t="s">
+        <v>1728</v>
       </c>
       <c r="H383" s="13">
         <f t="shared" si="1"/>
@@ -16310,19 +16355,19 @@
         <v>4.0</v>
       </c>
       <c r="C384" s="10" t="s">
+        <v>1729</v>
+      </c>
+      <c r="D384" s="26" t="s">
+        <v>1730</v>
+      </c>
+      <c r="E384" s="26" t="s">
+        <v>1731</v>
+      </c>
+      <c r="F384" s="26" t="s">
+        <v>1732</v>
+      </c>
+      <c r="G384" s="26" t="s">
         <v>1733</v>
-      </c>
-      <c r="D384" s="25" t="s">
-        <v>1734</v>
-      </c>
-      <c r="E384" s="25" t="s">
-        <v>1735</v>
-      </c>
-      <c r="F384" s="25" t="s">
-        <v>1736</v>
-      </c>
-      <c r="G384" s="25" t="s">
-        <v>1737</v>
       </c>
       <c r="H384" s="11">
         <f t="shared" si="1"/>
@@ -16337,19 +16382,19 @@
         <v>4.0</v>
       </c>
       <c r="C385" s="12" t="s">
+        <v>1734</v>
+      </c>
+      <c r="D385" s="8" t="s">
+        <v>1735</v>
+      </c>
+      <c r="E385" s="25" t="s">
+        <v>1736</v>
+      </c>
+      <c r="F385" s="25" t="s">
+        <v>1737</v>
+      </c>
+      <c r="G385" s="25" t="s">
         <v>1738</v>
-      </c>
-      <c r="D385" s="26" t="s">
-        <v>1739</v>
-      </c>
-      <c r="E385" s="26" t="s">
-        <v>1740</v>
-      </c>
-      <c r="F385" s="26" t="s">
-        <v>1741</v>
-      </c>
-      <c r="G385" s="26" t="s">
-        <v>64</v>
       </c>
       <c r="H385" s="13">
         <f t="shared" si="1"/>
@@ -16364,19 +16409,19 @@
         <v>4.0</v>
       </c>
       <c r="C386" s="10" t="s">
+        <v>1739</v>
+      </c>
+      <c r="D386" s="26" t="s">
+        <v>1740</v>
+      </c>
+      <c r="E386" s="26" t="s">
+        <v>1741</v>
+      </c>
+      <c r="F386" s="26" t="s">
         <v>1742</v>
       </c>
-      <c r="D386" s="25" t="s">
+      <c r="G386" s="26" t="s">
         <v>1743</v>
-      </c>
-      <c r="E386" s="25" t="s">
-        <v>1744</v>
-      </c>
-      <c r="F386" s="25" t="s">
-        <v>1745</v>
-      </c>
-      <c r="G386" s="25" t="s">
-        <v>1746</v>
       </c>
       <c r="H386" s="11">
         <f t="shared" si="1"/>
@@ -16391,19 +16436,19 @@
         <v>4.0</v>
       </c>
       <c r="C387" s="12" t="s">
+        <v>1744</v>
+      </c>
+      <c r="D387" s="25" t="s">
+        <v>1745</v>
+      </c>
+      <c r="E387" s="25" t="s">
+        <v>1746</v>
+      </c>
+      <c r="F387" s="25" t="s">
+        <v>1741</v>
+      </c>
+      <c r="G387" s="25" t="s">
         <v>1747</v>
-      </c>
-      <c r="D387" s="26" t="s">
-        <v>1748</v>
-      </c>
-      <c r="E387" s="26" t="s">
-        <v>1749</v>
-      </c>
-      <c r="F387" s="26" t="s">
-        <v>1750</v>
-      </c>
-      <c r="G387" s="26" t="s">
-        <v>1751</v>
       </c>
       <c r="H387" s="13">
         <f t="shared" si="1"/>
@@ -16418,19 +16463,19 @@
         <v>4.0</v>
       </c>
       <c r="C388" s="10" t="s">
+        <v>1748</v>
+      </c>
+      <c r="D388" s="26" t="s">
+        <v>1749</v>
+      </c>
+      <c r="E388" s="26" t="s">
+        <v>1750</v>
+      </c>
+      <c r="F388" s="26" t="s">
+        <v>1751</v>
+      </c>
+      <c r="G388" s="26" t="s">
         <v>1752</v>
-      </c>
-      <c r="D388" s="25" t="s">
-        <v>1753</v>
-      </c>
-      <c r="E388" s="25" t="s">
-        <v>1754</v>
-      </c>
-      <c r="F388" s="25" t="s">
-        <v>1755</v>
-      </c>
-      <c r="G388" s="25" t="s">
-        <v>1756</v>
       </c>
       <c r="H388" s="11">
         <f t="shared" si="1"/>
@@ -16445,19 +16490,19 @@
         <v>4.0</v>
       </c>
       <c r="C389" s="12" t="s">
-        <v>1757</v>
-      </c>
-      <c r="D389" s="26" t="s">
-        <v>1758</v>
-      </c>
-      <c r="E389" s="26" t="s">
-        <v>1759</v>
-      </c>
-      <c r="F389" s="26" t="s">
-        <v>1760</v>
-      </c>
-      <c r="G389" s="26" t="s">
-        <v>1761</v>
+        <v>1753</v>
+      </c>
+      <c r="D389" s="25" t="s">
+        <v>1754</v>
+      </c>
+      <c r="E389" s="25" t="s">
+        <v>1755</v>
+      </c>
+      <c r="F389" s="25" t="s">
+        <v>1756</v>
+      </c>
+      <c r="G389" s="25" t="s">
+        <v>64</v>
       </c>
       <c r="H389" s="13">
         <f t="shared" si="1"/>
@@ -16472,19 +16517,19 @@
         <v>4.0</v>
       </c>
       <c r="C390" s="10" t="s">
-        <v>1762</v>
-      </c>
-      <c r="D390" s="25" t="s">
-        <v>1763</v>
-      </c>
-      <c r="E390" s="25" t="s">
-        <v>1764</v>
-      </c>
-      <c r="F390" s="25" t="s">
-        <v>1765</v>
-      </c>
-      <c r="G390" s="25" t="s">
-        <v>1766</v>
+        <v>1757</v>
+      </c>
+      <c r="D390" s="26" t="s">
+        <v>1758</v>
+      </c>
+      <c r="E390" s="26" t="s">
+        <v>1759</v>
+      </c>
+      <c r="F390" s="26" t="s">
+        <v>1760</v>
+      </c>
+      <c r="G390" s="26" t="s">
+        <v>1761</v>
       </c>
       <c r="H390" s="11">
         <f t="shared" si="1"/>
@@ -16499,19 +16544,19 @@
         <v>4.0</v>
       </c>
       <c r="C391" s="12" t="s">
-        <v>1767</v>
-      </c>
-      <c r="D391" s="26" t="s">
-        <v>1768</v>
-      </c>
-      <c r="E391" s="26" t="s">
-        <v>1769</v>
-      </c>
-      <c r="F391" s="26" t="s">
-        <v>1770</v>
-      </c>
-      <c r="G391" s="26" t="s">
-        <v>1771</v>
+        <v>1762</v>
+      </c>
+      <c r="D391" s="25" t="s">
+        <v>1763</v>
+      </c>
+      <c r="E391" s="25" t="s">
+        <v>1764</v>
+      </c>
+      <c r="F391" s="25" t="s">
+        <v>1765</v>
+      </c>
+      <c r="G391" s="25" t="s">
+        <v>1766</v>
       </c>
       <c r="H391" s="13">
         <f t="shared" si="1"/>
@@ -16526,19 +16571,19 @@
         <v>4.0</v>
       </c>
       <c r="C392" s="10" t="s">
-        <v>1772</v>
-      </c>
-      <c r="D392" s="25" t="s">
-        <v>1773</v>
-      </c>
-      <c r="E392" s="25" t="s">
-        <v>1774</v>
-      </c>
-      <c r="F392" s="25" t="s">
-        <v>1775</v>
-      </c>
-      <c r="G392" s="25" t="s">
-        <v>1776</v>
+        <v>1767</v>
+      </c>
+      <c r="D392" s="26" t="s">
+        <v>1768</v>
+      </c>
+      <c r="E392" s="26" t="s">
+        <v>1769</v>
+      </c>
+      <c r="F392" s="26" t="s">
+        <v>1770</v>
+      </c>
+      <c r="G392" s="26" t="s">
+        <v>1771</v>
       </c>
       <c r="H392" s="11">
         <f t="shared" si="1"/>
@@ -16553,19 +16598,19 @@
         <v>4.0</v>
       </c>
       <c r="C393" s="12" t="s">
-        <v>1777</v>
-      </c>
-      <c r="D393" s="26" t="s">
-        <v>1778</v>
-      </c>
-      <c r="E393" s="26" t="s">
-        <v>1779</v>
-      </c>
-      <c r="F393" s="26" t="s">
-        <v>1780</v>
-      </c>
-      <c r="G393" s="26" t="s">
-        <v>1781</v>
+        <v>1772</v>
+      </c>
+      <c r="D393" s="25" t="s">
+        <v>1773</v>
+      </c>
+      <c r="E393" s="25" t="s">
+        <v>1774</v>
+      </c>
+      <c r="F393" s="25" t="s">
+        <v>1775</v>
+      </c>
+      <c r="G393" s="25" t="s">
+        <v>1776</v>
       </c>
       <c r="H393" s="13">
         <f t="shared" si="1"/>
@@ -16580,19 +16625,19 @@
         <v>4.0</v>
       </c>
       <c r="C394" s="10" t="s">
-        <v>1782</v>
-      </c>
-      <c r="D394" s="25" t="s">
-        <v>1783</v>
-      </c>
-      <c r="E394" s="25" t="s">
-        <v>1784</v>
-      </c>
-      <c r="F394" s="25" t="s">
-        <v>1785</v>
-      </c>
-      <c r="G394" s="25" t="s">
-        <v>1786</v>
+        <v>1777</v>
+      </c>
+      <c r="D394" s="26" t="s">
+        <v>1778</v>
+      </c>
+      <c r="E394" s="26" t="s">
+        <v>1779</v>
+      </c>
+      <c r="F394" s="26" t="s">
+        <v>1780</v>
+      </c>
+      <c r="G394" s="26" t="s">
+        <v>1781</v>
       </c>
       <c r="H394" s="11">
         <f t="shared" si="1"/>
@@ -16607,19 +16652,19 @@
         <v>4.0</v>
       </c>
       <c r="C395" s="12" t="s">
-        <v>1787</v>
-      </c>
-      <c r="D395" s="26" t="s">
-        <v>1788</v>
-      </c>
-      <c r="E395" s="26" t="s">
-        <v>1789</v>
-      </c>
-      <c r="F395" s="26" t="s">
-        <v>1790</v>
-      </c>
-      <c r="G395" s="26" t="s">
-        <v>1791</v>
+        <v>1782</v>
+      </c>
+      <c r="D395" s="25" t="s">
+        <v>1783</v>
+      </c>
+      <c r="E395" s="25" t="s">
+        <v>1784</v>
+      </c>
+      <c r="F395" s="25" t="s">
+        <v>1785</v>
+      </c>
+      <c r="G395" s="25" t="s">
+        <v>1786</v>
       </c>
       <c r="H395" s="13">
         <f t="shared" si="1"/>
@@ -16634,19 +16679,19 @@
         <v>4.0</v>
       </c>
       <c r="C396" s="10" t="s">
-        <v>1792</v>
-      </c>
-      <c r="D396" s="25" t="s">
-        <v>1773</v>
-      </c>
-      <c r="E396" s="25" t="s">
-        <v>1793</v>
-      </c>
-      <c r="F396" s="25" t="s">
-        <v>1775</v>
-      </c>
-      <c r="G396" s="25" t="s">
-        <v>1776</v>
+        <v>1787</v>
+      </c>
+      <c r="D396" s="26" t="s">
+        <v>1788</v>
+      </c>
+      <c r="E396" s="26" t="s">
+        <v>1789</v>
+      </c>
+      <c r="F396" s="26" t="s">
+        <v>1790</v>
+      </c>
+      <c r="G396" s="26" t="s">
+        <v>1791</v>
       </c>
       <c r="H396" s="11">
         <f t="shared" si="1"/>
@@ -16661,19 +16706,19 @@
         <v>4.0</v>
       </c>
       <c r="C397" s="12" t="s">
+        <v>1792</v>
+      </c>
+      <c r="D397" s="25" t="s">
+        <v>1793</v>
+      </c>
+      <c r="E397" s="25" t="s">
         <v>1794</v>
       </c>
-      <c r="D397" s="26" t="s">
+      <c r="F397" s="25" t="s">
         <v>1795</v>
       </c>
-      <c r="E397" s="26" t="s">
+      <c r="G397" s="25" t="s">
         <v>1796</v>
-      </c>
-      <c r="F397" s="26" t="s">
-        <v>1797</v>
-      </c>
-      <c r="G397" s="26" t="s">
-        <v>1798</v>
       </c>
       <c r="H397" s="13">
         <f t="shared" si="1"/>
@@ -16688,19 +16733,19 @@
         <v>4.0</v>
       </c>
       <c r="C398" s="10" t="s">
+        <v>1797</v>
+      </c>
+      <c r="D398" s="26" t="s">
+        <v>1798</v>
+      </c>
+      <c r="E398" s="26" t="s">
         <v>1799</v>
       </c>
-      <c r="D398" s="25" t="s">
+      <c r="F398" s="26" t="s">
         <v>1800</v>
       </c>
-      <c r="E398" s="25" t="s">
+      <c r="G398" s="26" t="s">
         <v>1801</v>
-      </c>
-      <c r="F398" s="25" t="s">
-        <v>1802</v>
-      </c>
-      <c r="G398" s="25" t="s">
-        <v>1803</v>
       </c>
       <c r="H398" s="11">
         <f t="shared" si="1"/>
@@ -16715,19 +16760,19 @@
         <v>4.0</v>
       </c>
       <c r="C399" s="12" t="s">
+        <v>1802</v>
+      </c>
+      <c r="D399" s="25" t="s">
+        <v>1803</v>
+      </c>
+      <c r="E399" s="25" t="s">
         <v>1804</v>
       </c>
-      <c r="D399" s="8" t="s">
+      <c r="F399" s="25" t="s">
         <v>1805</v>
       </c>
-      <c r="E399" s="26" t="s">
+      <c r="G399" s="25" t="s">
         <v>1806</v>
-      </c>
-      <c r="F399" s="26" t="s">
-        <v>1807</v>
-      </c>
-      <c r="G399" s="26" t="s">
-        <v>1808</v>
       </c>
       <c r="H399" s="13">
         <f t="shared" si="1"/>
@@ -16742,19 +16787,19 @@
         <v>4.0</v>
       </c>
       <c r="C400" s="10" t="s">
-        <v>1809</v>
-      </c>
-      <c r="D400" s="10" t="s">
-        <v>1810</v>
-      </c>
-      <c r="E400" s="10" t="s">
-        <v>1811</v>
-      </c>
-      <c r="F400" s="25" t="s">
-        <v>1812</v>
-      </c>
-      <c r="G400" s="25" t="s">
-        <v>1813</v>
+        <v>1807</v>
+      </c>
+      <c r="D400" s="26" t="s">
+        <v>1788</v>
+      </c>
+      <c r="E400" s="26" t="s">
+        <v>1808</v>
+      </c>
+      <c r="F400" s="26" t="s">
+        <v>1790</v>
+      </c>
+      <c r="G400" s="26" t="s">
+        <v>1791</v>
       </c>
       <c r="H400" s="11">
         <f t="shared" si="1"/>
@@ -16769,19 +16814,19 @@
         <v>4.0</v>
       </c>
       <c r="C401" s="12" t="s">
-        <v>1814</v>
-      </c>
-      <c r="D401" s="12" t="s">
-        <v>1815</v>
-      </c>
-      <c r="E401" s="12" t="s">
-        <v>1816</v>
-      </c>
-      <c r="F401" s="12" t="s">
-        <v>1817</v>
-      </c>
-      <c r="G401" s="12" t="s">
-        <v>1818</v>
+        <v>1809</v>
+      </c>
+      <c r="D401" s="25" t="s">
+        <v>1810</v>
+      </c>
+      <c r="E401" s="25" t="s">
+        <v>1811</v>
+      </c>
+      <c r="F401" s="25" t="s">
+        <v>1812</v>
+      </c>
+      <c r="G401" s="25" t="s">
+        <v>1813</v>
       </c>
       <c r="H401" s="13">
         <f t="shared" si="1"/>
@@ -16796,50 +16841,158 @@
         <v>4.0</v>
       </c>
       <c r="C402" s="10" t="s">
+        <v>1814</v>
+      </c>
+      <c r="D402" s="26" t="s">
+        <v>1815</v>
+      </c>
+      <c r="E402" s="26" t="s">
+        <v>1816</v>
+      </c>
+      <c r="F402" s="26" t="s">
+        <v>1817</v>
+      </c>
+      <c r="G402" s="26" t="s">
+        <v>1818</v>
+      </c>
+      <c r="H402" s="11">
+        <f t="shared" si="1"/>
+        <v>402</v>
+      </c>
+    </row>
+    <row r="403">
+      <c r="A403" s="7" t="s">
+        <v>1340</v>
+      </c>
+      <c r="B403" s="12">
+        <v>4.0</v>
+      </c>
+      <c r="C403" s="12" t="s">
         <v>1819</v>
       </c>
-      <c r="D402" s="10">
+      <c r="D403" s="8" t="s">
+        <v>1820</v>
+      </c>
+      <c r="E403" s="25" t="s">
+        <v>1821</v>
+      </c>
+      <c r="F403" s="25" t="s">
+        <v>1822</v>
+      </c>
+      <c r="G403" s="25" t="s">
+        <v>1823</v>
+      </c>
+      <c r="H403" s="13">
+        <f t="shared" si="1"/>
+        <v>403</v>
+      </c>
+    </row>
+    <row r="404">
+      <c r="A404" s="4" t="s">
+        <v>1340</v>
+      </c>
+      <c r="B404" s="10">
+        <v>4.0</v>
+      </c>
+      <c r="C404" s="10" t="s">
+        <v>1824</v>
+      </c>
+      <c r="D404" s="10" t="s">
+        <v>1825</v>
+      </c>
+      <c r="E404" s="10" t="s">
+        <v>1826</v>
+      </c>
+      <c r="F404" s="26" t="s">
+        <v>1827</v>
+      </c>
+      <c r="G404" s="26" t="s">
+        <v>1828</v>
+      </c>
+      <c r="H404" s="11">
+        <f t="shared" si="1"/>
+        <v>404</v>
+      </c>
+    </row>
+    <row r="405">
+      <c r="A405" s="7" t="s">
+        <v>1340</v>
+      </c>
+      <c r="B405" s="12">
+        <v>4.0</v>
+      </c>
+      <c r="C405" s="12" t="s">
+        <v>1829</v>
+      </c>
+      <c r="D405" s="12" t="s">
+        <v>1830</v>
+      </c>
+      <c r="E405" s="12" t="s">
+        <v>1831</v>
+      </c>
+      <c r="F405" s="12" t="s">
+        <v>1832</v>
+      </c>
+      <c r="G405" s="12" t="s">
+        <v>1833</v>
+      </c>
+      <c r="H405" s="13">
+        <f t="shared" si="1"/>
+        <v>405</v>
+      </c>
+    </row>
+    <row r="406">
+      <c r="A406" s="4" t="s">
+        <v>1340</v>
+      </c>
+      <c r="B406" s="10">
+        <v>4.0</v>
+      </c>
+      <c r="C406" s="10" t="s">
+        <v>1834</v>
+      </c>
+      <c r="D406" s="10">
         <v>30.06</v>
       </c>
-      <c r="E402" s="10">
+      <c r="E406" s="10">
         <v>29.86</v>
       </c>
-      <c r="F402" s="10">
+      <c r="F406" s="10">
         <v>29.61</v>
       </c>
-      <c r="G402" s="10">
+      <c r="G406" s="10">
         <v>30.86</v>
       </c>
-      <c r="H402" s="11">
-        <f t="shared" si="1"/>
-        <v>402</v>
-      </c>
-    </row>
-    <row r="403">
-      <c r="A403" s="27" t="s">
+      <c r="H406" s="11">
+        <f t="shared" si="1"/>
+        <v>406</v>
+      </c>
+    </row>
+    <row r="407">
+      <c r="A407" s="27" t="s">
         <v>1340</v>
       </c>
-      <c r="B403" s="28">
+      <c r="B407" s="28">
         <v>4.0</v>
       </c>
-      <c r="C403" s="28" t="s">
-        <v>1820</v>
-      </c>
-      <c r="D403" s="28" t="s">
-        <v>1821</v>
-      </c>
-      <c r="E403" s="28" t="s">
-        <v>1822</v>
-      </c>
-      <c r="F403" s="28" t="s">
-        <v>1823</v>
-      </c>
-      <c r="G403" s="28" t="s">
-        <v>1824</v>
-      </c>
-      <c r="H403" s="29">
-        <f t="shared" si="1"/>
-        <v>403</v>
+      <c r="C407" s="28" t="s">
+        <v>1835</v>
+      </c>
+      <c r="D407" s="28" t="s">
+        <v>1836</v>
+      </c>
+      <c r="E407" s="28" t="s">
+        <v>1837</v>
+      </c>
+      <c r="F407" s="28" t="s">
+        <v>1838</v>
+      </c>
+      <c r="G407" s="28" t="s">
+        <v>1839</v>
+      </c>
+      <c r="H407" s="29">
+        <f t="shared" si="1"/>
+        <v>407</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Added ground school questions
</commit_message>
<xml_diff>
--- a/public/questions.xlsx
+++ b/public/questions.xlsx
@@ -6,14 +6,14 @@
     <sheet state="visible" name="Sheet1" sheetId="1" r:id="rId4"/>
   </sheets>
   <definedNames>
-    <definedName hidden="1" localSheetId="0" name="_xlnm._FilterDatabase">Sheet1!$A$1:$H$407</definedName>
+    <definedName hidden="1" localSheetId="0" name="_xlnm._FilterDatabase">Sheet1!$A$1:$H$431</definedName>
   </definedNames>
   <calcPr/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2413" uniqueCount="1840">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2553" uniqueCount="1957">
   <si>
     <t>Topic</t>
   </si>
@@ -5534,14 +5534,366 @@
   </si>
   <si>
     <t>6° C</t>
+  </si>
+  <si>
+    <t>What does P.A.T. stand for in the P.A.T. principle?</t>
+  </si>
+  <si>
+    <t>Power, Attitude, Trim</t>
+  </si>
+  <si>
+    <t>Pitch, Attitude, Trim</t>
+  </si>
+  <si>
+    <t>Power, Altitude, Trim</t>
+  </si>
+  <si>
+    <t>Pitch, Altitude, Trim</t>
+  </si>
+  <si>
+    <t>At what speed do you slow to in the level speed change and what is the power setting at that speed?</t>
+  </si>
+  <si>
+    <t>55 kts, ~2100 RPM</t>
+  </si>
+  <si>
+    <t>65 kts, 2000 RPM</t>
+  </si>
+  <si>
+    <t>65 kts, ~2100 RPM</t>
+  </si>
+  <si>
+    <t>55 kts, 2000 RPM</t>
+  </si>
+  <si>
+    <t>What hp does the engine output when operating at 2700 rpm?</t>
+  </si>
+  <si>
+    <t>180 hp</t>
+  </si>
+  <si>
+    <t>160 hp</t>
+  </si>
+  <si>
+    <t>200 hp</t>
+  </si>
+  <si>
+    <t>150 hp</t>
+  </si>
+  <si>
+    <t>When checking the magnetos, the RPM drop should not exceed ______ RPM on either side or show greater than _____ RPM difference between magnetos</t>
+  </si>
+  <si>
+    <t>125, 50</t>
+  </si>
+  <si>
+    <t>100, 50</t>
+  </si>
+  <si>
+    <t>150, 75</t>
+  </si>
+  <si>
+    <t>125, 75</t>
+  </si>
+  <si>
+    <t>When checking the carb heat, how much of an RPM dorp should you see?</t>
+  </si>
+  <si>
+    <t>50-100</t>
+  </si>
+  <si>
+    <t>50-125</t>
+  </si>
+  <si>
+    <t>75-125</t>
+  </si>
+  <si>
+    <t>What is the first indication of carburetor icing?</t>
+  </si>
+  <si>
+    <t>A decrease in RPM, followed by engine roughness</t>
+  </si>
+  <si>
+    <t>Buffeting and loss of control</t>
+  </si>
+  <si>
+    <t>Decrease in airspeed as max engine output decreases</t>
+  </si>
+  <si>
+    <t>Engine bumps and bangs, before the engine eventually dies</t>
+  </si>
+  <si>
+    <t xml:space="preserve">ground </t>
+  </si>
+  <si>
+    <t>What is GLOC?</t>
+  </si>
+  <si>
+    <t>Gravity-induced loss of consciousness</t>
+  </si>
+  <si>
+    <t>The set g level during an autopilot maneuver</t>
+  </si>
+  <si>
+    <t>The maximum gs a pilot can withstand for 30 secs</t>
+  </si>
+  <si>
+    <t>The location on the pilot where g forces are concentrated</t>
+  </si>
+  <si>
+    <t>Each of these is one of the 4 principles of ORM EXCEPT?</t>
+  </si>
+  <si>
+    <t>Make risk decisions at the operational level</t>
+  </si>
+  <si>
+    <t>Accept risk when benefits outweigh the cost</t>
+  </si>
+  <si>
+    <t>Accept no unnecessary risk</t>
+  </si>
+  <si>
+    <t>Anticipate and manage risk by planning</t>
+  </si>
+  <si>
+    <t>Which of these are the classes of Mishaps?</t>
+  </si>
+  <si>
+    <t>A, B, C, D, E</t>
+  </si>
+  <si>
+    <t>Flight, Flight Related, Aviation Ground</t>
+  </si>
+  <si>
+    <t>A, B, C, D</t>
+  </si>
+  <si>
+    <t>Flight, Flight Related, Aviation Ground, Preflight</t>
+  </si>
+  <si>
+    <t>Who do you communicate with at non-towered airports?</t>
+  </si>
+  <si>
+    <t>Common traffic advisory frequency (CTAF)</t>
+  </si>
+  <si>
+    <t>Guard</t>
+  </si>
+  <si>
+    <t>Bolo Common</t>
+  </si>
+  <si>
+    <t>Approach/Departure</t>
+  </si>
+  <si>
+    <t>What are your 3 priorities in order during an emergency?</t>
+  </si>
+  <si>
+    <t>Aviate, Navigate, Communicate</t>
+  </si>
+  <si>
+    <t>Aviate, Communicate, Navigate</t>
+  </si>
+  <si>
+    <t>Airspeed, Heading, Controls</t>
+  </si>
+  <si>
+    <t>Aviate, Navigate, Checklists</t>
+  </si>
+  <si>
+    <t>Which of these are NOT one of the 5 steps of ORM?</t>
+  </si>
+  <si>
+    <t>Assess the situation</t>
+  </si>
+  <si>
+    <t>Make risk decisions</t>
+  </si>
+  <si>
+    <t>Implement controls</t>
+  </si>
+  <si>
+    <t>Supervise</t>
+  </si>
+  <si>
+    <t>What is the best definition of assertiveness in CRM?</t>
+  </si>
+  <si>
+    <t>The willingness or readiness to actively participate, state, and maintain a position until convinced by the facts that other options are better</t>
+  </si>
+  <si>
+    <t>The quality of being confident and not frightened to say what you want or believe</t>
+  </si>
+  <si>
+    <t>Disposed to or characterized by bold or confident statements and behavior</t>
+  </si>
+  <si>
+    <t>The ability to state your beliefs and actions without being swayed by others inputs</t>
+  </si>
+  <si>
+    <t>The critical skills of CRM are:</t>
+  </si>
+  <si>
+    <t>Communication, Adaptability, Mission Analysis, Assertiveness, Situational Awareness, Leadership, Decision Making</t>
+  </si>
+  <si>
+    <t>Decision Making, Critical Thinking, Communication, Adaptability, Delegation, Vision, and Conflict resolution</t>
+  </si>
+  <si>
+    <t>Situational Analysis, Decisiveness, Adaptability, Mission Analysis, Communication, Leadership, Assertiveness</t>
+  </si>
+  <si>
+    <t>Mission Analysis, Assertiveness, Leadership, Communication, Situational Assessment, Adaptability, Decision Making</t>
+  </si>
+  <si>
+    <t>Which of these are NOT required for day VFR flight?</t>
+  </si>
+  <si>
+    <t>Taxi and positional lights</t>
+  </si>
+  <si>
+    <t>Oil Pressure Gauge</t>
+  </si>
+  <si>
+    <t>Tachometer</t>
+  </si>
+  <si>
+    <t>Gas gauge</t>
+  </si>
+  <si>
+    <t>We rotate at ______ and usually climb out at ______</t>
+  </si>
+  <si>
+    <t>55 kts, 73 kts</t>
+  </si>
+  <si>
+    <t>62 kts, 73 kts</t>
+  </si>
+  <si>
+    <t>55 kts, 62 kts</t>
+  </si>
+  <si>
+    <t>65 kts, 73 kts</t>
+  </si>
+  <si>
+    <t>During a power on stall we pitch the nose to _____, while on a power off stall we pitch to ______</t>
+  </si>
+  <si>
+    <t>15-20°, 5-10°</t>
+  </si>
+  <si>
+    <t>10-15°, 5-10°</t>
+  </si>
+  <si>
+    <t>15-20°, 0-5°</t>
+  </si>
+  <si>
+    <t>15-20°, 10-15°</t>
+  </si>
+  <si>
+    <t>At smaller airports you generally get your weather from ______</t>
+  </si>
+  <si>
+    <t>AWOS/ASOS</t>
+  </si>
+  <si>
+    <t>ATIS</t>
+  </si>
+  <si>
+    <t>PIREPs</t>
+  </si>
+  <si>
+    <t>CTAF</t>
+  </si>
+  <si>
+    <t>_____ utilize just the static port pressure while ______ utilize static port and pitot tube pressure</t>
+  </si>
+  <si>
+    <t>Altimeter and vertical speed indicator --- airspeed indicator</t>
+  </si>
+  <si>
+    <t>Altimeter  --- vertical speed indicator and airspeed indicator</t>
+  </si>
+  <si>
+    <t>Altimeter --- airspeed indicator</t>
+  </si>
+  <si>
+    <t>Altimeter and airspeed indicator --- vertical speed indicator</t>
+  </si>
+  <si>
+    <t>The normal VFR scan area consist of _____ either side from center and _____ up and down</t>
+  </si>
+  <si>
+    <t>60°, 10°</t>
+  </si>
+  <si>
+    <t>120°, 20°</t>
+  </si>
+  <si>
+    <t>10°, 45°</t>
+  </si>
+  <si>
+    <t>90°, 10°</t>
+  </si>
+  <si>
+    <t>G-Suits provide ______ Gs increased tolerance</t>
+  </si>
+  <si>
+    <t>0.5-1.5</t>
+  </si>
+  <si>
+    <t>Which of these is the appropriate level of ORM to use during the execution of a mission with little to no time to make a plan</t>
+  </si>
+  <si>
+    <t>Time critical</t>
+  </si>
+  <si>
+    <t>Urgent</t>
+  </si>
+  <si>
+    <t>Deliberate</t>
+  </si>
+  <si>
+    <t>In-depth</t>
+  </si>
+  <si>
+    <t>Mishaps which cause more than $2.5 million in damage, total loss of aircraft, or death/permanent total disability of personnel are classified as</t>
+  </si>
+  <si>
+    <t>A</t>
+  </si>
+  <si>
+    <t>B</t>
+  </si>
+  <si>
+    <t>Flight Related</t>
+  </si>
+  <si>
+    <t>Flight</t>
+  </si>
+  <si>
+    <t>80% of mishaps are caused by ______</t>
+  </si>
+  <si>
+    <t>Human Error</t>
+  </si>
+  <si>
+    <t>Technical Malfunction</t>
+  </si>
+  <si>
+    <t>Weather</t>
+  </si>
+  <si>
+    <t>Maintenance error</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
-  <numFmts count="1">
+  <numFmts count="2">
     <numFmt numFmtId="164" formatCode="m/d"/>
+    <numFmt numFmtId="165" formatCode="m-d"/>
   </numFmts>
   <fonts count="3">
     <font>
@@ -5742,7 +6094,7 @@
   <cellStyleXfs count="1">
     <xf borderId="0" fillId="0" fontId="0" numFmtId="0" applyAlignment="1" applyFont="1"/>
   </cellStyleXfs>
-  <cellXfs count="30">
+  <cellXfs count="31">
     <xf borderId="0" fillId="0" fontId="0" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
       <alignment readingOrder="0" shrinkToFit="0" vertical="bottom" wrapText="0"/>
     </xf>
@@ -5824,6 +6176,9 @@
     <xf borderId="5" fillId="0" fontId="1" numFmtId="3" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1" applyNumberFormat="1">
       <alignment readingOrder="0" shrinkToFit="0" vertical="center" wrapText="0"/>
     </xf>
+    <xf borderId="5" fillId="0" fontId="1" numFmtId="165" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1" applyNumberFormat="1">
+      <alignment readingOrder="0" shrinkToFit="0" vertical="center" wrapText="0"/>
+    </xf>
     <xf borderId="10" fillId="0" fontId="1" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
       <alignment readingOrder="0" shrinkToFit="0" vertical="center" wrapText="0"/>
     </xf>
@@ -5891,8 +6246,14 @@
 </file>
 
 <file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" ref="A1:H407" displayName="Table1" name="Table1" id="1">
-  <autoFilter ref="$A$1:$H$407"/>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" ref="A1:H431" displayName="Table1" name="Table1" id="1">
+  <autoFilter ref="$A$1:$H$431">
+    <filterColumn colId="0">
+      <filters>
+        <filter val="ground"/>
+      </filters>
+    </filterColumn>
+  </autoFilter>
   <tableColumns count="8">
     <tableColumn name="Topic" id="1"/>
     <tableColumn name="Lecture" id="2"/>
@@ -6145,7 +6506,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="2">
+    <row r="2" hidden="1">
       <c r="A2" s="4" t="s">
         <v>8</v>
       </c>
@@ -6168,11 +6529,11 @@
         <v>13</v>
       </c>
       <c r="H2" s="6">
-        <f t="shared" ref="H2:H407" si="1">ROW()</f>
+        <f t="shared" ref="H2:H431" si="1">ROW()</f>
         <v>2</v>
       </c>
     </row>
-    <row r="3">
+    <row r="3" hidden="1">
       <c r="A3" s="7" t="s">
         <v>8</v>
       </c>
@@ -6199,7 +6560,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="4">
+    <row r="4" hidden="1">
       <c r="A4" s="4" t="s">
         <v>8</v>
       </c>
@@ -6226,7 +6587,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="5">
+    <row r="5" hidden="1">
       <c r="A5" s="7" t="s">
         <v>8</v>
       </c>
@@ -6253,7 +6614,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="6">
+    <row r="6" hidden="1">
       <c r="A6" s="4" t="s">
         <v>8</v>
       </c>
@@ -6280,7 +6641,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="7">
+    <row r="7" hidden="1">
       <c r="A7" s="7" t="s">
         <v>8</v>
       </c>
@@ -6307,7 +6668,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="8">
+    <row r="8" hidden="1">
       <c r="A8" s="4" t="s">
         <v>8</v>
       </c>
@@ -6334,7 +6695,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="9">
+    <row r="9" hidden="1">
       <c r="A9" s="7" t="s">
         <v>8</v>
       </c>
@@ -6361,7 +6722,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="10">
+    <row r="10" hidden="1">
       <c r="A10" s="4" t="s">
         <v>8</v>
       </c>
@@ -6388,7 +6749,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="11">
+    <row r="11" hidden="1">
       <c r="A11" s="7" t="s">
         <v>8</v>
       </c>
@@ -6415,7 +6776,7 @@
         <v>11</v>
       </c>
     </row>
-    <row r="12">
+    <row r="12" hidden="1">
       <c r="A12" s="4" t="s">
         <v>8</v>
       </c>
@@ -6442,7 +6803,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="13">
+    <row r="13" hidden="1">
       <c r="A13" s="7" t="s">
         <v>8</v>
       </c>
@@ -6469,7 +6830,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="14">
+    <row r="14" hidden="1">
       <c r="A14" s="4" t="s">
         <v>8</v>
       </c>
@@ -6496,7 +6857,7 @@
         <v>14</v>
       </c>
     </row>
-    <row r="15">
+    <row r="15" hidden="1">
       <c r="A15" s="7" t="s">
         <v>8</v>
       </c>
@@ -6523,7 +6884,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="16">
+    <row r="16" hidden="1">
       <c r="A16" s="4" t="s">
         <v>8</v>
       </c>
@@ -6550,7 +6911,7 @@
         <v>16</v>
       </c>
     </row>
-    <row r="17">
+    <row r="17" hidden="1">
       <c r="A17" s="7" t="s">
         <v>8</v>
       </c>
@@ -6577,7 +6938,7 @@
         <v>17</v>
       </c>
     </row>
-    <row r="18">
+    <row r="18" hidden="1">
       <c r="A18" s="4" t="s">
         <v>8</v>
       </c>
@@ -6604,7 +6965,7 @@
         <v>18</v>
       </c>
     </row>
-    <row r="19">
+    <row r="19" hidden="1">
       <c r="A19" s="7" t="s">
         <v>8</v>
       </c>
@@ -6631,7 +6992,7 @@
         <v>19</v>
       </c>
     </row>
-    <row r="20">
+    <row r="20" hidden="1">
       <c r="A20" s="4" t="s">
         <v>8</v>
       </c>
@@ -6658,7 +7019,7 @@
         <v>20</v>
       </c>
     </row>
-    <row r="21">
+    <row r="21" hidden="1">
       <c r="A21" s="7" t="s">
         <v>8</v>
       </c>
@@ -6685,7 +7046,7 @@
         <v>21</v>
       </c>
     </row>
-    <row r="22">
+    <row r="22" hidden="1">
       <c r="A22" s="4" t="s">
         <v>8</v>
       </c>
@@ -6712,7 +7073,7 @@
         <v>22</v>
       </c>
     </row>
-    <row r="23">
+    <row r="23" hidden="1">
       <c r="A23" s="7" t="s">
         <v>8</v>
       </c>
@@ -6739,7 +7100,7 @@
         <v>23</v>
       </c>
     </row>
-    <row r="24">
+    <row r="24" hidden="1">
       <c r="A24" s="4" t="s">
         <v>8</v>
       </c>
@@ -6766,7 +7127,7 @@
         <v>24</v>
       </c>
     </row>
-    <row r="25">
+    <row r="25" hidden="1">
       <c r="A25" s="7" t="s">
         <v>8</v>
       </c>
@@ -6793,7 +7154,7 @@
         <v>25</v>
       </c>
     </row>
-    <row r="26">
+    <row r="26" hidden="1">
       <c r="A26" s="4" t="s">
         <v>8</v>
       </c>
@@ -6820,7 +7181,7 @@
         <v>26</v>
       </c>
     </row>
-    <row r="27">
+    <row r="27" hidden="1">
       <c r="A27" s="7" t="s">
         <v>8</v>
       </c>
@@ -6847,7 +7208,7 @@
         <v>27</v>
       </c>
     </row>
-    <row r="28">
+    <row r="28" hidden="1">
       <c r="A28" s="4" t="s">
         <v>8</v>
       </c>
@@ -6874,7 +7235,7 @@
         <v>28</v>
       </c>
     </row>
-    <row r="29">
+    <row r="29" hidden="1">
       <c r="A29" s="7" t="s">
         <v>8</v>
       </c>
@@ -6901,7 +7262,7 @@
         <v>29</v>
       </c>
     </row>
-    <row r="30">
+    <row r="30" hidden="1">
       <c r="A30" s="4" t="s">
         <v>8</v>
       </c>
@@ -6928,7 +7289,7 @@
         <v>30</v>
       </c>
     </row>
-    <row r="31">
+    <row r="31" hidden="1">
       <c r="A31" s="7" t="s">
         <v>8</v>
       </c>
@@ -6955,7 +7316,7 @@
         <v>31</v>
       </c>
     </row>
-    <row r="32">
+    <row r="32" hidden="1">
       <c r="A32" s="4" t="s">
         <v>8</v>
       </c>
@@ -6982,7 +7343,7 @@
         <v>32</v>
       </c>
     </row>
-    <row r="33">
+    <row r="33" hidden="1">
       <c r="A33" s="7" t="s">
         <v>8</v>
       </c>
@@ -7009,7 +7370,7 @@
         <v>33</v>
       </c>
     </row>
-    <row r="34">
+    <row r="34" hidden="1">
       <c r="A34" s="4" t="s">
         <v>8</v>
       </c>
@@ -7036,7 +7397,7 @@
         <v>34</v>
       </c>
     </row>
-    <row r="35">
+    <row r="35" hidden="1">
       <c r="A35" s="7" t="s">
         <v>8</v>
       </c>
@@ -7063,7 +7424,7 @@
         <v>35</v>
       </c>
     </row>
-    <row r="36">
+    <row r="36" hidden="1">
       <c r="A36" s="4" t="s">
         <v>8</v>
       </c>
@@ -7090,7 +7451,7 @@
         <v>36</v>
       </c>
     </row>
-    <row r="37">
+    <row r="37" hidden="1">
       <c r="A37" s="7" t="s">
         <v>8</v>
       </c>
@@ -7117,7 +7478,7 @@
         <v>37</v>
       </c>
     </row>
-    <row r="38">
+    <row r="38" hidden="1">
       <c r="A38" s="4" t="s">
         <v>8</v>
       </c>
@@ -7144,7 +7505,7 @@
         <v>38</v>
       </c>
     </row>
-    <row r="39">
+    <row r="39" hidden="1">
       <c r="A39" s="7" t="s">
         <v>8</v>
       </c>
@@ -7171,7 +7532,7 @@
         <v>39</v>
       </c>
     </row>
-    <row r="40">
+    <row r="40" hidden="1">
       <c r="A40" s="4" t="s">
         <v>8</v>
       </c>
@@ -7198,7 +7559,7 @@
         <v>40</v>
       </c>
     </row>
-    <row r="41">
+    <row r="41" hidden="1">
       <c r="A41" s="7" t="s">
         <v>8</v>
       </c>
@@ -7225,7 +7586,7 @@
         <v>41</v>
       </c>
     </row>
-    <row r="42">
+    <row r="42" hidden="1">
       <c r="A42" s="4" t="s">
         <v>8</v>
       </c>
@@ -7252,7 +7613,7 @@
         <v>42</v>
       </c>
     </row>
-    <row r="43">
+    <row r="43" hidden="1">
       <c r="A43" s="7" t="s">
         <v>8</v>
       </c>
@@ -7279,7 +7640,7 @@
         <v>43</v>
       </c>
     </row>
-    <row r="44">
+    <row r="44" hidden="1">
       <c r="A44" s="4" t="s">
         <v>8</v>
       </c>
@@ -7306,7 +7667,7 @@
         <v>44</v>
       </c>
     </row>
-    <row r="45">
+    <row r="45" hidden="1">
       <c r="A45" s="7" t="s">
         <v>8</v>
       </c>
@@ -7333,7 +7694,7 @@
         <v>45</v>
       </c>
     </row>
-    <row r="46">
+    <row r="46" hidden="1">
       <c r="A46" s="4" t="s">
         <v>8</v>
       </c>
@@ -7360,7 +7721,7 @@
         <v>46</v>
       </c>
     </row>
-    <row r="47">
+    <row r="47" hidden="1">
       <c r="A47" s="7" t="s">
         <v>8</v>
       </c>
@@ -7387,7 +7748,7 @@
         <v>47</v>
       </c>
     </row>
-    <row r="48">
+    <row r="48" hidden="1">
       <c r="A48" s="4" t="s">
         <v>8</v>
       </c>
@@ -7414,7 +7775,7 @@
         <v>48</v>
       </c>
     </row>
-    <row r="49">
+    <row r="49" hidden="1">
       <c r="A49" s="7" t="s">
         <v>8</v>
       </c>
@@ -7441,7 +7802,7 @@
         <v>49</v>
       </c>
     </row>
-    <row r="50">
+    <row r="50" hidden="1">
       <c r="A50" s="4" t="s">
         <v>8</v>
       </c>
@@ -7468,7 +7829,7 @@
         <v>50</v>
       </c>
     </row>
-    <row r="51">
+    <row r="51" hidden="1">
       <c r="A51" s="7" t="s">
         <v>8</v>
       </c>
@@ -7495,7 +7856,7 @@
         <v>51</v>
       </c>
     </row>
-    <row r="52">
+    <row r="52" hidden="1">
       <c r="A52" s="4" t="s">
         <v>8</v>
       </c>
@@ -7522,7 +7883,7 @@
         <v>52</v>
       </c>
     </row>
-    <row r="53">
+    <row r="53" hidden="1">
       <c r="A53" s="7" t="s">
         <v>8</v>
       </c>
@@ -7549,7 +7910,7 @@
         <v>53</v>
       </c>
     </row>
-    <row r="54">
+    <row r="54" hidden="1">
       <c r="A54" s="4" t="s">
         <v>8</v>
       </c>
@@ -7576,7 +7937,7 @@
         <v>54</v>
       </c>
     </row>
-    <row r="55">
+    <row r="55" hidden="1">
       <c r="A55" s="7" t="s">
         <v>8</v>
       </c>
@@ -7603,7 +7964,7 @@
         <v>55</v>
       </c>
     </row>
-    <row r="56">
+    <row r="56" hidden="1">
       <c r="A56" s="4" t="s">
         <v>8</v>
       </c>
@@ -7630,7 +7991,7 @@
         <v>56</v>
       </c>
     </row>
-    <row r="57">
+    <row r="57" hidden="1">
       <c r="A57" s="7" t="s">
         <v>8</v>
       </c>
@@ -7657,7 +8018,7 @@
         <v>57</v>
       </c>
     </row>
-    <row r="58">
+    <row r="58" hidden="1">
       <c r="A58" s="4" t="s">
         <v>8</v>
       </c>
@@ -7684,7 +8045,7 @@
         <v>58</v>
       </c>
     </row>
-    <row r="59">
+    <row r="59" hidden="1">
       <c r="A59" s="7" t="s">
         <v>8</v>
       </c>
@@ -7711,7 +8072,7 @@
         <v>59</v>
       </c>
     </row>
-    <row r="60">
+    <row r="60" hidden="1">
       <c r="A60" s="4" t="s">
         <v>8</v>
       </c>
@@ -7738,7 +8099,7 @@
         <v>60</v>
       </c>
     </row>
-    <row r="61">
+    <row r="61" hidden="1">
       <c r="A61" s="7" t="s">
         <v>8</v>
       </c>
@@ -7765,7 +8126,7 @@
         <v>61</v>
       </c>
     </row>
-    <row r="62">
+    <row r="62" hidden="1">
       <c r="A62" s="4" t="s">
         <v>8</v>
       </c>
@@ -7792,7 +8153,7 @@
         <v>62</v>
       </c>
     </row>
-    <row r="63">
+    <row r="63" hidden="1">
       <c r="A63" s="7" t="s">
         <v>8</v>
       </c>
@@ -7819,7 +8180,7 @@
         <v>63</v>
       </c>
     </row>
-    <row r="64">
+    <row r="64" hidden="1">
       <c r="A64" s="4" t="s">
         <v>8</v>
       </c>
@@ -7846,7 +8207,7 @@
         <v>64</v>
       </c>
     </row>
-    <row r="65">
+    <row r="65" hidden="1">
       <c r="A65" s="7" t="s">
         <v>8</v>
       </c>
@@ -7873,7 +8234,7 @@
         <v>65</v>
       </c>
     </row>
-    <row r="66">
+    <row r="66" hidden="1">
       <c r="A66" s="4" t="s">
         <v>8</v>
       </c>
@@ -7900,7 +8261,7 @@
         <v>66</v>
       </c>
     </row>
-    <row r="67">
+    <row r="67" hidden="1">
       <c r="A67" s="7" t="s">
         <v>8</v>
       </c>
@@ -7927,7 +8288,7 @@
         <v>67</v>
       </c>
     </row>
-    <row r="68">
+    <row r="68" hidden="1">
       <c r="A68" s="4" t="s">
         <v>8</v>
       </c>
@@ -7954,7 +8315,7 @@
         <v>68</v>
       </c>
     </row>
-    <row r="69">
+    <row r="69" hidden="1">
       <c r="A69" s="7" t="s">
         <v>8</v>
       </c>
@@ -7981,7 +8342,7 @@
         <v>69</v>
       </c>
     </row>
-    <row r="70">
+    <row r="70" hidden="1">
       <c r="A70" s="4" t="s">
         <v>8</v>
       </c>
@@ -8008,7 +8369,7 @@
         <v>70</v>
       </c>
     </row>
-    <row r="71">
+    <row r="71" hidden="1">
       <c r="A71" s="7" t="s">
         <v>8</v>
       </c>
@@ -8035,7 +8396,7 @@
         <v>71</v>
       </c>
     </row>
-    <row r="72">
+    <row r="72" hidden="1">
       <c r="A72" s="4" t="s">
         <v>8</v>
       </c>
@@ -8062,7 +8423,7 @@
         <v>72</v>
       </c>
     </row>
-    <row r="73">
+    <row r="73" hidden="1">
       <c r="A73" s="7" t="s">
         <v>8</v>
       </c>
@@ -8089,7 +8450,7 @@
         <v>73</v>
       </c>
     </row>
-    <row r="74">
+    <row r="74" hidden="1">
       <c r="A74" s="4" t="s">
         <v>8</v>
       </c>
@@ -8116,7 +8477,7 @@
         <v>74</v>
       </c>
     </row>
-    <row r="75">
+    <row r="75" hidden="1">
       <c r="A75" s="7" t="s">
         <v>8</v>
       </c>
@@ -8143,7 +8504,7 @@
         <v>75</v>
       </c>
     </row>
-    <row r="76">
+    <row r="76" hidden="1">
       <c r="A76" s="4" t="s">
         <v>8</v>
       </c>
@@ -8170,7 +8531,7 @@
         <v>76</v>
       </c>
     </row>
-    <row r="77">
+    <row r="77" hidden="1">
       <c r="A77" s="7" t="s">
         <v>8</v>
       </c>
@@ -8197,7 +8558,7 @@
         <v>77</v>
       </c>
     </row>
-    <row r="78">
+    <row r="78" hidden="1">
       <c r="A78" s="4" t="s">
         <v>8</v>
       </c>
@@ -8224,7 +8585,7 @@
         <v>78</v>
       </c>
     </row>
-    <row r="79">
+    <row r="79" hidden="1">
       <c r="A79" s="7" t="s">
         <v>8</v>
       </c>
@@ -8251,7 +8612,7 @@
         <v>79</v>
       </c>
     </row>
-    <row r="80">
+    <row r="80" hidden="1">
       <c r="A80" s="4" t="s">
         <v>8</v>
       </c>
@@ -8278,7 +8639,7 @@
         <v>80</v>
       </c>
     </row>
-    <row r="81">
+    <row r="81" hidden="1">
       <c r="A81" s="7" t="s">
         <v>8</v>
       </c>
@@ -8305,7 +8666,7 @@
         <v>81</v>
       </c>
     </row>
-    <row r="82">
+    <row r="82" hidden="1">
       <c r="A82" s="4" t="s">
         <v>8</v>
       </c>
@@ -8332,7 +8693,7 @@
         <v>82</v>
       </c>
     </row>
-    <row r="83">
+    <row r="83" hidden="1">
       <c r="A83" s="7" t="s">
         <v>8</v>
       </c>
@@ -8359,7 +8720,7 @@
         <v>83</v>
       </c>
     </row>
-    <row r="84">
+    <row r="84" hidden="1">
       <c r="A84" s="4" t="s">
         <v>8</v>
       </c>
@@ -8386,7 +8747,7 @@
         <v>84</v>
       </c>
     </row>
-    <row r="85">
+    <row r="85" hidden="1">
       <c r="A85" s="7" t="s">
         <v>8</v>
       </c>
@@ -8413,7 +8774,7 @@
         <v>85</v>
       </c>
     </row>
-    <row r="86">
+    <row r="86" hidden="1">
       <c r="A86" s="4" t="s">
         <v>372</v>
       </c>
@@ -8440,7 +8801,7 @@
         <v>86</v>
       </c>
     </row>
-    <row r="87">
+    <row r="87" hidden="1">
       <c r="A87" s="7" t="s">
         <v>372</v>
       </c>
@@ -8467,7 +8828,7 @@
         <v>87</v>
       </c>
     </row>
-    <row r="88">
+    <row r="88" hidden="1">
       <c r="A88" s="4" t="s">
         <v>372</v>
       </c>
@@ -8494,7 +8855,7 @@
         <v>88</v>
       </c>
     </row>
-    <row r="89">
+    <row r="89" hidden="1">
       <c r="A89" s="7" t="s">
         <v>372</v>
       </c>
@@ -8521,7 +8882,7 @@
         <v>89</v>
       </c>
     </row>
-    <row r="90">
+    <row r="90" hidden="1">
       <c r="A90" s="4" t="s">
         <v>372</v>
       </c>
@@ -8548,7 +8909,7 @@
         <v>90</v>
       </c>
     </row>
-    <row r="91">
+    <row r="91" hidden="1">
       <c r="A91" s="7" t="s">
         <v>372</v>
       </c>
@@ -8575,7 +8936,7 @@
         <v>91</v>
       </c>
     </row>
-    <row r="92">
+    <row r="92" hidden="1">
       <c r="A92" s="4" t="s">
         <v>372</v>
       </c>
@@ -8602,7 +8963,7 @@
         <v>92</v>
       </c>
     </row>
-    <row r="93">
+    <row r="93" hidden="1">
       <c r="A93" s="7" t="s">
         <v>372</v>
       </c>
@@ -8629,7 +8990,7 @@
         <v>93</v>
       </c>
     </row>
-    <row r="94">
+    <row r="94" hidden="1">
       <c r="A94" s="4" t="s">
         <v>372</v>
       </c>
@@ -8656,7 +9017,7 @@
         <v>94</v>
       </c>
     </row>
-    <row r="95">
+    <row r="95" hidden="1">
       <c r="A95" s="7" t="s">
         <v>372</v>
       </c>
@@ -8683,7 +9044,7 @@
         <v>95</v>
       </c>
     </row>
-    <row r="96">
+    <row r="96" hidden="1">
       <c r="A96" s="4" t="s">
         <v>372</v>
       </c>
@@ -8710,7 +9071,7 @@
         <v>96</v>
       </c>
     </row>
-    <row r="97">
+    <row r="97" hidden="1">
       <c r="A97" s="7" t="s">
         <v>372</v>
       </c>
@@ -8737,7 +9098,7 @@
         <v>97</v>
       </c>
     </row>
-    <row r="98">
+    <row r="98" hidden="1">
       <c r="A98" s="4" t="s">
         <v>372</v>
       </c>
@@ -8764,7 +9125,7 @@
         <v>98</v>
       </c>
     </row>
-    <row r="99">
+    <row r="99" hidden="1">
       <c r="A99" s="7" t="s">
         <v>372</v>
       </c>
@@ -8791,7 +9152,7 @@
         <v>99</v>
       </c>
     </row>
-    <row r="100">
+    <row r="100" hidden="1">
       <c r="A100" s="4" t="s">
         <v>372</v>
       </c>
@@ -8818,7 +9179,7 @@
         <v>100</v>
       </c>
     </row>
-    <row r="101">
+    <row r="101" hidden="1">
       <c r="A101" s="7" t="s">
         <v>372</v>
       </c>
@@ -8845,7 +9206,7 @@
         <v>101</v>
       </c>
     </row>
-    <row r="102">
+    <row r="102" hidden="1">
       <c r="A102" s="4" t="s">
         <v>372</v>
       </c>
@@ -8872,7 +9233,7 @@
         <v>102</v>
       </c>
     </row>
-    <row r="103">
+    <row r="103" hidden="1">
       <c r="A103" s="7" t="s">
         <v>372</v>
       </c>
@@ -8899,7 +9260,7 @@
         <v>103</v>
       </c>
     </row>
-    <row r="104">
+    <row r="104" hidden="1">
       <c r="A104" s="4" t="s">
         <v>372</v>
       </c>
@@ -8926,7 +9287,7 @@
         <v>104</v>
       </c>
     </row>
-    <row r="105">
+    <row r="105" hidden="1">
       <c r="A105" s="7" t="s">
         <v>372</v>
       </c>
@@ -8953,7 +9314,7 @@
         <v>105</v>
       </c>
     </row>
-    <row r="106">
+    <row r="106" hidden="1">
       <c r="A106" s="4" t="s">
         <v>372</v>
       </c>
@@ -8980,7 +9341,7 @@
         <v>106</v>
       </c>
     </row>
-    <row r="107">
+    <row r="107" hidden="1">
       <c r="A107" s="7" t="s">
         <v>372</v>
       </c>
@@ -9007,7 +9368,7 @@
         <v>107</v>
       </c>
     </row>
-    <row r="108">
+    <row r="108" hidden="1">
       <c r="A108" s="4" t="s">
         <v>372</v>
       </c>
@@ -9034,7 +9395,7 @@
         <v>108</v>
       </c>
     </row>
-    <row r="109">
+    <row r="109" hidden="1">
       <c r="A109" s="7" t="s">
         <v>372</v>
       </c>
@@ -9061,7 +9422,7 @@
         <v>109</v>
       </c>
     </row>
-    <row r="110">
+    <row r="110" hidden="1">
       <c r="A110" s="4" t="s">
         <v>372</v>
       </c>
@@ -9088,7 +9449,7 @@
         <v>110</v>
       </c>
     </row>
-    <row r="111">
+    <row r="111" hidden="1">
       <c r="A111" s="7" t="s">
         <v>372</v>
       </c>
@@ -9115,7 +9476,7 @@
         <v>111</v>
       </c>
     </row>
-    <row r="112">
+    <row r="112" hidden="1">
       <c r="A112" s="4" t="s">
         <v>372</v>
       </c>
@@ -9142,7 +9503,7 @@
         <v>112</v>
       </c>
     </row>
-    <row r="113">
+    <row r="113" hidden="1">
       <c r="A113" s="7" t="s">
         <v>372</v>
       </c>
@@ -9169,7 +9530,7 @@
         <v>113</v>
       </c>
     </row>
-    <row r="114">
+    <row r="114" hidden="1">
       <c r="A114" s="4" t="s">
         <v>372</v>
       </c>
@@ -9196,7 +9557,7 @@
         <v>114</v>
       </c>
     </row>
-    <row r="115">
+    <row r="115" hidden="1">
       <c r="A115" s="7" t="s">
         <v>372</v>
       </c>
@@ -9223,7 +9584,7 @@
         <v>115</v>
       </c>
     </row>
-    <row r="116">
+    <row r="116" hidden="1">
       <c r="A116" s="4" t="s">
         <v>372</v>
       </c>
@@ -9250,7 +9611,7 @@
         <v>116</v>
       </c>
     </row>
-    <row r="117">
+    <row r="117" hidden="1">
       <c r="A117" s="7" t="s">
         <v>372</v>
       </c>
@@ -9277,7 +9638,7 @@
         <v>117</v>
       </c>
     </row>
-    <row r="118">
+    <row r="118" hidden="1">
       <c r="A118" s="4" t="s">
         <v>372</v>
       </c>
@@ -9304,7 +9665,7 @@
         <v>118</v>
       </c>
     </row>
-    <row r="119">
+    <row r="119" hidden="1">
       <c r="A119" s="7" t="s">
         <v>372</v>
       </c>
@@ -9331,7 +9692,7 @@
         <v>119</v>
       </c>
     </row>
-    <row r="120">
+    <row r="120" hidden="1">
       <c r="A120" s="4" t="s">
         <v>372</v>
       </c>
@@ -9358,7 +9719,7 @@
         <v>120</v>
       </c>
     </row>
-    <row r="121">
+    <row r="121" hidden="1">
       <c r="A121" s="7" t="s">
         <v>372</v>
       </c>
@@ -9385,7 +9746,7 @@
         <v>121</v>
       </c>
     </row>
-    <row r="122">
+    <row r="122" hidden="1">
       <c r="A122" s="4" t="s">
         <v>372</v>
       </c>
@@ -9412,7 +9773,7 @@
         <v>122</v>
       </c>
     </row>
-    <row r="123">
+    <row r="123" hidden="1">
       <c r="A123" s="7" t="s">
         <v>372</v>
       </c>
@@ -9439,7 +9800,7 @@
         <v>123</v>
       </c>
     </row>
-    <row r="124">
+    <row r="124" hidden="1">
       <c r="A124" s="4" t="s">
         <v>372</v>
       </c>
@@ -9466,7 +9827,7 @@
         <v>124</v>
       </c>
     </row>
-    <row r="125">
+    <row r="125" hidden="1">
       <c r="A125" s="7" t="s">
         <v>372</v>
       </c>
@@ -9493,7 +9854,7 @@
         <v>125</v>
       </c>
     </row>
-    <row r="126">
+    <row r="126" hidden="1">
       <c r="A126" s="4" t="s">
         <v>372</v>
       </c>
@@ -9520,7 +9881,7 @@
         <v>126</v>
       </c>
     </row>
-    <row r="127">
+    <row r="127" hidden="1">
       <c r="A127" s="7" t="s">
         <v>372</v>
       </c>
@@ -9547,7 +9908,7 @@
         <v>127</v>
       </c>
     </row>
-    <row r="128">
+    <row r="128" hidden="1">
       <c r="A128" s="4" t="s">
         <v>372</v>
       </c>
@@ -9574,7 +9935,7 @@
         <v>128</v>
       </c>
     </row>
-    <row r="129">
+    <row r="129" hidden="1">
       <c r="A129" s="7" t="s">
         <v>372</v>
       </c>
@@ -9601,7 +9962,7 @@
         <v>129</v>
       </c>
     </row>
-    <row r="130">
+    <row r="130" hidden="1">
       <c r="A130" s="4" t="s">
         <v>372</v>
       </c>
@@ -9628,7 +9989,7 @@
         <v>130</v>
       </c>
     </row>
-    <row r="131">
+    <row r="131" hidden="1">
       <c r="A131" s="7" t="s">
         <v>372</v>
       </c>
@@ -9655,7 +10016,7 @@
         <v>131</v>
       </c>
     </row>
-    <row r="132">
+    <row r="132" hidden="1">
       <c r="A132" s="4" t="s">
         <v>372</v>
       </c>
@@ -9682,7 +10043,7 @@
         <v>132</v>
       </c>
     </row>
-    <row r="133">
+    <row r="133" hidden="1">
       <c r="A133" s="7" t="s">
         <v>372</v>
       </c>
@@ -9709,7 +10070,7 @@
         <v>133</v>
       </c>
     </row>
-    <row r="134">
+    <row r="134" hidden="1">
       <c r="A134" s="4" t="s">
         <v>372</v>
       </c>
@@ -9736,7 +10097,7 @@
         <v>134</v>
       </c>
     </row>
-    <row r="135">
+    <row r="135" hidden="1">
       <c r="A135" s="7" t="s">
         <v>372</v>
       </c>
@@ -9763,7 +10124,7 @@
         <v>135</v>
       </c>
     </row>
-    <row r="136">
+    <row r="136" hidden="1">
       <c r="A136" s="4" t="s">
         <v>372</v>
       </c>
@@ -9790,7 +10151,7 @@
         <v>136</v>
       </c>
     </row>
-    <row r="137">
+    <row r="137" hidden="1">
       <c r="A137" s="7" t="s">
         <v>372</v>
       </c>
@@ -9817,7 +10178,7 @@
         <v>137</v>
       </c>
     </row>
-    <row r="138">
+    <row r="138" hidden="1">
       <c r="A138" s="4" t="s">
         <v>372</v>
       </c>
@@ -9844,7 +10205,7 @@
         <v>138</v>
       </c>
     </row>
-    <row r="139">
+    <row r="139" hidden="1">
       <c r="A139" s="7" t="s">
         <v>372</v>
       </c>
@@ -9871,7 +10232,7 @@
         <v>139</v>
       </c>
     </row>
-    <row r="140">
+    <row r="140" hidden="1">
       <c r="A140" s="4" t="s">
         <v>372</v>
       </c>
@@ -9898,7 +10259,7 @@
         <v>140</v>
       </c>
     </row>
-    <row r="141">
+    <row r="141" hidden="1">
       <c r="A141" s="7" t="s">
         <v>372</v>
       </c>
@@ -9925,7 +10286,7 @@
         <v>141</v>
       </c>
     </row>
-    <row r="142">
+    <row r="142" hidden="1">
       <c r="A142" s="4" t="s">
         <v>372</v>
       </c>
@@ -9952,7 +10313,7 @@
         <v>142</v>
       </c>
     </row>
-    <row r="143">
+    <row r="143" hidden="1">
       <c r="A143" s="7" t="s">
         <v>372</v>
       </c>
@@ -9979,7 +10340,7 @@
         <v>143</v>
       </c>
     </row>
-    <row r="144">
+    <row r="144" hidden="1">
       <c r="A144" s="4" t="s">
         <v>372</v>
       </c>
@@ -10006,7 +10367,7 @@
         <v>144</v>
       </c>
     </row>
-    <row r="145">
+    <row r="145" hidden="1">
       <c r="A145" s="7" t="s">
         <v>372</v>
       </c>
@@ -10033,7 +10394,7 @@
         <v>145</v>
       </c>
     </row>
-    <row r="146">
+    <row r="146" hidden="1">
       <c r="A146" s="4" t="s">
         <v>372</v>
       </c>
@@ -10060,7 +10421,7 @@
         <v>146</v>
       </c>
     </row>
-    <row r="147">
+    <row r="147" hidden="1">
       <c r="A147" s="7" t="s">
         <v>372</v>
       </c>
@@ -10087,7 +10448,7 @@
         <v>147</v>
       </c>
     </row>
-    <row r="148">
+    <row r="148" hidden="1">
       <c r="A148" s="4" t="s">
         <v>372</v>
       </c>
@@ -10114,7 +10475,7 @@
         <v>148</v>
       </c>
     </row>
-    <row r="149">
+    <row r="149" hidden="1">
       <c r="A149" s="7" t="s">
         <v>372</v>
       </c>
@@ -10141,7 +10502,7 @@
         <v>149</v>
       </c>
     </row>
-    <row r="150">
+    <row r="150" hidden="1">
       <c r="A150" s="4" t="s">
         <v>372</v>
       </c>
@@ -10168,7 +10529,7 @@
         <v>150</v>
       </c>
     </row>
-    <row r="151">
+    <row r="151" hidden="1">
       <c r="A151" s="7" t="s">
         <v>372</v>
       </c>
@@ -10195,7 +10556,7 @@
         <v>151</v>
       </c>
     </row>
-    <row r="152">
+    <row r="152" hidden="1">
       <c r="A152" s="4" t="s">
         <v>372</v>
       </c>
@@ -10222,7 +10583,7 @@
         <v>152</v>
       </c>
     </row>
-    <row r="153">
+    <row r="153" hidden="1">
       <c r="A153" s="7" t="s">
         <v>372</v>
       </c>
@@ -10249,7 +10610,7 @@
         <v>153</v>
       </c>
     </row>
-    <row r="154">
+    <row r="154" hidden="1">
       <c r="A154" s="4" t="s">
         <v>372</v>
       </c>
@@ -10276,7 +10637,7 @@
         <v>154</v>
       </c>
     </row>
-    <row r="155">
+    <row r="155" hidden="1">
       <c r="A155" s="7" t="s">
         <v>372</v>
       </c>
@@ -10303,7 +10664,7 @@
         <v>155</v>
       </c>
     </row>
-    <row r="156">
+    <row r="156" hidden="1">
       <c r="A156" s="4" t="s">
         <v>372</v>
       </c>
@@ -10330,7 +10691,7 @@
         <v>156</v>
       </c>
     </row>
-    <row r="157">
+    <row r="157" hidden="1">
       <c r="A157" s="7" t="s">
         <v>372</v>
       </c>
@@ -10357,7 +10718,7 @@
         <v>157</v>
       </c>
     </row>
-    <row r="158">
+    <row r="158" hidden="1">
       <c r="A158" s="4" t="s">
         <v>372</v>
       </c>
@@ -10384,7 +10745,7 @@
         <v>158</v>
       </c>
     </row>
-    <row r="159">
+    <row r="159" hidden="1">
       <c r="A159" s="7" t="s">
         <v>372</v>
       </c>
@@ -10411,7 +10772,7 @@
         <v>159</v>
       </c>
     </row>
-    <row r="160">
+    <row r="160" hidden="1">
       <c r="A160" s="4" t="s">
         <v>372</v>
       </c>
@@ -10438,7 +10799,7 @@
         <v>160</v>
       </c>
     </row>
-    <row r="161">
+    <row r="161" hidden="1">
       <c r="A161" s="7" t="s">
         <v>372</v>
       </c>
@@ -10465,7 +10826,7 @@
         <v>161</v>
       </c>
     </row>
-    <row r="162">
+    <row r="162" hidden="1">
       <c r="A162" s="4" t="s">
         <v>372</v>
       </c>
@@ -10492,7 +10853,7 @@
         <v>162</v>
       </c>
     </row>
-    <row r="163">
+    <row r="163" hidden="1">
       <c r="A163" s="7" t="s">
         <v>372</v>
       </c>
@@ -10519,7 +10880,7 @@
         <v>163</v>
       </c>
     </row>
-    <row r="164">
+    <row r="164" hidden="1">
       <c r="A164" s="4" t="s">
         <v>372</v>
       </c>
@@ -10546,7 +10907,7 @@
         <v>164</v>
       </c>
     </row>
-    <row r="165">
+    <row r="165" hidden="1">
       <c r="A165" s="7" t="s">
         <v>372</v>
       </c>
@@ -10573,7 +10934,7 @@
         <v>165</v>
       </c>
     </row>
-    <row r="166">
+    <row r="166" hidden="1">
       <c r="A166" s="4" t="s">
         <v>372</v>
       </c>
@@ -10600,7 +10961,7 @@
         <v>166</v>
       </c>
     </row>
-    <row r="167">
+    <row r="167" hidden="1">
       <c r="A167" s="7" t="s">
         <v>372</v>
       </c>
@@ -10627,7 +10988,7 @@
         <v>167</v>
       </c>
     </row>
-    <row r="168">
+    <row r="168" hidden="1">
       <c r="A168" s="4" t="s">
         <v>372</v>
       </c>
@@ -10654,7 +11015,7 @@
         <v>168</v>
       </c>
     </row>
-    <row r="169">
+    <row r="169" hidden="1">
       <c r="A169" s="7" t="s">
         <v>372</v>
       </c>
@@ -10681,7 +11042,7 @@
         <v>169</v>
       </c>
     </row>
-    <row r="170">
+    <row r="170" hidden="1">
       <c r="A170" s="4" t="s">
         <v>372</v>
       </c>
@@ -10708,7 +11069,7 @@
         <v>170</v>
       </c>
     </row>
-    <row r="171">
+    <row r="171" hidden="1">
       <c r="A171" s="7" t="s">
         <v>372</v>
       </c>
@@ -10735,7 +11096,7 @@
         <v>171</v>
       </c>
     </row>
-    <row r="172">
+    <row r="172" hidden="1">
       <c r="A172" s="4" t="s">
         <v>372</v>
       </c>
@@ -10762,7 +11123,7 @@
         <v>172</v>
       </c>
     </row>
-    <row r="173">
+    <row r="173" hidden="1">
       <c r="A173" s="7" t="s">
         <v>750</v>
       </c>
@@ -10789,7 +11150,7 @@
         <v>173</v>
       </c>
     </row>
-    <row r="174">
+    <row r="174" hidden="1">
       <c r="A174" s="4" t="s">
         <v>750</v>
       </c>
@@ -10816,7 +11177,7 @@
         <v>174</v>
       </c>
     </row>
-    <row r="175">
+    <row r="175" hidden="1">
       <c r="A175" s="7" t="s">
         <v>750</v>
       </c>
@@ -10843,7 +11204,7 @@
         <v>175</v>
       </c>
     </row>
-    <row r="176">
+    <row r="176" hidden="1">
       <c r="A176" s="4" t="s">
         <v>750</v>
       </c>
@@ -10870,7 +11231,7 @@
         <v>176</v>
       </c>
     </row>
-    <row r="177">
+    <row r="177" hidden="1">
       <c r="A177" s="7" t="s">
         <v>750</v>
       </c>
@@ -10897,7 +11258,7 @@
         <v>177</v>
       </c>
     </row>
-    <row r="178">
+    <row r="178" hidden="1">
       <c r="A178" s="4" t="s">
         <v>750</v>
       </c>
@@ -10924,7 +11285,7 @@
         <v>178</v>
       </c>
     </row>
-    <row r="179">
+    <row r="179" hidden="1">
       <c r="A179" s="7" t="s">
         <v>750</v>
       </c>
@@ -10951,7 +11312,7 @@
         <v>179</v>
       </c>
     </row>
-    <row r="180">
+    <row r="180" hidden="1">
       <c r="A180" s="4" t="s">
         <v>750</v>
       </c>
@@ -10978,7 +11339,7 @@
         <v>180</v>
       </c>
     </row>
-    <row r="181">
+    <row r="181" hidden="1">
       <c r="A181" s="7" t="s">
         <v>750</v>
       </c>
@@ -11005,7 +11366,7 @@
         <v>181</v>
       </c>
     </row>
-    <row r="182">
+    <row r="182" hidden="1">
       <c r="A182" s="4" t="s">
         <v>750</v>
       </c>
@@ -11032,7 +11393,7 @@
         <v>182</v>
       </c>
     </row>
-    <row r="183">
+    <row r="183" hidden="1">
       <c r="A183" s="7" t="s">
         <v>750</v>
       </c>
@@ -11059,7 +11420,7 @@
         <v>183</v>
       </c>
     </row>
-    <row r="184">
+    <row r="184" hidden="1">
       <c r="A184" s="4" t="s">
         <v>750</v>
       </c>
@@ -11086,7 +11447,7 @@
         <v>184</v>
       </c>
     </row>
-    <row r="185">
+    <row r="185" hidden="1">
       <c r="A185" s="7" t="s">
         <v>750</v>
       </c>
@@ -11113,7 +11474,7 @@
         <v>185</v>
       </c>
     </row>
-    <row r="186">
+    <row r="186" hidden="1">
       <c r="A186" s="4" t="s">
         <v>750</v>
       </c>
@@ -11140,7 +11501,7 @@
         <v>186</v>
       </c>
     </row>
-    <row r="187">
+    <row r="187" hidden="1">
       <c r="A187" s="7" t="s">
         <v>750</v>
       </c>
@@ -11167,7 +11528,7 @@
         <v>187</v>
       </c>
     </row>
-    <row r="188">
+    <row r="188" hidden="1">
       <c r="A188" s="4" t="s">
         <v>750</v>
       </c>
@@ -11194,7 +11555,7 @@
         <v>188</v>
       </c>
     </row>
-    <row r="189">
+    <row r="189" hidden="1">
       <c r="A189" s="7" t="s">
         <v>750</v>
       </c>
@@ -11221,7 +11582,7 @@
         <v>189</v>
       </c>
     </row>
-    <row r="190">
+    <row r="190" hidden="1">
       <c r="A190" s="4" t="s">
         <v>750</v>
       </c>
@@ -11248,7 +11609,7 @@
         <v>190</v>
       </c>
     </row>
-    <row r="191">
+    <row r="191" hidden="1">
       <c r="A191" s="7" t="s">
         <v>750</v>
       </c>
@@ -11275,7 +11636,7 @@
         <v>191</v>
       </c>
     </row>
-    <row r="192">
+    <row r="192" hidden="1">
       <c r="A192" s="4" t="s">
         <v>750</v>
       </c>
@@ -11302,7 +11663,7 @@
         <v>192</v>
       </c>
     </row>
-    <row r="193">
+    <row r="193" hidden="1">
       <c r="A193" s="7" t="s">
         <v>750</v>
       </c>
@@ -11329,7 +11690,7 @@
         <v>193</v>
       </c>
     </row>
-    <row r="194">
+    <row r="194" hidden="1">
       <c r="A194" s="4" t="s">
         <v>750</v>
       </c>
@@ -11356,7 +11717,7 @@
         <v>194</v>
       </c>
     </row>
-    <row r="195">
+    <row r="195" hidden="1">
       <c r="A195" s="7" t="s">
         <v>750</v>
       </c>
@@ -11383,7 +11744,7 @@
         <v>195</v>
       </c>
     </row>
-    <row r="196">
+    <row r="196" hidden="1">
       <c r="A196" s="4" t="s">
         <v>750</v>
       </c>
@@ -11410,7 +11771,7 @@
         <v>196</v>
       </c>
     </row>
-    <row r="197">
+    <row r="197" hidden="1">
       <c r="A197" s="7" t="s">
         <v>750</v>
       </c>
@@ -11437,7 +11798,7 @@
         <v>197</v>
       </c>
     </row>
-    <row r="198">
+    <row r="198" hidden="1">
       <c r="A198" s="4" t="s">
         <v>750</v>
       </c>
@@ -11464,7 +11825,7 @@
         <v>198</v>
       </c>
     </row>
-    <row r="199">
+    <row r="199" hidden="1">
       <c r="A199" s="7" t="s">
         <v>750</v>
       </c>
@@ -11491,7 +11852,7 @@
         <v>199</v>
       </c>
     </row>
-    <row r="200">
+    <row r="200" hidden="1">
       <c r="A200" s="4" t="s">
         <v>750</v>
       </c>
@@ -11518,7 +11879,7 @@
         <v>200</v>
       </c>
     </row>
-    <row r="201">
+    <row r="201" hidden="1">
       <c r="A201" s="7" t="s">
         <v>750</v>
       </c>
@@ -11545,7 +11906,7 @@
         <v>201</v>
       </c>
     </row>
-    <row r="202">
+    <row r="202" hidden="1">
       <c r="A202" s="4" t="s">
         <v>750</v>
       </c>
@@ -11572,7 +11933,7 @@
         <v>202</v>
       </c>
     </row>
-    <row r="203">
+    <row r="203" hidden="1">
       <c r="A203" s="7" t="s">
         <v>750</v>
       </c>
@@ -11599,7 +11960,7 @@
         <v>203</v>
       </c>
     </row>
-    <row r="204">
+    <row r="204" hidden="1">
       <c r="A204" s="4" t="s">
         <v>750</v>
       </c>
@@ -11626,7 +11987,7 @@
         <v>204</v>
       </c>
     </row>
-    <row r="205">
+    <row r="205" hidden="1">
       <c r="A205" s="7" t="s">
         <v>750</v>
       </c>
@@ -11653,7 +12014,7 @@
         <v>205</v>
       </c>
     </row>
-    <row r="206">
+    <row r="206" hidden="1">
       <c r="A206" s="4" t="s">
         <v>750</v>
       </c>
@@ -11680,7 +12041,7 @@
         <v>206</v>
       </c>
     </row>
-    <row r="207">
+    <row r="207" hidden="1">
       <c r="A207" s="7" t="s">
         <v>750</v>
       </c>
@@ -11707,7 +12068,7 @@
         <v>207</v>
       </c>
     </row>
-    <row r="208">
+    <row r="208" hidden="1">
       <c r="A208" s="4" t="s">
         <v>750</v>
       </c>
@@ -11734,7 +12095,7 @@
         <v>208</v>
       </c>
     </row>
-    <row r="209">
+    <row r="209" hidden="1">
       <c r="A209" s="7" t="s">
         <v>750</v>
       </c>
@@ -11761,7 +12122,7 @@
         <v>209</v>
       </c>
     </row>
-    <row r="210">
+    <row r="210" hidden="1">
       <c r="A210" s="4" t="s">
         <v>750</v>
       </c>
@@ -11788,7 +12149,7 @@
         <v>210</v>
       </c>
     </row>
-    <row r="211">
+    <row r="211" hidden="1">
       <c r="A211" s="7" t="s">
         <v>750</v>
       </c>
@@ -11815,7 +12176,7 @@
         <v>211</v>
       </c>
     </row>
-    <row r="212">
+    <row r="212" hidden="1">
       <c r="A212" s="4" t="s">
         <v>750</v>
       </c>
@@ -11842,7 +12203,7 @@
         <v>212</v>
       </c>
     </row>
-    <row r="213">
+    <row r="213" hidden="1">
       <c r="A213" s="7" t="s">
         <v>750</v>
       </c>
@@ -11869,7 +12230,7 @@
         <v>213</v>
       </c>
     </row>
-    <row r="214">
+    <row r="214" hidden="1">
       <c r="A214" s="4" t="s">
         <v>750</v>
       </c>
@@ -11896,7 +12257,7 @@
         <v>214</v>
       </c>
     </row>
-    <row r="215">
+    <row r="215" hidden="1">
       <c r="A215" s="7" t="s">
         <v>750</v>
       </c>
@@ -11923,7 +12284,7 @@
         <v>215</v>
       </c>
     </row>
-    <row r="216">
+    <row r="216" hidden="1">
       <c r="A216" s="4" t="s">
         <v>750</v>
       </c>
@@ -11950,7 +12311,7 @@
         <v>216</v>
       </c>
     </row>
-    <row r="217">
+    <row r="217" hidden="1">
       <c r="A217" s="7" t="s">
         <v>750</v>
       </c>
@@ -11977,7 +12338,7 @@
         <v>217</v>
       </c>
     </row>
-    <row r="218">
+    <row r="218" hidden="1">
       <c r="A218" s="4" t="s">
         <v>750</v>
       </c>
@@ -12004,7 +12365,7 @@
         <v>218</v>
       </c>
     </row>
-    <row r="219">
+    <row r="219" hidden="1">
       <c r="A219" s="7" t="s">
         <v>750</v>
       </c>
@@ -12031,7 +12392,7 @@
         <v>219</v>
       </c>
     </row>
-    <row r="220">
+    <row r="220" hidden="1">
       <c r="A220" s="4" t="s">
         <v>750</v>
       </c>
@@ -12058,7 +12419,7 @@
         <v>220</v>
       </c>
     </row>
-    <row r="221">
+    <row r="221" hidden="1">
       <c r="A221" s="7" t="s">
         <v>750</v>
       </c>
@@ -12085,7 +12446,7 @@
         <v>221</v>
       </c>
     </row>
-    <row r="222">
+    <row r="222" hidden="1">
       <c r="A222" s="4" t="s">
         <v>750</v>
       </c>
@@ -12112,7 +12473,7 @@
         <v>222</v>
       </c>
     </row>
-    <row r="223">
+    <row r="223" hidden="1">
       <c r="A223" s="7" t="s">
         <v>750</v>
       </c>
@@ -12139,7 +12500,7 @@
         <v>223</v>
       </c>
     </row>
-    <row r="224">
+    <row r="224" hidden="1">
       <c r="A224" s="4" t="s">
         <v>750</v>
       </c>
@@ -12166,7 +12527,7 @@
         <v>224</v>
       </c>
     </row>
-    <row r="225">
+    <row r="225" hidden="1">
       <c r="A225" s="7" t="s">
         <v>750</v>
       </c>
@@ -12193,7 +12554,7 @@
         <v>225</v>
       </c>
     </row>
-    <row r="226">
+    <row r="226" hidden="1">
       <c r="A226" s="4" t="s">
         <v>750</v>
       </c>
@@ -12220,7 +12581,7 @@
         <v>226</v>
       </c>
     </row>
-    <row r="227">
+    <row r="227" hidden="1">
       <c r="A227" s="7" t="s">
         <v>750</v>
       </c>
@@ -12247,7 +12608,7 @@
         <v>227</v>
       </c>
     </row>
-    <row r="228">
+    <row r="228" hidden="1">
       <c r="A228" s="4" t="s">
         <v>750</v>
       </c>
@@ -12274,7 +12635,7 @@
         <v>228</v>
       </c>
     </row>
-    <row r="229">
+    <row r="229" hidden="1">
       <c r="A229" s="7" t="s">
         <v>750</v>
       </c>
@@ -12301,7 +12662,7 @@
         <v>229</v>
       </c>
     </row>
-    <row r="230">
+    <row r="230" hidden="1">
       <c r="A230" s="4" t="s">
         <v>750</v>
       </c>
@@ -12328,7 +12689,7 @@
         <v>230</v>
       </c>
     </row>
-    <row r="231">
+    <row r="231" hidden="1">
       <c r="A231" s="7" t="s">
         <v>750</v>
       </c>
@@ -12355,7 +12716,7 @@
         <v>231</v>
       </c>
     </row>
-    <row r="232">
+    <row r="232" hidden="1">
       <c r="A232" s="4" t="s">
         <v>750</v>
       </c>
@@ -12382,7 +12743,7 @@
         <v>232</v>
       </c>
     </row>
-    <row r="233">
+    <row r="233" hidden="1">
       <c r="A233" s="7" t="s">
         <v>750</v>
       </c>
@@ -12409,7 +12770,7 @@
         <v>233</v>
       </c>
     </row>
-    <row r="234">
+    <row r="234" hidden="1">
       <c r="A234" s="4" t="s">
         <v>750</v>
       </c>
@@ -12436,7 +12797,7 @@
         <v>234</v>
       </c>
     </row>
-    <row r="235">
+    <row r="235" hidden="1">
       <c r="A235" s="7" t="s">
         <v>750</v>
       </c>
@@ -12463,7 +12824,7 @@
         <v>235</v>
       </c>
     </row>
-    <row r="236">
+    <row r="236" hidden="1">
       <c r="A236" s="4" t="s">
         <v>750</v>
       </c>
@@ -12490,7 +12851,7 @@
         <v>236</v>
       </c>
     </row>
-    <row r="237">
+    <row r="237" hidden="1">
       <c r="A237" s="7" t="s">
         <v>750</v>
       </c>
@@ -12517,7 +12878,7 @@
         <v>237</v>
       </c>
     </row>
-    <row r="238">
+    <row r="238" hidden="1">
       <c r="A238" s="4" t="s">
         <v>750</v>
       </c>
@@ -12544,7 +12905,7 @@
         <v>238</v>
       </c>
     </row>
-    <row r="239">
+    <row r="239" hidden="1">
       <c r="A239" s="7" t="s">
         <v>750</v>
       </c>
@@ -12571,7 +12932,7 @@
         <v>239</v>
       </c>
     </row>
-    <row r="240">
+    <row r="240" hidden="1">
       <c r="A240" s="4" t="s">
         <v>750</v>
       </c>
@@ -12598,7 +12959,7 @@
         <v>240</v>
       </c>
     </row>
-    <row r="241">
+    <row r="241" hidden="1">
       <c r="A241" s="7" t="s">
         <v>750</v>
       </c>
@@ -12625,7 +12986,7 @@
         <v>241</v>
       </c>
     </row>
-    <row r="242">
+    <row r="242" hidden="1">
       <c r="A242" s="4" t="s">
         <v>750</v>
       </c>
@@ -12652,7 +13013,7 @@
         <v>242</v>
       </c>
     </row>
-    <row r="243">
+    <row r="243" hidden="1">
       <c r="A243" s="7" t="s">
         <v>750</v>
       </c>
@@ -12679,7 +13040,7 @@
         <v>243</v>
       </c>
     </row>
-    <row r="244">
+    <row r="244" hidden="1">
       <c r="A244" s="4" t="s">
         <v>750</v>
       </c>
@@ -12706,7 +13067,7 @@
         <v>244</v>
       </c>
     </row>
-    <row r="245">
+    <row r="245" hidden="1">
       <c r="A245" s="7" t="s">
         <v>750</v>
       </c>
@@ -12733,7 +13094,7 @@
         <v>245</v>
       </c>
     </row>
-    <row r="246">
+    <row r="246" hidden="1">
       <c r="A246" s="4" t="s">
         <v>750</v>
       </c>
@@ -12760,7 +13121,7 @@
         <v>246</v>
       </c>
     </row>
-    <row r="247">
+    <row r="247" hidden="1">
       <c r="A247" s="7" t="s">
         <v>750</v>
       </c>
@@ -12787,7 +13148,7 @@
         <v>247</v>
       </c>
     </row>
-    <row r="248">
+    <row r="248" hidden="1">
       <c r="A248" s="4" t="s">
         <v>750</v>
       </c>
@@ -12814,7 +13175,7 @@
         <v>248</v>
       </c>
     </row>
-    <row r="249">
+    <row r="249" hidden="1">
       <c r="A249" s="7" t="s">
         <v>750</v>
       </c>
@@ -12841,7 +13202,7 @@
         <v>249</v>
       </c>
     </row>
-    <row r="250">
+    <row r="250" hidden="1">
       <c r="A250" s="4" t="s">
         <v>750</v>
       </c>
@@ -12868,7 +13229,7 @@
         <v>250</v>
       </c>
     </row>
-    <row r="251">
+    <row r="251" hidden="1">
       <c r="A251" s="7" t="s">
         <v>750</v>
       </c>
@@ -12895,7 +13256,7 @@
         <v>251</v>
       </c>
     </row>
-    <row r="252">
+    <row r="252" hidden="1">
       <c r="A252" s="4" t="s">
         <v>750</v>
       </c>
@@ -12922,7 +13283,7 @@
         <v>252</v>
       </c>
     </row>
-    <row r="253">
+    <row r="253" hidden="1">
       <c r="A253" s="7" t="s">
         <v>750</v>
       </c>
@@ -12953,9 +13314,7 @@
       <c r="A254" s="4" t="s">
         <v>1129</v>
       </c>
-      <c r="B254" s="10">
-        <v>1.0</v>
-      </c>
+      <c r="B254" s="10"/>
       <c r="C254" s="10" t="s">
         <v>1130</v>
       </c>
@@ -12980,9 +13339,7 @@
       <c r="A255" s="7" t="s">
         <v>1129</v>
       </c>
-      <c r="B255" s="12">
-        <v>1.0</v>
-      </c>
+      <c r="B255" s="12"/>
       <c r="C255" s="12" t="s">
         <v>1135</v>
       </c>
@@ -13007,9 +13364,7 @@
       <c r="A256" s="4" t="s">
         <v>1129</v>
       </c>
-      <c r="B256" s="10">
-        <v>1.0</v>
-      </c>
+      <c r="B256" s="10"/>
       <c r="C256" s="10" t="s">
         <v>1137</v>
       </c>
@@ -13034,9 +13389,7 @@
       <c r="A257" s="7" t="s">
         <v>1129</v>
       </c>
-      <c r="B257" s="12">
-        <v>1.0</v>
-      </c>
+      <c r="B257" s="12"/>
       <c r="C257" s="12" t="s">
         <v>1142</v>
       </c>
@@ -13061,9 +13414,7 @@
       <c r="A258" s="4" t="s">
         <v>1129</v>
       </c>
-      <c r="B258" s="10">
-        <v>1.0</v>
-      </c>
+      <c r="B258" s="10"/>
       <c r="C258" s="10" t="s">
         <v>1147</v>
       </c>
@@ -13088,9 +13439,7 @@
       <c r="A259" s="7" t="s">
         <v>1129</v>
       </c>
-      <c r="B259" s="12">
-        <v>1.0</v>
-      </c>
+      <c r="B259" s="12"/>
       <c r="C259" s="12" t="s">
         <v>1152</v>
       </c>
@@ -13115,9 +13464,7 @@
       <c r="A260" s="4" t="s">
         <v>1129</v>
       </c>
-      <c r="B260" s="10">
-        <v>1.0</v>
-      </c>
+      <c r="B260" s="10"/>
       <c r="C260" s="10" t="s">
         <v>1157</v>
       </c>
@@ -13142,9 +13489,7 @@
       <c r="A261" s="7" t="s">
         <v>1129</v>
       </c>
-      <c r="B261" s="12">
-        <v>2.0</v>
-      </c>
+      <c r="B261" s="12"/>
       <c r="C261" s="12" t="s">
         <v>1162</v>
       </c>
@@ -13238,7 +13583,7 @@
         <v>264</v>
       </c>
     </row>
-    <row r="265">
+    <row r="265" hidden="1">
       <c r="A265" s="7" t="s">
         <v>1182</v>
       </c>
@@ -13262,7 +13607,7 @@
         <v>265</v>
       </c>
     </row>
-    <row r="266">
+    <row r="266" hidden="1">
       <c r="A266" s="4" t="s">
         <v>1182</v>
       </c>
@@ -13286,7 +13631,7 @@
         <v>266</v>
       </c>
     </row>
-    <row r="267">
+    <row r="267" hidden="1">
       <c r="A267" s="7" t="s">
         <v>1182</v>
       </c>
@@ -13310,7 +13655,7 @@
         <v>267</v>
       </c>
     </row>
-    <row r="268">
+    <row r="268" hidden="1">
       <c r="A268" s="4" t="s">
         <v>1182</v>
       </c>
@@ -13334,7 +13679,7 @@
         <v>268</v>
       </c>
     </row>
-    <row r="269">
+    <row r="269" hidden="1">
       <c r="A269" s="7" t="s">
         <v>1182</v>
       </c>
@@ -13358,7 +13703,7 @@
         <v>269</v>
       </c>
     </row>
-    <row r="270">
+    <row r="270" hidden="1">
       <c r="A270" s="4" t="s">
         <v>1182</v>
       </c>
@@ -13382,7 +13727,7 @@
         <v>270</v>
       </c>
     </row>
-    <row r="271">
+    <row r="271" hidden="1">
       <c r="A271" s="7" t="s">
         <v>1182</v>
       </c>
@@ -13406,7 +13751,7 @@
         <v>271</v>
       </c>
     </row>
-    <row r="272">
+    <row r="272" hidden="1">
       <c r="A272" s="4" t="s">
         <v>1182</v>
       </c>
@@ -13430,7 +13775,7 @@
         <v>272</v>
       </c>
     </row>
-    <row r="273">
+    <row r="273" hidden="1">
       <c r="A273" s="7" t="s">
         <v>1182</v>
       </c>
@@ -13454,7 +13799,7 @@
         <v>273</v>
       </c>
     </row>
-    <row r="274">
+    <row r="274" hidden="1">
       <c r="A274" s="4" t="s">
         <v>1182</v>
       </c>
@@ -13478,7 +13823,7 @@
         <v>274</v>
       </c>
     </row>
-    <row r="275">
+    <row r="275" hidden="1">
       <c r="A275" s="7" t="s">
         <v>1182</v>
       </c>
@@ -13502,7 +13847,7 @@
         <v>275</v>
       </c>
     </row>
-    <row r="276">
+    <row r="276" hidden="1">
       <c r="A276" s="4" t="s">
         <v>1182</v>
       </c>
@@ -13526,7 +13871,7 @@
         <v>276</v>
       </c>
     </row>
-    <row r="277">
+    <row r="277" hidden="1">
       <c r="A277" s="7" t="s">
         <v>1182</v>
       </c>
@@ -13550,7 +13895,7 @@
         <v>277</v>
       </c>
     </row>
-    <row r="278">
+    <row r="278" hidden="1">
       <c r="A278" s="4" t="s">
         <v>1182</v>
       </c>
@@ -13574,7 +13919,7 @@
         <v>278</v>
       </c>
     </row>
-    <row r="279">
+    <row r="279" hidden="1">
       <c r="A279" s="7" t="s">
         <v>1182</v>
       </c>
@@ -13598,7 +13943,7 @@
         <v>279</v>
       </c>
     </row>
-    <row r="280">
+    <row r="280" hidden="1">
       <c r="A280" s="4" t="s">
         <v>1182</v>
       </c>
@@ -13622,7 +13967,7 @@
         <v>280</v>
       </c>
     </row>
-    <row r="281">
+    <row r="281" hidden="1">
       <c r="A281" s="7" t="s">
         <v>1182</v>
       </c>
@@ -13646,7 +13991,7 @@
         <v>281</v>
       </c>
     </row>
-    <row r="282">
+    <row r="282" hidden="1">
       <c r="A282" s="4" t="s">
         <v>1182</v>
       </c>
@@ -13670,7 +14015,7 @@
         <v>282</v>
       </c>
     </row>
-    <row r="283">
+    <row r="283" hidden="1">
       <c r="A283" s="7" t="s">
         <v>1182</v>
       </c>
@@ -13694,7 +14039,7 @@
         <v>283</v>
       </c>
     </row>
-    <row r="284">
+    <row r="284" hidden="1">
       <c r="A284" s="4" t="s">
         <v>1182</v>
       </c>
@@ -13718,7 +14063,7 @@
         <v>284</v>
       </c>
     </row>
-    <row r="285">
+    <row r="285" hidden="1">
       <c r="A285" s="7" t="s">
         <v>1182</v>
       </c>
@@ -13742,7 +14087,7 @@
         <v>285</v>
       </c>
     </row>
-    <row r="286">
+    <row r="286" hidden="1">
       <c r="A286" s="4" t="s">
         <v>1182</v>
       </c>
@@ -13766,7 +14111,7 @@
         <v>286</v>
       </c>
     </row>
-    <row r="287">
+    <row r="287" hidden="1">
       <c r="A287" s="7" t="s">
         <v>1182</v>
       </c>
@@ -13790,7 +14135,7 @@
         <v>287</v>
       </c>
     </row>
-    <row r="288">
+    <row r="288" hidden="1">
       <c r="A288" s="4" t="s">
         <v>1182</v>
       </c>
@@ -13814,7 +14159,7 @@
         <v>288</v>
       </c>
     </row>
-    <row r="289">
+    <row r="289" hidden="1">
       <c r="A289" s="7" t="s">
         <v>1182</v>
       </c>
@@ -13838,7 +14183,7 @@
         <v>289</v>
       </c>
     </row>
-    <row r="290">
+    <row r="290" hidden="1">
       <c r="A290" s="4" t="s">
         <v>1182</v>
       </c>
@@ -13862,7 +14207,7 @@
         <v>290</v>
       </c>
     </row>
-    <row r="291">
+    <row r="291" hidden="1">
       <c r="A291" s="7" t="s">
         <v>1182</v>
       </c>
@@ -13886,7 +14231,7 @@
         <v>291</v>
       </c>
     </row>
-    <row r="292">
+    <row r="292" hidden="1">
       <c r="A292" s="4" t="s">
         <v>1182</v>
       </c>
@@ -13910,7 +14255,7 @@
         <v>292</v>
       </c>
     </row>
-    <row r="293">
+    <row r="293" hidden="1">
       <c r="A293" s="7" t="s">
         <v>1182</v>
       </c>
@@ -13934,7 +14279,7 @@
         <v>293</v>
       </c>
     </row>
-    <row r="294">
+    <row r="294" hidden="1">
       <c r="A294" s="4" t="s">
         <v>1182</v>
       </c>
@@ -13958,7 +14303,7 @@
         <v>294</v>
       </c>
     </row>
-    <row r="295">
+    <row r="295" hidden="1">
       <c r="A295" s="7" t="s">
         <v>1182</v>
       </c>
@@ -13982,7 +14327,7 @@
         <v>295</v>
       </c>
     </row>
-    <row r="296">
+    <row r="296" hidden="1">
       <c r="A296" s="4" t="s">
         <v>1182</v>
       </c>
@@ -14006,7 +14351,7 @@
         <v>296</v>
       </c>
     </row>
-    <row r="297">
+    <row r="297" hidden="1">
       <c r="A297" s="7" t="s">
         <v>1182</v>
       </c>
@@ -14030,7 +14375,7 @@
         <v>297</v>
       </c>
     </row>
-    <row r="298">
+    <row r="298" hidden="1">
       <c r="A298" s="4" t="s">
         <v>1182</v>
       </c>
@@ -14054,7 +14399,7 @@
         <v>298</v>
       </c>
     </row>
-    <row r="299">
+    <row r="299" hidden="1">
       <c r="A299" s="23" t="s">
         <v>1182</v>
       </c>
@@ -14079,7 +14424,7 @@
         <v>299</v>
       </c>
     </row>
-    <row r="300">
+    <row r="300" hidden="1">
       <c r="A300" s="4" t="s">
         <v>1340</v>
       </c>
@@ -14106,7 +14451,7 @@
         <v>300</v>
       </c>
     </row>
-    <row r="301">
+    <row r="301" hidden="1">
       <c r="A301" s="7" t="s">
         <v>1340</v>
       </c>
@@ -14133,7 +14478,7 @@
         <v>301</v>
       </c>
     </row>
-    <row r="302">
+    <row r="302" hidden="1">
       <c r="A302" s="4" t="s">
         <v>1340</v>
       </c>
@@ -14160,7 +14505,7 @@
         <v>302</v>
       </c>
     </row>
-    <row r="303">
+    <row r="303" hidden="1">
       <c r="A303" s="7" t="s">
         <v>1340</v>
       </c>
@@ -14187,7 +14532,7 @@
         <v>303</v>
       </c>
     </row>
-    <row r="304">
+    <row r="304" hidden="1">
       <c r="A304" s="4" t="s">
         <v>1340</v>
       </c>
@@ -14214,7 +14559,7 @@
         <v>304</v>
       </c>
     </row>
-    <row r="305">
+    <row r="305" hidden="1">
       <c r="A305" s="7" t="s">
         <v>1340</v>
       </c>
@@ -14241,7 +14586,7 @@
         <v>305</v>
       </c>
     </row>
-    <row r="306">
+    <row r="306" hidden="1">
       <c r="A306" s="4" t="s">
         <v>1340</v>
       </c>
@@ -14268,7 +14613,7 @@
         <v>306</v>
       </c>
     </row>
-    <row r="307">
+    <row r="307" hidden="1">
       <c r="A307" s="7" t="s">
         <v>1340</v>
       </c>
@@ -14295,7 +14640,7 @@
         <v>307</v>
       </c>
     </row>
-    <row r="308">
+    <row r="308" hidden="1">
       <c r="A308" s="4" t="s">
         <v>1340</v>
       </c>
@@ -14322,7 +14667,7 @@
         <v>308</v>
       </c>
     </row>
-    <row r="309">
+    <row r="309" hidden="1">
       <c r="A309" s="7" t="s">
         <v>1340</v>
       </c>
@@ -14349,7 +14694,7 @@
         <v>309</v>
       </c>
     </row>
-    <row r="310">
+    <row r="310" hidden="1">
       <c r="A310" s="4" t="s">
         <v>1340</v>
       </c>
@@ -14376,7 +14721,7 @@
         <v>310</v>
       </c>
     </row>
-    <row r="311">
+    <row r="311" hidden="1">
       <c r="A311" s="7" t="s">
         <v>1340</v>
       </c>
@@ -14403,7 +14748,7 @@
         <v>311</v>
       </c>
     </row>
-    <row r="312">
+    <row r="312" hidden="1">
       <c r="A312" s="4" t="s">
         <v>1340</v>
       </c>
@@ -14430,7 +14775,7 @@
         <v>312</v>
       </c>
     </row>
-    <row r="313">
+    <row r="313" hidden="1">
       <c r="A313" s="7" t="s">
         <v>1340</v>
       </c>
@@ -14457,7 +14802,7 @@
         <v>313</v>
       </c>
     </row>
-    <row r="314">
+    <row r="314" hidden="1">
       <c r="A314" s="4" t="s">
         <v>1340</v>
       </c>
@@ -14484,7 +14829,7 @@
         <v>314</v>
       </c>
     </row>
-    <row r="315">
+    <row r="315" hidden="1">
       <c r="A315" s="7" t="s">
         <v>1340</v>
       </c>
@@ -14511,7 +14856,7 @@
         <v>315</v>
       </c>
     </row>
-    <row r="316">
+    <row r="316" hidden="1">
       <c r="A316" s="4" t="s">
         <v>1340</v>
       </c>
@@ -14538,7 +14883,7 @@
         <v>316</v>
       </c>
     </row>
-    <row r="317">
+    <row r="317" hidden="1">
       <c r="A317" s="7" t="s">
         <v>1340</v>
       </c>
@@ -14565,7 +14910,7 @@
         <v>317</v>
       </c>
     </row>
-    <row r="318">
+    <row r="318" hidden="1">
       <c r="A318" s="4" t="s">
         <v>1340</v>
       </c>
@@ -14592,7 +14937,7 @@
         <v>318</v>
       </c>
     </row>
-    <row r="319">
+    <row r="319" hidden="1">
       <c r="A319" s="7" t="s">
         <v>1340</v>
       </c>
@@ -14619,7 +14964,7 @@
         <v>319</v>
       </c>
     </row>
-    <row r="320">
+    <row r="320" hidden="1">
       <c r="A320" s="4" t="s">
         <v>1340</v>
       </c>
@@ -14646,7 +14991,7 @@
         <v>320</v>
       </c>
     </row>
-    <row r="321">
+    <row r="321" hidden="1">
       <c r="A321" s="7" t="s">
         <v>1340</v>
       </c>
@@ -14673,7 +15018,7 @@
         <v>321</v>
       </c>
     </row>
-    <row r="322">
+    <row r="322" hidden="1">
       <c r="A322" s="4" t="s">
         <v>1340</v>
       </c>
@@ -14700,7 +15045,7 @@
         <v>322</v>
       </c>
     </row>
-    <row r="323">
+    <row r="323" hidden="1">
       <c r="A323" s="7" t="s">
         <v>1340</v>
       </c>
@@ -14727,7 +15072,7 @@
         <v>323</v>
       </c>
     </row>
-    <row r="324">
+    <row r="324" hidden="1">
       <c r="A324" s="4" t="s">
         <v>1340</v>
       </c>
@@ -14754,7 +15099,7 @@
         <v>324</v>
       </c>
     </row>
-    <row r="325">
+    <row r="325" hidden="1">
       <c r="A325" s="7" t="s">
         <v>1340</v>
       </c>
@@ -14781,7 +15126,7 @@
         <v>325</v>
       </c>
     </row>
-    <row r="326">
+    <row r="326" hidden="1">
       <c r="A326" s="4" t="s">
         <v>1340</v>
       </c>
@@ -14808,7 +15153,7 @@
         <v>326</v>
       </c>
     </row>
-    <row r="327">
+    <row r="327" hidden="1">
       <c r="A327" s="7" t="s">
         <v>1340</v>
       </c>
@@ -14835,7 +15180,7 @@
         <v>327</v>
       </c>
     </row>
-    <row r="328">
+    <row r="328" hidden="1">
       <c r="A328" s="4" t="s">
         <v>1340</v>
       </c>
@@ -14862,7 +15207,7 @@
         <v>328</v>
       </c>
     </row>
-    <row r="329">
+    <row r="329" hidden="1">
       <c r="A329" s="7" t="s">
         <v>1340</v>
       </c>
@@ -14889,7 +15234,7 @@
         <v>329</v>
       </c>
     </row>
-    <row r="330">
+    <row r="330" hidden="1">
       <c r="A330" s="4" t="s">
         <v>1340</v>
       </c>
@@ -14916,7 +15261,7 @@
         <v>330</v>
       </c>
     </row>
-    <row r="331">
+    <row r="331" hidden="1">
       <c r="A331" s="7" t="s">
         <v>1340</v>
       </c>
@@ -14943,7 +15288,7 @@
         <v>331</v>
       </c>
     </row>
-    <row r="332">
+    <row r="332" hidden="1">
       <c r="A332" s="4" t="s">
         <v>1340</v>
       </c>
@@ -14970,7 +15315,7 @@
         <v>332</v>
       </c>
     </row>
-    <row r="333">
+    <row r="333" hidden="1">
       <c r="A333" s="7" t="s">
         <v>1340</v>
       </c>
@@ -14997,7 +15342,7 @@
         <v>333</v>
       </c>
     </row>
-    <row r="334">
+    <row r="334" hidden="1">
       <c r="A334" s="4" t="s">
         <v>1340</v>
       </c>
@@ -15024,7 +15369,7 @@
         <v>334</v>
       </c>
     </row>
-    <row r="335">
+    <row r="335" hidden="1">
       <c r="A335" s="7" t="s">
         <v>1340</v>
       </c>
@@ -15051,7 +15396,7 @@
         <v>335</v>
       </c>
     </row>
-    <row r="336">
+    <row r="336" hidden="1">
       <c r="A336" s="4" t="s">
         <v>1340</v>
       </c>
@@ -15078,7 +15423,7 @@
         <v>336</v>
       </c>
     </row>
-    <row r="337">
+    <row r="337" hidden="1">
       <c r="A337" s="7" t="s">
         <v>1340</v>
       </c>
@@ -15105,7 +15450,7 @@
         <v>337</v>
       </c>
     </row>
-    <row r="338">
+    <row r="338" hidden="1">
       <c r="A338" s="4" t="s">
         <v>1340</v>
       </c>
@@ -15132,7 +15477,7 @@
         <v>338</v>
       </c>
     </row>
-    <row r="339">
+    <row r="339" hidden="1">
       <c r="A339" s="7" t="s">
         <v>1340</v>
       </c>
@@ -15159,7 +15504,7 @@
         <v>339</v>
       </c>
     </row>
-    <row r="340">
+    <row r="340" hidden="1">
       <c r="A340" s="4" t="s">
         <v>1340</v>
       </c>
@@ -15186,7 +15531,7 @@
         <v>340</v>
       </c>
     </row>
-    <row r="341">
+    <row r="341" hidden="1">
       <c r="A341" s="7" t="s">
         <v>1340</v>
       </c>
@@ -15213,7 +15558,7 @@
         <v>341</v>
       </c>
     </row>
-    <row r="342">
+    <row r="342" hidden="1">
       <c r="A342" s="4" t="s">
         <v>1340</v>
       </c>
@@ -15240,7 +15585,7 @@
         <v>342</v>
       </c>
     </row>
-    <row r="343">
+    <row r="343" hidden="1">
       <c r="A343" s="7" t="s">
         <v>1340</v>
       </c>
@@ -15267,7 +15612,7 @@
         <v>343</v>
       </c>
     </row>
-    <row r="344">
+    <row r="344" hidden="1">
       <c r="A344" s="4" t="s">
         <v>1340</v>
       </c>
@@ -15294,7 +15639,7 @@
         <v>344</v>
       </c>
     </row>
-    <row r="345">
+    <row r="345" hidden="1">
       <c r="A345" s="7" t="s">
         <v>1340</v>
       </c>
@@ -15321,7 +15666,7 @@
         <v>345</v>
       </c>
     </row>
-    <row r="346">
+    <row r="346" hidden="1">
       <c r="A346" s="4" t="s">
         <v>1340</v>
       </c>
@@ -15348,7 +15693,7 @@
         <v>346</v>
       </c>
     </row>
-    <row r="347">
+    <row r="347" hidden="1">
       <c r="A347" s="7" t="s">
         <v>1340</v>
       </c>
@@ -15375,7 +15720,7 @@
         <v>347</v>
       </c>
     </row>
-    <row r="348">
+    <row r="348" hidden="1">
       <c r="A348" s="4" t="s">
         <v>1340</v>
       </c>
@@ -15402,7 +15747,7 @@
         <v>348</v>
       </c>
     </row>
-    <row r="349">
+    <row r="349" hidden="1">
       <c r="A349" s="7" t="s">
         <v>1340</v>
       </c>
@@ -15429,7 +15774,7 @@
         <v>349</v>
       </c>
     </row>
-    <row r="350">
+    <row r="350" hidden="1">
       <c r="A350" s="4" t="s">
         <v>1340</v>
       </c>
@@ -15456,7 +15801,7 @@
         <v>350</v>
       </c>
     </row>
-    <row r="351">
+    <row r="351" hidden="1">
       <c r="A351" s="7" t="s">
         <v>1340</v>
       </c>
@@ -15483,7 +15828,7 @@
         <v>351</v>
       </c>
     </row>
-    <row r="352">
+    <row r="352" hidden="1">
       <c r="A352" s="4" t="s">
         <v>1340</v>
       </c>
@@ -15510,7 +15855,7 @@
         <v>352</v>
       </c>
     </row>
-    <row r="353">
+    <row r="353" hidden="1">
       <c r="A353" s="7" t="s">
         <v>1340</v>
       </c>
@@ -15537,7 +15882,7 @@
         <v>353</v>
       </c>
     </row>
-    <row r="354">
+    <row r="354" hidden="1">
       <c r="A354" s="4" t="s">
         <v>1340</v>
       </c>
@@ -15564,7 +15909,7 @@
         <v>354</v>
       </c>
     </row>
-    <row r="355">
+    <row r="355" hidden="1">
       <c r="A355" s="7" t="s">
         <v>1340</v>
       </c>
@@ -15591,7 +15936,7 @@
         <v>355</v>
       </c>
     </row>
-    <row r="356">
+    <row r="356" hidden="1">
       <c r="A356" s="4" t="s">
         <v>1340</v>
       </c>
@@ -15618,7 +15963,7 @@
         <v>356</v>
       </c>
     </row>
-    <row r="357">
+    <row r="357" hidden="1">
       <c r="A357" s="7" t="s">
         <v>1340</v>
       </c>
@@ -15645,7 +15990,7 @@
         <v>357</v>
       </c>
     </row>
-    <row r="358">
+    <row r="358" hidden="1">
       <c r="A358" s="4" t="s">
         <v>1340</v>
       </c>
@@ -15672,7 +16017,7 @@
         <v>358</v>
       </c>
     </row>
-    <row r="359">
+    <row r="359" hidden="1">
       <c r="A359" s="7" t="s">
         <v>1340</v>
       </c>
@@ -15699,7 +16044,7 @@
         <v>359</v>
       </c>
     </row>
-    <row r="360">
+    <row r="360" hidden="1">
       <c r="A360" s="4" t="s">
         <v>1340</v>
       </c>
@@ -15726,7 +16071,7 @@
         <v>360</v>
       </c>
     </row>
-    <row r="361">
+    <row r="361" hidden="1">
       <c r="A361" s="7" t="s">
         <v>1340</v>
       </c>
@@ -15753,7 +16098,7 @@
         <v>361</v>
       </c>
     </row>
-    <row r="362">
+    <row r="362" hidden="1">
       <c r="A362" s="4" t="s">
         <v>1340</v>
       </c>
@@ -15780,7 +16125,7 @@
         <v>362</v>
       </c>
     </row>
-    <row r="363">
+    <row r="363" hidden="1">
       <c r="A363" s="7" t="s">
         <v>1340</v>
       </c>
@@ -15807,7 +16152,7 @@
         <v>363</v>
       </c>
     </row>
-    <row r="364">
+    <row r="364" hidden="1">
       <c r="A364" s="4" t="s">
         <v>1340</v>
       </c>
@@ -15834,7 +16179,7 @@
         <v>364</v>
       </c>
     </row>
-    <row r="365">
+    <row r="365" hidden="1">
       <c r="A365" s="7" t="s">
         <v>1340</v>
       </c>
@@ -15861,7 +16206,7 @@
         <v>365</v>
       </c>
     </row>
-    <row r="366">
+    <row r="366" hidden="1">
       <c r="A366" s="4" t="s">
         <v>1340</v>
       </c>
@@ -15888,7 +16233,7 @@
         <v>366</v>
       </c>
     </row>
-    <row r="367">
+    <row r="367" hidden="1">
       <c r="A367" s="7" t="s">
         <v>1340</v>
       </c>
@@ -15915,7 +16260,7 @@
         <v>367</v>
       </c>
     </row>
-    <row r="368">
+    <row r="368" hidden="1">
       <c r="A368" s="4" t="s">
         <v>1340</v>
       </c>
@@ -15942,7 +16287,7 @@
         <v>368</v>
       </c>
     </row>
-    <row r="369">
+    <row r="369" hidden="1">
       <c r="A369" s="7" t="s">
         <v>1340</v>
       </c>
@@ -15969,7 +16314,7 @@
         <v>369</v>
       </c>
     </row>
-    <row r="370">
+    <row r="370" hidden="1">
       <c r="A370" s="4" t="s">
         <v>1340</v>
       </c>
@@ -15996,7 +16341,7 @@
         <v>370</v>
       </c>
     </row>
-    <row r="371">
+    <row r="371" hidden="1">
       <c r="A371" s="7" t="s">
         <v>1340</v>
       </c>
@@ -16023,7 +16368,7 @@
         <v>371</v>
       </c>
     </row>
-    <row r="372">
+    <row r="372" hidden="1">
       <c r="A372" s="4" t="s">
         <v>1340</v>
       </c>
@@ -16050,7 +16395,7 @@
         <v>372</v>
       </c>
     </row>
-    <row r="373">
+    <row r="373" hidden="1">
       <c r="A373" s="7" t="s">
         <v>1340</v>
       </c>
@@ -16077,7 +16422,7 @@
         <v>373</v>
       </c>
     </row>
-    <row r="374">
+    <row r="374" hidden="1">
       <c r="A374" s="4" t="s">
         <v>1340</v>
       </c>
@@ -16104,7 +16449,7 @@
         <v>374</v>
       </c>
     </row>
-    <row r="375">
+    <row r="375" hidden="1">
       <c r="A375" s="7" t="s">
         <v>1340</v>
       </c>
@@ -16131,7 +16476,7 @@
         <v>375</v>
       </c>
     </row>
-    <row r="376">
+    <row r="376" hidden="1">
       <c r="A376" s="20" t="s">
         <v>1340</v>
       </c>
@@ -16158,7 +16503,7 @@
         <v>376</v>
       </c>
     </row>
-    <row r="377">
+    <row r="377" hidden="1">
       <c r="A377" s="23" t="s">
         <v>1340</v>
       </c>
@@ -16185,7 +16530,7 @@
         <v>377</v>
       </c>
     </row>
-    <row r="378">
+    <row r="378" hidden="1">
       <c r="A378" s="20" t="s">
         <v>1340</v>
       </c>
@@ -16212,7 +16557,7 @@
         <v>378</v>
       </c>
     </row>
-    <row r="379">
+    <row r="379" hidden="1">
       <c r="A379" s="23" t="s">
         <v>1340</v>
       </c>
@@ -16239,7 +16584,7 @@
         <v>379</v>
       </c>
     </row>
-    <row r="380">
+    <row r="380" hidden="1">
       <c r="A380" s="4" t="s">
         <v>1340</v>
       </c>
@@ -16266,7 +16611,7 @@
         <v>380</v>
       </c>
     </row>
-    <row r="381">
+    <row r="381" hidden="1">
       <c r="A381" s="7" t="s">
         <v>1340</v>
       </c>
@@ -16293,7 +16638,7 @@
         <v>381</v>
       </c>
     </row>
-    <row r="382">
+    <row r="382" hidden="1">
       <c r="A382" s="4" t="s">
         <v>1340</v>
       </c>
@@ -16320,7 +16665,7 @@
         <v>382</v>
       </c>
     </row>
-    <row r="383">
+    <row r="383" hidden="1">
       <c r="A383" s="7" t="s">
         <v>1340</v>
       </c>
@@ -16347,7 +16692,7 @@
         <v>383</v>
       </c>
     </row>
-    <row r="384">
+    <row r="384" hidden="1">
       <c r="A384" s="4" t="s">
         <v>1340</v>
       </c>
@@ -16374,7 +16719,7 @@
         <v>384</v>
       </c>
     </row>
-    <row r="385">
+    <row r="385" hidden="1">
       <c r="A385" s="7" t="s">
         <v>1340</v>
       </c>
@@ -16401,7 +16746,7 @@
         <v>385</v>
       </c>
     </row>
-    <row r="386">
+    <row r="386" hidden="1">
       <c r="A386" s="4" t="s">
         <v>1340</v>
       </c>
@@ -16428,7 +16773,7 @@
         <v>386</v>
       </c>
     </row>
-    <row r="387">
+    <row r="387" hidden="1">
       <c r="A387" s="7" t="s">
         <v>1340</v>
       </c>
@@ -16455,7 +16800,7 @@
         <v>387</v>
       </c>
     </row>
-    <row r="388">
+    <row r="388" hidden="1">
       <c r="A388" s="4" t="s">
         <v>1340</v>
       </c>
@@ -16482,7 +16827,7 @@
         <v>388</v>
       </c>
     </row>
-    <row r="389">
+    <row r="389" hidden="1">
       <c r="A389" s="7" t="s">
         <v>1340</v>
       </c>
@@ -16509,7 +16854,7 @@
         <v>389</v>
       </c>
     </row>
-    <row r="390">
+    <row r="390" hidden="1">
       <c r="A390" s="4" t="s">
         <v>1340</v>
       </c>
@@ -16536,7 +16881,7 @@
         <v>390</v>
       </c>
     </row>
-    <row r="391">
+    <row r="391" hidden="1">
       <c r="A391" s="7" t="s">
         <v>1340</v>
       </c>
@@ -16563,7 +16908,7 @@
         <v>391</v>
       </c>
     </row>
-    <row r="392">
+    <row r="392" hidden="1">
       <c r="A392" s="4" t="s">
         <v>1340</v>
       </c>
@@ -16590,7 +16935,7 @@
         <v>392</v>
       </c>
     </row>
-    <row r="393">
+    <row r="393" hidden="1">
       <c r="A393" s="7" t="s">
         <v>1340</v>
       </c>
@@ -16617,7 +16962,7 @@
         <v>393</v>
       </c>
     </row>
-    <row r="394">
+    <row r="394" hidden="1">
       <c r="A394" s="4" t="s">
         <v>1340</v>
       </c>
@@ -16644,7 +16989,7 @@
         <v>394</v>
       </c>
     </row>
-    <row r="395">
+    <row r="395" hidden="1">
       <c r="A395" s="7" t="s">
         <v>1340</v>
       </c>
@@ -16671,7 +17016,7 @@
         <v>395</v>
       </c>
     </row>
-    <row r="396">
+    <row r="396" hidden="1">
       <c r="A396" s="4" t="s">
         <v>1340</v>
       </c>
@@ -16698,7 +17043,7 @@
         <v>396</v>
       </c>
     </row>
-    <row r="397">
+    <row r="397" hidden="1">
       <c r="A397" s="7" t="s">
         <v>1340</v>
       </c>
@@ -16725,7 +17070,7 @@
         <v>397</v>
       </c>
     </row>
-    <row r="398">
+    <row r="398" hidden="1">
       <c r="A398" s="4" t="s">
         <v>1340</v>
       </c>
@@ -16752,7 +17097,7 @@
         <v>398</v>
       </c>
     </row>
-    <row r="399">
+    <row r="399" hidden="1">
       <c r="A399" s="7" t="s">
         <v>1340</v>
       </c>
@@ -16779,7 +17124,7 @@
         <v>399</v>
       </c>
     </row>
-    <row r="400">
+    <row r="400" hidden="1">
       <c r="A400" s="4" t="s">
         <v>1340</v>
       </c>
@@ -16806,7 +17151,7 @@
         <v>400</v>
       </c>
     </row>
-    <row r="401">
+    <row r="401" hidden="1">
       <c r="A401" s="7" t="s">
         <v>1340</v>
       </c>
@@ -16833,7 +17178,7 @@
         <v>401</v>
       </c>
     </row>
-    <row r="402">
+    <row r="402" hidden="1">
       <c r="A402" s="4" t="s">
         <v>1340</v>
       </c>
@@ -16860,7 +17205,7 @@
         <v>402</v>
       </c>
     </row>
-    <row r="403">
+    <row r="403" hidden="1">
       <c r="A403" s="7" t="s">
         <v>1340</v>
       </c>
@@ -16887,7 +17232,7 @@
         <v>403</v>
       </c>
     </row>
-    <row r="404">
+    <row r="404" hidden="1">
       <c r="A404" s="4" t="s">
         <v>1340</v>
       </c>
@@ -16914,7 +17259,7 @@
         <v>404</v>
       </c>
     </row>
-    <row r="405">
+    <row r="405" hidden="1">
       <c r="A405" s="7" t="s">
         <v>1340</v>
       </c>
@@ -16941,7 +17286,7 @@
         <v>405</v>
       </c>
     </row>
-    <row r="406">
+    <row r="406" hidden="1">
       <c r="A406" s="4" t="s">
         <v>1340</v>
       </c>
@@ -16968,31 +17313,631 @@
         <v>406</v>
       </c>
     </row>
-    <row r="407">
-      <c r="A407" s="27" t="s">
+    <row r="407" hidden="1">
+      <c r="A407" s="7" t="s">
         <v>1340</v>
       </c>
-      <c r="B407" s="28">
+      <c r="B407" s="12">
         <v>4.0</v>
       </c>
-      <c r="C407" s="28" t="s">
+      <c r="C407" s="12" t="s">
         <v>1835</v>
       </c>
-      <c r="D407" s="28" t="s">
+      <c r="D407" s="12" t="s">
         <v>1836</v>
       </c>
-      <c r="E407" s="28" t="s">
+      <c r="E407" s="12" t="s">
         <v>1837</v>
       </c>
-      <c r="F407" s="28" t="s">
+      <c r="F407" s="12" t="s">
         <v>1838</v>
       </c>
-      <c r="G407" s="28" t="s">
+      <c r="G407" s="12" t="s">
         <v>1839</v>
       </c>
-      <c r="H407" s="29">
+      <c r="H407" s="13">
         <f t="shared" si="1"/>
         <v>407</v>
+      </c>
+    </row>
+    <row r="408">
+      <c r="A408" s="20" t="s">
+        <v>1129</v>
+      </c>
+      <c r="B408" s="10"/>
+      <c r="C408" s="10" t="s">
+        <v>1840</v>
+      </c>
+      <c r="D408" s="10" t="s">
+        <v>1841</v>
+      </c>
+      <c r="E408" s="10" t="s">
+        <v>1842</v>
+      </c>
+      <c r="F408" s="10" t="s">
+        <v>1843</v>
+      </c>
+      <c r="G408" s="10" t="s">
+        <v>1844</v>
+      </c>
+      <c r="H408" s="11">
+        <f t="shared" si="1"/>
+        <v>408</v>
+      </c>
+    </row>
+    <row r="409">
+      <c r="A409" s="23" t="s">
+        <v>1129</v>
+      </c>
+      <c r="B409" s="12"/>
+      <c r="C409" s="12" t="s">
+        <v>1845</v>
+      </c>
+      <c r="D409" s="12" t="s">
+        <v>1846</v>
+      </c>
+      <c r="E409" s="12" t="s">
+        <v>1847</v>
+      </c>
+      <c r="F409" s="12" t="s">
+        <v>1848</v>
+      </c>
+      <c r="G409" s="12" t="s">
+        <v>1849</v>
+      </c>
+      <c r="H409" s="13">
+        <f t="shared" si="1"/>
+        <v>409</v>
+      </c>
+    </row>
+    <row r="410">
+      <c r="A410" s="20" t="s">
+        <v>1129</v>
+      </c>
+      <c r="B410" s="10"/>
+      <c r="C410" s="10" t="s">
+        <v>1850</v>
+      </c>
+      <c r="D410" s="10" t="s">
+        <v>1851</v>
+      </c>
+      <c r="E410" s="10" t="s">
+        <v>1852</v>
+      </c>
+      <c r="F410" s="10" t="s">
+        <v>1853</v>
+      </c>
+      <c r="G410" s="10" t="s">
+        <v>1854</v>
+      </c>
+      <c r="H410" s="11">
+        <f t="shared" si="1"/>
+        <v>410</v>
+      </c>
+    </row>
+    <row r="411">
+      <c r="A411" s="23" t="s">
+        <v>1129</v>
+      </c>
+      <c r="B411" s="12"/>
+      <c r="C411" s="12" t="s">
+        <v>1855</v>
+      </c>
+      <c r="D411" s="12" t="s">
+        <v>1856</v>
+      </c>
+      <c r="E411" s="12" t="s">
+        <v>1857</v>
+      </c>
+      <c r="F411" s="12" t="s">
+        <v>1858</v>
+      </c>
+      <c r="G411" s="12" t="s">
+        <v>1859</v>
+      </c>
+      <c r="H411" s="13">
+        <f t="shared" si="1"/>
+        <v>411</v>
+      </c>
+    </row>
+    <row r="412">
+      <c r="A412" s="20" t="s">
+        <v>1129</v>
+      </c>
+      <c r="B412" s="10"/>
+      <c r="C412" s="10" t="s">
+        <v>1860</v>
+      </c>
+      <c r="D412" s="10" t="s">
+        <v>1861</v>
+      </c>
+      <c r="E412" s="10">
+        <v>75.0</v>
+      </c>
+      <c r="F412" s="10" t="s">
+        <v>1862</v>
+      </c>
+      <c r="G412" s="10" t="s">
+        <v>1863</v>
+      </c>
+      <c r="H412" s="11">
+        <f t="shared" si="1"/>
+        <v>412</v>
+      </c>
+    </row>
+    <row r="413">
+      <c r="A413" s="23" t="s">
+        <v>1129</v>
+      </c>
+      <c r="B413" s="12"/>
+      <c r="C413" s="12" t="s">
+        <v>1864</v>
+      </c>
+      <c r="D413" s="12" t="s">
+        <v>1865</v>
+      </c>
+      <c r="E413" s="12" t="s">
+        <v>1866</v>
+      </c>
+      <c r="F413" s="12" t="s">
+        <v>1867</v>
+      </c>
+      <c r="G413" s="12" t="s">
+        <v>1868</v>
+      </c>
+      <c r="H413" s="13">
+        <f t="shared" si="1"/>
+        <v>413</v>
+      </c>
+    </row>
+    <row r="414">
+      <c r="A414" s="20" t="s">
+        <v>1869</v>
+      </c>
+      <c r="B414" s="10"/>
+      <c r="C414" s="10" t="s">
+        <v>1870</v>
+      </c>
+      <c r="D414" s="5" t="s">
+        <v>1871</v>
+      </c>
+      <c r="E414" s="10" t="s">
+        <v>1872</v>
+      </c>
+      <c r="F414" s="10" t="s">
+        <v>1873</v>
+      </c>
+      <c r="G414" s="10" t="s">
+        <v>1874</v>
+      </c>
+      <c r="H414" s="11">
+        <f t="shared" si="1"/>
+        <v>414</v>
+      </c>
+    </row>
+    <row r="415">
+      <c r="A415" s="23" t="s">
+        <v>1129</v>
+      </c>
+      <c r="B415" s="12"/>
+      <c r="C415" s="12" t="s">
+        <v>1875</v>
+      </c>
+      <c r="D415" s="8" t="s">
+        <v>1876</v>
+      </c>
+      <c r="E415" s="8" t="s">
+        <v>1877</v>
+      </c>
+      <c r="F415" s="8" t="s">
+        <v>1878</v>
+      </c>
+      <c r="G415" s="8" t="s">
+        <v>1879</v>
+      </c>
+      <c r="H415" s="13">
+        <f t="shared" si="1"/>
+        <v>415</v>
+      </c>
+    </row>
+    <row r="416">
+      <c r="A416" s="20" t="s">
+        <v>1129</v>
+      </c>
+      <c r="B416" s="10"/>
+      <c r="C416" s="10" t="s">
+        <v>1880</v>
+      </c>
+      <c r="D416" s="10" t="s">
+        <v>1881</v>
+      </c>
+      <c r="E416" s="10" t="s">
+        <v>1882</v>
+      </c>
+      <c r="F416" s="10" t="s">
+        <v>1883</v>
+      </c>
+      <c r="G416" s="10" t="s">
+        <v>1884</v>
+      </c>
+      <c r="H416" s="11">
+        <f t="shared" si="1"/>
+        <v>416</v>
+      </c>
+    </row>
+    <row r="417">
+      <c r="A417" s="23" t="s">
+        <v>1129</v>
+      </c>
+      <c r="B417" s="12"/>
+      <c r="C417" s="12" t="s">
+        <v>1885</v>
+      </c>
+      <c r="D417" s="12" t="s">
+        <v>1886</v>
+      </c>
+      <c r="E417" s="12" t="s">
+        <v>1887</v>
+      </c>
+      <c r="F417" s="12" t="s">
+        <v>1888</v>
+      </c>
+      <c r="G417" s="12" t="s">
+        <v>1889</v>
+      </c>
+      <c r="H417" s="13">
+        <f t="shared" si="1"/>
+        <v>417</v>
+      </c>
+    </row>
+    <row r="418">
+      <c r="A418" s="20" t="s">
+        <v>1129</v>
+      </c>
+      <c r="B418" s="10"/>
+      <c r="C418" s="10" t="s">
+        <v>1890</v>
+      </c>
+      <c r="D418" s="10" t="s">
+        <v>1891</v>
+      </c>
+      <c r="E418" s="10" t="s">
+        <v>1892</v>
+      </c>
+      <c r="F418" s="10" t="s">
+        <v>1893</v>
+      </c>
+      <c r="G418" s="10" t="s">
+        <v>1894</v>
+      </c>
+      <c r="H418" s="11">
+        <f t="shared" si="1"/>
+        <v>418</v>
+      </c>
+    </row>
+    <row r="419">
+      <c r="A419" s="23" t="s">
+        <v>1129</v>
+      </c>
+      <c r="B419" s="12"/>
+      <c r="C419" s="12" t="s">
+        <v>1895</v>
+      </c>
+      <c r="D419" s="12" t="s">
+        <v>1896</v>
+      </c>
+      <c r="E419" s="12" t="s">
+        <v>1897</v>
+      </c>
+      <c r="F419" s="12" t="s">
+        <v>1898</v>
+      </c>
+      <c r="G419" s="12" t="s">
+        <v>1899</v>
+      </c>
+      <c r="H419" s="13">
+        <f t="shared" si="1"/>
+        <v>419</v>
+      </c>
+    </row>
+    <row r="420">
+      <c r="A420" s="20" t="s">
+        <v>1129</v>
+      </c>
+      <c r="B420" s="10"/>
+      <c r="C420" s="10" t="s">
+        <v>1900</v>
+      </c>
+      <c r="D420" s="10" t="s">
+        <v>1901</v>
+      </c>
+      <c r="E420" s="10" t="s">
+        <v>1902</v>
+      </c>
+      <c r="F420" s="10" t="s">
+        <v>1903</v>
+      </c>
+      <c r="G420" s="10" t="s">
+        <v>1904</v>
+      </c>
+      <c r="H420" s="11">
+        <f t="shared" si="1"/>
+        <v>420</v>
+      </c>
+    </row>
+    <row r="421">
+      <c r="A421" s="23" t="s">
+        <v>1129</v>
+      </c>
+      <c r="B421" s="12"/>
+      <c r="C421" s="12" t="s">
+        <v>1905</v>
+      </c>
+      <c r="D421" s="8" t="s">
+        <v>1906</v>
+      </c>
+      <c r="E421" s="12" t="s">
+        <v>1907</v>
+      </c>
+      <c r="F421" s="8" t="s">
+        <v>1908</v>
+      </c>
+      <c r="G421" s="8" t="s">
+        <v>1909</v>
+      </c>
+      <c r="H421" s="13">
+        <f t="shared" si="1"/>
+        <v>421</v>
+      </c>
+    </row>
+    <row r="422">
+      <c r="A422" s="20" t="s">
+        <v>1129</v>
+      </c>
+      <c r="B422" s="10"/>
+      <c r="C422" s="10" t="s">
+        <v>1910</v>
+      </c>
+      <c r="D422" s="10" t="s">
+        <v>1911</v>
+      </c>
+      <c r="E422" s="10" t="s">
+        <v>1912</v>
+      </c>
+      <c r="F422" s="10" t="s">
+        <v>1913</v>
+      </c>
+      <c r="G422" s="10" t="s">
+        <v>1914</v>
+      </c>
+      <c r="H422" s="11">
+        <f t="shared" si="1"/>
+        <v>422</v>
+      </c>
+    </row>
+    <row r="423">
+      <c r="A423" s="23" t="s">
+        <v>1129</v>
+      </c>
+      <c r="B423" s="12"/>
+      <c r="C423" s="12" t="s">
+        <v>1915</v>
+      </c>
+      <c r="D423" s="12" t="s">
+        <v>1916</v>
+      </c>
+      <c r="E423" s="12" t="s">
+        <v>1917</v>
+      </c>
+      <c r="F423" s="12" t="s">
+        <v>1918</v>
+      </c>
+      <c r="G423" s="12" t="s">
+        <v>1919</v>
+      </c>
+      <c r="H423" s="13">
+        <f t="shared" si="1"/>
+        <v>423</v>
+      </c>
+    </row>
+    <row r="424">
+      <c r="A424" s="20" t="s">
+        <v>1129</v>
+      </c>
+      <c r="B424" s="10"/>
+      <c r="C424" s="10" t="s">
+        <v>1920</v>
+      </c>
+      <c r="D424" s="10" t="s">
+        <v>1921</v>
+      </c>
+      <c r="E424" s="10" t="s">
+        <v>1922</v>
+      </c>
+      <c r="F424" s="10" t="s">
+        <v>1923</v>
+      </c>
+      <c r="G424" s="10" t="s">
+        <v>1924</v>
+      </c>
+      <c r="H424" s="11">
+        <f t="shared" si="1"/>
+        <v>424</v>
+      </c>
+    </row>
+    <row r="425">
+      <c r="A425" s="23" t="s">
+        <v>1129</v>
+      </c>
+      <c r="B425" s="12"/>
+      <c r="C425" s="12" t="s">
+        <v>1925</v>
+      </c>
+      <c r="D425" s="12" t="s">
+        <v>1926</v>
+      </c>
+      <c r="E425" s="12" t="s">
+        <v>1927</v>
+      </c>
+      <c r="F425" s="12" t="s">
+        <v>1928</v>
+      </c>
+      <c r="G425" s="12" t="s">
+        <v>1929</v>
+      </c>
+      <c r="H425" s="13">
+        <f t="shared" si="1"/>
+        <v>425</v>
+      </c>
+    </row>
+    <row r="426">
+      <c r="A426" s="20" t="s">
+        <v>1129</v>
+      </c>
+      <c r="B426" s="10"/>
+      <c r="C426" s="10" t="s">
+        <v>1930</v>
+      </c>
+      <c r="D426" s="10" t="s">
+        <v>1931</v>
+      </c>
+      <c r="E426" s="10" t="s">
+        <v>1932</v>
+      </c>
+      <c r="F426" s="10" t="s">
+        <v>1933</v>
+      </c>
+      <c r="G426" s="10" t="s">
+        <v>1934</v>
+      </c>
+      <c r="H426" s="11">
+        <f t="shared" si="1"/>
+        <v>426</v>
+      </c>
+    </row>
+    <row r="427">
+      <c r="A427" s="23" t="s">
+        <v>1129</v>
+      </c>
+      <c r="B427" s="12"/>
+      <c r="C427" s="12" t="s">
+        <v>1935</v>
+      </c>
+      <c r="D427" s="12" t="s">
+        <v>1936</v>
+      </c>
+      <c r="E427" s="12" t="s">
+        <v>1937</v>
+      </c>
+      <c r="F427" s="12" t="s">
+        <v>1938</v>
+      </c>
+      <c r="G427" s="12" t="s">
+        <v>1939</v>
+      </c>
+      <c r="H427" s="13">
+        <f t="shared" si="1"/>
+        <v>427</v>
+      </c>
+    </row>
+    <row r="428">
+      <c r="A428" s="20" t="s">
+        <v>1129</v>
+      </c>
+      <c r="B428" s="10"/>
+      <c r="C428" s="10" t="s">
+        <v>1940</v>
+      </c>
+      <c r="D428" s="27">
+        <v>45659.0</v>
+      </c>
+      <c r="E428" s="10" t="s">
+        <v>1941</v>
+      </c>
+      <c r="F428" s="27">
+        <v>45691.0</v>
+      </c>
+      <c r="G428" s="27">
+        <v>45660.0</v>
+      </c>
+      <c r="H428" s="11">
+        <f t="shared" si="1"/>
+        <v>428</v>
+      </c>
+    </row>
+    <row r="429">
+      <c r="A429" s="23" t="s">
+        <v>1129</v>
+      </c>
+      <c r="B429" s="12"/>
+      <c r="C429" s="12" t="s">
+        <v>1942</v>
+      </c>
+      <c r="D429" s="12" t="s">
+        <v>1943</v>
+      </c>
+      <c r="E429" s="12" t="s">
+        <v>1944</v>
+      </c>
+      <c r="F429" s="12" t="s">
+        <v>1945</v>
+      </c>
+      <c r="G429" s="12" t="s">
+        <v>1946</v>
+      </c>
+      <c r="H429" s="13">
+        <f t="shared" si="1"/>
+        <v>429</v>
+      </c>
+    </row>
+    <row r="430">
+      <c r="A430" s="20" t="s">
+        <v>1129</v>
+      </c>
+      <c r="B430" s="10"/>
+      <c r="C430" s="10" t="s">
+        <v>1947</v>
+      </c>
+      <c r="D430" s="10" t="s">
+        <v>1948</v>
+      </c>
+      <c r="E430" s="10" t="s">
+        <v>1949</v>
+      </c>
+      <c r="F430" s="10" t="s">
+        <v>1950</v>
+      </c>
+      <c r="G430" s="10" t="s">
+        <v>1951</v>
+      </c>
+      <c r="H430" s="11">
+        <f t="shared" si="1"/>
+        <v>430</v>
+      </c>
+    </row>
+    <row r="431">
+      <c r="A431" s="28" t="s">
+        <v>1129</v>
+      </c>
+      <c r="B431" s="29"/>
+      <c r="C431" s="29" t="s">
+        <v>1952</v>
+      </c>
+      <c r="D431" s="29" t="s">
+        <v>1953</v>
+      </c>
+      <c r="E431" s="29" t="s">
+        <v>1954</v>
+      </c>
+      <c r="F431" s="29" t="s">
+        <v>1955</v>
+      </c>
+      <c r="G431" s="29" t="s">
+        <v>1956</v>
+      </c>
+      <c r="H431" s="30">
+        <f t="shared" si="1"/>
+        <v>431</v>
       </c>
     </row>
   </sheetData>

</xml_diff>